<commit_message>
fixed date_processor() in link_preprocesso.py
</commit_message>
<xml_diff>
--- a/AMS.xlsx
+++ b/AMS.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20224703\Documents\GitHub\DLL_Risk_Analysis\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F37A23-105A-4260-8E34-137A7CAFB030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="262">
   <si>
     <t>URL</t>
   </si>
@@ -55,40 +49,31 @@
     <t>https://strukton.maglr.nl/strukton-s-world-q1-2020-eng/allright</t>
   </si>
   <si>
+    <t>https://www.businessradar.com/company/63f72-nl-shv-nederland-bv/scandal/</t>
+  </si>
+  <si>
     <t>https://pledgetimes.com/controversial-gerard-sanderink-returns-as-director-at-strukton/</t>
   </si>
   <si>
-    <t>https://businessradar.com/company/6d56c-nl-strukton-international-bv/crisis/</t>
-  </si>
-  <si>
     <t>https://www.dutchnews.nl/news/2019/03/strukton-investigated-for-corruption-in-saudi-metro-deal/</t>
   </si>
   <si>
     <t>https://www.reuters.com/article/us-dutch-canals-idUKL2920999420080130</t>
   </si>
   <si>
-    <t>https://www.digitaljournal.com/pr/tamping-machine-market-to-discern-magnified-growth-during-2027</t>
+    <t>https://www.eco-business.com/news/indonesia-to-build-worlds-largest-tidal-power-plant/</t>
   </si>
   <si>
     <t>https://indianexpress.com/article/cities/mumbai/mumbai-inductor-delay-holds-up-trials-of-ac-rakes-2994807/</t>
   </si>
   <si>
-    <t>https://www.eco-business.com/news/indonesia-to-build-worlds-largest-tidal-power-plant/</t>
-  </si>
-  <si>
-    <t>https://www.dailymail.co.uk/sciencetech/article-2860418/End-line-autumn-train-delays-Dutch-begin-trials-zap-leaf-litter-tracks-LASERS.html</t>
-  </si>
-  <si>
     <t>https://www.waterkant.net/suriname/2014/11/07/vanaf-12-november-weer-ambassadeur-nederland-in-suriname/</t>
   </si>
   <si>
     <t>https://www.waterkant.net/suriname/2014/08/28/bouterse-blij-als-een-kind-om-energiebesparing/</t>
   </si>
   <si>
-    <t>https://www.ruetir.com/2022/11/03/enterprise-chamber-refuses-to-give-centric-ceo-sanderink-his-support/</t>
-  </si>
-  <si>
-    <t>https://www.ruetir.com/2022/10/24/om-takes-next-step-to-depose-sanderink/</t>
+    <t>https://www.ruetir.com/2022/11/02/will-gerard-sanderink-be-forced-to-resign-from-centric/</t>
   </si>
   <si>
     <t>https://struktonciviel.nl/project/2020/07/grond-en-grondwatersanering-voormalig-drugslab-gemeente-horst-aan-de-maas/</t>
@@ -103,10 +88,13 @@
     <t>https://pages.facebook.com/382663555435193/photos/a.382681052100110/1027158144319061/?type=3</t>
   </si>
   <si>
+    <t>https://www.globalconstructionreview.com/dutch-authorities-raid-strukton-suspicion-bribery/</t>
+  </si>
+  <si>
     <t>https://kokmilieu.nl/projecten/107/vier_k40_ibc_2c_fireguards_voor_strukton_milieutechniek</t>
   </si>
   <si>
-    <t>https://www.globalconstructionreview.com/dutch-authorities-raid-strukton-suspicion-bribery/</t>
+    <t>https://www.rtlnieuws.nl/economie/artikel/5341421/gerard-sanderink-ceo-centric-topman-strukton-rian-van-rijbroek</t>
   </si>
   <si>
     <t>https://menafn.com/1105203187/Railway-Maintenance-Machinery-Market-Growth-Global-Survey-Segments-Industry-Status-And-Forecast-2022-2027</t>
@@ -121,6 +109,9 @@
     <t>https://www.omroepbrabant.nl/nieuws/4169408/toon-francken-90-niet-geholpen-als-rijk-opruimen-drugsafval-betaalt</t>
   </si>
   <si>
+    <t>https://www.noordhollandsdagblad.nl/cnt/dmf20220203_24292664</t>
+  </si>
+  <si>
     <t>https://www.omroepbrabant.nl/nieuws/2971372/opruimen-1600-liter-drugsafval-in-eindhoven-flinke-klus-politie-zoekt-witte-bakwagen</t>
   </si>
   <si>
@@ -133,39 +124,33 @@
     <t>https://www.emerce.nl/nieuws/ban-via-rian-podcast-bizarre-bedrijfssoap</t>
   </si>
   <si>
-    <t>https://flevopost.nl/dronten/Muurschildering-De-Binding-oogst-waardering-27555565.html</t>
-  </si>
-  <si>
     <t>https://m.engineeringnews.co.za/article/dutch-solar-road-proves-successful-moves-on-to-heavy-traffic-road-trial-2018-10-19/rep_id:4433</t>
   </si>
   <si>
     <t>https://www.openpr.com/news/925553/global-railway-maintenance-machinery-market-2018-harsco-speno-strukton-vortok-international-plasser-theurer.html</t>
   </si>
   <si>
-    <t>https://www.ruetir.com/2022/11/02/will-gerard-sanderink-be-forced-to-resign-from-centric/</t>
-  </si>
-  <si>
     <t>https://www.lifegate.com/larantuka-straits-tidal-power-indonesia</t>
   </si>
   <si>
-    <t>https://www.progressiverailroading.com/internet-digital/article/University-of-Delawares-Big-Data-conference-explored-analytics-trends-in-a-rail-context--59675</t>
-  </si>
-  <si>
     <t>https://www.railjournal.com/regions/europe/get-set-for-innotrans-2016/</t>
   </si>
   <si>
     <t>https://www.cleantech.com/turning-tide-for-ocean-power-is-marine-energy-coming-of-age/</t>
   </si>
   <si>
-    <t>https://www.byggnadsarbetaren.se/flest-anstallda-30-storsta-bygg%C2%ADforetagen-i-sverige-2021/</t>
-  </si>
-  <si>
-    <t>https://www.emerce.nl/wire/studententeam-delft-hyperloop-onthult-nieuwe-hyperloop-capsule-atlas-02</t>
-  </si>
-  <si>
     <t>https://www.railtechnologymagazine.com/Rail-News/why-not-do-some-re-engineering-adrian-shooter-on-the-vivarail-d-train</t>
   </si>
   <si>
+    <t>https://www.nwboomerandseniornews.com/uncategorized/2022/on-board-systems-professional-market-2028-key-insights-and-leading-players-deuta-werke-gmbh-hubersuhner-strukton-rail-abb-knorr-bremse-ag-caf-group-etc/</t>
+  </si>
+  <si>
+    <t>https://www.ruetir.com/2022/10/22/who-is-gerard-sanderink-and-why-is-justice-demanding-his-resignation-from-centric/</t>
+  </si>
+  <si>
+    <t>https://112doetinchem.nl/page/nieuwsdetail/52747/tevreden-gezichten-bij-provinciale-brandweerwedstrijden-in-zutphen</t>
+  </si>
+  <si>
     <t>https://strukton.com/about-us/integrity/</t>
   </si>
   <si>
@@ -184,37 +169,49 @@
     <t>https://struktonciviel.nl/betonbouw/betonrenovatie/</t>
   </si>
   <si>
-    <t>https://www.nu.nl/economie/6225849/strukton-topman-sanderink-verdacht-van-omkoping-in-saoedi-arabie.html</t>
-  </si>
-  <si>
     <t>https://www.prorail.nl/nieuws/langdurig-geen-treinverkeer-flevoland</t>
   </si>
   <si>
-    <t>https://www.treinenweb.nl/nieuws/9594/mogelijk-wekenlang-geen-treinen-tussen-lelystad-en-zwolle-na-kortsluiting.html</t>
-  </si>
-  <si>
     <t>https://www.prorail.nl/nieuws/trein-in-botsing-met-lege-stadsbus</t>
   </si>
   <si>
-    <t>https://eindhovennews.com/news/2022/08/here-you-can-see-how-a-huge-tunnel-is-pushed-under-the-a2/</t>
+    <t>https://www.treinenweb.nl/nieuws/9671/treinverkeer-zeeland-deels-hervat-na-aanrijding.html</t>
   </si>
   <si>
     <t>https://www.railjournal.com/in_depth/irj-innotrans-2022-preview-r-z/</t>
   </si>
   <si>
+    <t>https://eindhovennews.com/news/2022/03/eindhoven-begins-construction-of-underpass-a2/</t>
+  </si>
+  <si>
     <t>https://www.prorail.nl/nieuws/prorail-op-pole-position</t>
   </si>
   <si>
     <t>https://www.rtvoost.nl/nieuws/1491859/Commissarissen-Strukton-roepen-topman-Sanderink-tot-de-orde-na-bedreiging-deurwaarder</t>
   </si>
   <si>
+    <t>https://www.nu.nl/tech/6002924/gegevens-van-waarschijnlijk-alle-oud-medewerkers-strukton-rail-gestolen.html</t>
+  </si>
+  <si>
+    <t>https://studio040.nl/nieuws/artikel/eindhoven-begint-met-aanleg-onderdoorgang-a2</t>
+  </si>
+  <si>
     <t>https://www.spoorpro.nl/spoorbouw/2018/08/09/prorail-en-strukton-rail-in-gesprek-om-veiligheid-kijfhoek-te-verbeteren/</t>
   </si>
   <si>
     <t>https://www.gim-international.com/case-study/phase-one-drone-supports-3d-bridge-inspection-in-the-netherlands</t>
   </si>
   <si>
-    <t>https://www.railway-technology.com/uncategorized/newsstrukton-secures-atb-vv-train-protection-system-installation-contract-prorail-4963221/</t>
+    <t>https://studio040.nl/nieuws/artikel/inleverpunt-voor-vuurwerk-oogst-vooral-onschuldige-sterretjes</t>
+  </si>
+  <si>
+    <t>https://www.spoorpro.nl/spoorbouw/2020/03/20/gvb-gunt-strukton-vernieuwing-metrospoorbrug-in-amsterdam/</t>
+  </si>
+  <si>
+    <t>https://www.nu.nl/beurs/3935465/reorganisatie-bij-strukton-rail.html</t>
+  </si>
+  <si>
+    <t>https://dutchitchannel.nl/620720/strukton-en-centric-hebben-vertrouwen-in-deskundigheid-rian-van-rijbroek.html</t>
   </si>
   <si>
     <t>https://www.spoorpro.nl/spoorbouw/2012/08/03/strukton-rail-neemt-belang-in-a1-elektronics/</t>
@@ -232,6 +229,9 @@
     <t>https://www.spoorpro.nl/management/2014/08/04/spoorbeheerder-prorail-sluit-vier-tienjarige-pgo-contracten-af/</t>
   </si>
   <si>
+    <t>https://www.transport-online.nl/site/14394/gefco-bouwt-lichtgewicht-bedrijfswageninrichting-voor-strukton/</t>
+  </si>
+  <si>
     <t>https://www.spoorpro.nl/spoorbouw/2018/08/03/stof-arm-los-trein-ingezet-bij-spoorwerkzaamheden-gouda/</t>
   </si>
   <si>
@@ -241,7 +241,7 @@
     <t>https://www.nieuwsblad.be/cnt/blero_04648155</t>
   </si>
   <si>
-    <t>https://www.nu.nl/binnenland/3774905/sanering-vervuilde-bodem-chemie-pack-begint.html</t>
+    <t>https://studio040.nl/nieuws/artikel/nog-steeds-frustraties-over-bouwongeval-internationale-school</t>
   </si>
   <si>
     <t>https://www.spoorpro.nl/materieel/2016/07/28/eerste-ervaringen-met-stofarme-werktrein-positief/</t>
@@ -253,39 +253,27 @@
     <t>https://www.rtlnieuws.nl/nieuws/artikel/4466311/een-giftige-cocktail-vier-dode-kinderen-paniek-en-house-cards</t>
   </si>
   <si>
-    <t>https://groningen.nieuws.nl/nieuws/830406/voorlopig-ontwerp-verbouwing-station-groningen-gepresenteerd/</t>
-  </si>
-  <si>
-    <t>https://www.railjournal.com/in_depth/riyadh-metro-megaproject-reaches-halfway-mark/</t>
-  </si>
-  <si>
     <t>strukton.maglr.nl</t>
   </si>
   <si>
+    <t>www.businessradar.com</t>
+  </si>
+  <si>
     <t>pledgetimes.com</t>
   </si>
   <si>
-    <t>businessradar.com</t>
-  </si>
-  <si>
     <t>www.dutchnews.nl</t>
   </si>
   <si>
     <t>www.reuters.com</t>
   </si>
   <si>
-    <t>www.digitaljournal.com</t>
+    <t>www.eco-business.com</t>
   </si>
   <si>
     <t>indianexpress.com</t>
   </si>
   <si>
-    <t>www.eco-business.com</t>
-  </si>
-  <si>
-    <t>www.dailymail.co.uk</t>
-  </si>
-  <si>
     <t>www.waterkant.net</t>
   </si>
   <si>
@@ -301,10 +289,13 @@
     <t>pages.facebook.com</t>
   </si>
   <si>
+    <t>www.globalconstructionreview.com</t>
+  </si>
+  <si>
     <t>kokmilieu.nl</t>
   </si>
   <si>
-    <t>www.globalconstructionreview.com</t>
+    <t>www.rtlnieuws.nl</t>
   </si>
   <si>
     <t>menafn.com</t>
@@ -316,6 +307,9 @@
     <t>www.omroepbrabant.nl</t>
   </si>
   <si>
+    <t>www.noordhollandsdagblad.nl</t>
+  </si>
+  <si>
     <t>nos.nl</t>
   </si>
   <si>
@@ -325,9 +319,6 @@
     <t>www.emerce.nl</t>
   </si>
   <si>
-    <t>flevopost.nl</t>
-  </si>
-  <si>
     <t>m.engineeringnews.co.za</t>
   </si>
   <si>
@@ -337,21 +328,21 @@
     <t>www.lifegate.com</t>
   </si>
   <si>
-    <t>www.progressiverailroading.com</t>
-  </si>
-  <si>
     <t>www.railjournal.com</t>
   </si>
   <si>
     <t>www.cleantech.com</t>
   </si>
   <si>
-    <t>www.byggnadsarbetaren.se</t>
-  </si>
-  <si>
     <t>www.railtechnologymagazine.com</t>
   </si>
   <si>
+    <t>www.nwboomerandseniornews.com</t>
+  </si>
+  <si>
+    <t>112doetinchem.nl</t>
+  </si>
+  <si>
     <t>strukton.com</t>
   </si>
   <si>
@@ -367,19 +358,22 @@
     <t>nl.linkedin.com</t>
   </si>
   <si>
+    <t>www.prorail.nl</t>
+  </si>
+  <si>
+    <t>www.treinenweb.nl</t>
+  </si>
+  <si>
+    <t>eindhovennews.com</t>
+  </si>
+  <si>
+    <t>www.rtvoost.nl</t>
+  </si>
+  <si>
     <t>www.nu.nl</t>
   </si>
   <si>
-    <t>www.prorail.nl</t>
-  </si>
-  <si>
-    <t>www.treinenweb.nl</t>
-  </si>
-  <si>
-    <t>eindhovennews.com</t>
-  </si>
-  <si>
-    <t>www.rtvoost.nl</t>
+    <t>studio040.nl</t>
   </si>
   <si>
     <t>www.spoorpro.nl</t>
@@ -388,7 +382,10 @@
     <t>www.gim-international.com</t>
   </si>
   <si>
-    <t>www.railway-technology.com</t>
+    <t>dutchitchannel.nl</t>
+  </si>
+  <si>
+    <t>www.transport-online.nl</t>
   </si>
   <si>
     <t>www.ovpro.nl</t>
@@ -400,12 +397,6 @@
     <t>www.quotenet.nl</t>
   </si>
   <si>
-    <t>www.rtlnieuws.nl</t>
-  </si>
-  <si>
-    <t>groningen.nieuws.nl</t>
-  </si>
-  <si>
     <t>Investigative Journal</t>
   </si>
   <si>
@@ -418,40 +409,31 @@
     <t>Allright</t>
   </si>
   <si>
+    <t>Scandal</t>
+  </si>
+  <si>
     <t>Controversial gerard sanderink returns as director at strukton</t>
   </si>
   <si>
-    <t>Crisis</t>
-  </si>
-  <si>
     <t>Strukton investigated for corruption in saudi metro deal</t>
   </si>
   <si>
     <t>Us dutch canals idUKL</t>
   </si>
   <si>
-    <t>Tamping machine market to discern magnified growth during</t>
+    <t>Indonesia to build worlds largest tidal power plant</t>
   </si>
   <si>
     <t>Mumbai inductor delay holds up trials of ac rakes</t>
   </si>
   <si>
-    <t>Indonesia to build worlds largest tidal power plant</t>
-  </si>
-  <si>
-    <t>End line autumn train delays Dutch begin trials zap leaf litter tracks LASERShtml</t>
-  </si>
-  <si>
     <t>Ambassador Netherlands in Suriname again from November</t>
   </si>
   <si>
     <t>Bouterse happy as a child about energy savings</t>
   </si>
   <si>
-    <t>Enterprise chamber refuses to give centric ceo sanderink his support</t>
-  </si>
-  <si>
-    <t>Om takes next step to depose sanderink</t>
+    <t>Will gerard sanderink be forced to resign from centric</t>
   </si>
   <si>
     <t>Soil and groundwater remediation of the former drug lab in the municipality of Horst aan de Maas</t>
@@ -466,10 +448,13 @@
     <t>type</t>
   </si>
   <si>
+    <t>Dutch authorities raid strukton suspicion bribery</t>
+  </si>
+  <si>
     <t>Vierkibccfireguardsforstructuretonenvironmental engineering</t>
   </si>
   <si>
-    <t>Dutch authorities raid strukton suspicion bribery</t>
+    <t>Gerard sanderink ceo centric top man strukton rian van breeches</t>
   </si>
   <si>
     <t>Railway Maintenance Machinery Market Growth Global Survey Segments Industry Status And Forecast</t>
@@ -484,6 +469,9 @@
     <t>Toon francken not helped if the rich pays to clean up drug waste</t>
   </si>
   <si>
+    <t>Dmf</t>
+  </si>
+  <si>
     <t>Cleaning up liters of drug waste in Eindhoven is a big job, police are looking for a white box truck</t>
   </si>
   <si>
@@ -493,39 +481,33 @@
     <t>Ban via rian podcast bizarre company soap</t>
   </si>
   <si>
-    <t>Mural The Binding Harvest Appreciation Html</t>
-  </si>
-  <si>
     <t>Repid</t>
   </si>
   <si>
     <t>Global railway maintenance machinery market  harsco speno strukton vortok international plasser theurerhtml</t>
   </si>
   <si>
-    <t>Will gerard sanderink be forced to resign from centric</t>
-  </si>
-  <si>
     <t>Larantuka straits tidal power Indonesia</t>
   </si>
   <si>
-    <t>University of Delawares Big Data conference explored analytics trends in a rail context</t>
-  </si>
-  <si>
     <t>Get set for innotrans</t>
   </si>
   <si>
     <t>Turning tide for ocean power is marine energy coming of age</t>
   </si>
   <si>
-    <t>Most employed largest construction CAD companies in Sweden</t>
-  </si>
-  <si>
-    <t>Student team Delft hyperloop unveils new hyperloop capsule atlas</t>
-  </si>
-  <si>
     <t>Why not do some re engineering adrian shooter on the vivarail d train</t>
   </si>
   <si>
+    <t>On board systems professional market  key insights and leading players deuta werke gmbh hubersuhner strukton rail abb knorr bremse ag caf group etc</t>
+  </si>
+  <si>
+    <t>Who is gerard sanderink and why is justice demanding his resignation from centric</t>
+  </si>
+  <si>
+    <t>Satisfied faces at provincial firefighting competitions in Zutphen</t>
+  </si>
+  <si>
     <t>Integrity</t>
   </si>
   <si>
@@ -541,37 +523,49 @@
     <t>Concrete renovation</t>
   </si>
   <si>
-    <t>Strukton CEO Sanderink suspected of bribery in Saudi Arabia</t>
-  </si>
-  <si>
     <t>No train traffic in Flevoland for a long time</t>
   </si>
   <si>
-    <t>Possibly no trains between Lelystad and Zwolle for weeks after a short circuit</t>
-  </si>
-  <si>
     <t>Train collides with empty city bus</t>
   </si>
   <si>
-    <t>Here you can see how a huge tunnel is pushed under the a</t>
+    <t>Train traffic in Zeeland partly resumed after collision</t>
   </si>
   <si>
     <t>Irj innotrans  preview r z</t>
   </si>
   <si>
+    <t>Eindhoven begins construction of underpass a</t>
+  </si>
+  <si>
     <t>Prorail on pole position</t>
   </si>
   <si>
     <t>Supervisory Board members of Strukton call CEO Sanderink to order after a threat from the bailiff</t>
   </si>
   <si>
+    <t>Data from probably all former employees of Strukton rail stolen</t>
+  </si>
+  <si>
+    <t>Eindhoven starts construction of underpass a</t>
+  </si>
+  <si>
     <t>ProRail and Strukton Rail in talks to improve safety dispute angle</t>
   </si>
   <si>
     <t>Phase one drone supports d bridge inspection in the netherlands</t>
   </si>
   <si>
-    <t>Newsstrukton secures atb vv train protection system installation contract prorail</t>
+    <t>Collection point for fireworks mainly harvests innocent stars</t>
+  </si>
+  <si>
+    <t>GVB awards Strukton the renewal of the metro railway bridge in Amsterdam</t>
+  </si>
+  <si>
+    <t>Reorganization at Strukton railhtml</t>
+  </si>
+  <si>
+    <t>Strukton and centric have confidence in the expertise of rian van breecheshtml</t>
   </si>
   <si>
     <t>Strukton rail takes an interest in a electronics</t>
@@ -589,6 +583,9 @@
     <t>Rail manager prorail concludes four ten-year PGO contracts</t>
   </si>
   <si>
+    <t>Gefco builds lightweight in-vehicle equipment for Strukton</t>
+  </si>
+  <si>
     <t>Dust arm loose train used for railway works in Gouda</t>
   </si>
   <si>
@@ -598,7 +595,7 @@
     <t>Sefa</t>
   </si>
   <si>
-    <t>Remediation of polluted soil chemistry pack starts html</t>
+    <t>Still frustrated about international school construction accident</t>
   </si>
   <si>
     <t>Positive initial experiences with low-dust work train</t>
@@ -610,50 +607,35 @@
     <t>A poisonous cocktail four dead kids panic and house cards</t>
   </si>
   <si>
-    <t>Preliminary design renovation station groningen presented</t>
-  </si>
-  <si>
-    <t>Riyadh metro megaproject reaches halfway mark</t>
-  </si>
-  <si>
     <t>Strukton publications</t>
   </si>
   <si>
-    <t>Controversial Gerard Sanderink returns as director at Strukton A spokesperson confirms that NRC after reporting in the Financial Newspaper. Sanderink succeeds Erik Hermsen, who took over his duties after Sanderink’s departure earlier this year. Hermsen worked at Strukton for 22 years until his immediate departure on Friday and will focus on other “administrative and supervisory roles”, according to the report. the press release. Sanderink has been discredited in recent years due to various quarrels and scandals within his companies, which, in addition to Strukton, also include IT company Centric and engineering company Antea. He therefore left both parent company Oranjewoud (of which Sanderink also owns) and Strukton, but is now a director there again. A spokesperson for Strukton answers questions from NRC unable to comment further on Hermsen’s departure. “He has contributed a lot to the company, but now he is going in a different direction in his career.” According to her, the unrest surrounding Sanderink is also “over”. To get the company out of the red, the company says it has recently tightened its strategy. According to the spokesperson, the management of Strukton Groep now has ‘shorter lines’ with the various parts. “We make better strategic choices, and no longer take on risky projects.” In 2019, the company still suffered a loss of 19.7 million euros, but according to the spokesperson, the profit has been made again in the first half of 2021. The company has more than 6,500 employees. Oranjewoud’s subsidiaries have been plagued by scandals since 2019, and one director or director after another has left. In February 2019, the FIOD raided Strukton’s headquarters in an investigation into corruption and forgery surrounding the contract for a metro project in Riad, Saudi Arabia. The investigation is still ongoing. There was also great dissatisfaction with the way in which Sanderink tried to solve Strukton’s financial problems by taking money away from the other companies. In addition, there was increasing concern within the companies about Sanderink’s own behavior. In July 2019, the fourth board member left IT company Centric, one of the other companies. The reason for this was an article in NRC about the influence of the controversial self-proclaimed cyber expert Van Rijbroek, with whom Sanderink has had a relationship since 2019, on the company. Also read: The last eruption was one too many for entrepreneur Gerard Sanderink Sanderink also accused his ex-girlfriend Brigitte van Egten, who headed several companies under Oranjewoud, of fraud and theft. However, the FIOD has found no evidence for this. Hermsen became involved in this conflict when Van Egten had information on Sanderink’s telephone and computer seized at Strukton’s office. Sanderink threatened both Hermsen and the inspector during the seizure, after which Hermsen asked Sanderink to calm down in another room. During the time-out, Sanderink’s phone was remotely erased, and evidence may have been destroyed, Van Egt’s counsel said. NRC know. In June it wrote FD that Hermsen would have been suspended, based on a conversation with Herman Spenkelink, a supervisory director at Oranjewoud. A spokesperson for Strukton denies this, saying that Hermsen had a conversation with Sanderink and was said to have been ill for a few days. Sanderink has long owned the vast majority of Oranjewoud’s shares. In February, the company announced that Sanderink’s investment company would own the remaining 0.9 percent of the shares wanted to buy up. At that time, that involved almost 575,000 shares. The intention is to end the listing of Oranjewoud on the Euronext Amsterdam after completion of the buy-out. It is not known when that will be, but the process is running “according to plan”, according to a spokesperson. Only a small volume of Oranjewoud shares are currently tradable. A version of this article also appeared in NRC on the morning of October 6, 2021 In St. Petersburg, a citizen of Belarus knocked down a 12-year-old schoolboy at a pedestrian crossingIn St. Petersburg, a driver,</t>
-  </si>
-  <si>
-    <t>Architectural services Until 2018, Gerard Sanderink, owner of ICT company Centric and construction company Strukton, seemed to be a modest businessman, despite his power and his fortune of 620 million. Until 2018, Gerard Sanderink, owner of ICT company Centric and construction company Strukton, seemed to be a modest businessman, despite his power and his fortune of 620 million. Centric and Strukton charged over smear campaign against ex Sanderink Centric and Strukton charged over smear campaign against ex Sanderink Will Centric and Strukton come into the hands of Rian van Rijbroek? Will Centric and Strukton come into the hands of Rian van Rijbroek? And: Gerard Sanderink is making a remarkable comeback as director of construction company Strukton. And: Gerard Sanderink is making a remarkable comeback as director of construction company Strukton. Gerard Sanderink back as CEO Strukton after Erik Hermsen's definitive departure Gerard Sanderink back as CEO Strukton after Erik Hermsen's definitive departure Uproar again at a Sanderink company: Strukton's CEO calls in sick – or has he been put on hold? Uproar again at a Sanderink company: Strukton's CEO calls in sick – or has he been put on hold? Strukton's chief executive Erik Hermsen has been suspended by owner Gerard Sanderink. Strukton's chief executive Erik Hermsen has been suspended by owner Gerard Sanderink. Controversial entrepreneur Sanderink suspends Strukton's CEO Controversial entrepreneur Sanderink suspends Strukton's CEO 'Topman Strukton put on hold by owner Gerard Sanderink' 'Topman Strukton put on hold by owner Gerard Sanderink' Millionaire Gerard Sanderink is stepping down as top executive of the Oranjewoud engineering and consultancy firm and its subsidiaries Antea Group and construction company Strukton. Millionaire Gerard Sanderink is stepping down as top executive of the Oranjewoud engineering and consultancy firm and its subsidiaries Antea Group and construction company Strukton. The judge also ruled that the eccentric entrepreneur must also rectify his fraud allegations against Van Egten on the homepages of Centric and Strukton, Sanderink's other large company. The judge also ruled that the eccentric entrepreneur must also rectify his fraud allegations against Van Egten on the homepages of Centric and Strukton, Sanderink's other large company. Click here to read all articles Get the full picture and Receive alerts on lawsuits, news articles, publications and more!</t>
+    <t>Member of the AFM Supervisory Board temporarily resigns due to SHV corruption scandal Bart Koolstra has withdrawn for the time being Member of the AFM Supervisory Board temporarily resigns due to SHV corruption scandal Bart Koolstra has withdrawn for the time being After criminal investigations against Ballast Nedam, Damen Shipyards and parts of SHV, it is now the turn of construction company Strukton. After criminal investigations against Ballast Nedam, Damen Shipyards and parts of SHV, it is now the turn of construction company Strukton. Dennis Mr – NRC journalists have another nice file in their hands: a major bribery affair at the recovery company Mammoet, a subsidiary of SHV that is again in the hands of the well-known entrepreneurial family Fentener van Vlissingen. Dennis Mr – NRC journalists have another nice file in their hands: a major bribery affair at the recovery company Mammoet, a subsidiary of SHV that is again in the hands of the well-known entrepreneurial family Fentener van Vlissingen. Member of the AFM Supervisory Board temporarily resigns due to SHV corruption scandal Member of the AFM Supervisory Board temporarily resigns due to SHV corruption scandal KPMG reports controversial SHV 'committee' as a bribe to FIU KPMG reports controversial SHV 'committee' as a bribe to FIU Click here to read all articles Get the full picture and Receive alerts on lawsuits, news articles, publications and more!</t>
+  </si>
+  <si>
+    <t>Controversial Gerard Sanderink returns as director at Strukton A spokesperson confirms that NRC after reporting in the Financial Newspaper. Sanderink succeeds Erik Hermsen, who took over his duties after Sanderink’s departure earlier this year. Hermsen worked at Strukton for 22 years until his immediate departure on Friday and will focus on other “administrative and supervisory roles”, according to the report. the press release. Sanderink has been discredited in recent years due to various quarrels and scandals within his companies, which, in addition to Strukton, also include IT company Centric and engineering company Antea. He therefore left both parent company Oranjewoud (of which Sanderink also owns) and Strukton, but is now a director there again. A spokesperson for Strukton answers questions from NRC unable to comment further on Hermsen’s departure. “He has contributed a lot to the company, but now he is going in a different direction in his career.” According to her, the unrest surrounding Sanderink is also “over”. To get the company out of the red, the company says it has recently tightened its strategy. According to the spokesperson, the management of Strukton Groep now has ‘shorter lines’ with the various parts. “We make better strategic choices, and no longer take on risky projects.” In 2019, the company still suffered a loss of 19.7 million euros, but according to the spokesperson, the profit has been made again in the first half of 2021. The company has more than 6,500 employees. Oranjewoud’s subsidiaries have been plagued by scandals since 2019, and one director or director after another has left. In February 2019, the FIOD raided Strukton’s headquarters in an investigation into corruption and forgery surrounding the contract for a metro project in Riad, Saudi Arabia. The investigation is still ongoing. There was also great dissatisfaction with the way in which Sanderink tried to solve Strukton’s financial problems by taking money away from the other companies. In addition, there was increasing concern within the companies about Sanderink’s own behavior. In July 2019, the fourth board member left IT company Centric, one of the other companies. The reason for this was an article in NRC about the influence of the controversial self-proclaimed cyber expert Van Rijbroek, with whom Sanderink has had a relationship since 2019, on the company. Also read: The last eruption was one too many for entrepreneur Gerard Sanderink Sanderink also accused his ex-girlfriend Brigitte van Egten, who headed several companies under Oranjewoud, of fraud and theft. However, the FIOD has found no evidence for this. Hermsen became involved in this conflict when Van Egten had information on Sanderink’s telephone and computer seized at Strukton’s office. Sanderink threatened both Hermsen and the inspector during the seizure, after which Hermsen asked Sanderink to calm down in another room. During the time-out, Sanderink’s phone was remotely erased, and evidence may have been destroyed, Van Egt’s counsel said. NRC know. In June it wrote FD that Hermsen would have been suspended, based on a conversation with Herman Spenkelink, a supervisory director at Oranjewoud. A spokesperson for Strukton denies this, saying that Hermsen had a conversation with Sanderink and was said to have been ill for a few days. Sanderink has long owned the vast majority of Oranjewoud’s shares. In February, the company announced that Sanderink’s investment company would own the remaining 0.9 percent of the shares wanted to buy up. At that time, that involved almost 575,000 shares. The intention is to end the listing of Oranjewoud on the Euronext Amsterdam after completion of the buy-out. It is not known when that will be, but the process is running “according to plan”, according to a spokesperson. Only a small volume of Oranjewoud shares are currently tradable. A version of this article also appeared in NRC on the morning of October 6, 2021 The "Atlas Lions" squad included: Yassin Bono - Ashraf Hakimi - Naseer Al-Mazrawi - Sufyan Amrabat - Nayef Akrad -</t>
   </si>
   <si>
     <t>Strukton investigated for corruption in Saudi metro deal Photo: Wikimedia Commons Building company Strukton is being investigated for paying millions of euros via an agent to a half brother of the current Saudi king, the Financieele Dagblad said on Friday. The FD says the payments to prince Mishaal bin Abudalaziz al Sauid via a middle man enabled Strukton to work on developing a metro network in Riyadh, the capital of Saudi Arabia. The prince has since died. The paper bases its claims on information received following a raid on Strukton’s headquarters in Utrecht on February 15. Strukton chairman Gerard Sanderink said in a reaction that there is no question of bribery being involved. ‘The project was awarded on the basis of the lowest price,’ he said. ‘We have been told that the FIOD based the decision for the raid on audits by the tax authorities, leading to suspicion of corruption and false declarations when obtaining a contract for the metro project in Riyadh. We fully cooperate and provide full insight to the FIOD,’ the company statement said. Strukton is one of several companies involved in the multi-billion euro project to build six metro lines in Riyadh that will run for a total length of 176 kilometres across the city and includes 85 stations. Thank you for donating to DutchNews.nlThe DutchNews.nl team would like to thank all the generous readers who have made a donation in recent weeks. Your financial support has helped us to expand our coverage of the coronavirus crisis into the evenings and weekends and make sure you are kept up to date with the latest developments. DutchNews.nl has been free for 14 years, but without the financial backing of our readers, we would not be able to provide you with fair and accurate news and features about all things Dutch. Your contributions make this possible. If you have not yet made a donation, but would like to, you can do so via Ideal, credit card or Paypal. The DutchNews.nl team would like to thank all the generous readers who have made a donation in recent weeks. Your financial support has helped us to expand our coverage of the coronavirus crisis into the evenings and weekends and make sure you are kept up to date with the latest developments. DutchNews.nl has been free for 14 years, but without the financial backing of our readers, we would not be able to provide you with fair and accurate news and features about all things Dutch. Your contributions make this possible. If you have not yet made a donation, but would like to, you can do so via Ideal, credit card or Paypal. © 2022 DutchNews | Cookie settings | website by Vindustries Many thanks to everyone who has donated to DutchNews.nl in recent days! We could not provide this service without you. If you have not yet made a contribution, you can do so here. The DutchNews.nl team</t>
   </si>
   <si>
     <t>Firm wants parking, shops under Amsterdam canals A pleasureboat cruises the Brouwersgracht canal in front of the paved over Palmgracht in Amsterdam, August 11, 2004. Amsterdam's trademark canals should be drained in sections so that underground parking, shops and cinemas can be built to ease the space shortage in the Dutch capital, according to an ambitious plan launched on Tuesday. REUTERS/Michael Kooren Construction company Strukton, owned by the Dutch railway, proposed building an underground city six floors deep under the picturesque canals, which would be drained section by section while construction takes place and then refilled with water. The web-like complex could be used for parking, sport halls, cinemas and warehouses, and accessed by car from the highway that circles the city, with exits for pedestrians around the city, Strukton said, launching architect's plans: here “It is a sustainable and realizable plan. Expanding a city underground is not futuristic but a necessity in today’s world,” said Bas Obladen, a senior Strukton adviser. The city has signaled support for the plan but would have to take a decision before work could go ahead, Strukton spokesman Youssef Eddini said. Residents of the historic houses that line Amsterdam’s central ring of canals have to wait years for parking permits and a garage space can cost as much as 100,000 euros ($147,800). The one-way streets on either side of the water are often blocked for hours by delivery and rubbish trucks, making it far quicker to travel by bicycle. Eddini said the plan could cost about 10 billion euros and take up to 20 years to realize, but would pay for itself by creating a huge amount of space, cutting the cost of a garage parking spot to 25,000 euros. “It’s a solution for the future of Amsterdam. If we continue in this way Amsterdam will be closed for cars,” he said. Strukton is working on a metro hub under Amsterdam central station for a much-delayed new subway line linking the north and south of the city that has caused traffic chaos for years. The old center of Amsterdam was built on swampy marshland and many of the houses along the canals are still supported by wooden poles, but Eddini said it would be easier to dig and build in the clay under the canal water. He said the new plan would not cause as much disruption as the new metro line: “All materials could be brought to the site by water. We can use the canals as a road.” Reporting by Emma Thomasson, editing by Tim Pearce Our Standards: The Thomson Reuters Trust Principles. All quotes delayed a minimum of 15 minutes. See here for a complete list of exchanges and delays</t>
-  </si>
-  <si>
-    <t>Tamping Machine Market to Discern Magnified Growth during 2027  The tamping machine market is projected to expand at a CAGR of 5% from 2019 to 2027 in terms of volume. Growth of the tamping machine market can be attributed to rising adoption of tamping machines for railway track geometry degradation, which has triggered their demand globally. Over the forecast period, Europe is anticipated to emerge as the leading tamping machine market, followed by Asia Pacific and North America. Rising Adoption of Tamping Machines for Railway Track Geometry Degradation Maintenance of tracks is one of the key requirements for a viable railroad system across the world. Maintaining aging railway networks with a robust and economic maintenance strategy is a crucial task for the government of any country. Thus, railway authorities and governments of various countries are adopting tamping machines to maintain railway tracks, by utilizing data on the network track geometry with available records of maintenance performed. This is one of the factors driving the tamping machine market. Furthermore, tamping machines help railway authorities to analyze the quality, conditions, and variations of track geometry, in order to check the possible parameters to lessen the consequent stress of increased volume of traffic and frequency of trains. This in turn is accelerating the growth of the tamping machine market across the world. Thus, rising adoption of tamping machines for railway track geometry degradation is expected to have a significant impact on the tamping machine market. Get PDF sample for Industrial Insights and business Intelligence – https://www.transparencymarketresearch.com/sample/sample.php?flag=S&amp;rep_id=74192 Tamping Machine: Market Segmentation The global tamping machine market has been segmented in terms of product type, application, and region. Based on product type, the tamping machine market has been classified into track tamping machines, points and crossing tamping machines, and multi-purpose tamping machines (MPT). Among applications, new railway lines construction segment dominated the global tamping machine market in 2018. Request for Custom Research –  https://www.transparencymarketresearch.com/sample/sample.php?flag=CR&amp;rep_id=74192 Tamping Machine Market: Regional Outlook In terms of region, the global tamping machine market has been segmented into North America, Europe, Asia Pacific, Middle East &amp; Africa, and South America. Europe is anticipated to lead the tamping machine market during the forecast period. Germany is estimated to hold a notable share of the market in the Europe region and the market in the country is projected to expand at a CAGR of 5.7% during the forecast period in terms of volume. Asia Pacific is expected to hold a significant share of the global tamping machine market, accounting for a substantial share in 2019, with India, China, and Japan being the major markets in the region. The tamping machine market in North America, Middle East &amp; Africa, and South America is also projected to increase moderately over the forecast period. The report provides in-depth segment analysis of the global tamping machine market, thereby providing valuable insights at macro as well as micro levels. Analysis of major countries, which hold growth opportunities or account for significant share has also been included as part of geographic analysis of the tamping machine market. Make an Enquiry Before Buying – https://www.transparencymarketresearch.com/sample/sample.php?flag=EB&amp;rep_id=74192 Tamping Machine Market: Competition Dynamics The research study includes profiles of leading companies operating in the global tamping machine market. Key players profiled in the report include CRCC High-Tech Equipment Co., Ltd., Gemac Engineering Machinery Co Ltd, Harsco Corporation, Kalugaputmash, MATISA MATÉRIEL INDUSTRIEL S.A., New Sorema Ferroviaria SpA, Plasser &amp; Theurer, Robel Bahnbaumaschinen Gmbh, Strukton, The Sinara Group, and Loram Maintenance of Way, Inc. About Transparency Market Research Transparency Market Research, a global market research company registered at Wilmington, Delaware, United States, provides custom research and consulting services. The firm scrutinizes factors shaping the dynamics of demand in various markets. The insights and perspectives on the markets evaluate opportunities in various segments. The opportunities in the segments based on source, application, demographics, sales channel, and end-use are analysed, which will determine growth in the markets over the next decade. Our exclusive blend of quantitative forecasting and trends analysis provides forward-looking insights for thousands of decision-makers, made possible by experienced teams of Analysts, Researchers, and Consultants. The proprietary data sources and various tools &amp; techniques we use always reflect the latest trends and information. With a broad research and analysis capability, Transparency Market Research employs rigorous primary and secondary research techniques in all of its business reports. Contact Nikhil Sawlani Transparency Market Research Inc. CORPORATE HEADQUARTER DOWNTOWN, 1000 N. West Street, Suite 1200, Wilmington, Delaware 19801 USA Tel: +1-518-618-1030 USA – Canada Toll Free: 866-552-3453 Website: https://www.transparencymarketresearch.com Blog: https://tmrblog.com Email: [email protected] The truck drives itself, and veteran driver Roger Nordqvist is at the ready only in case of unexpected problems. Meanwhile, everyone’s allowed to breathe as much and as many pollutants as they like. People living with HIV have a higher risk of lung cancer than the general population. China's factory activity shrank for a second straight month in November, official data showed Wednesday. COPYRIGHT © 1998 - 2022 DIGITAL JOURNAL INC. Sitemaps: XML / News . Digital Journal is not responsible for the content of external sites. Read more about our external linking</t>
-  </si>
-  <si>
-    <t>Mumbai: Still awaiting those local AC trains? Here’s why trial run has been held up Though the order for the inductor was made in June, much time has been wasted in bringing it to Kurla car-shed, where currently the train is undergoing maintenance, officials said. The AC rake manufactured by the Bharat Heavy Electricals Limited (BHEL) and Strukton, a Netherlands-based firm, had arrived in Mumbai on April 1. CR authorities had already missed its earlier deadlines (May 16, June 30 and August 31) of conducting static trials. “Improper co-ordination between the manufacturers and CR authorities delayed the inductor for conducting trials. The instrument supposed to come in June will now be hopefully received by September, post which commissioning can be expected to begin trials,” a CR official said. Static trials of the rake will test the interface between the software and the equipment installed. Officials confirmed that out of a fourteen-day schedule of this phase of trials, thirteen have already been completed and the wait continues for the inductor. “Our team has successfully completed majority of trials of the AC rake. We are waiting for the inductor to be received, post which trials will be re-run to check smooth co-ordination between the motor coach and other coaches. The rake cannot be considered fit to run without doing so,” he added. Commissioning permission can be availed of by mid-September if the inductor is in place with CR authorities by September 1. The trials can begin from September 30 post which dynamic trials of the rake can be started. However, officials seem puzzled on deciding the line for conducting the trials. “As height of the AC rake could clash with some railway-over- bridges (ROBs) between route of Chhatrapati Shivaji Terminus (CST)-Kurla, conducting dynamic trials there will be difficult. Also, problems exist with conducting trials on trans-harbor line as well. It may thus run on the route between Kurla-Karjat or Kasara and then on Western Railway (WR) line for trials,” a senior CR official said. Also, officials confirmed it is too early to think about deciding fares or marking routes. “The rake is yet to qualify many trials. It may run on WR if Commission of Railway Safety certifies so. There is also a possibility that other AC rakes manufactured would be lower in height and would run on CR,” the official added. It is only after the prototype rake is set in place that the other AC rakes are constructed on a similar model. “After specifications are given to the Integral Coach Factory (ICF) about smooth running of this rake, the next one will come within a month. It is necessary that the first AC rake runs with the second in place as any operational issue with the first will require an immediate replacement with the second,” the official added. The Railways had placed an order for ten air-conditioned rakes from BHEL. Built at a cost of Rs 54 crore, the entire rake would be vestibule-connected and has a seating capacity of 1,208 and standing capacity of 4,936 passengers.   Mississippi man sentenced to 8 years for trying to join Islamic State Neha Kulkarni</t>
   </si>
   <si>
     <t>Indonesia to build 'world's largest' tidal power plant
  The new plant, known as the Palmerah Tidal Bridge, will be built into a floating 800 metre-long bridge on the Larantuka Strait in East Flores, and promises to deliver power capacity of 18 to 23 megawatts (MW), providing enough electricity for 100,000 people in the area. It is the first deal to emerge from a strategic hydropower alliance between the Indonesian and Dutch governments. A second phase of construction could see capacity increased to 90 to 115 MW, enough power for more than half a million Indonesians in a region that largely relies on polluting diesel generators for electricity. An artist’s impression of the Palmerah Tidal Bridge. Image: Tidal Bridge BV  Environmental group Greenpeace has said that it approves of the project as an alternative to coal in fossil fuels-dependent Indonesia, but that caution is needed to ensure that the biodiversity of the marine environment is not affected. Tidal power is a relatively uncommon form of renewable energy that harnesses the energy of marine currents, a potentially more reliable power source than wind or the sun. The International Energy Agency estimates that in 2014, global tidal power capacity was about 0.5GW, compared to 128GW of solar and 8.8GW of offshore wind. Indonesia is an ideal location for tidal power, because of strong ocean currents that move between the world’s largest archipelago’s thousands of islands. The Larantuka Strait between Flores and Adonara is one such area, with a number of sites now being considered by the Indonesian government. The Palmerah Tidal Bridge is also being trumpeted as a way of improving grid connectivity in the eastern part of Indonesia, and giving people in the area better access to education, healthcare and job opportunities. The project has been awarded to Tidal Bridge BV, a joint venture between Dutch engineering firm Strukton International and venture capital fund Dutch Expansion Capital. It is slated to be completed by 2019 at a cost of US$550 million. The companies behind the project claim Palmerah Tidal Bridge will be the largest tidal power facility in the world. However, South Korea’s Sihwa Lake Tidal Power Station, with power output of 254 MW, has around double the capacity of the Palmerah project, as does the Rance Tidal Power Station in France, with power capacity of 240 MW. Greenpeace Indonesia climate and energy campaigner Hindun Mulaika told Eco-Business that the organisation supported the development of renewable energy in Indonesia, a country that is a big coal extractor and user, and continues to approve plans to build new coal-fired power plants to meet its growing energy demands. Around 50 million Indonesians are without reliable electricity, and president Joko Widowo’s 35,000 MW plan to electrify the country is slated to use mostly coal (20,000 MW, or 57 per cent) to deliver power to those without it. A report by Greenpeace released in January predicted that if plans to build new coal power plants go ahead in Indonesia, it will suffer more deaths as a result of air pollution than any country in Southeast Asia. Hindun said that the group “supports the development of renewable energy to foster the transition away from huge coal dependencies in the country.” “We found a perfect example in Palmerah Tidal Power Plant where the energy source can be found in local resources, which will surely cut distribution costs that commonly occur in big centralised power plants,” she noted. “But for any renewable project that is developed in Indonesia, it needs to be based on comprehensive research, in this case fish passage design for the tidal bridge and power plant development for the mitigation measures,” she said. “The project design and its implementation should consider and ensure it does not harm the environment and biodiversity, particularly marine mammals, turtles and whale sharks and their ecosystems,” added Hindun, stressing that the environmental assessment of this project should also take into account migration routes of fish and other marine mammals.  The tidal plant should also allow fishermen to pass through the straight easily, and consideration is also needed for the potentially increased sedimentation above and below the dams, so as not to impact local fisheries, she said. Eric van den Eijnden, chief executive officer, Tidal Bridge, told Eco-Business that research had been done to assess the environmental impact of the bridge on biodiversity in the area, and that the consequences would be “very limited”. He said that water speed would decrease as a result of the bridge, but this has “no known” environmental consequences. Eco-Business has requested for Tidal Bridge BV to share the results of its research, including the likely impact on local communities. The company has yet to produce its findings.  Van den Eijnden added that fish mortality at the hands of the massive turbines that power the plant would be “negligible” because the turbines are “fish-friendly”— designed to prevent fish from being crushed when they pass through it. Van den Eijnden added: “[Local] fishermen are very enthusiastic because we respect the shipping lanes and they can use the electricity to build cool cells. With this [electricity], they are able to freeze the catch and are thus able to build up a proper industry.”  Tidal power has proved to be controversial in Korea, home of the world’s largest tidal power plants, despite the technology’s renewable status. Environmental groups and fishermen in Korea have predicted that large tidal power plants will bring about deep and lasting harm to tidal ecosystems, fisheries and the landscape. They have also complained about a lack of environmental impact studies to investigate the potential impact of tidal power plants. Your support helps keep our journalism independent and our content free for everyone to read. Join our community here</t>
   </si>
   <si>
-    <t>Dutch begin trials to zap leaf litter from the tracks with LASERS By Richard Gray for MailOnline Published: 12:03 GMT, 4 December 2014 | Updated: 10:46 GMT, 30 July 2015 18 View comments For commuters it is perhaps the most baffling annual excuse for delays and cancellations on the railways: Leaves on the line. But there may now be a solution to the problem and it involves zapping autumn litter into oblivion with lasers. Dutch rail company Nederlandse Spoorwegen has revealed it is working with the Delft University of Technology and a British inventor to fit powerful lasers under two of its trains to burn away leaves from the tracks.  Scroll down for video  Falling leaves from trees beside railway tracks led to 4.5 million hours of passenger delays last year, so rail operators hope a new laser system will help them clear the dangerous leafy mulch that builds up on rails The technology will use intense beams of infrared light to vaporise the build up of material on the rails before the wheels of the train passes over them. Fallen leaves cause delays on the rail network because they can cover and stick to the tracks when wet. This can make the tracks slippery in itself, but the problem becomes worse when heavy metal train wheels pass over the top, as the leaves get sucked under the wheels and crushed, compacting the material into a hard, shiny substance that has been compared to Teflon. When this layer becomes wet, the tracks become excessively slippery and braking distances can double. Once stationary, trains can also struggle to get going again as they are unable to get traction on the tracks. Leaf mulch can also insulate train wheels from the rails, meaning signallers get less information about the location of trains on the network, meaning trains need to run with bigger spaces between them. Yet despite this, leaves on the line remains the excuse most likely to infuriate train travellers each autumn as they struggle to understand why rail companies cannot be better prepared for this problem. The perennial excuse of fallen leaves causing travel chaos has long been seen as a running joke, but according to Network Rail in the UK, leaves caused 4.5 million hours of passenger delays in 2013. The laser device sits just in front of the wheels while a specially designed suspension system helps to keep the high powered beam focused on the layer of mulch that builds up on rails as leaves get wet and break down Methods including brushing and grinding the rails, washing with jets of water or ice have all been tried, but with limited success. Now researchers at Delft University of Technology have been developing a system with the Dutch rail engineering firm Strukton Rail, the national network ProRail and train operator Nederlandse Spoorwegen. ‘We are now investigating whether offers laser solution,’ Jurjen Hendriks, one of the researchers at Delft University of Technology told the website Kennislink. The Laser Railhead Cleaner (LRC) which has been installed by the researchers on a Nederlandse Spoorwegen DM-90 train, sits under the train just in front of the wheels. Most current methods for removing mulch from train tracks use high powered jets of water to wash the rails The device uses a Nd:YAG laser to pulses of laser light with a wavelength of around 1,064 nanometres, which is infrared. According to experts the wavelength used is specifically absorbed by the leaves and other organic matter that can build up on the tracks, but not by metal. This means that the energy from the lasers is reflected off the rails without damaging them while the leaf material is vaporised, a process known as ablation. A spokesman for Strukton Rail said: ‘The LRC briefly heats the organic material on the rails and because the organic material expands more rapidly it separates from the rails. The Laser Railhead Cleaner system is being trialed underneath Nederlandse Spoorwegen DM-90 trains Lasers can be used to detect when fruits like apples, bananas, pears and tomatoes reach their 'peak' for eating. Researchers from Saint Joseph University in Lebanon and the Université de Bretagne Occidentale de Brest in France have developed a technique that looks at the speckling of the skin of fruits. As climacteric fruits like apples and bananas mature and ripen on the tree, it is important to pick them at exactly the right moment. After this point the fruit becomes vulnerable to fungi or starts to rot. The researchers found they could analyse the speckle patterns on the skin of Golden apples as they ripened by looking at the way the laser light was scattered and reflected from apple skin. This changed as the fruit ripened. The researchers hope the technique can be used to help farmers pick their fruit at exactly the right time. ‘What’s more, rust bursts away as well. The rails are cleaned and dried as a result, preventing any other material from adhering to them for some time. ‘Tests have shown that because they are solid, rails and other infrastructural objects are not damaged by the ablation process.’ The Laser Railhead Cleaner technology was first invented by a former Royal Navy Officer called Malcolm Higgins, who has developed the technology under the company name LaserThor. Tests on his technology between 1999 and 2004 were conducted by RailTrack and its predecessor Network Rail but revealed that it struggled to focus the laser correctly on the track due to vibrations as the trains picked up speed. However, Mr Higgins proved that dirt and moisture were vaporised from the track at speeds just over 6mph. He later teamed up with the German Fraunhofer institute in Aachen and the Rofin Sinar laser firm in Hamburg to develop a more powerful laser. This used a two kilowatts of infrared laser light that produced 25,000 pulses per second. This heated the leafy mulch to temperatures of more than 5,000 degrees, causing it to vanish from the rails. Further tests with Network Rail showed it was successful at speaks of up to 40mph, but Network Rail said it chose not to take the tests further. Mr Higgins has now been working with Strukton Rail and Delft University as a consultant on the project. They have been able to improve the system so that it can clean 20mm of rail head on both sides of the track at speeds of up to 50mph. Their device also uses a suspension system to help protect the optics of the laser from vibrations while the laser also temporarily switches off if it misses its target. Instead of lasers, Network rail said it is now concentrating on using high pressure jet washing technology to bash away leaf mulch and laying down a composite of sand and aluminium onto the tracks to aid traction. The laser is focused onto the rail head so that pulses of intense light vaporise any organic material that has built up on the surface of the tracks This year Network Rail has also begun using new technology called a tribometer, a handheld device that accurately measures how slippery the rails are, on its network in Merseyside. Data from this device is then used to assess the effectiveness of treatments and whether more are needed, according to the company. But lasers also have advantages as sand and water tanks need to be regularly refilled while water jets can damage the rails. They claim their laser is so precise it can etch a diagram into the head of a match without setting it alight.  Professor Rolf Dollevoet, who is leading the new trials at Delft University of Technology, said: ‘The question is not so much whether the laser system works, but for how long the rails will remain clean. ‘We’ll measure the remaining friction over time during rain, drizzle, frost and snowfall. ‘From these measurements NS and Prorail can derive at what frequency the 6,000km of track need to be lasered and how many trains have to be equipped with lasers to achieve that.’ Share what you think The comments below have been moderated in advance. The views expressed in the contents above are those of our users and do not necessarily reflect the views of MailOnline. We are no longer accepting comments on this article. Prince and Princess of Wales are bombarded with cheers of 'USA' and a smattering of boos at Boston Celtics basketball game - one hour after black Reverend gave lecture on 'colonialism and racism' at Earthshot launch amid Palace race row Published by Associated Newspapers Ltd Part of the Daily Mail, The Mail on Sunday &amp; Metro Media Group</t>
+    <t>Mumbai: Still awaiting those local AC trains? Here’s why trial run has been held up Though the order for the inductor was made in June, much time has been wasted in bringing it to Kurla car-shed, where currently the train is undergoing maintenance, officials said. The AC rake manufactured by the Bharat Heavy Electricals Limited (BHEL) and Strukton, a Netherlands-based firm, had arrived in Mumbai on April 1. CR authorities had already missed its earlier deadlines (May 16, June 30 and August 31) of conducting static trials. “Improper co-ordination between the manufacturers and CR authorities delayed the inductor for conducting trials. The instrument supposed to come in June will now be hopefully received by September, post which commissioning can be expected to begin trials,” a CR official said. Static trials of the rake will test the interface between the software and the equipment installed. Officials confirmed that out of a fourteen-day schedule of this phase of trials, thirteen have already been completed and the wait continues for the inductor. “Our team has successfully completed majority of trials of the AC rake. We are waiting for the inductor to be received, post which trials will be re-run to check smooth co-ordination between the motor coach and other coaches. The rake cannot be considered fit to run without doing so,” he added. Commissioning permission can be availed of by mid-September if the inductor is in place with CR authorities by September 1. The trials can begin from September 30 post which dynamic trials of the rake can be started. However, officials seem puzzled on deciding the line for conducting the trials. “As height of the AC rake could clash with some railway-over- bridges (ROBs) between route of Chhatrapati Shivaji Terminus (CST)-Kurla, conducting dynamic trials there will be difficult. Also, problems exist with conducting trials on trans-harbor line as well. It may thus run on the route between Kurla-Karjat or Kasara and then on Western Railway (WR) line for trials,” a senior CR official said. Also, officials confirmed it is too early to think about deciding fares or marking routes. “The rake is yet to qualify many trials. It may run on WR if Commission of Railway Safety certifies so. There is also a possibility that other AC rakes manufactured would be lower in height and would run on CR,” the official added. It is only after the prototype rake is set in place that the other AC rakes are constructed on a similar model. “After specifications are given to the Integral Coach Factory (ICF) about smooth running of this rake, the next one will come within a month. It is necessary that the first AC rake runs with the second in place as any operational issue with the first will require an immediate replacement with the second,” the official added. The Railways had placed an order for ten air-conditioned rakes from BHEL. Built at a cost of Rs 54 crore, the entire rake would be vestibule-connected and has a seating capacity of 1,208 and standing capacity of 4,936 passengers.   Mississippi man sentenced to 8 years for trying to join Islamic State Neha Kulkarni</t>
   </si>
   <si>
     <t>Ambassador of the Netherlands will present letters of credence to Bouterse Then Ernst Noorman(PHOTO), hitherto chargé d'affaires, will be allowed to present his credentials to President Desiré Bouterse. It's been over a year and a half. The adoption of the amnesty law caused the noise, The Hague recalled its ambassador. Since then, mutual efforts have been made to restore and improve. “We never argued. Diplomatic relations were just a bit difficult," says Foreign Minister Winston Lackin to de Ware Tijd. That there is some friction every now and then should not spoil the fun. The important thing is that both sides recognize the importance of stable relations. From the Surinamese side, it is in any case recognized that there is an advantage to be gained. The Dutch business community can make a substantial contribution to the development of Suriname. The Strukton company does this on a large scale with projects in the field of energy and railway development. The Dutch banking system finances several major projects. The Surinamese diaspora and tourism are also good reasons for healthy relationships. That's right, doing business with criminals is certainly not wrong. Especially if you can look into the future and see that Alibouta is always up for a Dutch party</t>
   </si>
   <si>
-    <t>Bouterse 'happy as a child' about energy savings ” This is how President Desiré Bouterse describes his mood about the substantial cuts in national energy consumption. More than seventeen megawatts were saved in one day and the head of state thanks society for that. “People have understood what it is all about,” said Bouterse in the radio program Bakana Tori. The savings far exceed expectations.” I had thought after our call that we would save four to five megawatts. But our people have proven that they understand what it's all about,” says Bouterse. The direct result is that the shortage of energy has almost been eliminated. Bauxite company Suralco had already promised to supply an additional twenty megawatts from the Afobakka power station. With the cuts, energy company EBS is now almost able to cover the need. The shortage was caused by the sudden shortening of the delivery. EBS does have a new diesel power plant with extra energy and Staatsolie also supplies tens of megawatts. The problem is that the infrastructure is not meant to handle more load. The Dutch company Strukton has been brought in to improve distribution. Bakabana torie is an NDP propaganda show of slimes of this killer. Report fortune teller, I think you are frustrated to make such statements Report ……</t>
-  </si>
-  <si>
-    <t>Enterprise Chamber refuses to give Centric CEO Sanderink his ‘support’ Sanderink seems unable to keep Centric’s interest separate from his private interests. Recent events give rise to doubts about Sanderink’s ability to make rational decisions.” The Enterprise Chamber of the Amsterdam Court of Appeal is unprecedentedly harsh on Thursday in its judgment on Centric CEO Gerard Sanderink. The IT service provider had drawn this along in the private quarrel that he had been fighting with his ex-girlfriend Brigitte van Egten for several years. And that was sufficient reason to grant the request of the Public Prosecution Service to immediately suspend Sanderink as director of Centric. He must also at least temporarily transfer his shares in the company to an external manager. According to the Enterprise Chamber, the public interest is being damaged too much by the lawsuits that Sanderink and Van Egten have been conducting back and forth for three and a half years. By instructing Centric to start a case against his ex-girlfriend earlier this year, Sanderink involved a company that performs crucial functions for governments, among others, in his private perils. The 2,500 employees in the Netherlands also suffer from the resulting loss of customers. “The recruitment of new staff is stalling, Centric’s Dutch activities have now become loss-making,” the Enterprise Chamber motivated its decision. “This poses an acute threat to the company. There is good reason to doubt the correctness of the policy pursued at Centric.” Two weeks ago, the Public Prosecution Service asked the Enterprise Chamber for further investigation into possible mismanagement at Centric after Sanderink had reappointed himself as CEO of the company. At the beginning of 2021, he had just left because of the unrest that had arisen. The case is unprecedented in the Netherlands. Rarely did the Public Prosecution Service start proceedings at the Enterprise Chamber to start an investigation into mismanagement at such a large company (turnover 2021: 422 million euros, approximately 3,800 employees). The request arose from a longer-running investigation by the justice system itself into the state of affairs at the company. The Public Prosecution Service was concerned that the continuity of the company’s services for customers (such as governments) and employees would be jeopardized if it did not intervene. Centric has not been doing well for a long time. Since Sanderink got into a relationship with the self-proclaimed and controversial cyber expert Rian van Rijbroek in 2018, several drivers had to leave or resigned themselves. Those involved have repeatedly outlined to NRC, among others, that Van Rijbroek’s involvement in the company had to do with this. She would make important decisions in the background and also draft emails on behalf of Sanderink. Read more about the key players in the Sanderink case here: Will Gerard Sanderink be forced to resign from Centric? Sanderink also fought and lost several legal battles with his ex-girlfriend, Brigitte van Egten, since the beginning of 2019. The entrepreneur has accused her for years of fraud at one of his companies, solar panel manufacturer DSS, where she was director. She would also have put terabytes of porn on that company’s server. The judge has never found any evidence for the various allegations. Sanderink now has to pay Van Egten for millions in penalty payments. Sanderink left little doubt on Thursday about who is to blame for his suspension: his ex-girlfriend and the media. “I made this company great. I got Strukton on track, I got Antea [Group] helped out,” he said, referring to other companies in his empire. “And now I can do that again. But I am being killed by negative reporting.” According to Sanderink and his lawyer Paul Acda, there is nothing wrong with Centric. When Acda gives his speech during the session on Thursday, it will only be about the negative way in which Sanderink would have been portrayed in the media for pages. Until the chairman of the Enterprise Chamber intervenes. “Mr. Acda, this case is about Centric. The first place in your defense that mentions that company is on page 5.” The immediate reason for the preliminary investigation that the Public Prosecution Service launched into Centric at the beginning of this summer was a seizure by the company at Van Egten. Centric claimed to have lost tens of millions of euros due to Sanderink’s ex-girlfriend. Customers would have walked away because of the negative publicity that all the legal battles have entailed. The IT company therefore had an attachment for 1.96 million euros from Van Egten. Coincidentally, that was exactly the amount that Sanderink had outstanding from his ex-girlfriend in previous lawsuits in penalties still to be paid. The judge therefore made short shrift of the attachment and accused Centric of abuse of law. This led to the resignation of several Centric directors who no longer wanted to be used for Sanderink’s private whims. Also read how the soap around Centric started: How the Automater Was Bewitched by the Cyber ​​Guru The Public Prosecution Service wanted to see how the unrest around Centric could be removed. According to the judiciary, which spoke to several former executives, the automation company is now in the red due to the high costs of hiring external staff and recruiting new customers. According to Sanderink, hiring external staff is necessary to “serve customers with specific knowledge that Centric does not have in-house”. To ward off the unrest, Centric itself wanted to expand the powers of its own works council (OR). He or she could also investigate abuses within the company itself. The condition was that Sanderink would not return as director. The works council and all directors of Centric outside Sanderink had already agreed to this. However, the option was blocked by the entrepreneur himself. He returned to the company shortly afterwards, after which several directors resigned. The only remaining member of the board – non-executive board member Peter Mous – was suspended by Sanderink on Wednesday afternoon after it turned out that he would support the request of the Public Prosecution Service. The works council itself was incredibly fierce about his owner on Thursday. “Customers want a supplier of impeccable conduct. Not a top executive who just throws all kinds of conspiracies into the world. It is extremely annoying that customers who are satisfied with the service still cancel contracts because they no longer want to be associated with Centric.” Sanderink himself did not want to hear it all. He said it was clear who should lead the company. Although there may be a director appointed by the Enterprise Chamber next to him who “does not have the deciding vote”. “You have seen that I can cause a turn-around in companies. I have the power and strength to get companies back on their feet.” And: “But will I get support from the judicial system? No. My mouth is being gagged. It would be nice if you would support us today by rejecting this request for suspension.” That support was not forthcoming on Thursday. A version of this article also appeared in the newspaper of November 4, 2022 Your email address will not be published. Required fields are marked * Comment * Name * Email * Website Save my name, email, and website in this browser for the next time I comment. Ruetir| Latest News, World News, Breaking News, Games,Technology, Business, Lifestyle, Fashion, Sports, Food &amp; Technology. Contact Us : [email protected] © Ruetir 2022. All Rights Reserved. © Ruetir 2022. All Rights Reserved</t>
-  </si>
-  <si>
-    <t>OM takes next step to depose Sanderink The company had been given until this Monday by law enforcement to take action, but that did not happen. The automation company announced last Wednesday that Sanderink, at the age of 74, will once again be in charge of the company that he set up in 1992 and of which he is still wholly owner. Also read: The Public Prosecution Service is reaching for a heavy means to depose Gerard Sanderink Sanderink’s companies (besides Centric, among others, infrastructure builder Strukton) have been restless for years because of the many changes at the top and the private legal conflicts that the entrepreneur is fighting with his ex-girlfriend. Those involved previously spoke in NRC about the important role that Sanderink’s current girlfriend – the controversial and self-proclaimed cyber expert Rian van Rijbroek – plays. It would, among other things, encourage the departure of several directors. Board members also became frustrated with her involvement in the companies. One of the reasons that the Public Prosecution Service is involved in the case is that many governments are customers of Centric. The Enterprise Chamber must now consider measures that are necessary to ‘guarantee the stability and continuity of Centric’. One of the questions that the Enterprise Chamber must now answer is whether there are reasons to conduct further investigation into the state of affairs at the IT company. At the same time, the Enterprise Section can impose temporary measures as long as the investigation is ongoing. Sanderink may then be temporarily suspended. In a second phase of the procedure, the Enterprise Section must consider whether there has been mismanagement at Centric. The appointed investigators have then completed their report with findings. If mismanagement is established, the Enterprise Section may decide to permanently remove Sanderink from his position as director. The voting rights that the Twente entrepreneur has as owner and with which he is concerned with the appointment of a new director may also be withdrawn. Centric has not yet responded to questions from NRC. Your email address will not be published. Required fields are marked * Comment * Name * Email * Website Save my name, email, and website in this browser for the next time I comment. Ruetir| Latest News, World News, Breaking News, Games,Technology, Business, Lifestyle, Fashion, Sports, Food &amp; Technology. Contact Us : [email protected] © Ruetir 2022. All Rights Reserved. © Ruetir 2022. All Rights Reserved</t>
+    <t>Bouterse 'happy as a child' about energy savings ” This is how President Desiré Bouterse describes his mood about the substantial cuts in national energy consumption. More than seventeen megawatts were saved in one day and the head of state thanks society for that. “People have understood what it is all about,” said Bouterse in the radio program Bakana Tori. The savings far exceed expectations.” I had thought after our call that we would save four to five megawatts. But our people have proven that they understand what it's all about,” says Bouterse. The direct result is that the shortage of energy has almost been eliminated. Bauxite company Suralco had already promised to supply an additional twenty megawatts from the Afobakka power station. With the cuts, energy company EBS is now almost able to cover the need. The shortage was caused by the sudden shortening of the delivery. EBS does have a new diesel power plant with extra energy and Staatsolie also supplies dozens of megawatts. The problem is that the infrastructure is not meant to handle more load. The Dutch company Strukton has been brought in to improve distribution. Bakabana torie is an NDP propaganda show of slimes of this killer. Report fortune teller, I think you are frustrated to make such statements Report ……</t>
+  </si>
+  <si>
+    <t>Will Gerard Sanderink be forced to resign from Centric? After the meeting between the two, more than four years of decisions followed that jeopardized the future of his companies to such an extent that the Public Prosecution Service deemed it necessary to intervene. On Thursday afternoon, the Public Prosecution Service demands further investigation into mismanagement at IT service provider Centric for the Enterprise Chamber at the Amsterdam Court of Appeal. In the meantime, Sanderink must be suspended as CEO and his shares – he also owns infrastructure builder Strukton, among others – must be placed with an external manager. The case is the next chapter in an unprecedented soap opera in the enterprising Netherlands. Rarely did a businessman listed in the Quote 500 make the news in such a way. Several executives and senior managers left his companies or were fired. He conducted dozens of lawsuits against his ex-girlfriend Brigitte van Egten, whom he accuses of, among other things, fraud and placing porn on the servers of one of his companies. Both claims have been brushed aside by the judge several times. In recent years, those involved have been clear about who is behind the accusations: his current girlfriend Van Rijbroek. She would feed Sanderink with information about conspiracies inside and outside his companies. In this way she would have set up Sanderink against administrators and other close contacts. Read more about the resignation of Centric directors in June 2022 here: Drivers leave again after a conflict with Gerard Sanderink In 2018, for example, the Centric board was in negotiations with a major customer, regulator De Nederlandsche Bank (DNB), when Sanderink suddenly threatened to intervene. He had understood through Van Rijbroek that DNB could not be trusted as a contract partner. The board managed to prevent the negotiations from ending in a fiasco after a tender that had been won, but the conflict did lay the foundation for an exodus of personnel from Centric and later Strukton and the engineering firm Antea Group. For the first time it became clear what influence Van Rijbroek had on Sanderink and what this could mean for his companies. Van Rijbroek is not officially employed by Centric, but he did think about, for example, a cybersecurity division that the company would start a few years ago (it is unclear whether this ever got off the ground). It is also suspected that various emails with accusations about Sanderink’s ex-wife Van Egten are from the Veghelse. At the beginning of 2021, things seemed to calm down around Sanderink’s companies. After Sanderink fell out against a bailiff, he left Strukton and Centric as a director. Sanderink had again had a dubious report with fraud allegations about his ex-girlfriend. The source of the allegations would again have been Van Rijbroek. The judge ordered the entrepreneur to rectify those allegations, but Van Egten wanted to know with whom they had been shared and had Sanderink’s mailbox and telephone seized from Strukton. When a bailiff came at the end of 2020 to copy the data, Sanderink threatened him and had his phone erased remotely. The fuss that arose about this led to such pressure from customers, among others, on the entrepreneur that he resigned from his board positions. However, he remained involved as a shareholder. It didn’t take long: later that year he made a comeback in Strukton’s group management. In June of this year, things got restless around Centric again. Three drivers left. In their view, Sanderink had abused his power by claiming compensation of 1.9 million euros through Centric previously awarded by the court to Van Egten. Sanderink thought that the company would have been damaged by statements that Van Egten made about Centric in various legal proceedings. The court rejected that claim at the time and accused Centric and Sanderink of abuse of rights. Also read: The Public Prosecution Service is reaching for a heavy means to depose Gerard Sanderink At the beginning of July of this year, the Public Prosecution Service announced that it would start a preliminary civil investigation into Centric. This happened after MP Pieter Omtzigt, among others, expressed his concerns about the consequences of the unrest at the company for government services (for example, in recent years it provided part of the IT infrastructure at the regulator DNB and many municipalities also use of Centric’s software). Central question in the Public Prosecution Service investigation: how can the continuity of the company be guaranteed? That research showed that there is a high turnover of staff, which makes the service provision vulnerable. Recently, several important customers have also canceled their contract with the automation company. While the investigation was in its final phase, Sanderink announced two weeks ago that he would return to Centric as a top executive. That was enough for the Public Prosecution Service. It asks the Enterprise Chamber to start an investigation into possible mismanagement at the company and to suspend Sanderink in the meantime and to transfer the shares to external management. For example, Sanderink cannot make important decisions at his companies during his possible suspension. The entrepreneur can defend himself against this on Thursday. Gerard Sanderink (74) from Twente founded the Sanderink Groep in 1992, later renamed Centric (turnover 2021: 422 million euros, approximately 3,800 employees). With the company, Sanderink provides IT services for, among others, (local) governments. Companies such as ASML and Spar also belonged to the clientele. Centric grew into one of the most important IT companies in the Netherlands through acquisitions of smaller competitors. In 2005 Sanderink took over the listed engineering firm Oranjewoud. Five years later, infrastructure builder and NS subsidiary Strukton (2020 turnover: 1.9 billion euros, 6,500 employees) was added. That company also came to hang under the Oranjewoud coat rack. Strukton was visited by the tax investigation service FIOD at the beginning of 2019. The Public Prosecution Service suspects that Strukton may be involved in paying bribes for a metro project in Saudi Arabia. At the beginning of 2022, Sanderink bought out the last strand of shareholders and took Oranjewoud off the stock exchange. In addition, Sanderink also owns solar panel company DSS. His net worth is now estimated by Quote at 505 million euros. Sanderink has been together with Rian van Rijbroek since the autumn of 2018. He previously had a long-standing relationship with Brigitte van Egten. Brigitte van Egten is Gerard Sanderink’s ex-girlfriend. During their relationship, Van Egten was director of Sanderink’s solar panel company DSS, from 2003 to 2018. The relationship lasted until November 2018, when Sanderink was now together with Rian van Rijbroek. Shortly afterwards, Sanderink accused Van Egten of, among other things, fraud at DSS. She also allegedly had several terabytes of porn put on DSS servers. No evidence has ever been found for this. Sanderink also said that Van Egten was behind the FIOD raid on Strukton. The two have been involved in lawsuits for years about Sanderink’s accusations and his statements. Sanderink has been sentenced to rectification several times. He has also been ordered to pay fines worth millions. Rian van Rijbroek (1969) is a cyber entrepreneur from Brabant (with his own company: MaMoMo, Make More Money) who gained national fame in 2018 with a highly criticized performance at Nieuwsuur. In it she stated, among other things, that the North Korean secret service was behind a series of (at the time recent) DDos attacks on Dutch banks. It later turned out that an eighteen-year-old Dutch boy was behind the attacks. Tech experts dismissed the claims as scaremongering and said they did not know Van Rijbroek. Research by various media also showed that at least part of Van Rijbroek’s CV turned out to be incorrect. Shortly afterwards, the Veghelse made the news again. A book she wrote with former politician and professor Willem Vermeend was withdrawn from the market when it turned out that various passages had been copied without citing the source. Since Van Rijbroek has been together with Sanderink, she has also become involved in several lawsuits. For example, Sanderink’s ex-girlfriend Brigitte van Egten tries to show that Van Rijbroek is the source of various accusations about her. Last year, Van Egten had several terabytes of data from Rian van Rijbroek seized. A judge is currently examining the extent to which Van Egten may gain access to this. Your email address will not be published. Required fields are marked * Comment * Name * Email * Website Save my name, email, and website in this browser for the next time I comment. Ruetir| Latest News, World News, Breaking News, Games,Technology, Business, Lifestyle, Fashion, Sports, Food &amp; Technology. Contact Us : [email protected] © Ruetir 2022. All Rights Reserved. © Ruetir 2022. All Rights Reserved</t>
   </si>
   <si>
     <t>Ground and groundwater remediation former drug lab After removing and disposing of the chemicals found, Strukton Milieutechniek carried out an exploratory and further soil investigation. These investigations showed that there was a soil and groundwater contamination with acetone and 2-propanol as a result of the production of hard drugs. Subsequently, soil remediation was carried out, in which the existing pavements, vegetation and underground foundations were removed, the highly contaminated soil was excavated and removed and the excavation was supplemented with clean sand. Subsequently, groundwater remediation took place. After treatment, the extracted groundwater was discharged into the Groote Molenbeek. The legal duty of care has been complied with, after which the location is again suitable for its original use. Ground and groundwater remediation in the municipality of Horst aan de Maas Activities By means of soil investigation, the extent of the contamination has been mapped out, as well as the parameters that are important for the approach and costs of the remediation. Subsequently, the existing soil and groundwater contamination was removed. The legal duty of care has been complied with and the location is once again suitable for its original use. By means of soil investigation, the extent of the contamination has been mapped out, as well as the parameters that are important for the approach and costs of the remediation. Subsequently, the existing soil and groundwater contamination was removed. The legal duty of care has been complied with and the location is once again suitable for its original use. Maximum unburdening for the client By taking care of the entire process of research, design, budgeting, permits and notifications and realization, Strukton Milieutechniek has unburdened the client as much as possible, achieving maximum results with minimal costs. Important aspects of this were a customized Water Act permit for the discharge of the treated water, the consideration of several remediation variants and the application, in addition to regular soil remediation, of an intermittent extraction regime with buffering to achieve specific flow dynamics in the soil for groundwater remediation. The remediation work was carried out in the built-up area. Strukton Milieutechniek has kept the nuisance for the surrounding area to a minimum by acting proactively and making sound agreements with the municipality, informing the surrounding area in good time and carrying out air quality measurements. As one Strukton Civiel, we have the professional and innovative clout to serve our customers – nationally and regionally. And we are building infrastructure on which the Netherlands can move smoothly</t>
@@ -662,10 +644,13 @@
     <t>Drug Lab Dismantling We have specialists with the experience and knowledge to dismantle a drug lab safely and professionally. Garage boxes, barns, stables or in a house: drug labs can be found everywhere. Recognizable mainly by the chemical smell. This smell arises because they process and mix chemical substances. A toxic and dangerous process. Strukton Milieutechniek has a great deal of experience in dismantling drug laboratories. We have specialists with the experience and knowledge to dismantle a drug lab safely and professionally. In addition, we have the right material and we can realize ADR transport. Drug dumping and drug labs are a common problem in the south of the Netherlands and are also becoming more frequent in other parts of the Netherlands. The source of the drug waste is a drug laboratory, the place where the production of drugs and the formation of the drug waste takes place. In almost all cases, the locations where the drug lab is located are highly contaminated with hazardous chemicals. For example, mercury chloride is used in the production of Crystal Meth. Mercury is a volatile substance which can cause serious contamination. This contamination can cause short and long-term damage to humans, animals and the environment. It also happens that drug labs are found on agricultural sites. The drug waste can then be dumped in manure cellars. Strukton Milieutechniek is immediately available to rid such manure pits of manure with drug waste or, in the worst case, drug waste with manure. After the clearing, we like to think along about a follow-up approach. Because walls and soil are polluted, a manure cellar can "evaporate" for a long time, with consequences for the immediate environment. We have specialists with the experience and knowledge to dismantle a drug lab safely and professionally. When dismantling a drug laboratory, it is important to check whether the soil is contaminated. Strukton Milieutechniek is also a soil specialist and is the right partner for clearing up drug laboratories for complete restoration of the crime scene in accordance with laws and regulations. Thanks to our extensive experience, we can immediately assist in clearing the drug waste after an evacuation of a drug laboratory. Because we have a unique environmentally licensed location and ADR transport, we can ensure the acceptance of the drug waste. We use our own waste flow numbers, then report it to the National Waste Reporting Center and then forward it to an accredited processor. Cleaning manure cellars can be extra difficult because manure grids can collapse. Even after cleaning, the manure cellar can continue to 'evaporate'. If this is the case, Strukton Milieutechniek can clean the air with its own 'air washing installation'. Strukton Milieutechniek offers advice, support and is available 24/7. In addition, we can offer various activities and supervise the entire process. Call 0800 - 2211 221. Available 24/7. The drug lab has been demolished and now needs to be cleaned up before we can remediate the soil Back of a drug lab A drug lab hidden in a separate room of a building A drug lab has burned down completely Manure cellars are increasingly crime scenes when drug waste is found Page Page Page</t>
   </si>
   <si>
+    <t>Dutch authorities raid Strukton on suspicion of bribery in Saudi Arabia Reach 97,000 UK and global construction experts. Strukton said yesterday it was "unpleasantly surprised" by the raid on 15 February conducted by the Dutch Fiscal Information and Investigation Service (FIOD). Strukton’s visualisation of the Riyadh metro It denied ever paying bribes, and has described circumstances of the tender by the FAST consortium, consisting of FCC, Alstom, Samsung and Strukton, for the metro project. "These events affect me personally and I am very sorry for all Strukton employees," said Strukton chief executive Gerard Sanderink. "I think it is important to emphasise that there is no question of bribery whatsoever. The project was awarded based on the lowest price." Strukton had a limited role in the consortium with share of around 15%, the company said. The consortium’s tender was submitted to the customer on 20 February 2013, and offered the lowest price for all six lines to be built, it said. In the end FAST got the contract for three of the lines – 4, 5 and 6 – with the other lines going to two other consortia. "We have now received some further information and we have been told that the FIOD based the decision for the raid on audits by the tax authorities, leading to suspicion of corruption and false declarations when obtaining a contract for the metro project in Riyadh. We fully cooperate and provide full insight to the FIOD," Strukton said in its statement. Strukton described the appointment of a company called Somo as an agent for the Riyadh project. Somo received a fixed percentage of the contract sum for its work to "facilitate us in this major, logistic challenge in a busy metropolis during the years of execution", Strukton said, adding Somo had no role in the pricing and submission of the tender. Payments to Somo were all transparent and traceable, Strukton said. Somo also provided "support by eliminating obstacles preventing us to operate in e.g. the case of political unrest", the company said</t>
+  </si>
+  <si>
     <t>Four K40 IBC 2C Fireguards for Strukton Milieutechniek Fire-resistant or insulated. Fire compartments for the safe storage of small packages and more. Heat storage Cooling or heating. Store at a constant temperature. Gas bottle storage - gas bottle storage according to all requirements. Fire resistant and ventilating. Strukton Milieutechniek The workshop is working hard to build four rack containers for Strukton Milieutechniek in Breda. When the K40 IBC 2C Fireguards are installed at the customer, they are used for drug waste storage. Strukton cleans up drug waste and thus contributes to 'the war on drugs'. We are happy that we can help them with this by supplying containers. To store the waste safely, each storage system has two fire-resistant compartments. This ensures that incompatible substances are kept separate. Each compartment has space for 6 IBCs and has a drip tray with a capacity of 1,100 litres. You can therefore use a shelf container with several fire-resistant compartments for the storage of hazardous and incompatible substances. We supply such storage systems in various shapes and sizes. Your wishes are central to us, so let us know how we can help you by calling 0487-560077 or sending an email to info@kokmilieu.nl. KOK offers environmental containers for the storage of environmentally hazardous substances. Expert in the field of customized environmental containers. More info? Visit the site! View storage systems that we can deliver directly</t>
   </si>
   <si>
-    <t>Dutch authorities raid Strukton on suspicion of bribery in Saudi Arabia Reach 97,000 UK and global construction experts. Strukton said yesterday it was "unpleasantly surprised" by the raid on 15 February conducted by the Dutch Fiscal Information and Investigation Service (FIOD). Strukton’s visualisation of the Riyadh metro It denied ever paying bribes, and has described circumstances of the tender by the FAST consortium, consisting of FCC, Alstom, Samsung and Strukton, for the metro project. "These events affect me personally and I am very sorry for all Strukton employees," said Strukton chief executive Gerard Sanderink. "I think it is important to emphasise that there is no question of bribery whatsoever. The project was awarded based on the lowest price." Strukton had a limited role in the consortium with share of around 15%, the company said. The consortium’s tender was submitted to the customer on 20 February 2013, and offered the lowest price for all six lines to be built, it said. In the end FAST got the contract for three of the lines – 4, 5 and 6 – with the other lines going to two other consortia. "We have now received some further information and we have been told that the FIOD based the decision for the raid on audits by the tax authorities, leading to suspicion of corruption and false declarations when obtaining a contract for the metro project in Riyadh. We fully cooperate and provide full insight to the FIOD," Strukton said in its statement. Strukton described the appointment of a company called Somo as an agent for the Riyadh project. Somo received a fixed percentage of the contract sum for its work to "facilitate us in this major, logistic challenge in a busy metropolis during the years of execution", Strukton said, adding Somo had no role in the pricing and submission of the tender. Payments to Somo were all transparent and traceable, Strukton said. Somo also provided "support by eliminating obstacles preventing us to operate in e.g. the case of political unrest", the company said</t>
+    <t>Who is Gerard Sanderink and why is Justice demanding his resignation from Centric? The Public Prosecution Service demands that Centric reverse the appointment before Monday. What is going on here? Five questions and answers. Where shall we start? First of all, a successful businessman, it must be said. The 74-year-old Sanderink built an impressive empire of companies from the ground up. We can rightly call the farmer's son born in Weerselo a self-made millionaire. Business magazine Quote estimated his assets at 550 million euros last year. That entrepreneurship started in 1978, when Sanderink founded his first company, ICT Automatisering, together with partner Hans Quellhorst. After selling his shares, he went his own way in 1992 and founded the Sanderink Group. In the years that follow, one company after another is taken over. Sanderink's merit is that it is often underperforming companies that he cleans up and incorporates. The rapidly growing company that was created in this way specializes in software and secondment and was renamed Centric around the turn of the century. With the proceeds, Sanderink also acquires engineering firm Oranjewoud (2005) and railway construction company Strukton (2010). But that reputation as a business doctor melts like snow in the sun from the end of 2018, after his breakup with his girlfriend Brigitte van Egten. According to insiders, she is also Sanderink's business support and rock, the two have known each other since 2002. Sanderink's new girlfriend is Rian van Rijbroek, a woman who steps out of the shadows in early 2018 and poses as cybersecurity expert and former Secret Service hacker. All fingers point to Van Rijbroek. She would play Sanderink and set him up against Van Egten and several executives of his companies. A period full of mudslinging and lawsuits begins. Nine top managers will leave Centric in 2019. Clients such as Action and NN ask questions about Sanderink's close relationship with the controversial Van Rijbroek, who at that time would help Centric set up a cybersecurity department. But for a man of his stature that may be too easy to think. Before that time, Sanderink was portrayed as a down-to-earth Twente native, averse to expensive stuff or outward display. Would someone with such a reputation, plus years of experience as a shrewd businessman, be so easily fooled? It is a question that will linger if a media storm arises around Sanderink and his affairs from 2019. Sanderink would see conspiracies everywhere and be convinced that the Public Prosecution Service and the government want to take everything away from him. Due to the 'unrest' surrounding his person, the underemployment of employees and the many lawsuits, Sanderink will step down in 2021 as a director at his companies Centric, Oranjewoud and Strukton. He still owns it. Now, more than a year later, several podcasts and a book have been published about the IT multimillionaire from Twente. With the same question every time: what happened to the man who built up his empire with 15,000 employees in relative peace for years? That is because on Wednesday it was suddenly announced that Sanderink will return as chairman of the board at Centric. The same press release states that two non-executive directors 'in good harmony' resign their duties and leave Centric. Incidentally, the company announced that Sanderink will focus on a new strategy for the ICT service provider in the coming period. A day later, the Public Prosecution Service makes itself heard. The Ministry of Justice announced publicly on Thursday afternoon that it had contacted Centric about the reappointment of Sanderink and the resignation of the two directors. "This reinforces the already prevailing unrest within Centric", the Public Prosecution Service writes, which immediately sets a deadline for Centric. The company has until next Monday to reverse the decision. This has everything to do with the services that Centric offers. The company (annual turnover 422 million euros) is part of the Dutch government. Municipalities use Centric for various matters such as their administration, digital services to citizens and have maintenance contracts with the company. Centric manages data centers and supplies software developers and IT managers to local governments, among others. Well-known companies such as ASML and Action also purchase services from Centric. Just like BNG Bank, the house bank of Dutch municipalities, provinces, housing associations and healthcare institutions, among others. The question is for how long. For example, the Social Insurance Bank (which manages and pays the AOW and child benefit, among other things) and the regulator De Nederlandsche Bank have already dropped out. BNG Bank is also said to be considering this. Then the Public Prosecution Service will report to the Enterprise Chamber of the Amsterdam Court of Appeal, the court for the business community. A highly unusual step, since the judiciary rarely interferes directly with the management of a company. The Enterprise Chamber has the right to intervene in the event of mismanagement at companies and to suspend directors. This usually happens after complaints from employees or shareholders involved. But in the case of Centric that is difficult: Sanderink is in control. "Stability at Centric is of great importance to the many employees and customers who depend on Centric's software, including a number of government agencies," the OM wrote on Thursday. But according to Justice, Centric itself is insufficiently able to restore peace. "The Public Prosecution Service therefore concludes that it is appropriate to request the Enterprise Chamber to decide whether, and if so, what measures are necessary to guarantee the stability and continuity of Centric." So to be continued</t>
   </si>
   <si>
     <t>Railway Maintenance Machinery Market Growth, Global Survey, ...| MENAFN.COM Forgot Username or Password Date (MENAFN- EIN Presswire) Railway Maintenance Machinery Market Railway maintenance machinery refers to the equipment used to maintain, repair and monitor railway tracks. SHERIDAN, WYOMING, UNITED STATES, November 18, 2022 /einpresswire.com / -- According to IMARC Group latest report titled“Railway Maintenance Machinery Market: Global Industry Trends, Share, Size, Growth, Opportunity and Forecast 2022-2027”, offers a comprehensive analysis of the industry, which comprises insights on railway maintenance machinery market research report . The report also includes competitor and regional analysis, and contemporary advancements in the global market. The global railway maintenance machinery market reached a value of US$ 4.25 Billion in 2021. Looking forward, IMARC Group expects the market to reach US$ 6.30 Billion by 2027, exhibiting a CAGR of 6.42% during 2022-2027. Railway maintenance machinery represents the equipment used to monitor and fix damages on railway tracks. They are primarily used for inspecting, repairing, and maintaining railway tracks to ensure smooth functioning and enhanced operational life of the railway tracks. Some of the commonly available railway maintenance machinery include tampers, ballast regulators, dynamic track stabilizers, ballast cleaners, undercutters, etc. They are extensively utilized for the mechanical maintenance of vertical and horizontal alignment of railway tracks. These devices find extensive applications in both ballast and non-ballast tracks to lift the sleeper and pack the ballast to prevent abrasion, deformation, change of geometry, damage to various components, etc. Request to Get the Free Sample Report: As the novel coronavirus (COVID-19) crisis takes over the world, we are continuously tracking the changes in the markets, as well as the purchase behaviours of the consumers globally and our estimates about the latest market trends and forecasts are being done after considering the impact of this pandemic. Market Trends: Continuous improvements in the railway infrastructures are among the key factors stimulating the railway maintenance machinery market. Apart from this, the rising investments by government bodies across countries in refurbishing the existing railway tracks to provide a secure, safe, and efficient travel experience to individuals are acting as significant growth-inducing factors. Furthermore, the increasing incidents of railway accidents and train derailments and the growing utilization of periodic maintenance activities that aid in preventing such incidents and minimizing the loss of lives and property are also propelling the market growth. Besides this, the widespread adoption of electric trains in place of fuel-powered trains and the inflating consumer environmental consciousness are also positively influencing the global market. Additionally, numerous technological advancements, such as the elevating integration of connected devices with the internet of things (iot) and artificial intelligence (AI) solutions, are expected to fuel the railway maintenance machinery market over the forecasted period. View Full Report with TOC &amp; List of Figure: Competitive Landscape with Key players:The report has also analysed the competitive landscape of the market with some of the key players being.•American Equipment Company Inc •China Railway Construction Corporation Limited •Geatech Group srl•Harsco Corporation•Loram Maintenance of Way Inc. •MATISA Industrial Materials S.A•Plasser &amp; Theurer•Speno International SA•Strukton•Teräspyörä-Steelwheel Oy Railway Maintenance Machinery Market Segmentation:Our report has categorized the market based on region, product type, application and sales type. Breakup by Product Type:•Tamping Machine•Stabilizing Machinery•Rail Handling Machinery•Ballast Cleaning Machinery•Others Breakup by Application:•Ballast Track•Non-Ballast Track Breakup by Sales Type:•New Sales•Aftermarket Breakup by Region:•North America (United States, Canada)•Europe (Germany, France, United Kingdom, Italy, Spain, Others)•Asia Pacific (China, Japan, India, Australia, Indonesia, Korea, Others)•Latin America (Brazil, Mexico, Others)•Middle East and Africa (United Arab Emirates, Saudi Arabia, Qatar, Iraq, Other) Key highlights of the report:•Market Performance (2016-2021) •Market Outlook (2022-2027)•Porter's Five Forces Analysis•Market Drivers and Success Factors•SWOT Analysis•Value Chain•Comprehensive Mapping of the Competitive Landscape We are updating our reports, If you want latest primary and secondary data (2022-2027) with Cost Module, Business Strategy, Competitive landscape, etc. Click request free sample report, the report will be delivered to you in PDF format via email within 24 to 48 hours after the payment confirmation. Browse Other Reports of IMARC Group: Location Based Advertising (LBA) Market: Third-Party Logistics (3PL) Market: Sterile Medical Packaging Market: Subscription E-commerce Market: Gasoline Market: About Us IMARC Group is a leading market research company that offers management strategy and market research worldwide. We partner with clients in all sectors and regions to identify their highest-value opportunities, address their most critical challenges, and transform their businesses. IMARC's information products include major market, scientific, economic and technological developments for business leaders in pharmaceutical, industrial, and high technology organizations. Market forecasts and industry analysis for biotechnology, advanced materials, pharmaceuticals, food and beverage, travel and tourism, nanotechnology and novel processing methods are at the top of the company's expertise.Elena Anderson IMARC Services Private Limited +1 631-791-1145 email us here MENAFN18112022003118003196ID1105203187 Railway Maintenance Machinery Market Railway maintenance machinery refers to the equipment used to maintain, repair and monitor railway tracks. SHERIDAN, WYOMING, UNITED STATES, November 18, 2022 /einpresswire.com / -- According to IMARC Group latest report titled“Railway Maintenance Machinery Market: Global Industry Trends, Share, Size, Growth, Opportunity and Forecast 2022-2027”, offers a comprehensive analysis of the industry, which comprises insights on railway maintenance machinery market research report . The report also includes competitor and regional analysis, and contemporary advancements in the global market. The global railway maintenance machinery market reached a value of US$ 4.25 Billion in 2021. Looking forward, IMARC Group expects the market to reach US$ 6.30 Billion by 2027, exhibiting a CAGR of 6.42% during 2022-2027. Railway maintenance machinery represents the equipment used to monitor and fix damages on railway tracks. They are primarily used for inspecting, repairing, and maintaining railway tracks to ensure smooth functioning and enhanced operational life of the railway tracks. Some of the commonly available railway maintenance machinery include tampers, ballast regulators, dynamic track stabilizers, ballast cleaners, undercutters, etc. They are extensively utilized for the mechanical maintenance of vertical and horizontal alignment of railway tracks. These devices find extensive applications in both ballast and non-ballast tracks to lift the sleeper and pack the ballast to prevent abrasion, deformation, change of geometry, damage to various components, etc. Request to Get the Free Sample Report: As the novel coronavirus (COVID-19) crisis takes over the world, we are continuously tracking the changes in the markets, as well as the purchase behaviours of the consumers globally and our estimates about the latest market trends and forecasts are being done after considering the impact of this pandemic. Market Trends: Continuous improvements in the railway infrastructures are among the key factors stimulating the railway maintenance machinery market. Apart from this, the rising investments by government bodies across countries in refurbishing the existing railway tracks to provide a secure, safe, and efficient travel experience to individuals are acting as significant growth-inducing factors. Furthermore, the increasing incidents of railway accidents and train derailments and the growing utilization of periodic maintenance activities that aid in preventing such incidents and minimizing the loss of lives and property are also propelling the market growth. Besides this, the widespread adoption of electric trains in place of fuel-powered trains and the inflating consumer environmental consciousness are also positively influencing the global market. Additionally, numerous technological advancements, such as the elevating integration of connected devices with the internet of things (iot) and artificial intelligence (AI) solutions, are expected to fuel the railway maintenance machinery market over the forecasted period. View Full Report with TOC &amp; List of Figure: Competitive Landscape with Key players:The report has also analysed the competitive landscape of the market with some of the key players being.•American Equipment Company Inc •China Railway Construction Corporation Limited •Geatech Group srl•Harsco Corporation•Loram Maintenance of Way Inc. •MATISA Industrial Materials S.A•Plasser &amp; Theurer•Speno International SA•Strukton•Teräspyörä-Steelwheel Oy Railway Maintenance Machinery Market Segmentation:Our report has categorized the market based on region, product type, application and sales type. Breakup by Product Type:•Tamping Machine•Stabilizing Machinery•Rail Handling Machinery•Ballast Cleaning Machinery•Others Breakup by Application:•Ballast Track•Non-Ballast Track Breakup by Sales Type:•New Sales•Aftermarket Breakup by Region:•North America (United States, Canada)•Europe (Germany, France, United Kingdom, Italy, Spain, Others)•Asia Pacific (China, Japan, India, Australia, Indonesia, Korea, Others)•Latin America (Brazil, Mexico, Others)•Middle East and Africa (United Arab Emirates, Saudi Arabia, Qatar, Iraq, Other) Key highlights of the report:•Market Performance (2016-2021) •Market Outlook (2022-2027)•Porter's Five Forces Analysis•Market Drivers and Success Factors•SWOT Analysis•Value Chain•Comprehensive Mapping of the Competitive Landscape We are updating our reports, If you want latest primary and secondary data (2022-2027) with Cost Module, Business Strategy, Competitive landscape, etc. Click request free sample report, the report will be delivered to you in PDF format via email within 24 to 48 hours after the payment confirmation. Browse Other Reports of IMARC Group: Location Based Advertising (LBA) Market: Third-Party Logistics (3PL) Market: Sterile Medical Packaging Market: Subscription E-commerce Market: Gasoline Market: About Us IMARC Group is a leading market research company that offers management strategy and market research worldwide. We partner with clients in all sectors and regions to identify their highest-value opportunities, address their most critical challenges, and transform their businesses. IMARC's information products include major market, scientific, economic and technological developments for business leaders in pharmaceutical, industrial, and high technology organizations. Market forecasts and industry analysis for biotechnology, advanced materials, pharmaceuticals, food and beverage, travel and tourism, nanotechnology and novel processing methods are at the top of the company's expertise. Elena Anderson IMARC Services Private Limited +1 631-791-1145 email us here MENAFN18112022003118003196ID1105203187 MENAFN18112022003118003196ID1105203187 Legal Disclaimer: MENAFN provides the information “as is” without warranty of any kind. We do not accept any responsibility or liability for the accuracy, content, images, videos, licenses, completeness, legality, or reliability of the information contained in this article. If you have any complaints or copyright issues related to this article, kindly contact the provider above. Tags Comments Category Date Followers    Likes itunes App Store RSS Daily(English) Daily(Arabic) All() World and Middle East business and financial news, Stocks, Currencies, Market Data, Research, Weather and other data. Contact Us Click here Tel: +962 6 5690450 Copyright © 2000 MENAFN. All rights reserved. Design &amp; Devleopment by MENAFN</t>
@@ -680,19 +665,19 @@
     <t>Toon Francken (90) 'not helped' if the government pays for cleaning up drug waste At the end of last week it was announced that citizens or municipalities whose drug waste is dumped on their territory can largely recover the cleaning costs from the national government from next year. This concerns an amount of up to 200,000 euros. In three cases, all of which occurred in Brabant, the cabinet has adopted a more generous attitude. The entire remediation operation is hereby reimbursed: Faton Bajrami, lawyer for the nineties: “I call it a wasp. The letter to parliament does indeed state that two hundred thousand will be released, but at the end it can also be read that governments such as the province and municipality must continue their attempts to recover the damage from the perpetrator. It is a gesture for the stage," the Breda lawyer clarifies. "I understand through the grapevine that the municipality of Zundert is sticking to its intention to pass on the costs to my client. She has already seized his house. B and W maintain that he is responsible for the dumping, even if experts prove otherwise.” Urgently requested In the meantime, Bajrami is of course not sitting still either. He had already initiated proceedings before the Council of State. The lawyer wants to challenge the decision of the mayor and aldermen of Zundert to have Francken pay for the costs. This week he will urgently urge the highest judicial body in our country. He will also request documents from the municipality that would show that Strukton Militeutechniek already concluded at the end of April 2020 that the contamination had originated in a ditch and therefore outside Francken's plot. It would also have been established that the contamination had spread via the ditch and the groundwater under the piece of land belonging to his client. The counselor will also ask BIJ12 for clarification. This nationally operating organization supervises the implementation of the subsidy scheme for the clearance of drug waste. Bajrami: “So extra money is set aside for cleaning up drugs from people like my client. Then it seems that you are innocent, but in practice I have serious doubts about the legal feasibility. Why else would the municipality stand firm like that?” Things are not going well with FranckenIncidentally, Francken hardly gets any of the discussion about the drug waste that was partly found on his territory. His (mental) health has taken a turn for the worse, partly due to the persistent accusations made by the municipality. Bajrami hopes to keep him out of the wind as much as possible. With new developments, he mainly has contact with his daughter. The municipality of Zundert confirms that it will recover the costs from Francken as the owner of the plot on Pater Taksweg. According to her, the drug discharge can be attributed to him, according to soil investigations. A spokesperson could not yet say when the soil remediation would begin. He also says that the municipality is pleased with the news that the government wants to think along and is willing to offer tailor-made financial solutions in this matter. READ ALSO: Drug waste dumped: this is how it is cleaned up (for a lot of money) Drug waste in nature, forest ranger Erik fought for years for compensation Toon Francken (90) must clean up drug waste: the municipality stands firm Did you see a mistake or do you have a comment about this article? Then please contact us. facebook twitter flickr instagram youtube soundcloud linkedin whatsapp</t>
   </si>
   <si>
+    <t>The Texel beach is full of wood and rubbish after storm Corrie. It takes days before everything is removed. Many balloon strings are also entangled in the waste, which are dangerous for birds.© Photo Sytske Dijksen Storm Corrie has left a lot of washing up on the Texel North Sea beach. On Thursday, Strukton Civiel started work on behalf of the municipality to remove wood and other bulky material. It is expected that the company will continue to do so on Friday. In addition to pallets, poles, branches and plates, many nets have washed ashore. Normally, wood - with the exception of pallets - is not disposed of because it is a natural product. In this case, however, large quantities are involved. Bulky plastic waste and nets are also taken along to ensure that they do not end up in the sea again. Large or heavy items washed ashore can also affect the foundations of beach pavilions. (Text continues below the photo) Strukton is cleaning up the North Sea beach on behalf of the municipality of Texel. © Photo Sytske Dijksen Nature photographer Sytske Dijksen from Den Hoorn, who can be found on the beach almost every day, noticed that the waste is all piled up in large heaps between Post 9 and Post 12 lay. There was nothing to be found at De Hors and at Paal 17. “Probably because there is so much coastal erosion here,” she thinks. She was also surprised that there is a lot of balloon ribbon on the beach again, while she had the impression that these ribbons, which are dangerous for birds, had decreased in number. Jutter Maarten Brugge had also noticed it and knows the reason: ,,Most balloon strings come from under the sand. Due to the exit, the old tide lines have been washed out again.” For example, he found Coca Cola labels from 2017 at Paal 22 north of De Koog. Do you want all the highlights from the news in your inbox every day?</t>
+  </si>
+  <si>
     <t>Cleaning up 1600 liters of drug waste in Eindhoven is a big job, the police are looking for a white box truck The police are looking for the perpetrator(s). Among other things, she adheres to a report from a witness who saw a white box truck driving around a quarter to ten on Sunday evening near a parking lot on Anconalaan. A liquid was leaking from this closed truck and a pungent chemical smell was said to be coming from it. The police strongly suspect that this vehicle was involved in the dumping. 'Busy days for Strukton'The waste was in three IBC Containers, which are large barrels with a volume of approximately one thousand litres. After part of the rubbish was discharged into the parking lot, the perpetrators continued until halfway along the service road along Eindhovenseweg, between Eindhoven and Son. This is where the containers were left behind. Claereboets: "These are busy days for us. Yesterday we had to clean up such a container in Nuenen. Now again in Eindhoven. It is unbelievable that this is happening more and more in the neighborhood where people live." The mess ended up on the service road and in the verge. A single sealing cap, hydrochloric acid and stench reminded us of the dumping in the early afternoon on Monday. Most of the road had to be closed for the cleanup. Claereboets: "It takes a lot of effort to clean up everything safely and responsibly." For example, a special transport had to be used to pump over the contents of the barrels that were not yet empty. The job will cost ten to twenty thousand euros, estimates Claereboets. Damage to the sewer seems to be not too bad. According to the police, part of the polluted area must be excavated and the sewer will also have to be cleaned. A spokeswoman for De Dommel Water Board reports that the damage to the sewer system seems to be not too bad. "There is so much water flowing through it that the water treatment plant will not be affected despite the horrible stuff. The sewer may have to be flushed with a thinner," she said. As a precaution, the water board was warned of possible damage on Sunday evening. Exactly what kind of rubbish it is is still being investigated. Specialists are conducting a trace investigation. 'Dumped from car before' The junk was dumped from a car or other vehicle. A spokesman for the police: "There are more examples of dumping from moving vehicles, at least it looked very similar given the way the waste was found." Mayor John Jorritsma of the municipality of Eindhoven reacted furiously: “This is yet another proof of the brutality and nonchalance of XTC criminals. It is unacceptable and very harmful. It undermines our society: nature, public health and safety and also our wallet, because municipalities are responsible for the clean-up costs. That is why we work closely with the police, Public Prosecution Service, Tax and Customs Administration, FIOD and other government services to tackle crime. Because every dumping is one too many. Perhaps festival-goers who use a pill can also realize this.”READ ALSO: Drug waste dumped from moving car, hydrochloric acid ends up in roadsides and sewersMore frequent hit in Eindhoven-NoordIt is the third drug bust in Eindhoven-Noord in a relatively short time. Last Monday, a cellar containing a cannabis nursery was found in a piece of forest on the border between Eindhoven and Son. In October last year, an underground hemp nursery was also found on the Anconalaan, near the Unitas '59 sports park. READ ALSO: Suddenly there are more drug dumping in Brabant, what is going on? Have you seen a mistake or do you have a comment about this article? Then please contact us. facebook twitter flickr instagram youtube soundcloud linkedin whatsapp</t>
   </si>
   <si>
     <t>Police are puzzled: where is the drug waste? Hanneke de Jonge Hanneke de Jonge The police are puzzled: last year more drug laboratories were dismantled than the year before, but less dumped drug waste was found than expected. Big question: where does that waste go? The images of leaking barrels and jerry cans dumped in a forest, ditch or along the road are well known. Manufacturers of synthetic drugs such as ecstasy and crystal meth easily discharge the chemical waste into nature. Two years ago this happened almost 300 times, last year that number had dropped by more than 100 dumping. While the number of drug labs found rose by a quarter. According to Max Daniel, Drugs portfolio holder of the National Police, one of the explanations is that the police receive reports more often when vans are driving around in a nature reserve. "You can no longer do that in good conscience, because then you run the risk that walkers - and there are now a lot of them - call and say: could this possibly be a dumping?" Daniel does not have the impression that fewer drugs are being produced in the Netherlands. "We see in all labs that we find, and there are more and more, that they are becoming more professional with faster procedures and larger boilers where larger quantities of drugs are made." It is inevitable that criminals get rid of their waste in a smarter way," he says. An example of such a smart way is the 'drug pit' that was found last March in the Brabant woods near Bergen op Zoom by forest ranger Erik de Jonge. He found a covered well on a hill of sandy soil where drug waste has probably been discharged for years. "We have never seen this before, I don't think it has ever been found in the Netherlands. But we had been afraid for a while that we would find this." Forest ranger Erik de Jonge would rather have seen that the waste was 'just' dumped in jerry cans. "They stand out, then you are often there in time . This well is a disaster." He suspects that the remediation of the soil could cost hundreds of thousands of euros. But rapid action is also important with a classic dumping. Leaking barrels pose a direct threat to the environment and public health. Leon van Zoggel in action. As a Dangerous Substances expert at Strukton, he and 24 colleagues are responsible for clearing up the chemical mess. They are ready day and night. They recently had a major job in Asten in Brabant. There was 1700 liters of drug waste dumped on a country road "I assume a lorry drove into this and tipped its load. And that is why the barrels have opened," says Van Zoggel. But he also sees this type of dumping decreasing. Where does it go? Van Zoggel suspects that it mainly disappears in manure cellars. "At the beginning of this year, we cleared three locations where the manure cellar of drug waste had been dumped. If you consider: rural area, there is no supervision, there is no social control, it is so easy to pull the lid off the draw pit where the farmer gets his slurry and then let your stuff run in there, a quick action" , explains Van Zoggel. The police are also aware that this is happening. "We regularly receive signals like this that farmers have been approached. We cannot exclude that there are people who are forced to do this and feel pressure from the criminal organization to make their space available. And there will probably be a few who turn a blind eye because it suits them financially," Daniel thinks. "We don't have a complete view of where the drug waste ends up. We also have signals that it is disappearing abroad, for example, where there is less supervision of the environment." But the police do not have hard evidence. And then there is the sewer. That is discharged into it, researchers from the KWR Water Research Institute have shown. They tested the sewage water of the Eindhoven region every day for three years, for three months. The large quantities we find can never be the result of use, these are traces of waste," says researcher Thomas ter Laak. Would it help the police if there were a national investigation? "That would indeed help. Combined with tips and our own information, it would certainly help us in the investigation," said Max Daniel. Nieuwsuur Binnenland Share article:</t>
   </si>
   <si>
-    <t>Kruispunt Deldenerstraat – Marskant weer open! Op 10 mei 2021 werd deze belangrijke kruising afgesloten. Een nieuwe inrichting voor de Deldenerstraat (vanaf de Langestraat tot aan de kruising Tuindorpstraat (inclusief Mitchamplein) en Marskant volgde. Iets meer dan een jaar later is de volledige kruising heringericht én weer open. Wethouder Gerard Gerrits is blij met de afronding van de vernieuwing van de Deldenerstraat: ‘Werkzaamheden aan een belangrijke invalsweg hebben veel impact in de stad. Ik ben blij met het begrip én geduld wat we de afgelopen jaren van onze inwoners hebben gekregen’. Want met het openen van de kruising komt er een einde aan een groot herinrichtingsproject in de Hengelose binnenstad. Dat project startte in 2019 met een nieuwe inrichting voor het deel tussen kruispunt Bornsestraat tot aan de Langestraat. In 2020 volgde het deel tussen de kruising Tuindorpstraat en kruising Geerdinksweg. De herinrichting van de Marskant, Deldenerstraat én de kruising rondom het Mitchamplein was de laatste horde. Door een prettige samenwerking met aannemer Strukton Civiel én gunstige omstandigheden is het project sneller afgerond dan oorspronkelijk de bedoeling was. Boven de grond is de herinrichting van het gebied duidelijk zichtbaar. Langs de Marskant en het Mitchamplein is de F35 doorgetrokken. Op de Bankastraat na ligt er nu door heel Hengelo een mooie veilige fietsverbinding. Ook zijn beide weghelften wat versmald, wat snel rijden ontmoedigt. Auto- en fietsverkeer heeft een eigen plek gekregen, zo veilig mogelijk voor alle partijen. Gerrits: ‘verkeersveiligheid is in ons beleid één van de speerpunten, de automobilist, fietser én voetganger hebben een eigen plek en dat bevordert de verkeersveiligheid’. Naast een verkeersveilige inrichting is het nieuwe ontwerp ook gericht op een efficiënte doorstroming voor alle verkeersdeelnemers. Nieuwe intelligente verkeerslichten zorgen voor efficiënte afwikkeling van het verkeer. Gerrits: ‘Mooi dat dit nu gerealiseerd is langs de gehele Deldenerstraat. Zo langzamerhand zien we die intelligente systemen op steeds meer plekken in de stad en dat komt de afwikkeling van alle verkeersstromen zeker ten goede!’ In het afgelopen jaar is ook veel werk verricht waar nu niets meer van te zien is. Onder de grond is het vuilwaterriool vernieuwd. Daarnaast is er een nieuw regenwaterriool aangelegd. Dit riool zorgt voor de afvoer van regenwater naar de Berflobeek. Dus geen schoon regenwater meer naar de rioolwaterzuivering maar afvoer via de natuurlijke manier: de beek. Klimaatadaptatie is dan ook een belangrijk onderdeel in dit project. Belangrijke wegen moeten toegankelijk blijven tijdens flinke hoosbuien. Door de rioolstelsels van elkaar te scheiden wordt het water op deze plek tijdens piekbuien beter afgevoerd. Verkeer heeft er op deze manier zo weinig mogelijk last van. In het hele gebied is ook meer ruimte gecreëerd voor groen. Het Mitchamplein heeft de parkeerfunctie behouden maar is flink vergroend. Ook langs de wegen zijn diverse plantvakken aangelegd. Aannemer Strukton Civiel zorgt de komende weken nog voor een finishing touch van het gebied. Het verkeer zal hier geen hinder meer van ondervinden. Nieuw toegangsbeleid Hengelose binnenstad Het bestaande toegangsbeleid voor de Hengelose binnenstad voldoet niet meer. Dat is de conclusie van uitgebreid onderzoek naar het verkeer en het gedrag van verkeersgebruikers in de binnenstad. Uit het onderzoek komt het rapport ‘Advies actualisatie toegangsbeleid binnenstad Hengelo’ voort. In dit rapport worden de maatregelen geadviseerd die de binnenstad weer autovrij moeten maken. Het college heeft ingestemd met het verder uitwerken en aanpassen van het toegangsbeleid zoals beschreven in het adviesrapport. Mobiliteitsplan: Heel Hengelo in beweging Hengelo is volop in beweging. We willen meer en betaalbare woningen bouwen. En onze economische positie als technologische topregio versterken. Dat betekent meer inwoners, meer bedrijvigheid en daarmee ook meer verplaatsingen. Daarom is er de afgelopen maanden hard gewerkt aan een mobiliteitsplan voor Hengelo. Wethouder Hanneke Steen is blij met het resultaat: ‘De titel ‘Heel Hengelo in beweging’ zegt het al, er gebeurt een hoop in onze mooie gemeente. En om de leefbaarheid, verkeersveiligheid en bereikbaarheid in Hengelo in de toekomst goed te houden, moeten we keuzes maken. Dat doen we in het mobiliteitsplan.’ Samenwerkende Twentse gemeenten sluiten contract met Vattenfall voor de levering van aardgas De Samenwerkende Twentse Gemeenten (DSTG) Borne, Enschede, Dinkelland, Haaksbergen, Hellendoorn, Hengelo, Hof van Twente, Losser, Oldenzaal, Tubbergen, Wierden en een aantal partners krijgen met ingang van 1 januari 2023 het aardgas dat ze verbruiken geleverd door Vattenfall. Drie gemeenten - Enschede, Hof van Twente en Losser - tekenden bovendien een overeenkomst met Twence voor de levering van groengas: een belangrijke bijdrage aan de duurzaamheidsdoelstellingen van zowel Twence als de gemeenten. Energiekrediet voor Hengelose bedrijven De gemeente Hengelo biedt een kredietmogelijkheid aan voor Hengelose bedrijven die door gestegen energielasten in de problemen komen. Deze kredietmogelijkheid geldt tijdelijk totdat de landelijke regeling ‘Tegemoetkoming Energie Kosten’ (TEK) van kracht wordt. Vraag van de maand Elke laatste dinsdag van de maand leest u hier over een kwestie waar veel mensen over belden naar de gemeente. Of waarover ze informatie zochten op deze site. Deze keer: Hengelose bushaltes worden aangepakt De komende maanden vernieuwt de provincie Overijssel de borden met reisinformatie bij bushaltes in de gemeente Hengelo. De nieuwe digitale informatieborden zijn moderner en een stuk energiezuiniger dan de oude. Op de digitale borden staat hoe laat de bussen vertrekken, informatie over vertragingen, omleidingen en alternatieve routes. De verwachting is dat de werkzaamheden aan de haltes eind juni 2023 zijn afgerond. College stelt bijna half miljoen beschikbaar voor zonneveld Boeldershoek De komst van een zonneveld in de Boeldershoek is weer een stap dichterbij. Het college van B en W wil een zogenoemd voorbereidingskrediet beschikbaar stellen van €489.120,-. De gemeenteraad moet dit bedrag nog goedkeuren. Het geld komt beschikbaar voor de netaansluiting, het opstellen van een plan en ontwerp voor de ontwikkeling en exploitatie van het zonneveld, aanvullend onderzoek en het participatietraject. Hengelo ontvangt van Rijksoverheid subsidie van € 15 miljoen Hengelo heeft vandaag vanuit Meerjarenprogramma Infrastructuur, Ruimte en Transport (MIRT) een subsidie van maar liefst € 15 miljoen ontvangen. De subsidie is bestemd voor de versnelde bouw van in totaal 1500 woningen in de binnenstad en Hart van Zuid. Om die versnelling te realiseren moeten nieuwe woningbouwlocaties goed bereikbaar zijn. Speciaal daarvoor heeft het Rijk het MIRT-programma in het leven geroepen. Twente Board blij met impuls van 30 miljoen euro voor spoorlijn Zwolle-Twente-Münster Twente Board is blij met de toezegging van het Rijk van 30 miljoen euro voor de treinverbinding Zwolle-Twente-Münster. Dit is van doorslaggevende betekenis voor het voortbestaan van deze spoorverbinding met onze Oosterburen. En dat is hard nodig, want alleen al tussen Enschede en Münster reizen dagelijks ruim tienduizend mensen op en neer. Wat gaat de gemeente doen in 2023? De Hengelose gemeenteraad heeft ingestemd met de Beleidsbegroting 2023 – 2026. Met daarin ruimte en ambitie voor nieuwe investeringen in de stad. Hengelo zoekt Junior Cyber Agents Een smartphone, laptop en/of tablet zijn niet meer weg te denken. Even snel wat opzoeken op Google of een Instagram story maken, we zijn er de hele dag mee bezig! Helaas niet altijd zonder gevaren! Welkom in het stadhuis van Hengelo! Bent u benieuwd hoe uw stadhuis er van binnen uitziet? De gemeente Hengelo nodigt u van harte uit voor het Open Huis op zaterdag 26 november van 10.00 tot 16.00 uur. Oekraïners langer in woningen Nijverheid De Oekraïense vluchtelingen die tijdelijk in de woningen van Welbions in de Nijverheid wonen, kunnen daar enkele maanden langer blijven. Welbions stelt de werkzaamheden voor de sloop en vervolgens nieuwbouw van de betreffende woningen in de Nijverheid uit tot na de zomervakantie van 2023. De reden hiervoor is de lange levertijd van de benodigde bouwmaterialen voor de nieuwbouw en het tekort aan personeel in de bouw. Aandacht voor Week van de Pleegzorg Soms zijn er omstandigheden waardoor een kind (tijdelijk) niet kan terugvallen op een veilige thuisomgeving. Gelukkig zijn er in Hengelo veel mensen die iets voor een ander willen betekenen, zoals pleegouders. Dat zijn vrijwilligers die een kind van een ander in hun huis én hart opnemen, tijdelijk of langer. En dat is hard nodig! Elk jaar zijn er veel nieuwe pleeggezinnen nodig. De gemeente is heel blij met de bijna 80 Hengelose pleeggezinnen. Daarom biedt de gemeente alle pleeggezinnen een cadeaukaart aan. College stemt in met omgevingsvisie ‘Hart van Hengelo’ Het college van B en W heeft op 11 oktober ingestemd met de omgevingsvisie ‘Hart van Hengelo’. Deze visie gaat over de Binnenstad en Hart van Zuid. Het college stelt de gemeenteraad voor om de omgevingsvisie vast te stellen. Vraag van de maand Elke laatste dinsdag van de maand leest u hier over een kwestie waar veel mensen over belden naar de gemeente. Of waarover ze informatie zochten op deze site. Gemeente zet duizenden lichten uit Op zaterdagavond 29 oktober is het van 20.00 tot 21.00 uur pikkedonker in de stad. De gemeente zet dan duizenden openbare lichtpunten uit. Aanleiding is de jaarlijkse Nacht van de Nacht. Op deze avond vragen verschillende organisaties en instellingen aandacht voor lichtvervuiling en energiebesparing. In de bibliotheek zijn op deze avond activiteiten in het donker. Verlichte tocht Licht in het donker en Allerzielenviering Nabestaanden kunnen hun dierbaren gedenken tijdens twee gezamenlijke herdenkingsbijeenkomsten. Op woensdag 26 oktober is er een verlichte tocht over het begraaf- en gedenkpark aan de Oldenzaalsestraat. Op zondag 6 november is de Allerzielenviering op het begraaf- en gedenkpark aan de Deurningerstraat. Bladruimen start 24 oktober Het is herfst, de tijd van vallende bladeren en mooie kiekjes. De gevallen bladeren kunnen soms ook zorgen voor gevaarlijke situaties bijvoorbeeld op straten en fietspaden. Daarom starten Gildebor en groenaannemers vanaf maandag 24 oktober met het verwijderen van bladeren in de openbare ruimte. Door de warme en droge zomer is dat een weekje eerder dan u gewend bent. Lambertusbasiliek op zwart voor duurzaamheidscampagne Op maandagavond 17 oktober blijft de Lambertusbasiliek donker. Op deze manier wil de gemeente Hengelo aandacht vragen voor de lancering van de landelijke campagne ‘Zet ook de knop om’. Deze campagne is in het leven geroepen om mensen te helpen met energie besparen. Wolfkaterweg in beeld voor woningbouw De gemeente Hengelo heeft met twee grondeigenaren een optieovereenkomst gesloten om twee percelen grond aan te kopen aan de Wofkaterweg in Beckum. De gemeente is met onder meer de Dorpsraad Bruisend Beckum de mogelijkheden aan het onderzoeken om woningen te bouwen in en rondom Beckum. Dat is nodig voor de leefbaarheid in Beckum. Energieregeling Hengelo: 800 euro en gratis energieadvies De gemeente Hengelo gaat huishoudens die niet in aanmerking komen voor de landelijke energietoeslag dit jaar nog helpen. De gemeenteraad heeft ingestemd met de Hengelose energieregeling van eenmalig 800 euro én gratis energieadvies. De raad stelt hier 2,8 miljoen euro voor beschikbaar. Aanvragen kan vanaf 10 oktober a.s. Trebbe ontwikkelt samen met Stork en gemeente Hengelo visie op Stork-locatie De gemeente Hengelo, Stork en Trebbe gaan samen een integrale herontwikkelingsvisie opstellen voor de voormalige Koninklijke Machinefabriek Stork (KMS) locatie aan het Industrieplein in Hart van Zuid in Hengelo. Taalpunt Hengelo gecertificeerd Wethouder Jacqueline Freriksen heeft het kwaliteitscertificaat van het CBCT uitgereikt aan Taalpunt Hengelo. Met de certificering wordt nog duidelijker wat voor belangrijke schakel Het Taalpunt is. Coming Out Dag: 11 oktober 2022 Dinsdag 11 oktober is het internationale Coming Out Dag. Dit is de dag waarop we wereldwijd stilstaan bij het uit-de-kast-komen van lhbti's en queer-personen. Dit is nog lang niet voor iedereen vanzelfsprekend. Hengelo hangt dan de Progressvlag uit, de opvolger van de regenboogvlag. Als symbool dat iedereen erbij hoort in Hengelo. Investeren in de toekomst ondanks onzekere tijden Het college van B en W biedt een structureel sluitende Beleidsbegroting 2023-2026 aan de gemeenteraad aan. Met daarin ruimte en ambitie voor nieuwe investeringen in de stad, ondanks onzekere gemeentefinanciën op de lange termijn. Hanneke Steen, wethouder Financiën: ‘Juist nu willen en moeten we investeren daar waar dat het hardst nodig is’. Het college werkt aan een strategische agenda, om hier richting aan te geven. Burgemeestersontbijt Burgemeester Sander Schelberg ontbijt vrijdag 7 oktober met kinderen van IKC Esrein. Dit in het kader van de week van het jaarlijks Nationaal Schoolontbijt. Bakkerij Nollen zorgt voor een lekker en gezond ontbijt. Zilveren Erepenning voor Hengelose Amateur Fotografen Vereniging Zaterdag 1 oktober 2022 zal wethouder Marie-José Luttikholt de Zilveren Erepenning van de stad overhandigen aan de voorzitter van de Hengelose Amateur Fotografen Vereniging (HAFV) Jan van Asveld. Dit gebeurt om 15.00 uur op het Evenementenplein bij het stadhuis aan het Burgemeester Jansenplein, bij de opening van de expositie Hengelo Bepalend. Vluchtelingen Nijverheid naar Hazenweg Begin volgend jaar verandert er iets voor de Oekraïense vluchtelingen die nu verblijven in de woningen van Welbions in de Nijverheid. Zij verhuizen in februari 2023 naar de bestaande opvanglocatie aan de Hazenweg. De vluchtelingen en de omwonenden van de Hazenweg zijn daar afgelopen weekend over geïnformeerd. Week tegen Eenzaamheid Van 29 september tot en met 6 oktober is het de Week tegen Eenzaamheid. Ook u kunt vandaag iets betekenen voor iemand die zich eenzaam voelt. Hebt u een familielid, vriend of buur die hier last van heeft? Er is altijd wel iets dat iemand leuk vindt om te doen, samen met u of met anderen. Een steuntje in de rug kan veel betekenen. Duurzaamheidsmarkt bij stadhuis Op zaterdag 8 oktober staat er op het plein voor het stadhuis een grote duurzaamheidsmarkt. Belangstellenden kunnen hier bij verschillende kraampjes terecht voor alles wat met duurzaamheid te maken heeft. De wooncoaches van Hengelo Energie zijn bijvoorbeeld aanwezig om advies te geven over isoleren en besparen, maar ook over de aanschaf van een warmtepomp of zonnepanelen. Gemeente zet veteranen weer in het zonnetje Op zaterdag 24 september zet Hengelo voor de 14e keer de Hengelose veteranen in het zonnetje. Zo’n 135 veteranen reageerden op de uitnodiging van burgemeester Sander Schelberg en komen naar de Hengelose Veteranendag. Omgevingsvisie stedelijk gebied Zoals u weet zijn we al druk bezig met de omgevingsvisie Hengelo. Op dit moment zijn we bezig met de derde fase van de omgevingsvisie, het stedelijk gebied. Vanaf 3 september gaan we inwoners en ondernemers uit het visiegebied bevragen over hun (fysieke) leefomgeving. Sluiting pand aan Slachthuisweg Burgemeester Sander Schelberg heeft een pand aan de Slachthuisweg in Hengelo voor zes maanden gesloten. Dit op grond van de APV en de Gemeentewet naar aanleiding van (politie)onderzoeken in dit pand. Tijdens de laatste doorzoeking van het rechercheteam zijn meerdere goederen in beslag genomen. De sluiting van het pand gaat per direct in. Update: Vervanging verkeerslichten Oldenzaalsestraat en Weideweg Van 12 september tot en met 2 december worden verkeerslichten op zeven locaties in Hengelo vervangen. Er wordt gestart aan de Weideweg, vanaf 17 oktober is de Oldenzaalsestraat aan de beurt. Het verkeer kan, met enige hinder, gebruik blijven maken van de kruispunten. Zilveren Erepenning voor Wijkcentrum ’t Lansink Op donderdag 1 september reikte wethouder Marie-José Luttikholt de zilveren Erepenning uit aan de voorzitter van het Wijkcentrum ’t Lansink, de heer Jan Willem Korenromp. Dit ter ere van het 100-jarig jubileum bij Wijkcentrum. Hengelo ontvangt van ministerie van EZK subsidie van € 4,8 miljoen Vandaag heeft het ministerie van Economische Zaken en Klimaat (EZK) bekend gemaakt een subsidie van € 4,8 miljoen aan Hengelo te verstrekken. De subsidie komt voort uit het programma Impulsaanpak Winkelgebieden (IW). Het is bestemd voor de herinrichting van het gebied achter het voormalige V&amp;D pand. Het gaat om de locatie tussen de Marskant en de Beekstraat. Dit gebied wordt getransformeerd van winkelgebied naar woongebied. Lambertuskermis allereerste kermis zonder uitstoot van fossiele brandstof Een primeur op de Hengelose Lambertuskermis dit jaar! Van 14 tot en met 18 september draaien alle attracties op accustroom. Dit betekent dat de attracties voor het eerst niet aangedreven worden door een dieselaggregaat; een unicum. Nog niet eerder heeft een kermis in Nederland volledig gedraaid op accustroom. Winkelcentrum Slangenbeek bijna 700 m2 groen rijker In het voorjaar van 2021 won de vergroening van het Winkelcentrum Slangenbeek de stemronde voor Van Grijs naar Groen in Slangenbeek. Bijna 700 vierkante meter verharding in het winkelcentrum is vergroend. Een prachtig resultaat! En er gebeurt nog veel meer! 30 nieuwe inwoners in de opvanglocatie aan de Hazenweg Dinsdagavond 12 juli hebben dertig nieuwe inwoners intrek genomen in de vluchtelingenopvanglocatie aan de Hazenweg. Het gaat om kinderen met hun moeders en enkele vaders, van diverse nationaliteiten. Veiligheidsregio Twente heeft samen met de veertien Twentse gemeenten toegezegd om voor 225 noodplekken en dus extra opvang te zorgen om de locatie in Ter Apel te ontlasten. Wooncoaches klaar om Hengeloërs te helpen met verduurzamen De gemeente Hengelo en Coöperatie Hengelo Energie willen huiseigenaren stimuleren om hun woningen te verduurzamen. Dat houdt in dat de wooncoaches adviezen gaan geven hoe Hengeloërs energie kunnen besparen door bijvoorbeeld hun woning goed te isoleren, maar ook hoe ze zelf energie kunnen opwekken met bijvoorbeeld zonnepanelen; de meest groene energie is immers de energie die niet gebruikt hoeft de worden. Ook moet deze aanpak armoede als gevolg van hoge energielasten tegengaan. 200 tijdelijke huurwoningen in Groot Driene Voor jongeren, studenten en spoedzoekers is het momenteel moeilijk om betaalbare en geschikte woonruimte te vinden. Gemeente Hengelo, woningcorporatie Welbions en ontwikkelcombinatie Leyten-Trebbe slaan de handen ineen om snel enige verlichting op de woningmarkt te brengen. Het resultaat is dat er 200 tijdelijke huurwoningen worden geplaatst op de voormalige ROC-locatie aan de Sportlaan Driene in Hengelo. Reset van sociaal domein Het college van B en W windt er geen doekjes om; het sociale domein van de gemeente Hengelo moet grondig veranderen en wel nu. IKEA opent nieuwe zonnecarports met meer dan 3400 zonnepanelen IKEA Hengelo heeft 3.460 zonnepanelen geplaatst op de parkeerplaats. De vestiging heeft extra oppervlakte voor de panelen gecreëerd met zogenoemde zonnecarports boven de parkeerplaatsen. De zonnepanelen van IKEA Hengelo wekken 1.8 megawattpiek per jaar op. Strategische agenda voor gezonde toekomst Het college van B en W wil de komende jaren samen met de gemeenteraad, inwoners en partners bouwen aan een strategische agenda voor de toekomst. Zodat er geld beschikbaar is en blijft om te investeren in de stad, juist daar waar dat het hardste nodig is. Het college stelt de raad voor om deze agenda binnen een jaar op te stellen. In de Zomerbrief geeft het college een eerste aanzet voor de strategische koers. De gemeenteraad bespreekt de Zomerbrief op 12 juli tijdens een politieke markt. Intrekkingsbesluit 'noodverordening boerenprotest Twence' De toegangswegen naar de afvalverbrandingsinstallatie van Twence waren geblokkeerd. Politieke Markt Vanavond in het stadhuis Bus en aanhanger met ‘drugsvaten’ zorgt voor meldingen van Twentse inwoners De afgelopen weken heeft op verschillende plekken in Twente een bus en aanhanger vol met ‘drugsvaten’ en materialen voor de productie van drugs gestaan. Met deze actie vragen politie en gemeenten in Twente aandacht voor het thema drugscriminaliteit en werd er gekeken in hoeverre inwoners bereid zijn een verdachte situatie te melden. Dit leverde een wisselend beeld op. SchouwArt mag podium voor beeldende kunst vormgeven Hengelo is weer een stap dichterbij een permanent podium voor beeldende kunst. Vernieuwde Elsbeek feestelijk geopend Op donderdag 23 juni werd de vernieuwde Elsbeek in Hengelo officieel geopend. Het terrein naast de Elsbeek was voor deze gelegenheid feestelijk aangekleed en samen met omwonenden en samenwerkende partijen werd de opening van de Elsbeek gevierd. Woninginbraak: Je zou het maar meemaken Stel je voor. Na en dag werken, ga je nog even samen met de hond op bezoek bij familie. Rond 17.00 uur ga je weg en twee uur later word je gebeld door de buurvrouw ‘volgens mij is er ingebroken bij jou’. In paniek rijd je naar huis en wat je daar aantreft, blijft je tot op de dag van vandaag bij. Tweede omgevingsvisie ter inzage De wereld om ons heen verandert snel. Op hetzelfde moment spelen diverse grote trends op het gebied van demografie, technologie en klimaat. Deze leiden in ons land tot een aantal grote ruimtelijke opgaven. De komst van online winkelen zet centrumgebieden onder druk, de inwoners en behoeftes veranderen, er is een grote vraag naar woningen en we hebben samen een grote duurzaamheidsopgave. Met de omgevingsvisie wordt ingespeeld op deze maatschappelijke ontwikkelingen en wordt er richting gegeven aan de toekomstbestendige stad. De visie ligt tot en met 26 juli ter inzage en op 23 juni is er een informatieavond in de stadhuishal. Een exclusief interview met Special Olympics-atleten Friso Roeleveld en Sanne Droste! Nog een paar dagen en dan gaan de Special Olympics Nationale Spelen (SONS) Twente officieel van start met een grandioze openingsceremonie en atletenparade in het FBK-stadion. Boeldershoek in beeld voor zonneveld Vattenfall wil een zonneveld ontwikkelen in het energiegebied bij Twence en heeft een principeverzoek ingediend bij de gemeente. De gemeente is hiermee akkoord. De locatie van Vattenfall grenst aan het gebied waar de gemeente Hengelo ook een zonneveld wil ontwikkelen. De gemeente heeft Vattenfall uitgenodigd om in gesprek te gaan over de invulling en voorwaarden, zoals de participatie van omwonenden en omliggende bedrijven. Avondopenstelling Milieupark Ook dit jaar is het Milieupark aan de Wegtersweg in augustus op donderdagavond tot 20.00 uur geopend. Op donderdag 2 juni is dit jaar de eerste avondopenstelling. Met de avondopenstelling in de zomermaanden is het voor meer mensen mogelijk het Milieupark te bezoeken. Nieuwe wethouders benoemd Tijdens een speciale raadsvergadering op 25 mei zijn de Hengelose wethouders benoemd. Voor BurgerBelangen neemt Jacqueline Freriksen deel aan het college, voor de VVD Gerard Gerrits, voor het CDA Hanneke Steen-Klok, voor de PvdA Marie-José Luttikholt en voor D66 Claudio Bruggink. Kruispunt Deldenerstraat – Marskant weer open! Op woensdag 25 mei is het kruispunt Deldenerstraat weer open voor alle verkeer. Op 10 mei 2021 werd deze belangrijke kruising afgesloten. Een nieuwe inrichting voor de Deldenerstraat (vanaf de Langestraat tot aan de kruising Tuindorpstraat (inclusief Mitchamplein) en Marskant volgde. Iets meer dan een jaar later is de volledige kruising heringericht én weer open. Wethouder Gerard Gerrits is blij met de afronding van de vernieuwing van de Deldenerstraat: ‘Werkzaamheden aan een belangrijke invalsweg hebben veel impact in de stad. Ik ben blij met het begrip én geduld wat we de afgelopen jaren van onze inwoners hebben gekregen’. Erepenning voor Volksuniversiteit Hengelo Op vrijdag 20 mei reikt wethouder Claudio Bruggink de gemeentelijke Erepenning uit aan de Volksuniversiteit Hengelo. De uitreiking vindt om 13.30 uur plaats bij de Gieterij (ROC van Twente) tijdens de viering van het 100-jarig bestaan van de Volksuniversiteit. Dit jubileum wordt een klein jaar later gevierd, omdat het vanwege de eerdere coronabeperkingen niet door kon gaan. Inwonerspeiling Doe mee en vul de vragenlijst in! Nog geen rookmelders? Er komt een nieuwe wet aan: vanaf 1 juli 2022 zijn rookmelders op iedere verdieping verplicht. Gelukkig is het plaatsen zo gedaan. Heb je het altijd uitgesteld? Dan is dit het moment om rookmelders te plaatsen. Peter Schuurmans van Veiligheidsregio Rotterdam-Rijnmond legt uit hoe je in drie eenvoudige stappen rookmelders kunt plaatsen. Uitkomst college-onderhandelingen De afgelopen weken hebben de partijen BurgerBelangen Hengelo, VVD, CDA, PvdA en D66 intensief met elkaar gesproken over de (toekomst)plannen voor Hengelo. Met een goed resultaat, er is overeenstemming bereikt! Uitreiking Nijverbij aan Erwin Bolhaar Op dinsdag 17 mei reikt wethouder Bas van Wakeren het Stadscompliment, De Nijverbij, uit aan de heer Erwin Bolhaar. De uitreiking vindt plaats om ca. 14.30 uur in Woonzorgcentrum Herinckhave, Backenhagenlaan 76. Pas uw huis aan met ‘Lang zult u wonen’! U woont met plezier in uw eigen buurt en hoopt zo lang mogelijk te kunnen blijven wonen waar u nu woont. Hoe maakt u uw huis daar geschikt voor? Scholen uit Hengelo, Twenterand en Berkelland strijden tegen textielafval De Textiel Race is een initiatief van Knol Recycling. Het project is officieel van start gegaan met een kick-off met Wethouder Bas van Wakeren op de Wilbertschool. Positieve waardering binnenstad blijft De waardering voor de binnenstad handhaaft zich op een stabiel niveau. Sinds 2019 stijgt de waardering voor de binnenstad na jarenlange afname. Dit blijkt uit de jaarlijkse binnenstadspeiling onder leden van het Hengelopanel in 2021. Aan de ondervraagden zijn elf te waarderen aspecten voorgelegd. Ten opzichte van 2020 is er meer variatie in de waardering te zien. De positieve waardering van de sfeer en ‘de binnenstad in het algemeen’ is licht gestegen. Opvallend deze keer is toename van de waardering voor het ‘groen’ en de daling voor ‘de kwaliteit van het winkelaanbod’. Alleen folders in de bus met Ja-sticker Vanaf 1 juni 2022 geldt in Hengelo de Ja-sticker. U ontvangt dan alleen reclamefolders als u een Ja-sticker op uw brievenbus plakt. Doet u niets, dan krijgt u geen reclamefolders. Met de Ja-sticker wil de gemeente papierverspilling verminderen. Een gemiddeld huishouden ontvangt per jaar zo’n 26 kilo reclamedrukwerk. Een groot deel hiervan belandt ongelezen bij het oud papier. Primeur in Hengelo; groen licht voor groepen fietsers Op de kruising van de Rondweg/Bornsestraat (afrit A1) ter hoogte van Plein Westermaat, starten provincie Overijssel en de gemeente Hengelo de allereerste proef met de zogeheten Fietsketting. Gemeente gesloten op 5 mei De gemeente is donderdag 5 mei (Bevrijdingsdag) gesloten. Hengelo krijgt er fraaie woonlocaties bij Binnen afzienbare tijd start de verkoop van 28 bouwkavels aan de Marskant en 13 bouwkavels van het plan ‘Broek aan het Pad’. Geïnteresseerden kunnen donderdagavond 12 mei tijdens een informatieavond terecht in het stadhuis in Hengelo. Vrijheid in Verbondenheid Op donderdag 5 mei vieren wij Nationale Bevrijdingsdag. Op de vooravond daarvan, op woensdag 4 mei, worden ook in Hengelo de slachtoffers herdacht die in Nederland of waar ook ter wereld zijn omgekomen of vermoord sinds het uitbreken van de Tweede Wereldoorlog, in oorlogssituaties en bij vredesoperaties. Daarom wordt om 20.00 uur twee minuten stilte in acht genomen. Bij het herdenkingsmonument voor het stadhuis worden kransen gelegd. € 145.000 voor vernieuwing en versterking culturele programmering Afgelopen winter moesten veel culturele instellingen de deuren weer sluiten door de lockdown. Nu er weer van alles mag, is het voor de culturele sector belangrijk dat ze nieuwe activiteiten kunnen organiseren. De omvang van budgetten is vaak beperkt, waardoor nieuwe activiteiten opzetten niet mogelijk is of een te groot risico is. Het Rijk heeft daarom subsidie beschikbaar gesteld om de culturele sector te ondersteunen. Gemeente Hengelo zet daarvan € 145.000 in zodat de culturele sector kan investeren voor de lange termijn en zorgen dat er weer innovatie plaats kan vinden in de sector. Lintjesregen in Hengelo Op dinsdag 26 april reikt burgemeester Sander Schelberg zes Koninklijke Onderscheidingen uit aan Hengeloërs die zich jarenlang vrijwillig inzetten voor de maatschappij. Dit gebeurt tijdens een bijeenkomst in de Burgerzaal in het stadhuis tussen 10.00 en 12.00 uur. Herinrichting: Nieuwstraat en eerste deel Brinkstraat afgerond Al een aantal maanden is aannemer Dusseldorp druk bezig met de werkzaamheden in het kernwinkelgebied en op het marktplein. De eerste winkelstraten zijn inmiddels ingericht tonen hun nieuwe gezicht graag aan de stad. Duurzaamheidsroute A35 kan energie opwekken voor 25.000 huishoudens De Duurzaamheidsroute A35 kan naar verwachting minimaal 75 GWh tot maximaal 100 GWh aan energie opwekken. Dat is genoeg voor zo’n 25.000 tot 35.000 huishoudens in Twente. Dat blijkt uit een verkenningsrapport van verschillende samenwerkingspartners in Twente. Uit de verkenning blijkt dat de grond langs de A35 en een deel van de A1 geschikt is voor zonnevelden. De Hengelose Beren logeren tijdelijk ergens anders Vanaf februari is aannemer Dusseldorp druk bezig met de werkzaamheden op het marktplein. De beren hebben vanwege de overlast van de werkzaamheden hun koffers gepakt en zijn op zoek gegaan naar een tijdelijk onderkomen. Maar het marktplein blijft hun thuis. Na de oplevering van het vernieuwde plein krijgen ze een mooie plek in de vijver bij de Brinktoren. Nieuwe tijdelijke invulling in voormalige MTS De komende periode ontstaat er weer meer levendigheid in de voormalige Hofstede MTS aan het Industrieplein. Oplevering Informatieverslag Informateur Stefan Kuks heeft woensdagavond 13 april zijn informatieverslag gepresenteerd aan de gemeenteraad. Bestrijding eikenprocessierups weer van start De eerste eikenprocessierupsen zijn op 8 april weer uit het ei gekropen. Dat betekent dat de preventieve bestrijding van de rups weer gaat beginnen. Als de weersomstandigheden meezitten start dit op 13 april. Gildebor komt de komende weken tussen 19.00 en 02.30 uur twee keer langs om alle zomereiken te bespuiten met aaltjes. Waar kwamen al die kindergeluiden vandaan? Een heleboel kinderen waren het! Met heel veel enthousiasme. Het nieuwe Actieplan ’22-’26 staat voor een sfeervolle en levendige binnenstad Het Actieplan voor een vitale Hengelose binnenstad voor 2022-2026 is realistisch en net zo ambitieus als het Actieplan 2017-2021. Vrijwel alle ambities uit het vorige Actieplan zijn gerealiseerd of in gang gezet. In de periode 2022-2026 verschuift de focus geleidelijk naar de rand van de binnenstad. Het gaat hierbij vooral om de aanloopstraten en transformatie naar wonen en werken van gebieden in het centrum maar buiten het compacte hart van binnenstad. De omgevingsvisie Binnenstad-Hart van Zuid en de ontwikkeling van de spoorzone Hengelo-Enschede bieden kansen en uitdagingen voor de verdere ontwikkeling van de binnenstad in de komende jaren. Een groot en belangrijk onderdeel is de verdere uitwerking en realisatie van het plan Lange Wemen. Stadscompliment De Nijverbij voor de heer Marinus van Rooij Als blijk van dank voor zijn vrijwillige inzet Netwerk van laadpalen in de hele stad De gemeente Hengelo heeft een kaart gemaakt waar alle bestaande en toekomstige laadpalen op staan in Hengelo. Hulp voor gedupeerde ouders van de toeslagenaffaire Bent u in de problemen gekomen door de toeslagenaffaire van de kinderopvang? Dan kan de gemeente u helpen. Koper voor historische villa Markant Het plan van investeerder Hephaistos-Skapa is als winnaar uit de bus gekomen bij de verkoopprocedure van villa Markant. Verbod gebruik lachgas in binnenstad Het recreatief gebruik van lachgas op een openbare plaats in combinatie met overlast of een verstoring van de openbare orde is in de gehele gemeente Hengelo al geruime tijd verboden. Nu gaat er op 30 maart een algemeen gebruiksverbod in waarbij lachgas in de gehele binnenstad wordt verboden. De boete voor het gebruik van lachgas in de binnenstad bedraagt €100. Tegemoetkoming bij veel medisch afval Hengeloërs met veel medisch afval, zoals stomamateriaal, incontinentiemateriaal en dialysemateriaal, maken vaker gebruik van de ondergrondse container of laten vaker hun zorgcontainer legen. Daarom vergoedt de gemeente een deel van de afva</t>
+    <t>Kruispunt Deldenerstraat – Marskant weer open! Deel deze pagina Op woensdag 25 mei is het kruispunt Deldenerstraat weer open voor alle verkeer. Op 10 mei 2021 werd deze belangrijke kruising afgesloten. Een nieuwe inrichting voor de Deldenerstraat (vanaf de Langestraat tot aan de kruising Tuindorpstraat (inclusief Mitchamplein) en Marskant volgde. Iets meer dan een jaar later is de volledige kruising heringericht én weer open. Wethouder Gerard Gerrits is blij met de afronding van de vernieuwing van de Deldenerstraat: ‘Werkzaamheden aan een belangrijke invalsweg hebben veel impact in de stad. Ik ben blij met het begrip én geduld wat we de afgelopen jaren van onze inwoners hebben gekregen’. Want met het openen van de kruising komt er een einde aan een groot herinrichtingsproject in de Hengelose binnenstad. Dat project startte in 2019 met een nieuwe inrichting voor het deel tussen kruispunt Bornsestraat tot aan de Langestraat. In 2020 volgde het deel tussen de kruising Tuindorpstraat en kruising Geerdinksweg. De herinrichting van de Marskant, Deldenerstraat én de kruising rondom het Mitchamplein was de laatste horde. Door een prettige samenwerking met aannemer Strukton Civiel én gunstige omstandigheden is het project sneller afgerond dan oorspronkelijk de bedoeling was. Boven de grond is de herinrichting van het gebied duidelijk zichtbaar. Langs de Marskant en het Mitchamplein is de F35 doorgetrokken. Op de Bankastraat na ligt er nu door heel Hengelo een mooie veilige fietsverbinding. Ook zijn beide weghelften wat versmald, wat snel rijden ontmoedigt. Auto- en fietsverkeer heeft een eigen plek gekregen, zo veilig mogelijk voor alle partijen. Gerrits: ‘verkeersveiligheid is in ons beleid één van de speerpunten, de automobilist, fietser én voetganger hebben een eigen plek en dat bevordert de verkeersveiligheid’. Naast een verkeersveilige inrichting is het nieuwe ontwerp ook gericht op een efficiënte doorstroming voor alle verkeersdeelnemers. Nieuwe intelligente verkeerslichten zorgen voor efficiënte afwikkeling van het verkeer. Gerrits: ‘Mooi dat dit nu gerealiseerd is langs de gehele Deldenerstraat. Zo langzamerhand zien we die intelligente systemen op steeds meer plekken in de stad en dat komt de afwikkeling van alle verkeersstromen zeker ten goede!’ In het afgelopen jaar is ook veel werk verricht waar nu niets meer van te zien is. Onder de grond is het vuilwaterriool vernieuwd. Daarnaast is er een nieuw regenwaterriool aangelegd. Dit riool zorgt voor de afvoer van regenwater naar de Berflobeek. Dus geen schoon regenwater meer naar de rioolwaterzuivering maar afvoer via de natuurlijke manier: de beek. Klimaatadaptatie is dan ook een belangrijk onderdeel in dit project. Belangrijke wegen moeten toegankelijk blijven tijdens flinke hoosbuien. Door de rioolstelsels van elkaar te scheiden wordt het water op deze plek tijdens piekbuien beter afgevoerd. Verkeer heeft er op deze manier zo weinig mogelijk last van. In het hele gebied is ook meer ruimte gecreëerd voor groen. Het Mitchamplein heeft de parkeerfunctie behouden maar is flink vergroend. Ook langs de wegen zijn diverse plantvakken aangelegd. Aannemer Strukton Civiel zorgt de komende weken nog voor een finishing touch van het gebied. Het verkeer zal hier geen hinder meer van ondervinden. Eén toegankelijke en complete energieregeling moet verduurzaming versnellen Minister Hugo de Jonge voor Volkshuisvesting en Ruimtelijke Ordening en minister Rob Jetten voor Klimaat en Energie brachten maandag 5 december een werkbezoek aan Twente. Op uitnodiging van de gemeenten Enschede, Hengelo en Almelo spraken zij in Almelo over de energietransitie. De drie steden staan met de stedelijke corporaties en diverse marktpartijen een radicaal andere aanpak voor als het gaat om de energietransitie. Geen afzonderlijke subsidies en regelingen waar inwoners in verzeild raken, maar één toegankelijke en complete energieregeling. De Twentse steden vragen 846 miljoen euro van het Rijk om inwoners te ondersteunen die het op eigen kracht niet lukt te verduurzamen. Nieuw toegangsbeleid Hengelose binnenstad Het bestaande toegangsbeleid voor de Hengelose binnenstad voldoet niet meer. Dat is de conclusie van uitgebreid onderzoek naar het verkeer en het gedrag van verkeersgebruikers in de binnenstad. Uit het onderzoek komt het rapport ‘Advies actualisatie toegangsbeleid binnenstad Hengelo’ voort. In dit rapport worden de maatregelen geadviseerd die de binnenstad weer autovrij moeten maken. Het college heeft ingestemd met het verder uitwerken en aanpassen van het toegangsbeleid zoals beschreven in het adviesrapport. Mobiliteitsplan: Heel Hengelo in beweging Hengelo is volop in beweging. We willen meer en betaalbare woningen bouwen. En onze economische positie als technologische topregio versterken. Dat betekent meer inwoners, meer bedrijvigheid en daarmee ook meer verplaatsingen. Daarom is er de afgelopen maanden hard gewerkt aan een mobiliteitsplan voor Hengelo. Wethouder Hanneke Steen is blij met het resultaat: ‘De titel ‘Heel Hengelo in beweging’ zegt het al, er gebeurt een hoop in onze mooie gemeente. En om de leefbaarheid, verkeersveiligheid en bereikbaarheid in Hengelo in de toekomst goed te houden, moeten we keuzes maken. Dat doen we in het mobiliteitsplan.’ Samenwerkende Twentse gemeenten sluiten contract met Vattenfall voor de levering van aardgas De Samenwerkende Twentse Gemeenten (DSTG) Borne, Enschede, Dinkelland, Haaksbergen, Hellendoorn, Hengelo, Hof van Twente, Losser, Oldenzaal, Tubbergen, Wierden en een aantal partners krijgen met ingang van 1 januari 2023 het aardgas dat ze verbruiken geleverd door Vattenfall. Drie gemeenten - Enschede, Hof van Twente en Losser - tekenden bovendien een overeenkomst met Twence voor de levering van groengas: een belangrijke bijdrage aan de duurzaamheidsdoelstellingen van zowel Twence als de gemeenten. Energiekrediet voor Hengelose bedrijven De gemeente Hengelo biedt een kredietmogelijkheid aan voor Hengelose bedrijven die door gestegen energielasten in de problemen komen. Deze kredietmogelijkheid geldt tijdelijk totdat de landelijke regeling ‘Tegemoetkoming Energie Kosten’ (TEK) van kracht wordt. Vraag van de maand Elke laatste dinsdag van de maand leest u hier over een kwestie waar veel mensen over belden naar de gemeente. Of waarover ze informatie zochten op deze site. Deze keer: Hengelose bushaltes worden aangepakt De komende maanden vernieuwt de provincie Overijssel de borden met reisinformatie bij bushaltes in de gemeente Hengelo. De nieuwe digitale informatieborden zijn moderner en een stuk energiezuiniger dan de oude. Op de digitale borden staat hoe laat de bussen vertrekken, informatie over vertragingen, omleidingen en alternatieve routes. De verwachting is dat de werkzaamheden aan de haltes eind juni 2023 zijn afgerond. College stelt bijna half miljoen beschikbaar voor zonneveld Boeldershoek De komst van een zonneveld in de Boeldershoek is weer een stap dichterbij. Het college van B en W wil een zogenoemd voorbereidingskrediet beschikbaar stellen van €489.120,-. De gemeenteraad moet dit bedrag nog goedkeuren. Het geld komt beschikbaar voor de netaansluiting, het opstellen van een plan en ontwerp voor de ontwikkeling en exploitatie van het zonneveld, aanvullend onderzoek en het participatietraject. Hengelo ontvangt van Rijksoverheid subsidie van € 15 miljoen Hengelo heeft vandaag vanuit Meerjarenprogramma Infrastructuur, Ruimte en Transport (MIRT) een subsidie van maar liefst € 15 miljoen ontvangen. De subsidie is bestemd voor de versnelde bouw van in totaal 1500 woningen in de binnenstad en Hart van Zuid. Om die versnelling te realiseren moeten nieuwe woningbouwlocaties goed bereikbaar zijn. Speciaal daarvoor heeft het Rijk het MIRT-programma in het leven geroepen. Twente Board blij met impuls van 30 miljoen euro voor spoorlijn Zwolle-Twente-Münster Twente Board is blij met de toezegging van het Rijk van 30 miljoen euro voor de treinverbinding Zwolle-Twente-Münster. Dit is van doorslaggevende betekenis voor het voortbestaan van deze spoorverbinding met onze Oosterburen. En dat is hard nodig, want alleen al tussen Enschede en Münster reizen dagelijks ruim tienduizend mensen op en neer. Wat gaat de gemeente doen in 2023? De Hengelose gemeenteraad heeft ingestemd met de Beleidsbegroting 2023 – 2026. Met daarin ruimte en ambitie voor nieuwe investeringen in de stad. Hengelo zoekt Junior Cyber Agents Een smartphone, laptop en/of tablet zijn niet meer weg te denken. Even snel wat opzoeken op Google of een Instagram story maken, we zijn er de hele dag mee bezig! Helaas niet altijd zonder gevaren! Welkom in het stadhuis van Hengelo! Bent u benieuwd hoe uw stadhuis er van binnen uitziet? De gemeente Hengelo nodigt u van harte uit voor het Open Huis op zaterdag 26 november van 10.00 tot 16.00 uur. Oekraïners langer in woningen Nijverheid De Oekraïense vluchtelingen die tijdelijk in de woningen van Welbions in de Nijverheid wonen, kunnen daar enkele maanden langer blijven. Welbions stelt de werkzaamheden voor de sloop en vervolgens nieuwbouw van de betreffende woningen in de Nijverheid uit tot na de zomervakantie van 2023. De reden hiervoor is de lange levertijd van de benodigde bouwmaterialen voor de nieuwbouw en het tekort aan personeel in de bouw. Aandacht voor Week van de Pleegzorg Soms zijn er omstandigheden waardoor een kind (tijdelijk) niet kan terugvallen op een veilige thuisomgeving. Gelukkig zijn er in Hengelo veel mensen die iets voor een ander willen betekenen, zoals pleegouders. Dat zijn vrijwilligers die een kind van een ander in hun huis én hart opnemen, tijdelijk of langer. En dat is hard nodig! Elk jaar zijn er veel nieuwe pleeggezinnen nodig. De gemeente is heel blij met de bijna 80 Hengelose pleeggezinnen. Daarom biedt de gemeente alle pleeggezinnen een cadeaukaart aan. College stemt in met omgevingsvisie ‘Hart van Hengelo’ Het college van B en W heeft op 11 oktober ingestemd met de omgevingsvisie ‘Hart van Hengelo’. Deze visie gaat over de Binnenstad en Hart van Zuid. Het college stelt de gemeenteraad voor om de omgevingsvisie vast te stellen. Vraag van de maand Elke laatste dinsdag van de maand leest u hier over een kwestie waar veel mensen over belden naar de gemeente. Of waarover ze informatie zochten op deze site. Gemeente zet duizenden lichten uit Op zaterdagavond 29 oktober is het van 20.00 tot 21.00 uur pikkedonker in de stad. De gemeente zet dan duizenden openbare lichtpunten uit. Aanleiding is de jaarlijkse Nacht van de Nacht. Op deze avond vragen verschillende organisaties en instellingen aandacht voor lichtvervuiling en energiebesparing. In de bibliotheek zijn op deze avond activiteiten in het donker. Verlichte tocht Licht in het donker en Allerzielenviering Nabestaanden kunnen hun dierbaren gedenken tijdens twee gezamenlijke herdenkingsbijeenkomsten. Op woensdag 26 oktober is er een verlichte tocht over het begraaf- en gedenkpark aan de Oldenzaalsestraat. Op zondag 6 november is de Allerzielenviering op het begraaf- en gedenkpark aan de Deurningerstraat. Bladruimen start 24 oktober Het is herfst, de tijd van vallende bladeren en mooie kiekjes. De gevallen bladeren kunnen soms ook zorgen voor gevaarlijke situaties bijvoorbeeld op straten en fietspaden. Daarom starten Gildebor en groenaannemers vanaf maandag 24 oktober met het verwijderen van bladeren in de openbare ruimte. Door de warme en droge zomer is dat een weekje eerder dan u gewend bent. Lambertusbasiliek op zwart voor duurzaamheidscampagne Op maandagavond 17 oktober blijft de Lambertusbasiliek donker. Op deze manier wil de gemeente Hengelo aandacht vragen voor de lancering van de landelijke campagne ‘Zet ook de knop om’. Deze campagne is in het leven geroepen om mensen te helpen met energie besparen. Wolfkaterweg in beeld voor woningbouw De gemeente Hengelo heeft met twee grondeigenaren een optieovereenkomst gesloten om twee percelen grond aan te kopen aan de Wofkaterweg in Beckum. De gemeente is met onder meer de Dorpsraad Bruisend Beckum de mogelijkheden aan het onderzoeken om woningen te bouwen in en rondom Beckum. Dat is nodig voor de leefbaarheid in Beckum. Energieregeling Hengelo: 800 euro en gratis energieadvies De gemeente Hengelo gaat huishoudens die niet in aanmerking komen voor de landelijke energietoeslag dit jaar nog helpen. De gemeenteraad heeft ingestemd met de Hengelose energieregeling van eenmalig 800 euro én gratis energieadvies. De raad stelt hier 2,8 miljoen euro voor beschikbaar. Aanvragen kan vanaf 10 oktober a.s. Trebbe ontwikkelt samen met Stork en gemeente Hengelo visie op Stork-locatie De gemeente Hengelo, Stork en Trebbe gaan samen een integrale herontwikkelingsvisie opstellen voor de voormalige Koninklijke Machinefabriek Stork (KMS) locatie aan het Industrieplein in Hart van Zuid in Hengelo. Taalpunt Hengelo gecertificeerd Wethouder Jacqueline Freriksen heeft het kwaliteitscertificaat van het CBCT uitgereikt aan Taalpunt Hengelo. Met de certificering wordt nog duidelijker wat voor belangrijke schakel Het Taalpunt is. Coming Out Dag: 11 oktober 2022 Dinsdag 11 oktober is het internationale Coming Out Dag. Dit is de dag waarop we wereldwijd stilstaan bij het uit-de-kast-komen van lhbti's en queer-personen. Dit is nog lang niet voor iedereen vanzelfsprekend. Hengelo hangt dan de Progressvlag uit, de opvolger van de regenboogvlag. Als symbool dat iedereen erbij hoort in Hengelo. Investeren in de toekomst ondanks onzekere tijden Het college van B en W biedt een structureel sluitende Beleidsbegroting 2023-2026 aan de gemeenteraad aan. Met daarin ruimte en ambitie voor nieuwe investeringen in de stad, ondanks onzekere gemeentefinanciën op de lange termijn. Hanneke Steen, wethouder Financiën: ‘Juist nu willen en moeten we investeren daar waar dat het hardst nodig is’. Het college werkt aan een strategische agenda, om hier richting aan te geven. Burgemeestersontbijt Burgemeester Sander Schelberg ontbijt vrijdag 7 oktober met kinderen van IKC Esrein. Dit in het kader van de week van het jaarlijks Nationaal Schoolontbijt. Bakkerij Nollen zorgt voor een lekker en gezond ontbijt. Zilveren Erepenning voor Hengelose Amateur Fotografen Vereniging Zaterdag 1 oktober 2022 zal wethouder Marie-José Luttikholt de Zilveren Erepenning van de stad overhandigen aan de voorzitter van de Hengelose Amateur Fotografen Vereniging (HAFV) Jan van Asveld. Dit gebeurt om 15.00 uur op het Evenementenplein bij het stadhuis aan het Burgemeester Jansenplein, bij de opening van de expositie Hengelo Bepalend. Vluchtelingen Nijverheid naar Hazenweg Begin volgend jaar verandert er iets voor de Oekraïense vluchtelingen die nu verblijven in de woningen van Welbions in de Nijverheid. Zij verhuizen in februari 2023 naar de bestaande opvanglocatie aan de Hazenweg. De vluchtelingen en de omwonenden van de Hazenweg zijn daar afgelopen weekend over geïnformeerd. Week tegen Eenzaamheid Van 29 september tot en met 6 oktober is het de Week tegen Eenzaamheid. Ook u kunt vandaag iets betekenen voor iemand die zich eenzaam voelt. Hebt u een familielid, vriend of buur die hier last van heeft? Er is altijd wel iets dat iemand leuk vindt om te doen, samen met u of met anderen. Een steuntje in de rug kan veel betekenen. Duurzaamheidsmarkt bij stadhuis Op zaterdag 8 oktober staat er op het plein voor het stadhuis een grote duurzaamheidsmarkt. Belangstellenden kunnen hier bij verschillende kraampjes terecht voor alles wat met duurzaamheid te maken heeft. De wooncoaches van Hengelo Energie zijn bijvoorbeeld aanwezig om advies te geven over isoleren en besparen, maar ook over de aanschaf van een warmtepomp of zonnepanelen. Gemeente zet veteranen weer in het zonnetje Op zaterdag 24 september zet Hengelo voor de 14e keer de Hengelose veteranen in het zonnetje. Zo’n 135 veteranen reageerden op de uitnodiging van burgemeester Sander Schelberg en komen naar de Hengelose Veteranendag. Omgevingsvisie stedelijk gebied Zoals u weet zijn we al druk bezig met de omgevingsvisie Hengelo. Op dit moment zijn we bezig met de derde fase van de omgevingsvisie, het stedelijk gebied. Vanaf 3 september gaan we inwoners en ondernemers uit het visiegebied bevragen over hun (fysieke) leefomgeving. Sluiting pand aan Slachthuisweg Burgemeester Sander Schelberg heeft een pand aan de Slachthuisweg in Hengelo voor zes maanden gesloten. Dit op grond van de APV en de Gemeentewet naar aanleiding van (politie)onderzoeken in dit pand. Tijdens de laatste doorzoeking van het rechercheteam zijn meerdere goederen in beslag genomen. De sluiting van het pand gaat per direct in. Update: Vervanging verkeerslichten Oldenzaalsestraat en Weideweg Van 12 september tot en met 2 december worden verkeerslichten op zeven locaties in Hengelo vervangen. Er wordt gestart aan de Weideweg, vanaf 17 oktober is de Oldenzaalsestraat aan de beurt. Het verkeer kan, met enige hinder, gebruik blijven maken van de kruispunten. Zilveren Erepenning voor Wijkcentrum ’t Lansink Op donderdag 1 september reikte wethouder Marie-José Luttikholt de zilveren Erepenning uit aan de voorzitter van het Wijkcentrum ’t Lansink, de heer Jan Willem Korenromp. Dit ter ere van het 100-jarig jubileum bij Wijkcentrum. Hengelo ontvangt van ministerie van EZK subsidie van € 4,8 miljoen Vandaag heeft het ministerie van Economische Zaken en Klimaat (EZK) bekend gemaakt een subsidie van € 4,8 miljoen aan Hengelo te verstrekken. De subsidie komt voort uit het programma Impulsaanpak Winkelgebieden (IW). Het is bestemd voor de herinrichting van het gebied achter het voormalige V&amp;D pand. Het gaat om de locatie tussen de Marskant en de Beekstraat. Dit gebied wordt getransformeerd van winkelgebied naar woongebied. Lambertuskermis allereerste kermis zonder uitstoot van fossiele brandstof Een primeur op de Hengelose Lambertuskermis dit jaar! Van 14 tot en met 18 september draaien alle attracties op accustroom. Dit betekent dat de attracties voor het eerst niet aangedreven worden door een dieselaggregaat; een unicum. Nog niet eerder heeft een kermis in Nederland volledig gedraaid op accustroom. Winkelcentrum Slangenbeek bijna 700 m2 groen rijker In het voorjaar van 2021 won de vergroening van het Winkelcentrum Slangenbeek de stemronde voor Van Grijs naar Groen in Slangenbeek. Bijna 700 vierkante meter verharding in het winkelcentrum is vergroend. Een prachtig resultaat! En er gebeurt nog veel meer! 30 nieuwe inwoners in de opvanglocatie aan de Hazenweg Dinsdagavond 12 juli hebben dertig nieuwe inwoners intrek genomen in de vluchtelingenopvanglocatie aan de Hazenweg. Het gaat om kinderen met hun moeders en enkele vaders, van diverse nationaliteiten. Veiligheidsregio Twente heeft samen met de veertien Twentse gemeenten toegezegd om voor 225 noodplekken en dus extra opvang te zorgen om de locatie in Ter Apel te ontlasten. Wooncoaches klaar om Hengeloërs te helpen met verduurzamen De gemeente Hengelo en Coöperatie Hengelo Energie willen huiseigenaren stimuleren om hun woningen te verduurzamen. Dat houdt in dat de wooncoaches adviezen gaan geven hoe Hengeloërs energie kunnen besparen door bijvoorbeeld hun woning goed te isoleren, maar ook hoe ze zelf energie kunnen opwekken met bijvoorbeeld zonnepanelen; de meest groene energie is immers de energie die niet gebruikt hoeft de worden. Ook moet deze aanpak armoede als gevolg van hoge energielasten tegengaan. 200 tijdelijke huurwoningen in Groot Driene Voor jongeren, studenten en spoedzoekers is het momenteel moeilijk om betaalbare en geschikte woonruimte te vinden. Gemeente Hengelo, woningcorporatie Welbions en ontwikkelcombinatie Leyten-Trebbe slaan de handen ineen om snel enige verlichting op de woningmarkt te brengen. Het resultaat is dat er 200 tijdelijke huurwoningen worden geplaatst op de voormalige ROC-locatie aan de Sportlaan Driene in Hengelo. Reset van sociaal domein Het college van B en W windt er geen doekjes om; het sociale domein van de gemeente Hengelo moet grondig veranderen en wel nu. IKEA opent nieuwe zonnecarports met meer dan 3400 zonnepanelen IKEA Hengelo heeft 3.460 zonnepanelen geplaatst op de parkeerplaats. De vestiging heeft extra oppervlakte voor de panelen gecreëerd met zogenoemde zonnecarports boven de parkeerplaatsen. De zonnepanelen van IKEA Hengelo wekken 1.8 megawattpiek per jaar op. Strategische agenda voor gezonde toekomst Het college van B en W wil de komende jaren samen met de gemeenteraad, inwoners en partners bouwen aan een strategische agenda voor de toekomst. Zodat er geld beschikbaar is en blijft om te investeren in de stad, juist daar waar dat het hardste nodig is. Het college stelt de raad voor om deze agenda binnen een jaar op te stellen. In de Zomerbrief geeft het college een eerste aanzet voor de strategische koers. De gemeenteraad bespreekt de Zomerbrief op 12 juli tijdens een politieke markt. Intrekkingsbesluit 'noodverordening boerenprotest Twence' De toegangswegen naar de afvalverbrandingsinstallatie van Twence waren geblokkeerd. Politieke Markt Vanavond in het stadhuis Bus en aanhanger met ‘drugsvaten’ zorgt voor meldingen van Twentse inwoners De afgelopen weken heeft op verschillende plekken in Twente een bus en aanhanger vol met ‘drugsvaten’ en materialen voor de productie van drugs gestaan. Met deze actie vragen politie en gemeenten in Twente aandacht voor het thema drugscriminaliteit en werd er gekeken in hoeverre inwoners bereid zijn een verdachte situatie te melden. Dit leverde een wisselend beeld op. SchouwArt mag podium voor beeldende kunst vormgeven Hengelo is weer een stap dichterbij een permanent podium voor beeldende kunst. Vernieuwde Elsbeek feestelijk geopend Op donderdag 23 juni werd de vernieuwde Elsbeek in Hengelo officieel geopend. Het terrein naast de Elsbeek was voor deze gelegenheid feestelijk aangekleed en samen met omwonenden en samenwerkende partijen werd de opening van de Elsbeek gevierd. Woninginbraak: Je zou het maar meemaken Stel je voor. Na en dag werken, ga je nog even samen met de hond op bezoek bij familie. Rond 17.00 uur ga je weg en twee uur later word je gebeld door de buurvrouw ‘volgens mij is er ingebroken bij jou’. In paniek rijd je naar huis en wat je daar aantreft, blijft je tot op de dag van vandaag bij. Tweede omgevingsvisie ter inzage De wereld om ons heen verandert snel. Op hetzelfde moment spelen diverse grote trends op het gebied van demografie, technologie en klimaat. Deze leiden in ons land tot een aantal grote ruimtelijke opgaven. De komst van online winkelen zet centrumgebieden onder druk, de inwoners en behoeftes veranderen, er is een grote vraag naar woningen en we hebben samen een grote duurzaamheidsopgave. Met de omgevingsvisie wordt ingespeeld op deze maatschappelijke ontwikkelingen en wordt er richting gegeven aan de toekomstbestendige stad. De visie ligt tot en met 26 juli ter inzage en op 23 juni is er een informatieavond in de stadhuishal. Een exclusief interview met Special Olympics-atleten Friso Roeleveld en Sanne Droste! Nog een paar dagen en dan gaan de Special Olympics Nationale Spelen (SONS) Twente officieel van start met een grandioze openingsceremonie en atletenparade in het FBK-stadion. Boeldershoek in beeld voor zonneveld Vattenfall wil een zonneveld ontwikkelen in het energiegebied bij Twence en heeft een principeverzoek ingediend bij de gemeente. De gemeente is hiermee akkoord. De locatie van Vattenfall grenst aan het gebied waar de gemeente Hengelo ook een zonneveld wil ontwikkelen. De gemeente heeft Vattenfall uitgenodigd om in gesprek te gaan over de invulling en voorwaarden, zoals de participatie van omwonenden en omliggende bedrijven. Avondopenstelling Milieupark Ook dit jaar is het Milieupark aan de Wegtersweg in augustus op donderdagavond tot 20.00 uur geopend. Op donderdag 2 juni is dit jaar de eerste avondopenstelling. Met de avondopenstelling in de zomermaanden is het voor meer mensen mogelijk het Milieupark te bezoeken. Nieuwe wethouders benoemd Tijdens een speciale raadsvergadering op 25 mei zijn de Hengelose wethouders benoemd. Voor BurgerBelangen neemt Jacqueline Freriksen deel aan het college, voor de VVD Gerard Gerrits, voor het CDA Hanneke Steen-Klok, voor de PvdA Marie-José Luttikholt en voor D66 Claudio Bruggink. Kruispunt Deldenerstraat – Marskant weer open! Op woensdag 25 mei is het kruispunt Deldenerstraat weer open voor alle verkeer. Op 10 mei 2021 werd deze belangrijke kruising afgesloten. Een nieuwe inrichting voor de Deldenerstraat (vanaf de Langestraat tot aan de kruising Tuindorpstraat (inclusief Mitchamplein) en Marskant volgde. Iets meer dan een jaar later is de volledige kruising heringericht én weer open. Wethouder Gerard Gerrits is blij met de afronding van de vernieuwing van de Deldenerstraat: ‘Werkzaamheden aan een belangrijke invalsweg hebben veel impact in de stad. Ik ben blij met het begrip én geduld wat we de afgelopen jaren van onze inwoners hebben gekregen’. Erepenning voor Volksuniversiteit Hengelo Op vrijdag 20 mei reikt wethouder Claudio Bruggink de gemeentelijke Erepenning uit aan de Volksuniversiteit Hengelo. De uitreiking vindt om 13.30 uur plaats bij de Gieterij (ROC van Twente) tijdens de viering van het 100-jarig bestaan van de Volksuniversiteit. Dit jubileum wordt een klein jaar later gevierd, omdat het vanwege de eerdere coronabeperkingen niet door kon gaan. Inwonerspeiling Doe mee en vul de vragenlijst in! Nog geen rookmelders? Er komt een nieuwe wet aan: vanaf 1 juli 2022 zijn rookmelders op iedere verdieping verplicht. Gelukkig is het plaatsen zo gedaan. Heb je het altijd uitgesteld? Dan is dit het moment om rookmelders te plaatsen. Peter Schuurmans van Veiligheidsregio Rotterdam-Rijnmond legt uit hoe je in drie eenvoudige stappen rookmelders kunt plaatsen. Uitkomst college-onderhandelingen De afgelopen weken hebben de partijen BurgerBelangen Hengelo, VVD, CDA, PvdA en D66 intensief met elkaar gesproken over de (toekomst)plannen voor Hengelo. Met een goed resultaat, er is overeenstemming bereikt! Uitreiking Nijverbij aan Erwin Bolhaar Op dinsdag 17 mei reikt wethouder Bas van Wakeren het Stadscompliment, De Nijverbij, uit aan de heer Erwin Bolhaar. De uitreiking vindt plaats om ca. 14.30 uur in Woonzorgcentrum Herinckhave, Backenhagenlaan 76. Pas uw huis aan met ‘Lang zult u wonen’! U woont met plezier in uw eigen buurt en hoopt zo lang mogelijk te kunnen blijven wonen waar u nu woont. Hoe maakt u uw huis daar geschikt voor? Scholen uit Hengelo, Twenterand en Berkelland strijden tegen textielafval De Textiel Race is een initiatief van Knol Recycling. Het project is officieel van start gegaan met een kick-off met Wethouder Bas van Wakeren op de Wilbertschool. Positieve waardering binnenstad blijft De waardering voor de binnenstad handhaaft zich op een stabiel niveau. Sinds 2019 stijgt de waardering voor de binnenstad na jarenlange afname. Dit blijkt uit de jaarlijkse binnenstadspeiling onder leden van het Hengelopanel in 2021. Aan de ondervraagden zijn elf te waarderen aspecten voorgelegd. Ten opzichte van 2020 is er meer variatie in de waardering te zien. De positieve waardering van de sfeer en ‘de binnenstad in het algemeen’ is licht gestegen. Opvallend deze keer is toename van de waardering voor het ‘groen’ en de daling voor ‘de kwaliteit van het winkelaanbod’. Alleen folders in de bus met Ja-sticker Vanaf 1 juni 2022 geldt in Hengelo de Ja-sticker. U ontvangt dan alleen reclamefolders als u een Ja-sticker op uw brievenbus plakt. Doet u niets, dan krijgt u geen reclamefolders. Met de Ja-sticker wil de gemeente papierverspilling verminderen. Een gemiddeld huishouden ontvangt per jaar zo’n 26 kilo reclamedrukwerk. Een groot deel hiervan belandt ongelezen bij het oud papier. Primeur in Hengelo; groen licht voor groepen fietsers Op de kruising van de Rondweg/Bornsestraat (afrit A1) ter hoogte van Plein Westermaat, starten provincie Overijssel en de gemeente Hengelo de allereerste proef met de zogeheten Fietsketting. Gemeente gesloten op 5 mei De gemeente is donderdag 5 mei (Bevrijdingsdag) gesloten. Hengelo krijgt er fraaie woonlocaties bij Binnen afzienbare tijd start de verkoop van 28 bouwkavels aan de Marskant en 13 bouwkavels van het plan ‘Broek aan het Pad’. Geïnteresseerden kunnen donderdagavond 12 mei tijdens een informatieavond terecht in het stadhuis in Hengelo. Vrijheid in Verbondenheid Op donderdag 5 mei vieren wij Nationale Bevrijdingsdag. Op de vooravond daarvan, op woensdag 4 mei, worden ook in Hengelo de slachtoffers herdacht die in Nederland of waar ook ter wereld zijn omgekomen of vermoord sinds het uitbreken van de Tweede Wereldoorlog, in oorlogssituaties en bij vredesoperaties. Daarom wordt om 20.00 uur twee minuten stilte in acht genomen. Bij het herdenkingsmonument voor het stadhuis worden kransen gelegd. € 145.000 voor vernieuwing en versterking culturele programmering Afgelopen winter moesten veel culturele instellingen de deuren weer sluiten door de lockdown. Nu er weer van alles mag, is het voor de culturele sector belangrijk dat ze nieuwe activiteiten kunnen organiseren. De omvang van budgetten is vaak beperkt, waardoor nieuwe activiteiten opzetten niet mogelijk is of een te groot risico is. Het Rijk heeft daarom subsidie beschikbaar gesteld om de culturele sector te ondersteunen. Gemeente Hengelo zet daarvan € 145.000 in zodat de culturele sector kan investeren voor de lange termijn en zorgen dat er weer innovatie plaats kan vinden in de sector. Lintjesregen in Hengelo Op dinsdag 26 april reikt burgemeester Sander Schelberg zes Koninklijke Onderscheidingen uit aan Hengeloërs die zich jarenlang vrijwillig inzetten voor de maatschappij. Dit gebeurt tijdens een bijeenkomst in de Burgerzaal in het stadhuis tussen 10.00 en 12.00 uur. Herinrichting: Nieuwstraat en eerste deel Brinkstraat afgerond Al een aantal maanden is aannemer Dusseldorp druk bezig met de werkzaamheden in het kernwinkelgebied en op het marktplein. De eerste winkelstraten zijn inmiddels ingericht tonen hun nieuwe gezicht graag aan de stad. Duurzaamheidsroute A35 kan energie opwekken voor 25.000 huishoudens De Duurzaamheidsroute A35 kan naar verwachting minimaal 75 GWh tot maximaal 100 GWh aan energie opwekken. Dat is genoeg voor zo’n 25.000 tot 35.000 huishoudens in Twente. Dat blijkt uit een verkenningsrapport van verschillende samenwerkingspartners in Twente. Uit de verkenning blijkt dat de grond langs de A35 en een deel van de A1 geschikt is voor zonnevelden. De Hengelose Beren logeren tijdelijk ergens anders Vanaf februari is aannemer Dusseldorp druk bezig met de werkzaamheden op het marktplein. De beren hebben vanwege de overlast van de werkzaamheden hun koffers gepakt en zijn op zoek gegaan naar een tijdelijk onderkomen. Maar het marktplein blijft hun thuis. Na de oplevering van het vernieuwde plein krijgen ze een mooie plek in de vijver bij de Brinktoren. Nieuwe tijdelijke invulling in voormalige MTS De komende periode ontstaat er weer meer levendigheid in de voormalige Hofstede MTS aan het Industrieplein. Oplevering Informatieverslag Informateur Stefan Kuks heeft woensdagavond 13 april zijn informatieverslag gepresenteerd aan de gemeenteraad. Bestrijding eikenprocessierups weer van start De eerste eikenprocessierupsen zijn op 8 april weer uit het ei gekropen. Dat betekent dat de preventieve bestrijding van de rups weer gaat beginnen. Als de weersomstandigheden meezitten start dit op 13 april. Gildebor komt de komende weken tussen 19.00 en 02.30 uur twee keer langs om alle zomereiken te bespuiten met aaltjes. Waar kwamen al die kindergeluiden vandaan? Een heleboel kinderen waren het! Met heel veel enthousiasme. Het nieuwe Actieplan ’22-’26 staat voor een sfeervolle en levendige binnenstad Het Actieplan voor een vitale Hengelose binnenstad voor 2022-2026 is realistisch en net zo ambitieus als het Actieplan 2017-2021. Vrijwel alle ambities uit het vorige Actieplan zijn gerealiseerd of in gang gezet. In de periode 2022-2026 verschuift de focus geleidelijk naar de rand van de binnenstad. Het gaat hierbij vooral om de aanloopstraten en transformatie naar wonen en werken van gebieden in het centrum maar buiten het compacte hart van binnenstad. De omgevingsvisie Binnenstad-Hart van Zuid en de ontwikkeling van de spoorzone Hengelo-Enschede bieden kansen en uitdagingen voor de verdere ontwikkeling van de binnenstad in de komende jaren. Een groot en belangrijk onderdeel is de verdere uitwerking en realisatie van het plan Lange Wemen. Stadscompliment De Nijverbij voor de heer Marinus van Rooij Als blijk van dank voor zijn vrijwillige inzet Netwerk van laadpalen in de hele stad De gemeente Hengelo heeft een kaart gemaakt waar alle bestaande en toekomstige laadpalen op staan in Hengelo. Hulp voor gedupeerde ouders van de toeslagenaffaire Bent u in de problemen gekomen door de toeslagenaffaire van de kinderopvang? Dan k</t>
   </si>
   <si>
     <t>Under the spell via Rian: podcast about a bizarre company soap You wonder whether Rian van Rijbroek will see the many reports about her controversial relationship with Twente multimillionaire and businessman Gerard Sanderink herself. Probably so, because the shutters of her villa in Veghel are firmly closed and she is constantly hiding behind pseudonyms, Tubantia reports. In any case, the Twente newspaper fully exploits her affair. A book by research editor Angelique Kunst has already been published and a podcast is now running. Which isn't very flattering either. The main question is how it is that a 52-year-old woman with a very fat Brabant accent from Veghel has one of the richest IT entrepreneurs in the Netherlands completely in her power. And crazy. His IT company Centric, which supplies ICT systems for governments, would falter due to dismissed top executives and ongoing lawsuits that were partly caused by Van Rijbroek. Employees hold the IT millionaire responsible for the recent management crisis around Centric and fear that it will result in an implosion. The Public Prosecution Service (OM) has launched a preliminary civil investigation. Last year, the childless Sanderink contradicted reports that Centric and his construction company Strukton are partly owned by Van Rijbroek. She would also have become a certificate holder in the foundation that manages the shares. After a whole series of DDoS attacks on banks and government institutions, Van Rijbroek was actually invited by Nieuwsuur as a cybersecurity expert by coincidence (another expert fell ill) in 2018. She had just written a book with PvdA politician Willem Vermeend. Who, like Sanderink, had come under the pressure of her a little too quickly. The book De wereld van Cybersecurity en Cybercrime was withdrawn after proven plagiarism. And Nieuwsuur later had to apologize: the DDoS attacks came from Dutch teenagers, not from North Korea or Iran, as Van Rijbroek had firmly claimed. A year later there was another book of hers, Unhacked. Even with the necessary errors. The media did little to debunk her claims anyway. She said she was a secret agent, worked for foreign powers and large companies. She had obtained the source codes from Kaspersky, a company for which she would also have worked. Kaspersky had never heard of the "cyber charlatan." Nor were cyber specialists who had never encountered this woman. What the podcast makes clear is that Van Rijbroek has preferred to seduce older entrepreneurs all her life. She knows how to impress these men with knowledge that they themselves do not have enough. Before 2017, this was mainly asset and pension management. At the time of her meeting with Vermeend, it was no coincidence that a new Mamomo BV (Mamomo stands for Make more money) had been set up, specializing in 'the development, production and publishing of software'. The podcast suggests that her brother Marc van Rijbroek may have been the inspiration. He sold a SAP-certified tax tool Taxmarc for a lot of money to consultancy firm PwC. According to experts, the fact that Sanderink (73) would be her biggest catch can be explained very well: although he was once a computer specialist in aircraft and aerospace construction, the entrepreneur nowadays still does not know how to send an e-mail or operate a smartphone. He does not read online news. Others do that for him. In particular Van Rijbroek himself, who would have sent quite a few emails on his behalf and feeds him with conspiracies. Sanderink had had a relationship with Brigitte van Egten from Enschede for many years. But it ended with a crazy phone call. Out of the blue, Sanderink suddenly accused her of theft and of 'sex with Africans'. According to him, all this had come to light thanks to "investigations by secret services". The stories had been whispered to him by Van Rijbroek. Your email address will not be displayed on the site. All rights reserved © Emerce</t>
-  </si>
-  <si>
-    <t>Wall art on De Binding in Biddinghuizen is appreciated. The wall painting shows various expressions that have something to do with Biddinghuizen and the polder. Photo: De Binding The mural was a gift from architect Martijn Linde, Hemm project management, Strukton and the contractor Knol bouw. Last week the mural was realized by the company Graffiti for You. The artwork shows various expressions that have something to do with Biddinghuizen and the polder. All together recognizable images for everyone. The work of art already garnered appreciation during the work. Children in particular responded very enthusiastically. Release: 8adcdd1d09e878a893d7757bc39c5648f71e4a3c</t>
   </si>
   <si>
     <t>Dutch solar road proves successful, moves on to heavy traffic road trial
@@ -702,31 +687,27 @@
     <t>Global Railway Maintenance Machinery Market 2018 - Harsco, Speno, Strukton, Vortok International, Plasser &amp; Theurer Railway Maintenance Machinery Market 2017 Permanent link to this press release: Delete press release Edit press release All 5 Releases</t>
   </si>
   <si>
-    <t>Will Gerard Sanderink be forced to resign from Centric? After the meeting between the two, more than four years of decisions followed that jeopardized the future of his companies to such an extent that the Public Prosecution Service deemed it necessary to intervene. On Thursday afternoon, the Public Prosecution Service demands further investigation into mismanagement at IT service provider Centric for the Enterprise Chamber at the Amsterdam Court of Appeal. In the meantime, Sanderink must be suspended as CEO and his shares – he also owns infrastructure builder Strukton, among others – must be placed with an external manager. The case is the next chapter in an unprecedented soap opera in the enterprising Netherlands. Rarely did a businessman listed in the Quote 500 make the news in such a way. Several executives and senior managers left his companies or were fired. He conducted dozens of lawsuits against his ex-girlfriend Brigitte van Egten, whom he accuses of, among other things, fraud and placing porn on the servers of one of his companies. Both claims have been brushed aside by the judge several times. In recent years, those involved have been clear about who is behind the accusations: his current girlfriend Van Rijbroek. She would feed Sanderink with information about conspiracies inside and outside his companies. In this way she would have set up Sanderink against administrators and other close contacts. Read more about the resignation of Centric directors in June 2022 here: Drivers leave again after a conflict with Gerard Sanderink In 2018, for example, the Centric board was in negotiations with a major customer, regulator De Nederlandsche Bank (DNB), when Sanderink suddenly threatened to intervene. He had understood through Van Rijbroek that DNB could not be trusted as a contract partner. The board managed to prevent the negotiations from ending in a fiasco after a tender that had been won, but the conflict did lay the foundation for an exodus of personnel from Centric and later Strukton and the engineering firm Antea Group. For the first time it became clear what influence Van Rijbroek had on Sanderink and what this could mean for his companies. Van Rijbroek is not officially employed by Centric, but he did think about, for example, a cybersecurity division that the company would start a few years ago (it is unclear whether this ever got off the ground). It is also suspected that various emails with accusations about Sanderink’s ex-wife Van Egten are from the Veghelse. At the beginning of 2021, things seemed to calm down around Sanderink’s companies. After Sanderink fell out against a bailiff, he left Strukton and Centric as a director. Sanderink had again had a dubious report with fraud allegations about his ex-girlfriend. The source of the allegations would again have been Van Rijbroek. The judge ordered the entrepreneur to rectify those allegations, but Van Egten wanted to know with whom they had been shared and had Sanderink’s mailbox and telephone seized from Strukton. When a bailiff came at the end of 2020 to copy the data, Sanderink threatened him and had his phone erased remotely. The fuss that arose about this led to such pressure from customers, among others, on the entrepreneur that he resigned from his board positions. However, he remained involved as a shareholder. It didn’t take long: later that year he made a comeback in Strukton’s group management. In June of this year, things got restless around Centric again. Three drivers left. In their view, Sanderink had abused his power by claiming compensation of 1.9 million euros through Centric previously awarded by the court to Van Egten. Sanderink thought that the company would have been damaged by statements that Van Egten made about Centric in various legal proceedings. The court rejected that claim at the time and accused Centric and Sanderink of abuse of rights. Also read: The Public Prosecution Service is reaching for a heavy means to depose Gerard Sanderink At the beginning of July of this year, the Public Prosecution Service announced that it would start a preliminary civil investigation into Centric. This happened after MP Pieter Omtzigt, among others, expressed his concerns about the consequences of the unrest at the company for government services (for example, in recent years it provided part of the IT infrastructure at the regulator DNB and many municipalities also use of Centric’s software). Central question in the Public Prosecution Service investigation: how can the continuity of the company be guaranteed? That research showed that there is a high turnover of staff, which makes the service provision vulnerable. Recently, several important customers have also canceled their contract with the automation company. While the investigation was in its final phase, Sanderink announced two weeks ago that he would return to Centric as a top executive. That was enough for the Public Prosecution Service. It asks the Enterprise Chamber to start an investigation into possible mismanagement at the company and to suspend Sanderink in the meantime and to transfer the shares to external management. For example, Sanderink cannot make important decisions at his companies during his possible suspension. The entrepreneur can defend himself against this on Thursday. Gerard Sanderink (74) from Twente founded the Sanderink Groep in 1992, later renamed Centric (turnover 2021: 422 million euros, approximately 3,800 employees). With the company, Sanderink provides IT services for, among others, (local) governments. Companies such as ASML and Spar also belonged to the clientele. Centric grew into one of the most important IT companies in the Netherlands through acquisitions of smaller competitors. In 2005 Sanderink took over the listed engineering firm Oranjewoud. Five years later, infrastructure builder and NS subsidiary Strukton (2020 turnover: 1.9 billion euros, 6,500 employees) was added. That company also came to hang under the Oranjewoud coat rack. Strukton was visited by the tax investigation service FIOD at the beginning of 2019. The Public Prosecution Service suspects that Strukton may be involved in paying bribes for a metro project in Saudi Arabia. At the beginning of 2022, Sanderink bought out the last strand of shareholders and took Oranjewoud off the stock exchange. In addition, Sanderink also owns solar panel company DSS. His net worth is now estimated by Quote at 505 million euros. Sanderink has been together with Rian van Rijbroek since the autumn of 2018. He previously had a long-standing relationship with Brigitte van Egten. Brigitte van Egten is Gerard Sanderink’s ex-girlfriend. During their relationship, Van Egten was director of Sanderink’s solar panel company DSS, from 2003 to 2018. The relationship lasted until November 2018, when Sanderink was now together with Rian van Rijbroek. Shortly afterwards, Sanderink accused Van Egten of, among other things, fraud at DSS. She also allegedly had several terabytes of porn put on DSS servers. No evidence has ever been found for this. Sanderink also said that Van Egten was behind the FIOD raid on Strukton. The two have been involved in lawsuits for years about Sanderink’s accusations and his statements. Sanderink has been sentenced to rectification several times. He has also been ordered to pay fines worth millions. Rian van Rijbroek (1969) is a cyber entrepreneur from Brabant (with his own company: MaMoMo, Make More Money) who gained national fame in 2018 with a highly criticized performance at Nieuwsuur. In it she stated, among other things, that the North Korean secret service was behind a series of (at the time recent) DDos attacks on Dutch banks. It later turned out that an eighteen-year-old Dutch boy was behind the attacks. Tech experts dismissed the claims as scaremongering and said they did not know Van Rijbroek. Research by various media also showed that at least part of Van Rijbroek’s CV turned out to be incorrect. Shortly afterwards, the Veghelse made the news again. A book she wrote with former politician and professor Willem Vermeend was withdrawn from the market when it turned out that various passages had been copied without citing the source. Since Van Rijbroek has been together with Sanderink, she has also become involved in several lawsuits. For example, Sanderink’s ex-girlfriend Brigitte van Egten tries to show that Van Rijbroek is the source of various accusations about her. Last year, Van Egten had several terabytes of data from Rian van Rijbroek seized. A judge is currently examining the extent to which Van Egten may gain access to this. Your email address will not be published. Required fields are marked * Comment * Name * Email * Website Save my name, email, and website in this browser for the next time I comment. Ruetir| Latest News, World News, Breaking News, Games,Technology, Business, Lifestyle, Fashion, Sports, Food &amp; Technology. Contact Us : [email protected] © Ruetir 2022. All Rights Reserved. © Ruetir 2022. All Rights Reserved</t>
-  </si>
-  <si>
     <t>Larantuka Straits, Indonesia will be home to the largest tidal power plant in the world It will serve 100,000 people and help overcome some of the challenges of energy provision in Indonesia. The largest tidal power plant in the world will be built in the Larantuka Straits in the island of Flores, eastern Indonesia: it will provide energy for at least 100,000 people. Indonesia is an archipelago of more than 17,500 islands, with nearly 260 million people occupying less than half of these, which means that building efficient energy provision infrastructure is a challenge, particularly in the eastern part, where the islands are small (except for Papua) and spread over a wide area. Whilst the country relies mostly on coal, as it has significant reserves of this dirty fuel that can be extracted and processed at a low cost, about 20 million people remained without electricity in 2017. In addition, it has significant unutilised renewable energy potential, including a total of 60 gigawatts from tidal waves. As has been widely demonstrated, the use of fossil fuels is ridden with serious problems, including increasing costs, depleting resources and the negative impact of coal-based plants on surrounding communities and the environment. Also, it puts Indonesia among the biggest contributors to climate change. Its government has made a commitment to increasing the share of renewable energy in national energy provision, from the current level of a little under 8 per cent to almost a quarter by 2025 (through government regulation 79/2014). This will be aligned with international climate change mitigation efforts, with the country stating it will voluntarily reduce emissions by around a third by 2030. About 314 million tonnes of CO2 are expected to be cut from the energy sector. Renewable energy is actually an effective solution for an extensive archipelago such as Indonesia, as small islands and remote areas are mostly not connected to the electricity grid. Stretching the grid to these from the nearest major islands is also too costly and has been proven to be ineffective. Instead, renewable energy can be harvested directly on small and remote islands. The Larantuka Straits project will begin with the construction of the Pancasila-Palmerah Bridge that will function as a barrage (dam) where state-of-the-art turbines turbines will be installed to transform the kinetic energy of tides’ rise and fall of the tides into electricity. As simple as that. The construction, which should be complete by 2020, is integrated with other development projects that will represent an economic boost for more than 250,000 people, as well as a concrete contribution to mitigating climate change. Following completion of a feasibility study that included an environmental impact assessment, the government formed a consortium to run the project. According to Strukton International, one of the companies responsible for cosntructing the tidal bridge, it is estimated that the first phase of the project will absorb 200 million dollars in investments and will have an installed capacity of 18 to 23 megawatts, though tidal power in the area has a potential of 300 megawatts. The following stage will see the extension of the power plant to a capacity of 90 to 115 megawatts, backed by another 350 million dollars in investments. By then it is expected that the structure could provide energy for about half a million people. The project is doubly aimed at establishing reliable energy provision and boosting local infrastructure, states Luhut Pandjaitan, Coordinating Minister for Political, Legal and Security Affairs. The 800-metre bridge will connect Adonara Island to the eastern tip of Flores, enabling economic activity to be opened up. It will also be integrated with a container hub as part of President Joko Widodo’s Sea Toll Programme to turn the country into a global maritime hub, as well as the extension of Gewayantana Airport’s runway. Indonesia is one of the most thriving economies in the world, where growth is stable at about 5-6 per cent per year. Its huge population creates a large domestic market, where nearly 60 per cent of growth is fuelled by private consumption backed by a growing and affluent middle class. The government is aware that this positive trend can only last if the underpinning factor, which is infrastructure, is well-developed. Economic growth can only stand on adequate roads, ports, airport, railways, water provision structures and power plants, over all regions. And all these require energy. Joko Widodo’s administration has been working on a very ambitious infrastructure development programme. To support this, a fast-track policy has been launched to add 35,000 megawatts of new power by the end of its term in 2019, and the the Larantuka Straits tidal power plant will contribute to this objective. Tidal energy is released by tidal movements as a result of the gravitational and centrifugal forces of the Earth, moon and sun, resulting in two high tides and two low ones for every landmass. These occur at regular times during the day, meaning that this form of energy is stable, periodic and predictable. This also differentiates them from oceanic currents, which are slow-moving and unpredictable. Tidal energy involves the installation of clean infrastructure undersea and its efficiency is high. For example, compared to wind power, which applies similar technology, the output of tidal power is 80 per cent higher because water is much denser than wind. The highest tidal ranges, the difference between its low and high points, in the world include the Baie du Mont-Saint-Michel in France (13.5 metres), Severn Estuary in the UK (15 metres) and the Bay of Fundy in Canada (16 metres). The tidal range in Larantuka Straits has been evaluated to be adequate, meeting the required speed for energy production, therefore moving Indonesia in the right direction to fuel the growth of its booming economy whilst respecting the limits of the environment. Quest'opera è distribuita con Licenza Creative Commons Attribuzione - Non commerciale - Non opere derivate 4.0 Internazionale. Read more on these topics: Renewable energy, Sea, Indonesia, Islands A group of experts in Tokyo suggested pouring radioactive water from Fukushima into the open sea. A marine biochemist explains the consequences of this absurd decision. A federal court in Washington, D.C. has struck down the Dakota Access Pipeline, following years of campaigning by the Standing Rock Sioux tribe. The Scottish island of Eigg is self-sufficient for its energy needs, relying almost entirely on renewable sources, especially thanks to a coordinated community effort. President Magufuli in unmovable in going ahead with the Stiegler’s Gorge dam despite conservationists’ warnings of the damage it will cause the Selous Game Reserve’s ecosystem and wildlife. A large dam along the Luangwa River in Zambia would have posed a serious risk to local people and wildlife, leading hundreds of thousands to oppose it. A call to which the government responded by halting plans to build it. The first one megawatt solar power plant in the Chernobyl exclusion zone has become operational. This is the first step in a renewable energy development project promoted by the Ukrainian government in the area. Gas explosions are frequent in Nigeria, where safety standards are poor. In the latest incident, a gas tanker blast killed 35 people in Nasarawa state. Robben Island’s solar energy micro-grid project will produce almost one million kilowatt hours of electricity annually, significantly reducing the cost and impact of buying diesel. The Balikpapan oil spill off the coast or Borneo in Indonesia covers 120 square kilometres. It has caused the death of 5 people, health and economic problems for local communities, as well as threatening wildlife and local ecosystems</t>
   </si>
   <si>
-    <t>University of Delaware's Big Data conference explored analytics trends in a rail context February 2020 By Jeff Stagl, Managing Editor When it comes to efficiently processing and analyzing massive amounts of data, traditional techniques no longer cut it for railroads. They need more modern options like Big Data, a process aimed at analyzing and systematically extracting information from data sets that are too large or complex to handle via traditional processing methods. Through the process, railroads can convert data into usable information that can help them better plan annual maintenance and capital programs. Since Big Data is growing in value as railroads continue to gather and process more information generated from technological advances, the University of Delaware offers a conference each year that focuses on the trending topic — specifically, data analytics and associated statistical analysis techniques. The sixth iteration of the Big Data in Railroad Maintenance Planning Conference was held Dec. 11-12, 2019, at the Trabant University center in Newark, Delaware. The event is organized by the University of Delaware’s railroad engineering and safety program, Big Data center and professional engineering outreach arm. The 2019 edition aimed to expand on previous years’ conferences by introducing new and emerging analysis techniques, and showing how they can be applied to the large volume of inspection data collected by railroads, says Allan Zarembski, a University of Delaware professor who directs the conference. The more than 30 presentations were targeted at helping railroads improve their capital and maintenance program planning efforts, including for both track infrastructure and rolling stock. “We usually have had mostly a track audience, but we’re finding that more and more people want presentations on the mechanical side or operating side,” says Zarembski, who also is the director of the university’s railroad engineering and safety program. “They want to learn about different approaches.” Speakers hailed from a wide range of rail industry stakeholders, including Amtrak, BNSF Railway Co., CN, CSX, Brazil’s MRS Logistica, the Federal Railroad Administration, Penn State Altoona, State University of New York at Buffalo, Alstom, Railinc, Georgetown Rail Equipment Co., Plasser &amp; Theurer, Strukton Rail, ENSCO Inc. and Uptake Technologies Inc. Presentations addressed managing data and data analytics, combining data streams with different technologies, using machine learning to focus on maintenance needs and employing text mining in data analysis. Machine learning is the scientific study of algorithms and statistical models that computer systems use to perform a specific task using patterns and inference. Rutgers University Professor Trefor Williams and Collaborative Solutions LLC Managing Member John Betak discussed the use of topic modeling — or text mining — to identify overriding themes in U.S. and Great Britain rail accidents, says Zarembski. “They talked about using word recognition technology to analyze rail accidents, to look for words that are often repeated in accident reports,” he says. “There’s more to data analysis than just crunching numbers.” The sessions helmed by several universities offered more aggressive takes on data analytics, such as pattern recognition techniques, Zarembski says. For example, Milan Afzalan, Farrokh Jazizadeh Karimi and Mehdi Ahmadian from Virginia Polytechnic Institute and State University — or more commonly Virginia Tech — talked about assessing track conditions by using scalable onboard data and machine learning. A major conference highlight was the Dec. 11 keynote address from Southeastern Pennsylvania Transportation Authority (SEPTA) General Manager Jeff Knueppel, says Zarembski. Knueppel — who retired at 2019’s end — described the authority’s journey with Big Data, an effort aimed at forging a more effective organization. SEPTA is counting on Big Data to help improve safety and the customer experience, optimize spending and workforce planning, spur more informed decisions, and eventually increase the predictability of operations, maintenance and capital programming. The authority long has tried to replace old manual and formulaic processes with automated ones, says SEPTA Director of Innovation Erik Johanson, who helped with Knueppel’s presentation and reviewed it last month. For example, real-time remote condition monitoring of assets can provide automatic alerts of any unusual conditions. SEPTA has employed a TekTracking LLC remote monitoring system proof of concept at its 40th Street trolley portal. Such automation is targeted to help authority officials better understand the root causes of problems, recalibrate maintenance intervals and — over time — increase the potential to predict component failures. SEPTA has nearly reached the automated stage and now is in the preliminary stages of moving toward the predictive stage, which is the “holy grail,” says Johanson. To be predictive, the authority will need to evaluate and invest in new data sources, promote data-driven decision making and turn data into actionable insights. “Data now is in silos, so we need to break them down,” Johanson says. “The goal is to have an organizational pool of data that everyone has access to.” Service quality would improve substantially because arrival times would be more predictable, he says. Plus, maintenance personnel would know when switches or other components would fail. “You can better understand various aspects of your business,” Johanson says. For now, as part of the ongoing automation push, SEPTA continues to implement a new fare card system featuring an open payment system that requires no tokens or paper fares. The authority wants to continue leveraging data to modernize and boost efficiency, including the constant search for better ways to gather, store and disseminate all data sources, says Johanson. For example, SEPTA continues to adopt a second generation of an automated passenger counter (APC) technology that’s more sophisticated than the prior generation. The APC provides time-stamped and geocoded data with limitless analytical potential, and affords opportunities for customer rewards or more dynamic pricing, says Johanson. SEPTA also employs cellular modems on all buses and most of its rail fleet. A radio-based dispatch system previously polled the location of a rail car or bus every three minutes, but the modems poll every 30 seconds, providing better vehicle locations for customers, says Johanson. Coupled with a new mobile application, the modems also help improve fleet management and scheduling. “It’s all about going from old to better ways for a predictive platform,” Johanson says. The future in leveraging data will focus on safety and inspections, such as the use of GPS-enabled drones to inspect infrastructure above ground and GPS-denied drones to inspect tunnels or subways underground using special sensors, he says. In addition, SEPTA is considering or adopting the use of ground-penetrating radar and ultrasonic testing devices for inspections. Rail asset inspections and maintenance in a Big Data context also were the crux of a Dec. 11 presentation conducted jointly by CSX and VisioStack Inc. The session was a prime example of leveraging advanced data analytics, says the University of Delaware’s Zarembski. CSX Manager of Inspection and Records Stephen Love and VisioStack Data Scientist Joshua Doran discussed the Class I’s use of VisioStack’s RaiLinks™ tool for rail inspections and maintenance. CSX and VisioStack began working together in early 2018 to better align and synch the massive amounts of inspection and maintenance data the railroad was generating from many sources, says Love, who reviewed the presentation last month. The VisioStack data alignment tool enables CSX to visualize and disseminate data on cell phones, tablets and laptops, he says. Data — including high-resolution images and potential rail defects — is gathered from unmanned and manual test cars, other detection cars, LIDAR devices and visual inspections conducted by field inspectors. The tool is designed to support data organization, searches and sharing on a high scale. “We can see changes in data over time, see what’s trending or if there’s been a critical exception,” Love says. “It helps with making decisions — we can better plan work windows and how capital dollars are spent.” CSX began to provide RaiLinks to field managers in second-quarter 2019, and more than 100 of them now use it. The Class I plans to continue developing the tool with VisioStack while gathering feedback from users, says Love. “It’s customizable, so it can be suited to our needs,” he says. CSX aims to roll out RaiLinks to field personnel in the second quarter. The tool currently is used for track maintenance, but there will be other applications in the future, says Love. In 2018, the railroad covered more than 57,000 miles of track with test cars, but in 2019 — after using an unmanned test car and the VisioStack tool for the first time — about 200,000 miles of track were covered. “Without the tool, that would have been very difficult to do,” Love says. CSX expects to cover even more track miles in 2020 because the railroad will be using a total of three unmanned test cars, he says. Such positive results from Big Data are driven by research and development, and the academic world plays a large role in R&amp;D. To that end, the University of Delaware aims to incorporate graduate students’ projects into the conference through poster sessions. Held in conjunction with an evening reception on Dec. 11, the sessions enabled seven graduate students to display and explain their research. “Many found the opportunity to talk to the students very enlightening,” Zarembski says, adding that the university might expand the poster sessions at the 2020 conference. One thing that likely won’t change at the next event: the attendance fee. The conference is free because the university relies on sponsors to cover costs, says Zarembski. The 2019 edition drew six platinum and seven gold sponsors. “We have heard from people that it’s easier for them to attend if they don’t have to worry about a fee,” says Zarembski. Email questions or comments to jeff.stagl@tradepress.com</t>
-  </si>
-  <si>
     <t>Get set for InnoTrans 2016 Kevin Smith and Dan Templeton are here to guide you though some of the highlights. Suppliers from around the globe will be out in force to provide a vast shop window of the latest innovations that are set to drive the railway industry forward over the next few years. Indeed, Messe Berlin reports, as it does every two years, that records are set to fall in 2016 with well over 100,000 visitors expected, and 2940 exhibitors - 200 of them making their debut - from 60 countries. Of these exhibitors, 60% are from outside Germany, reflecting the international importance of the event, with leading railway executives and politicians expected to visit the show throughout the four days. Navigating such a large event is inevitably a major challenge. But fear not, IRJ has done some of the hard work for you in our traditional event preview, and features some of the most note-worthy innovations that will be on display in Berlin. We hope you enjoy the show! Plasser and Theurer (Hall 26, stand 222) will introduce a newly-developed universal two-sleeper tamping unit for tracks and turnouts. The 8x4 unit combines the flexibility of universal one-sleeper tamping units in split-head design with the increased output of two-sleeper tamping operations. The new unit can control the speed of the vibration drive, saving time by increasing the output in encrusted ballast while reducing maintenance costs. Outside Plasser will show two machines: a TIF tunnel inspection vehicle (Outside track T8/45) and Unimat 09-32/4S Dynamic E(3^) which uses a hybrid drive. Railshine, France (Hall 23a, stand 708) will display its Global Railway Service-Station concept for rolling stock depots and workshops. The solution is based on its Train Feeding Solutions range and the available features include retractable rigid catenary, locomotive sand filling systems, exhaust fume extraction systems, and an anti-icing system. It also includes a remotely-managed and supervised fuel service station. The highlight exhibit for Frauscher (Hall 25, stand 232) is Frauscher Tracking Solutions (FTS), a wheel detection and train tracking technology system. The company will also present the new Frauscher Alarming and Maintenance System (FAMS) which allows operators to monitor all of their Frauscher axle counter components at a glance. Stadler (Hall 2.2, stand 103) will unveil its EC250, which will be one of the star exhibits of this year’s outside track area. The EC250 or Giruno train high-speed train for Swiss Federal Railways (SBB) is set to begin operating passenger services through the Gotthard Base Tunnel from 2019. Stadler received a SFr 970m ($US 985.3m) order for 29 11-car EC250 sets in October 2014 and the first few completed coaches will be on display at T8/40. Stadler says the train will represent a new level of comfort for transalpine passengers, with high specifications in terms of acoustics and pressure protection. The train also features low-floor boarding, making it straightforward for passengers to board and alight, including those with reduced mobility, and includes a digital passenger information system which indicates where there are available seats on the train. This low-floor design has also influenced the construction of the car body, which demanded creativity from engineers, particularly in the entrance areas, and for installing sub-systems due to the reduced space available below the floor of the train. In addition, engineers had to consider the unique challenges of travelling through the 57km Gotthard Base Tunnel, particularly the air pressure, high levels of humidity and 35oC temperatures. A pressure-protected interior, air-conditioning control and air-flow around the pantograph are some of the adjustments made to ensure the train can operate effectively through the tunnel, while the train is designed to continue operating under its own power in order to be able to reach an emergency stop in the event of a fire. While the first few coaches will be on show in Berlin, the first 11-car train will not begin testing until spring 2017, while it is set to undergo testing at the Rail Tec Arsenal facility in Vienna in the second half of next year. In addition to Giruno, Stadler will show several new trains at the outside track area, including the Flirt EMU for Netherlands Railways (NS) (T9/40), Variobahn tram-train for Aarhus, Denmark (T4/15), and sleeping cars for Azerbaijan Railways (ADDV) (T9/42). The Swiss manufacturer will also display products from its new plant in Valencia, which it acquired from Vossloh in December 2015, including the Eurodual locomotive for British rail freight operator, Direct Rail Services, (T8/43), and Citylink tram-train for Chemnitz (T4/29). CAF (Hall 3.2, stand 401) will highlight its Civity range of trains at InnoTrans. CAF has continued to expand its European export activities in 2016, particularly in the British market, where it has signed contracts for the supply of Civity UK trains to Arriva UK, First Group, and Eversholt Rail. Civity UK features an aluminium carbody and lightweight Arin bogies, and is available as an EMU, DMU, DEMU or hybrid variant. The train is available in two to eight-car configurations. Other highlights of the CAF exhibit include its new fully-automated metro train for Istanbul and Santiago de Chile, as well as Urbos LRVs for cities such as Utrecht, Luxembourg and Canberra. The company will also show examples of civil works, electromechanical systems, and driving simulators. Meanwhile CAF Signalling will showcase its ETCS Level 2 system for the Mexico City - Toluca project, for which CAF is also supplying 30 five-car Civia EMUs, which will have a maximum speed of 160km/h. Škoda Transportation (Hall 2.1, stand 101) will be displaying its new fully air-conditioned ForCity Plus LRV for Bratislava (V/200). Škoda will also show its new Emil Zatopek type 109E electric locomotive for DB Regio (T5/40) which will operate with Škoda double-deck coaches for high-speed regional services on the Nuremberg - Ingolstadt - Munich line from December. The highlight exhibit for Mersen (Hall 11.1, stand 201) is its EcoDesign third-rail shoe, which employs a new assembly concept that makes it possible to replace only the carbon wear strip allowing the re-use of all metal components and eliminating the need for lead soldering. ZTR Control Systems’ (Hall 6.2, stand 507) will demonstrate its new ONE i3 solution, a customisable platform which enables companies to introduce complex industrial Internet of Things (IoT) processes. It will also launch its KickStart battery solution in the European market, which uses supercapacitor technology to provide reliable starts and extend battery life. In addition, the company will show its SmartStart automatic engine start-stop (AESS) system. Eltra Sistemi, Italy, (Hall 2.1, stand 416) will present its new line of RFID card dispensers which aim to increase automation and reduce the need for manual operators. The machines have a re-fill system in order to reduce reloading frequency. Safety glass is a leading feature of Romag’s stand (Hall 1.1b, stand 205). Romag will showcase a range of customer-based displays featuring body-side windows for Hitachi and Bombardier, and windscreens for Bombardier’s Aventra, Voyager and London Underground S-Stock trains. AMGC, Italy, (Hall 5.2, stand 228) will display Smir, a low-profile infrared array detector for early fire detection that has been designed specifically for reliable detection of fire on rolling stock. The system relies on an algorithm that quickly detects fire by identifying flames, temperature, and temperature gradient. International Railway Journal launches IRJ Pro at InnoTrans. International Railway Journal (IRJ) (Hall 6.2, stand 101) will launch IRJ Pro, a new market intelligence product for the rail industry at InnoTrans. IRJ Pro is a subscription-based service, divided into three segments - Project Monitor, Fleet Monitor and Global Rail Tenders. Project Monitor enables the user to access up-to-date information on every known new-build railway project currently underway across the world, including the estimated project cost, the length of the new line, and expected completion date. Similarly, Fleet Monitor enables users to access information on all known current open fleet orders across the world, including the quantity and type of passenger vehicles and locomotives on order, and their expected delivery date. The service will offer subscribers easily-accessible and continuously-updated intelligence on what is happening in the industry, while highlighting potential opportunities for suppliers. This is supported by Global Rail Tenders, IRJ’s bespoke railway tendering service which provides details of active tenders in the rail industry. IRJ’s Sales Executive Chloe Pickering will present IRJ Pro at the IRJ stand and will host regular demonstrations of the platform throughout InnoTrans. IRJ’s international sales managers, Louise Cooper and Julie Richardson, along with Fabio Potesta and Elda Guidi from Italy, will also be available to discuss IRJ’s other products and services. They will be joined by publisher Jonathan Chalon. In addition, IRJ’s editorial team will have all corners of Messe Berlin covered throughout the four days of the show, reporting live from the event on social media (@railjournal) and posting regular updates on railjournal.com. Editor-in-chief David Briginshaw will be joined by Associate Editor, Keith Barrow, Features Editor, Kevin Smith, and News and Features Writer Dan Templeton. The IRJ stand will be managed by Sue Morant who will be available to answer your questions. We look forward to meeting you in Berlin, and introducing you to IRJ Pro. Thales (Hall 4.2, stand 103) has divided its exhibit into four key highlights around the theme of “Vision 2020”: Security 2020 will help viewers experience how automatic video analytics technology can help improve the security of transport infrastructure, while Maintenance 2020 will show how cloud analytics and augmented reality technologies can improve efficiency and reduce the cost of rail infrastructure services. Cyber 2020 will highlight how to protect critical systems from external attacks using modern tools designed for rail infrastructure protection. Lastly, Thales will demonstrate Ticketing 2020, which includes its TransCity cloud-based ticketing solution, a mobile ticketing application and proximity detection technology. Oleo (Hall 1.2, stand 310) will launch its new Sentry coupler range which can be supplied in standard and bespoke configurations. The company will also show its range of buffer solutions. Perpetuum (Hall 2.2, stand 206), with 7000 diagnostics sensors now in service, will showcase its rolling stock and track condition monitoring services for rail assets and infrastructure. Robel (Hall 26, stand 234) is premiering the Robel 30.73 PSM (O/598,) a hydraulic precision wrenching machine. The company will also display a new infrastructure maintenance system for Cologne Transport (KVB) during the show (T10/47-49.) This includes three track vehicles, two of which are fitted with a 11.5m-loading crane, five trailers with a ballast lorry, two low-floor trailers, a wagon for rails up to 180m, and a trailer with high-pressure purging and vacuum system for underground facilities. Amberg (Hall 25, stand 314) will launch IMS 5000. The solution incorporates Amberg’s existing GRP 5000 system, which is used for clearance and as-built surveying, with its inertial measurement (IMU) technology to survey relative and absolute track geometry, and to identify objects close to track using laser scanning. Using 3D control points, the system executes topographic surveys without using total station or GPS, allowing the system to measure up to 4km/h. Egis Rail (Hall 8.1, stand 114), which offers engineering, project management and operations services, will present its portfolio of Virtual Reality technologies. It will also highlight its use of 3D modelling solutions in project design, and its engineering, project structuring and operations services. Japan Transport Engineering Company (J-TREC) (CityCube A, stand 43) will showcase its range of hybrid technologies, including Sustina hybrid trains. Pandrol Track Systems (Hall 23, stand 210) will show various solutions for track-related systems including from its subsidiary companies. This includes Vortok’s measure and detect wayside monitoring systems, which include options for continuous monitoring; Rosenqvist’s electric CD 200 rail clipping machines; and Pandrol CDM Track’s QTrack system, which is a one-stop-shop for equipment installations, support and up-cycled environmentally-friendly rubber profiles. Pandrol Electrification will also display its Rigid Overhead Catenary System for tunnels, depots, bridges and rapid battery charging stations, and its complete third-rail systems, which are based on a co-extruded conductor rail. In addition, Railtech Welding and Equipment will display its rail welding equipment and services. Kapsch (Hall 4.1, stand 415) will show its dedicated railway networks portfolio as well as its latest smart solutions for public transport, which emphasise enhanced cyber security. It will have demonstrations of its IP-based railway communication solutions, including the SIP-based Functional Addressing call. In addition, visitors to the stand will be able to conduct a “security-self-test”. IntelliDesk, a new design concept for driver consoles which is suitable for a variety of information equipment is the highlight exhibit for Schaltbau (Hall 2.2, stand 102). The company will also show C195x a bidirectional variant of its high-voltage contractor for 1500V and 320A, and its new range of cable connectors: Schaltbau Connections. Pöyry (Hall 5.2, stand 401) will display its solutions for tunnel construction and equipment, rail engineering and address topics such as surveying and the environment.­­­­­­­­ CRRC (Hall 2.2, stand 310) is set to have a major presence with the company exhibiting for the first time since the merger of CSR and CNR was confirmed in 2015. Among the products that the manufacturer will highlight are its 100km/h EMU for Brazil, electric locomotives for South Africa and diesel locomotives, including its HX range developed in cooperation with EMD. The manufacturer has also promised to reveal several new products for the first time, including a high-speed train. Getzner (Hall 25, stand 213) will display its range of elastic mountings for turnouts and transition zones which are designed to reduce maintenance costs by balancing out variations in stiffness while reducing the impact of passing trains. The Austrian company will also show its latest under-ballast mats, mass-spring systems and sleeper pads. Crane and switch renewal systems supplier Kirow (Hall 26a, stand 228) will showcase its solutions for point renewal using the Multi Tasker 910 (T5/43), the Self-Leveling Beam and the Kirow Switch Tilter. It will also display its Multi Tasker 1100 railway crane (T5/43), which Swiss Molinari has purchased for the Awash - Woldia/Hara Gebeya project in Ethiopia. Parker Hannifin (Hall 10.2, stand 209) will present a range of components and solutions, including air treatment and filtration equipment for pneumatic systems, control valves, and integrated control systems for applications such as pantographs, door mechanisms and couplings. ABB (Hall 9, stand 310) will present two world premieres: the lightweight traction transformer Efflight, and the next generation battery charger, Bordline BC. Efflight’s technology significantly reduces oil volume, providing notable energy savings for operators and weight reductions for train manufacturers. Bordline BC incorporates silicon carbide technology which enables a compact design, high power density, high reliability and easy maintenance. The charger is compatible with most railway applications and many train batteries. The company will also display its new Enviline withdrawable diode rectifier for dc traction power supplies, modular Conceptpower DPA 120 uninterruptable power supply system, and a high-speed dc circuit breaker. Cummins (Hall 18, stand 202) will introduce QSK60, a 60-litre engine with Cummins’ Modular Common Rail Fuel system, which is available in outputs ranging from 1723-2013kW and has secured Stage IIIb emissions certification. Another highlight is the QSK95, a 16-cylinder high-speed diesel engine, which was recently certified to meet United States EPA Tier 4 emissions standards. Highlights of the British Steel (Hall 26, stand 107) exhibit include the SF350 a stress-free heat-treated rail offering wear resistance with low residual stress, minimising the risk of foot fatigue; the ML330, a grooved rail; and Zinoco, a premium-coated rail for aggressive environments. Hübner (Hall 1.2, stand 211) is celebrating its 70th anniversary in 2016, and will host an executive presentation of its latest product developments and services, including a new track geometry recording system which can record the complete physical characteristics of specific track sections. The company will also showcase a real-time testing simulator and acoustical insulation solutions. SHC Heavy Industry (Hall 9, stand 603) will display vehicle carbodies formed using the company’s roll forming process as well as its welded assemblies for passenger coaches. This includes roof assembly, underframe sub-assembly, and wall sub-assembly parts. Gummi-Metall-Technik (Hall 9, stand 625), a specialist in rubber-to-metal bonded suspension components and systems, will highlight the performance and progress of its MERP wheel set axle-protector, which the company launched at InnoTrans 2014. As well as its portfolio of freight and passenger locomotives, GE Transportation (Hall 6.2, stand 501) will showcase its Digital Solutions software portfolio, including the GoLinc platform, which converts any locomotive into a mobile data centre and creates an edge-to-cloud-enabled device. Moxa (Hall 4.1, stand 320) will present Vport 06-2 and VPort P16-2MR series rugged IP cameras for onboard CCTV applications. The cameras support 1080P HD video and are EN 50155 certified. Moxa will also show its two-wire ethernet technology, which supports upgrades to an IP network using existing wiring, and its new ioPAC 8600 all-in-one controller which combines serial, I/O, and ethernet interfaces in a single device. European Railway Industry Association (Unife) (Hall 4.2, stand 302) will host a full programme of presentations and discussions during the show, including the signing of a memorandum of understanding on ERTMS on the Tuesday morning, and a presentation on the Fourth Railway Package later in the day. The Shift2Rail programme, Unife’s digitalisation strategy, and various research projects will also be discussed. In addition to an extensive indoor exhibit Alstom (Hall 3.2, stand 308) will show two vehicles at the outside track area: its new “zero-emissions train” (T6/40) will break cover for the first time following a project agreed in 2014 with the German states of Lower Saxony, North Rhine-Westphalia, Baden-Württemberg, and the public transport authorities of Hesse. The company will also display its H3 Hybrid shunting locomotive (T1/16). Hitachi and Johnson Controls’ joint-venture, Johnson Controls-Hitachi Air Conditioning (Hall 3.1, stand 337) will display its scroll compressor as well as an expanding line up of R407C/R134a horizontal and vertical scroll compressors, including inverter-driven models. Sécheron Hasler Group, Switzerland, recently acquired a 60% majority share in Saira Electronics, Italy and both companies will exhibit in Hall 6.2, stand 218. Their highlight exhibit is the newly-developed Hasler EVA+ data management and evaluation software. The solution combines ETCS and national data evaluation, voice and front/rear view data evaluation, GPS tracking, data comparison into a single web-based software. Safety controllers for applications including interlockings, level crossings and rolling stock will be at the forefront of the HIMA (Hall 6.2, stand 406) exhibit, including the company’s HiMax and HiMatrix which have Cenelec SIL 4 approval. Loccioni Group (Hall 26, stand 131d) will showcase its Felix Robot which the company says is the first mobile robot capable of carrying out measurements on points, crossings and track. Aucotec (Hall 6.2, stand 102) will launch its new configuration concept for rail vehicles. The Advanced Typical Manager (ATM) based on Engineering Base (EB) software provides a centralised management system for complicated route and cross-border operations. The user can change data entries at a single point, which appears immediately in both a graphic and list format, and shows a representation of the changed object at each point in the process. Turbo Power Systems (TPS) (CityCube A, stand 225) will showcase its auxiliary power supply (APS) products, including for monorail projects in Riyadh and São Paulo. Among the features of the APS is a liquid cooling system designed as modular line replaceable units (LRUs), power modules, and extensive diagnostic and data logging facilities. TPS will also highlight its at-seat power supply products. Max Bögl (Hall 26, stand 227) will display its proven slab track system, Feste Fahrbahn Bögl (FBB), which is suitable for high-speed applications. The company will also show its mass-spring systems for reducing noise and vibrations. Lütze Transportation (Hall 6.2, stand 203) will present the new Lütze solid state relay which is able to outperform conventional relays by switching inductive and ohmic loads to up to 7A. The component is suitable for all control cabinets and is available in two versions: with a control voltage of 24-110V dc and secondly with 72-110V dc. Scheidt &amp; Bachmann (Hall 2.1, stand 203) will demonstrate its updated ticketing solutions for public transport, including a world-premiere of its ID-based ticketing system. The system utilises a Be-in/Be-out concept based on ID-based ticketing and is compatible with smart cards, NFC devices, or credit cards. Be-in/Be-out is reliant on a cloud-based database, enabling centralised management of all systems and straightforward introduction of new features. Lapp (Hall 10.1, stand 103) is making its first steps into the European rail market and will show various cables and connections, including its original Öflex train cables, Unitronic data network cables, Etherline data communication systems, Epic industrial connectors, Skintop cable glands and Fleximark marking systems. Among SKF’s (Hall 22, stand 606) exhibits is its new class of wheel tapered roller bearing units (TBUs), which are designed to run for 1.7 million km between overhauls thus matching typical wheel replacement intervals. The company will also display its new Centrifugal Lip Seal that switches between contacting and non-contacting sealing modes in wheelset bearing units. SelectraVision, Italy, (Hall 5.2, stand 312) will show its WheelCheck system which uses lasers and high-speed cameras to analyse train wheel profiles at up to 150km/h in order to prevent train derailments. It will also display its 3D obstacle detection system which uses a 3D laser scanner to measure the position and the size of any object in a detection zone at level crossings, station platforms and in front of trams. KLW (Hall 21, stand 508) will present a range of new products and additional services for customers, including its CNC machining centres, which are suitable for finish machining of wheel bores and can undertake various types of web drillings. KLW will also show its new rough machined railway axles and new wheels which meet AAR standards. HTV (Hall 11.1, stand 231) will show its capabilities in long-term conservation and storage by presenting its TAB platform for electronic components of up to 50 years. It will also show HTV Revivec, a product for the removal of oxidation and impurities from component connections, and HTV-NovaTin, which offers highly-durable retinning of electronic components to restore solderability. Lucchini (Hall 21, stand 401) will exhibit various solutions including wheels, axles, wheelsets, anti-ballast protection, and noise damping solutions. The Italian company will also show castings and forgings for heavy industry applications such as oil and gas, power generation, and high-tech engineering. MAN (Hall 18, stand 218) will present an extended portfolio based on the D3876 six-cylinder engine as well as the downgraded version of its previously most powerful 12-cylinder D2862 prime mover. MAN Engines will also display its modular exhaust gas after-­­­treatment system which will comply with future emission standards. Greenwood Engineering (Hall 23, stand 606) will highlight its MiniProf Wheel, rail and brake contact measurement system. Miniprof supports Bluetooth, and the company says the solution offers fast, reliable, and high-quality profile measurements. The system is also available with Envision, a complete data analysis toolbox. A full-size working jack will be the centrepiece of Mechan’s (Hall 2.2, stand 206E) exhibit. The jacks are suitable for all types of rail vehicle, including high-speed trains and heavy on-track plant. The British manufacturer will also demonstrate its Megalink control system, which enables synchronised control of an unlimited number of jack units. Fraunhofer IPM (Hall 23, stand 206) is presenting its new contactless Contact Wire Inspection System (CIS) which records the vertical and horizontal position and wear of up to 10 contact wires at the same time and can operate at up to 350km/h. The company will also exhibit its laser and camera-based railway measurement system, Clearance Profile Scanner (CPS), for measuring clearance profiles, and small and lightweight laser-based measurement systems for use on unmanned aerial vehicles (UAV). The French Pavillion (Halls 3.2, 11.2 and 26b) will feature five companies from the industrial and high technology fields:Centralp, which specialises in embedded electronics, CIM, a group specialising in rolling stock maintenance, Corys, which designs and manufactures driving simulators, Flertex, an expert in brake linings and brake shoes, and Nexter Electronics, embedded electronic systems engineering professionals. Saft (Hall 15.1, stand 205) is launching a new remote battery monitoring solution Comm Batt, a new Internet of Things (IoT) service which combines remote, wireless real-time data monitoring and collection with modelling algorithms to help rail operators transition to a predictive battery maintenance regime. Vossloh’s (Hall 26, stand 310) exhibit is divided into three key themes: solutions to protect against noise and vibration, efficient availability of tracks, and long-term reduction of costs across the complete lifecycle. Among the exhibits that will showcase these capabilities are its highly-elastic rail fastenings, vibration damping rail pads, intermediate plates made from cellentic, and its High Speed Grinding technology for preventative rail maintenance. The company will also launch a dowel-bolt combination, which promises to extend the life of concrete sleepers. From its Transportation Division the company will show lightweight bogies; and diesel locomotives DE 18 (T1/29) and G 6 (T1/28). Vossloh Kiepe will show a new CO2 air-conditioning system, while Vossloh Locomotives will launch a new engine management system, which can restrict power output and save energy. Visitors will also be invited for a multimedia tour of the new Vossloh locomotive factory in Kiel-Suchdorf. Flexicon (Hall 2.2, stand 206) will launch a new flexible conduit fitting for rail electrical and data installations that require uninterrupted supply. The one-piece Flexicon Ultra has all-round teeth providing a tensile strength of up to 70kg and high levels of anti-vibration and shock protection performance. Mios Elettronica, Italy, (Hall 6.2, stand 307) will exhibit a new Train Real-time Data Protocol (TRDP) solution for its portfolio of train communication networks and train control and monitoring systems for items such as crash-protected memory modules, event recorders, vehicle control units and door controllers. It will also launch a programmable logic controller language feature on its RIO and MVB-ETH converters, and a gigabit ethernet solution.­ Voestalpine (Hall 21b, stand 210) will present several world premieres, including interactive rail lifecycle cost tools, which can help infrastructure owners assess the relative cost of different investment and maintenance strategies. The company will also display a new range of heat-treated hypereutectoid rails based on the steel grade 400 UHC HSH, and the iSwitch intelligent point machine, which has a wireless and battery-powered device to monitor comprehensive data inside the machine and send it to the Roadmaster server. The PHS1601 point heating system will also make its market debut along with the UNIAC2 axle counter. NEM Solutions (Hall 21, stand 509) will launch Aura Desk, an intelligent workstation which combines economic and technical data of a fleet’s health, and can help users to quickly identify and monitor existing problems. In addition, with the generation of smart data from components, users are able to understand key data from their fleets which can inform the decision-making process. TE Connectivity (Hall 12, stand 210) will show a prototype of a new generation modular roofline system, a solution which transmits electrical power from the catenary to the traction transformer and includes components such as the pantograph, surge arrestors, circuit breakers, power cables, insulated bushings and metering transformers. TE will also highlight its products and systems for trackside, power and signal, and cable identification.Automatic Passenger Counting (APC) sensor supplier g Iris (Hall 2.1, stand 418) will show its Irma Matrix sensor, the most recent generation of Iris’ APC sensors. This new generation system is based on 3D distance measurement and can detect the real contour of passengers for accurate and reliable counting. In parallel, Iris can also offer a bicycle counting solution. Strukton Rail (Hall 26, stand 235) will display its range of traction converters, auxiliary power supply, and train control management systems. The company will also highlight its expertise in infrastructure. Hitachi (Hall 4.2, stand 304) is focusing its exhibit on its Internet of Things (IoT) solutions, predictive maintenance, and plans for using big data. The event is the first time that Hitachi, Hitachi Rail Europe, Hitachi Rail Italy, and Ansaldo STS will exhibit together. Among the highlights for Ansaldo STS is details of its work at the Ersatt test-track in Cagliari, Italy, where it carried out the first trials of the satellite-based 3InSat project. The system is based on ERTMS signalling standards and uses the company’s Location Determination System (LDS). Among the infrastructure maintenance and support vehicles that Herzog Railroad Services (HRSI) (Hall 22b, stand 310) will showcase is its new Automated Conveyor Train (ACT) which can be used to stockpile material for crossing work, new construction, shoulder rebuilding, flood work and more. The company’s multi-purpose machine (MPM), road-worthy rail unloading machine, (RUM) and automated tie-down car will also be highlighted. AZD Praha (Hall 9, stand 302) will present its portfolio of signalling and telecommunications products and systems, including station interlockings and lineside signalling systems and products for ETCS. LB Foster (Hall 25, stand 220) will showcase its core range of track components along with friction management solutions and engineering technology applications. Products and services, including the Level Crossing Obstacle Detection (Lidar OD) system, customer information touchscreen wayfinders, and the driver-only CCTV system for Crossrail, will be demonstrated. Inside the stand there will be a display screen dedicated to Netpractice’s wayfinding, larger screen passenger information and OIS stations, and a premiere of its unique Arriva fingerprint platform. Among the highlights for insulation specialist Armacell (Hall 8.2, stand 316) is the Armaflex Rail SD, an elastomeric insulation material which offers improved flame-retardant properties and low smoke density. The material features Microban technology for additional protection against mould. Armacell will also present its Rail SD-C, the first closed cell-insulation material for use in areas requiring the highest hazard level. Huawei (Hall 7.1b, stand 201) will showcase its latest achievements under its All-</t>
   </si>
   <si>
     <t>Cleantech Group Below is a quick overview of what we’re seeing in terms of trends, innovators, and partnerships, but for a closer look at this space, please do get in touch with us at research@cleantech.com. There are at least four different technologies to harness the energy of the sea – ocean thermal energy, salinity gradient energy, tidal energy, and wave energy. Ocean thermal conversion exploits the difference in temperature between deep and surface waters, while salinity gradient generation converts the difference in salt concentration between fresh and saltwater, typically found in fjords and deltas. Although a few start-ups such as Bluerise and REDstack are active in this space, these technologies remain largely in the concept stage and we’ll therefore focus on the latter two below. While wave energy converters capture energy from the motion of waves through either floating or submerged devices, tidal turbines generate electricity from the tides caused by the gravitational force of the moon and can be mounted to the seabed like submarine wind turbines (tidal stream), or integrated within a barrier impounding a lagoon (tidal range). Advantages of tidal energy – apart from being clean and renewable – are its potential efficiency and predictability. As water is much denser than air, turbines can be smaller and generate energy from far slower velocities than wind turbines. Even more importantly, tides are not as erratic as winds but happen twice a day, which has the potential to offset the intermittent nature of solar and wind and makes annual production calculations much easier. Benefits of wave energy converters, on the other hand, include a very low impact on aquatic life, and the high power density resulting from multiple planes of movement (waves not only roll past the device, but push it up and down and side-to-side). Both technologies could also be deployed at smaller scales for offgrid applications and energy security on small islands that typically suffer from energy scarcity and/or high electricity prices. Carnegie Clean Energy, for example, has been awarded $2.5M by the Australian Renewable Energy Agency late last year for a wave-powered microgrid project to be implemented on Garden Island in Western Australia in the coming months.      (Photo credits: clockwise from the top left, Wello, Carnegie Clean Energy, Atlantis Resources, Sabella,) Similar to offshore wind farms, the deployment of these technologies faces challenges from difficulties in grid connections, as well as the harsh (salty &amp; stormy) and remote (underwater) environment in which they are to be implemented. This explains in part why no single dominant design has yet to emerge for wave energy converters, and also why progress has been stymied by a few bankruptcies of early movers, such as Pelamis Wave Power and Aquamarine Power, gone out of business in 2014 and 2015, respectively. However, we’ve also seen a plethora of new start-ups appear in our i3 platform in recent years. Relatedly, investment activity in the scene seems to have picked up the pace again with a number of equity and project financing rounds for innovators such as the InnoEnergy Spin-off CorPower Ocean, AW-Energy and Carnegie Clean Energy. Large utilities are taking up the race as well, with players such as ENEL Green Power partnering with the Italian start-up, 40SouthEnergy, and Finnish utility Fortum aiming to deploy the first multi-megawatt wave farm in 2020 off the coast of Scotland in a partnership with the Finnish start-up, Wello. More research, pilot projects and experimentation like these will still be necessary before wave technologies become viable and competitive enough for wider industrial rollout. The tidal energy industry has already seen initial large-scale capabilities deployed last year, and has more than one multi-megawatt project under construction. With a total lease capacity of 398MW, the MeyGen project installed in Pentland Firth (Scotland) by Atlantis Resources is the largest tidal energy farm in operation to date. But more are yet to come. Just last month, Tidal Bridge BV, a joint venture of DEC and Strukton International has been awarded the Palmerah Tidal Bridge Project in Indonesia, which will have an installed capacity of up to 115MV and has a contract value of an estimated $550 million. Other known names include Engie, Alstom, EDF, and Repsol, who have all been involved early on and have partnered with start-ups, such as Sabella or Tocardo, to speed up the development of tidal turbines. The Swedish company, Minesto, received attention two months ago when it closed a limited public share offering with $8 million in proceeds for an innovative tidal kite design, pointing out that the last word has not been said on the shape of tidal technologies to come. While Europe is clearly spearheading innovation for ocean power, other countries such as Israel and Canada are advancing fast. With the potential for off grid applications, more developments for island states and remote coastal areas can be expected. Capitalizing on existing offshore infrastructures, naval capabilities, and under-used harbors might open up additional new pathways for deployments. For years, the spotlight has focussed on green energy, with blue energy gaining momentum in fits and starts. While tidal energy now seems on the crest of maturity with various deployments being carried out worldwide, wave energy has yet to breach the surface</t>
   </si>
   <si>
-    <t>Most employees? 30 largest construction companies in Sweden in 2021
- Open the e-magazine Three companies on the top 30 list have more employees than the other 27 combined. Peab, Skanska and NCC continue to dominate in Byggsverige. It is Byggföretagen that produced a compilation in which the employers' organization ranked the 30 largest construction companies in the country according to the number of employees in the country. Peab is at the top closely followed by Skanska and NCC. Then there is a big gap down to Veidekke in fourth place. - When it comes to the number of employees and turnover, Peab, Skanska and NCC are in a class of their own. With a total turnover of more than SEK 100 billion and over 25,000 employees in Sweden, these three are bigger than the other 27 companies on the list combined, says Emil Flodin, analyst at Byggföretagen in a comment. This year, for the first time, the companies are ranked according to the number of employees instead of, as before, according to how much they turnover. Something else that also differs from before is the selection, as Byggföretagen clearly wants to bring out companies that are more purely construction and construction companies. In addition, only Swedish companies that prepared an annual report in Sweden were included in the list. Below in the facts box, you can read the entire list. There are also which subsidiaries are included for each group 1. Peab: 9,188 2. Skanska: 8,430 3. NCC: 8,220 4. Veidekke: 2,124 5. JM: 2,058 6. Svevia: 1,830 7 Infranord AB: 1,781 8. Serneke: 1,046 9. Strukton Rail: 949 10. Eleda Group: 700 11. AF Gruppen: 637 12. MVB: 554 13. Brixly: 522 14. Implenia Sverige AB: 514 15. Erlandssonbolagen : 493 16. NRC Group: 456 17. ByggPartner: 452 18. Sh bygg: 442 19. Åhlin &amp; Ekeroth: 411 20. Belstroj AB: 407 21. Contractor Bygg: 399 22. Sveab: 345 23. JSB: 336 24. Strabag: 315 25. Sehed Byggmästargruppen: 299 26. Thage i Skåne AB: 284 27. Bonava: 280 28. BAB: 267 29. Wästbygg: 259 30. Karaten Bygg: 257 The compilation applies to the entire group in cases where it is relevant. Here you can see which group companies were included for each company: Peab: AB Smidmek, Annehem Fastigheter AB, G Nilssons Last &amp; Planering i Ranseröd AB, HälsingeBygg i Hudiksvall AB, Lambertsson Kran AB, Olof Mobjer Entreprenad AB, Peab AB, Peab Anläggning AB, Peab Asfalt AB, Peab Bemanning AB, Peab Bostad AB, Peab Byggservice AB, Peab Fastighet AB, Peab Grundläggingn AB, Peab Industribyggnad i Norr AB, Peab PGS AB, Peab Support AB, Peab Sweden AB, TRANAB Markbyggnad AB Skanska: Skanska AB, Skanska Commercial Development Europe AB, Skanska Fastigheter Gothenburg AB, Skanska Fastigheter Stockholm AB, Skanska Financial Services AB, Skanska Industrial Solutions AB, Skanska Kommersiell Utveckling Norden AB, Skanska Sweden AB, Skanska Sweden IT AB, Skanska Öresund AB NCC: Hercules Foundation AB, NCC AB, NCC Fräs AB, NCC Industry AB, NCC Industry Nordic AB, NCC Property Development AB, NCC Property Development Nordic AB, NCC Sweden AB, Nybergs Entreprenad AB, Släryds Grus &amp; Entreprena d AB Veidekke: Arcona AB, Billström Riemer Andersson Bygg AB, Billström Riemer Andersson Mark AB, Billström Riemer Andersson Teknik AB, Lillhagen Byggnads AB, Sydobälingar AB, Veidekke Entreprenad AB, Veidekke Grundläggingn AB, Veidekke Industri AB, Veidekke Sweden AB, Vilande Brinkab AB, Vilande B&amp;B AB JM: JM AB, JM Entreprenad AB, JM@Home AB Svevia: Arento AB, Svevia AB, Svevia Betong AB Serneke: SERNEKE Group AB, Serneke Sweden AB Eleda Group: Installation &amp; Cable Entreprenad i Malmö AB, Annebergs Bygg och Anläggning AB, AXEDA Entreprenad AB, Göteborg Land och Betong Entreprenad AB, Järfälla VA- &amp; Byggetreprenad AB, Land &amp; Energibyggarna i Göteborg AB, Palms Sprängtjänst AB, Salboheds Bygg och Anläggningstjänst AB, Sandins Entreprenad AB, Sandins Rail AB, Västkustens Anläggnings AB, Westcoast Concrete AB AF Gruppen: AF Anläggning AB, AF Bygg Göteborg AB, AF Bygg Syd AB, AF Gruppen Sverige AB, AF Härnösand Byggreturer AB, AF Projektutveckling AB, Bergbolaget i Götaland AB, Betonm ast Anläggning AB, Betonmast Göteborg AB, Betonmast Malmö AB, Betonmast Mälardalen AB, Betonmast Stockholm AB, Betonmast Sweden AB, Kanonaden Entreprenad AB, Kanonaden Entreprenad Mälardalen AB MVB: MVB Astor Bygg AB, MVB Holding AB, MVB Syd AB, MVB Öst AB . JM Entreprenad AB, Jord &amp; Berg i Kungsbacka AB, Kron &amp; Karlsson Bygg &amp; Mark AB, Lunds Shakt &amp; Planering i Borlänge AB, Skölsta Mark- och Rivningsentreprenader AB, Svenska Land- och Anläggningbolagen i Kungsbacka AB, SweGrund AB, Sawing &amp; Concrete Drilling i Uddevalla AB, Tobbes Schakt AB, Tre M Bygg &amp; Fönster AB, Tångabergs Schakt AB, Västkustens Mark &amp; ​​Asfalt AB, Westins Maskin AB NRC Group: Nordic Railway Construction AB, Nordic Railway Construction Sverige AB, Nordi c Railway Construction Underhåll AB Byggpartner: Bygg Partner i Dalarna AB, ByggPartner i Dalarna Holding AB, ByggPartner i Dalarna Service AB, JUF Byggnadställningen AB Sh build: APJ Prefab AB, JMG Betong AB, Sh Asfalt AB, Sh bygg, sten och anlaging AB , Sh machine in Uppsala AB, Vallentuna Betong AB Åhlin &amp; Ekeroth: Åhlin &amp; Ekeroth Byggnads AB, Åhlin &amp; Ekeroth Invest AB Contractor Building: Contractor Bygg Holding Norr AB, Contractor Bygg i Hemavan AB, Contractor Bygg i Lycksele AB, Contractor Bygg i Skellefteå AB, Contractor Bygg i Sundsvall AB, Contractor Bygg i Umeå AB, Contractor Land i Skellefteå AB Sveab: SVEAB Anläggning AB, Sveab Järnväg AB, SVEAB Materialförädling AB, SVEAB Projektutveckling AB, SVEAB Verkasamhetstöd AB JSB: Minjar AB, JSB CONSTRUCTION AB, JSB Gruppen AB Strabag: CML Construction Services AB, NIMAB Entreprenad AB, Nimab Support AB, STRABAG Sweden AB, Züblin Scandinavia AB SEHED Byggmästargruppen: AB Tresson Balkong, AB Tresson fasad, Byggmästargruppen Stockholm BMG AB, SEHED BYGG AB, SEHED Bygg Gävleborg AB, SEHED Bygg Hälsingland AB, SEHED Tresson AB Bonava: Bonava AB, Bonava Sweden AB BAB: BAB anlægg AB, BAB bygg AB Wästbygg: Logistic Contractor AB, Logistic Contractor Entreprenad AB, WB Projektutveckling Entreprenad AB, Wästbygg Entreprenad AB, Wästbygg Gruppen AB, Wästbygg Projektutveckling AB Karaten Bygg: Karaten Bygg AB, Karaten Bygg Entreprenad Väst AB, Karaten Bygg Väst AB, VVS &amp; Kakeltjänst Sverige AB. Source: Byggföretagen. Read the latest issue of the magazine. You can also search the newspaper archive. Get in touch with web reporter Tomasz Pozar 072-215 83 36 Send e-mail This is how you who tip us off are protected Byggnadsarbetaren Box 519 101 30 Stockholm Visiting address: Hagagatan 2 113 48 Stockholm red@byggarb.se More contact details Isabella Iverus Editor-in-chief and responsible publisher Tel 010-601 10 81, 070-269 07 88 Tomasz Pozar Editor-in-chief Tel 072-215 83 36 Advertise Subscribe Change subscription address RSS Information about cookies © Copyright Byggnadsarbetaren All material on the website is protected according to the copyright law. Quote us, but please indicate the source</t>
-  </si>
-  <si>
-    <t>Student team Delft Hyperloop unveils new hyperloop capsule Atlas 02 On Monday 3 June, student team Delft Hyperloop will unveil their new hyperloop capsule, Atlas 02, in the Auditorium of Delft University of Technology. With this capsule, also called pod , the team will participate in the SpaceX Hyperloop Pod Competition in the summer of 2019. The fastest pod in the vacuum tube will be the winner of this competition taking place in Los Angeles, California. The team's goal is to win and break the current world record of 467 km/h on a one kilometer track. The TU Delft Hyperloop team consists of 40 students who build a fully working prototype for the race in one year. This race will take place on July 21 in Hawthorn on the SpaceX site. Of the 22 globally selected teams, only three teams will actually be allowed to enter the tube to race. These three teams are chosen based on 122 safety tests conducted in the week leading up to the race. “These tests are intended to demonstrate that our vehicle is working properly and that all safety requirements are met. There are elements that are tested such as: the braking system, whether the pod can handle the vacuum in the tube and whether the software works properly. These tests must all be completed successfully before the final run”, says Team Captain Rieneke van Noort. In order to prepare as well as possible for the test week, the student team is currently already busy carrying out comparable tests. For example, parts such as the motors, wheels and brakes have already been tested on a flywheel; a spinning aluminum disc that can simulate the material, movement and weight of the pod to mimic a run in the tube of SpaceX. In addition, the subsystems were also tested in vacuum by letting the pod 'run' in the vacuum tube of startup Hardt global. Since vehicle testing is a crucial factor in increasing the chances of winning, the team has been given the unique opportunity to test their entire pod on a section of track next to Hilversum Station. The team was able to realize this 300-metre long test track in collaboration with Voestalpine RailPro, ProRail and Strukton. Now that the pod has been unveiled, the team can start testing on this test track. With the vehicle, the Hyperloop team aims to go faster than 500 km/h within one kilometer. In this kilometer you will have to accelerate and slow down. For this reason, the vehicle will have to brake several times faster than a Formula 1 car. The vehicle will be powered by an electric motor. Next month the Delft Hyperloop team will leave for Los Angeles. This means moving the vehicle, all team members and the workplace to Hawthorne, California; the space of SpaceX, to dot the i's and cross the t's here before the race. Chief Engineer Elja Ebbens: “With the knowledge that the team has gathered during testing, we are now extremely well prepared for the test week. We therefore consider the chances of reaching the final and being allowed to race in the tube.” This article is a submission to the editor and is not the responsibility of the editors. All rights reserved © Emerce</t>
-  </si>
-  <si>
     <t>Latest Rail News “It’s not surprising that people should be sceptical, that’s absolutely fine,” he told us, acknowledging that their low speed makes them unsuitable for TransPennine Express, and he is “not talking to any bidders” for that new franchise. The ex-chair of Chiltern Railways now leads Vivarail, which bought much or all of the D78 stock from TfL – about 150 driving motor cars and enough vehicles altogether to form 75 units of two or three car trains. With electrification timescales looking shaky, there could be a growing need for diesel alternatives in the short to medium term, which Vivarail think they can provide. Their vision is for a new, cheap 60mph DEMU that could plug the gap – using Ford automotive engines on re-engineered District Line stock that originally came into service in 1980. Although the RMT union and others have criticised the trains as “London’s cast-offs” and branded them 'Crawlers' because of their speed, Shooter insisted in an interview with RTM that the D-Train has so many elements being replaced or upgraded that “this is effectively a new train – but we’re making it very affordable by reusing the body shell, which is aluminium and has no corrosion, and the bogies, which are only about 10 years old”. This is where Vivarail has gotten lucky. The original bogies from the D78 stock “fell to pieces”, as Shooter put it (they were too rigid and suffered cracking on the inconsistent District Line track), and from 2000-03 were replaced with Bombardier bogies (Adtranz, then) that are still in good condition, the same as used on the 1995 Stock on the Northern Line. “The result is a train that is very affordable but it will have a lot of absolutely up-to-date facilities, in terms of the engines and the alternators, the IGBT electronic power control and a number of other features and communications systems,” Shooter said. Conversion Vivarail received the first of the D78 stock on 19 January and the conversion began immediately. All of the existing DC control gear, including cam shaft control and all of the underfloor equipment used on Underground trains, was removed from the driving cars. This will be replaced by two 3L Ford Diesel engines combining to create 400hp for each driving car, plus a modern alternator and inverter with an output of 750v DC, plus a compressor. The trains will also have IGBTs (insulated gate bipolar transistors) made by Strukton Rail in Holland, and while early versions of the D-Train will come with rheostatic braking, Vivarail is looking to fit later models with a braking system that recovers and reuses the energy. “We’ve got some recycled parts clearly, but people really aren’t that bothered about bogies provided they’re unobtrusive and work and the same with the body shells,” Shooter said. “Our principal objective is that when passengers travel in this train they say ‘Isn’t this a fantastic new train?’ That’s our desired end.” Vivarail plans to have its prototype up and running on the test track at Long Marston by June, and approved by the autumn to run out on Network Rail track. Lightweight and low maintenance The D-Train will come with several notable benefits: at 25 tonnes per vehicle in the three-car formation, they will be a lot lighter than other trains (a Class 150 comes in at 35 tonnes). That helps keep fuel consumption low, as do the modern automotive engines, which shut off when the train idles. Shooter has focused on finding ways to “substantially reduce maintenance costs”, such as designing the engine units and bogies to be easily removable and replaceable. He claims the engine units can be swapped out in 10 minutes and Vivarail has also designed a notional depot that would allow the bogies to be swapped very quickly too. After Vivarail has finished overhauling the train, replacing the lights with modern LED lighting, and all the old components, there will be very little other than the bogies and engines that will require maintenance. Shooter says this gives the D-Train a big bonus: maintenance can be kept local to the line it is operating on. “There are quite a few branch lines around the country that are a long way from a maintenance depot. It might make sense to put a ‘mini-depot’ somewhere along the line, because this train does not need to go back to a proper, conventional maintenance depot,” he said. “Now if you think about the fact that you can start to keep these trains local to the line where they operate, it means that you haven’t got to waste a lot of time and money in sending them miles to a maintenance depot. That incurs fuel cost, driver cost, track access cost, and also possibly means Network Rail has to keep a line open at times when it would be more efficient for them to get on and be maintaining it at night. So there are a number of angles there and these trains would be very suitable for that.” Commuter routes, not fast routes Shooter has a particular vision where he can see the D-Train being used. Although he couldn’t go into details, he has been in talks with all of the bidders for the next Northern franchise, but he has not contacted anyone bidding for TransPennine Express. “This would not be the right train for somewhere where there’s going to be a lot of faster running. For example, I am not talking to any bidders for the TPE franchise, because the nature of their runs is quite fast running and this is not the right train for that. What this might do of course, is free up some other faster, older DMUs that can then be redeployed on some of those routes.” The D-Train will have a maximum speed of only 60mph, although it does have relatively good acceleration. Shooter believes this will make it ideal for a route with a lot of station stops. With the different configurations that Vivarail offer for the carriages, it will also be suitable for both long and short routes. Shooter also sees the D-Train as an ideal way to deal with rush-hour commuters. “Take commuting in and out of cities where there’s very heavy crowding on trains that are not going tremendously fast. Because this train is very affordable, one option would be to acquire some just to do a morning trip into the city, park up all day and then bring a load of people out in the evening,” he said. “If it’s not too long a distance what you’d probably do is keep the configuration similar to what they are now, as used on the District Line, and then it’s an efficient way of shifting a lot of people quickly in reasonable circumstances. So that’s one option.” What makes the D-Train ideal for commuter journeys is it is what the old D78 stock was originally designed for. In their original configuration they would come with four doors, making it very efficient in loading and off-loading, reducing station dwell time. However for longer routes, Shooter said that Vivarail will offer alternative configurations with some of the doors taken out to make way for more seating. Getting the Department for Transport on board As promising as the D-Train sounds, it’s hard to imagine it becoming a success without the support of the Department for Transport (DfT), which has been lukewarm on the subject of old District Line stock to say the least – publicly mindful of the potentially bad PR of being seen to replace decrepit Pacers with “London’s cast-offs”. In December a DfT spokesperson told RTM: “There is no government proposal to replace Pacer trains with old London Underground trains. “We are committed to improving services for passengers across the north. We recognise that Pacers fall short of passengers’ expectations, which is why we will be specifically requiring bidders for the next Northern franchise to phase these outdated trains out. These bids must include improved rolling stock. “The industry is best placed to tell us how more modern, better quality trains can be introduced, and it is only right that we look to them as we push ahead with our ambitious plans to transform the north’s rail network.” But Shooter says that things have moved on a lot since then. “We hadn’t been very forthcoming on what we’re doing until relatively recently, so in the absence of knowing what we’re doing, it’s not surprising that people should be sceptical, that’s absolutely fine,” he explained. “What I can say is that we’re now being much more public about what we’re doing and explaining just how much time and money we’ve put into this, which is quite considerable. And of course I’ve been briefing officials at the DfT so that they’re now aware in a great deal of detail what it is that we’re offering to operators.” (Library image of Adrian Shooter) With the rolling stock problems facing the rail network the D-Train could just be the right solution and the right time. But what inspired Shooter in coming up with the scheme in the first place? “I bought some of the last DMUs that were bought in this country, the 172s, which we bought for Chiltern and London Overground. They’re a good train but they’re very expensive,” he said. “So I looked around at what the alternative might be, and the fact that there is going to be, at least for a few years, a shortage of DMUs until electrification catches up. Leasing companies are not going to want to lease something that’s probably got a 40-year life if they can only really see 10 years’ worth of use. So I said to myself, if we could produce something that was affordable, maybe we can fill that gap – so why not do some re-engineering?” Interview by Sam McCaffrey Tell us what you think – have your say below, or email us directly at [email protected] Mick   23/01/2015 at 12:05 What a refreshing attitude from Mr Shooter; cheap and cheerful, an understanding of what the passengers need. Easy to get on and off is just the job for commuters. Probably be ideal on local lines around Bristol, Exeter and Cornwall branches at peak times</t>
   </si>
   <si>
+    <t>On Board Systems Professional Market 2028 Key Insights and Leading Players DEUTA-WERKE GmbH, HUBER+SUHNER, Strukton Rail, ABB, Knorr-Bremse AG, CAF GROUP, etc The study provides an overview of how business professionals in the Global On Board Systems Professional Market report have established a globally unique model to strategize the policies to contain the deleterious impact of the COVID-19 pandemic. The report highlights those market sectors that present a positive growth trend and a positive future outlook for the market participants by 2022-2027. This report analyzes the economic performance of On Board Systems Professional market taking into consideration various analytical frameworks such as SWOT analysis, PEST analysis, competitive analysis, etc methods. The segments that have witnessed increase in the annual sales, market share because of the significant factors like trade and other. Key Players in the On Board Systems Professional market: DEUTA-WERKE GmbH HUBER+SUHNER Strukton Rail ABB Knorr-Bremse AG CAF GROUP MEN Mikro Elektronik GmbH Siemens AG Thales Group Amaronia Rail Ltd ALSTOM SA ASELSAN A Eke Group Leroy Automation Request a sample report : https://www.orbisresearch.com/contacts/request-sample/6797158 The On Board Systems Professional report outlines business models and marketing strategies incorporated by market players to sustain the competition and accelerate business growth in market. Through various market scenarios, it recommends some solutions to implement in future to stay ahead of the competition and gives detailed insights about the covid-19 impact on the market. The report highlights the trends that influenced or hampered the market during covid-19 and identifies existing opportunities and strategies to be adopted to stay competitive in market in the post-pandemic world are highlighted in the report. The report identifies the investment opportunities in the market by country and by sectors and provides assessment and comparative analysis of over 100 countries and companies operating in the market. On Board Systems Professional Market Types: GSM-R Wi-Fi TETRA) On Board Systems Professional Market Applications: Train Metro The report highlights government initiatives that enabled On Board Systems Professional infrastructural support. The report details the value added products and services that can further enhance customer retention. The dominant market segment region-wise and country-wise are identified in the report with associated investment opportunities and recommendations to accelerate growth. The report identifies market sizes of the dominating segments, industry players, and classifications of the sectors based in product types. It studies the performance of market across the major geographic regions. The report classifies each segment, determines the current market size, growth projection in forecast years 2021-2028, and products and services offered. The report highlights the policies implemented by different governments in steering the growth of the On Board Systems Professional market at regional and global fronts. Do Inquiry before Accessing Report at: https://www.orbisresearch.com/contacts/enquiry-before-buying/6797158 About Us: Orbis Research (orbisresearch.com) is a single point aid for all your market research requirements. We have a vast database of reports from leading publishers and authors across the globe. We specialize in delivering customized reports as per the requirements of our clients. We have complete information about our publishers and hence are sure about the accuracy of the industries and verticals of their specialization. This helps our clients to map their needs and we produce the perfect required market research study for our clients. Contact Us: Hector CostelloSenior Manager – Client Engagements4144N Central Expressway,Suite 600, Dallas,Texas – 75204, U.S.A.Phone No.: USA: +1 (972)-362-8199 | IND: +91 895 659 5155Email ID: sales@orbisresearch.com</t>
+  </si>
+  <si>
+    <t>Who is Gerard Sanderink and why is Justice demanding his resignation from Centric? Sanderink, 74, has built up an impressive empire of companies from the ground up. We can rightly call the farmer’s son, who was born in Weerselo, a self-made millionaire. Business magazine Quote estimated his net worth last year at 550 million euros. This entrepreneurship started in 1978, when Sanderink founded his first company, ICT Automatisering, together with his partner Hans Quellhorst. After selling his shares, he went his own way in 1992 and founded the Sanderink Groep. In the years that follow, one company after another is taken over. Sanderink’s credit is that they are often failing companies that he cleans up and incorporates. The rapidly growing company that was created in this way specializes in software and secondment and was renamed Centric around the turn of the century. With the proceeds, Sanderink also acquires Oranjewoud engineering firm (2005) and railway builder Strukton (2010). But that reputation as a company doctor will melt like snow in the sun from the end of 2018, after his split with his girlfriend Brigitte van Egten. According to insiders, she is also the business support and rock of Sanderink, the two have known each other since 2002. Sanderink’s new girlfriend is Rian van Rijbroek, a woman who steps out of the shadows at the beginning of 2018 and presents herself in much-discussed broadcasts of Nieuwsuur and BNR Nieuwsradio as cybersecurity expert and former secret service hacker. All fingers point to Van Rijbroek. She would play Sanderink and set him up against Van Egten and several executives of his companies. A period full of mud-slinging and lawsuits begins. Nine top managers will leave Centric in 2019. Clients such as Action and NN are asking questions about Sanderink’s close relationship with the controversial Van Rijbroek, who would help Centric set up a cybersecurity department at the time. But of a man of his stature, that may have been thought too easily. Before that time, Sanderink was portrayed as a down-to-earth local from Twente, averse to expensive stuff or ostentation. Would someone with such a reputation, plus years of experience as a shrewd businessman, be so easily deceived? It is a question that will stick if a media storm around Sanderink and his affairs arises from 2019 onwards. Sanderink would see conspiracies everywhere and be convinced that the Public Prosecution Service and the government want to take everything from him. Due to the ‘unrest that has arisen’ around his person, the exodus of employees and the many lawsuits, Sanderink will step down as director of his companies Centric, Oranjewoud and Strukton in 2021. He still owns it. Now more than a year later, several podcasts and a book have been published about the Twente IT multimillionaire. Always asking the same question: what happened to the man who for years built his empire with 15,000 employees in relative peace? That is because on Wednesday it was suddenly announced that Sanderink will return as chairman of the board at Centric. The same press release states that two non-executive directors are resigning from their duties “in good harmony” and are leaving Centric. In passing, the company announced that Sanderink will focus on a new strategy for the ICT service provider in the coming period. A day later, the Public Prosecution Service makes itself heard. Justice announced publicly on Thursday afternoon that it had contacted Centric about the reappointment of Sanderink and the resignation of the two directors. “That reinforces the already prevailing unrest within Centric,” writes the Public Prosecution Service, which immediately sets a deadline. The company has until Monday to reverse the decision. This has everything to do with the services that Centric offers. The company (annual turnover 422 million euros) is in the capillaries of the Dutch government. Municipalities use Centric for various matters such as their administration, digital services to citizens and have maintenance contracts with the company. Centric manages data centers and supplies software developers and IT administrators to local authorities, among others. But well-known companies such as ASML and Action also purchase services from Centric. Just like BNG Bank, the main bank of Dutch municipalities, provinces, housing associations and healthcare institutions, among others. The question is for how long. For example, the Social Insurance Bank (which manages and pays, among other things, the AOW and child benefits) and the regulator De Nederlandsche Bank have already dropped out. BNG Bank is also reportedly considering this. Then the Public Prosecution Service reports to the Enterprise Chamber of the Amsterdam Court of Appeal, the court for business. A highly unusual move, as the Justice Department rarely interferes directly in the management of a company. The Enterprise Chamber has the right to intervene in the case of mismanagement at companies and to suspend directors. This usually happens after complaints from involved employees or shareholders. But in the case of Centric, that is difficult: Sanderink is in full control. “Stability at Centric is of great importance for the many employees and for the customers who depend on Centric’s software, including a number of government agencies,” the Public Prosecution Service wrote on Thursday. But according to Justice, Centric itself appears to be insufficiently able to restore peace. “The Public Prosecution Service therefore concludes that it is appropriate to request the Enterprise Chamber to decide whether, and if so which measures are necessary to guarantee the stability and continuity of Centric.” So to be continued. Your email address will not be published. Required fields are marked * Comment * Name * Email * Website Save my name, email, and website in this browser for the next time I comment. Ruetir| Latest News, World News, Breaking News, Games,Technology, Business, Lifestyle, Fashion, Sports, Food &amp; Technology. Contact Us : [email protected] © Ruetir 2022. All Rights Reserved. © Ruetir 2022. All Rights Reserved</t>
+  </si>
+  <si>
+    <t>Satisfied faces at provincial firefighter competitions in Zutphen These are organized by the (ABWC) General firefighter competition committee. The TAS-HD track was located in the former building of Bührmann Ubbens, the 112 track in the Strukton Rail workshop. TAS-HDParticipating forces were alerted for a police assistance. In the beginning it was not yet clear what was happening in the building. Once on the road, the emergency center (AC) reported that it was a fire. On site, the first firefighters went to reconnoitre and found out that a fire was raging on the first floor. Upon entering the building, the arrest team immediately came downstairs with an arrested person. Although he came out loudly, he turned out to have burns on his hands. The firefighters and women remained professional and went on further reconnaissance. Eventually they ended up in a room that was full of smoke. After some detective work, including a thermal imaging camera, the second victim was soon found. It took them the necessary effort to bring him to safety. This because he had chained himself to a concrete post with a chain. But?? He asked the firefighters to pack his things. They turned out to be packages of drugs. A fire was started by a drug lab. After he was freed and brought outside, they started looking for the third victim. He was also found quickly, quite drunk. He apparently liked it so much that it wanted to get a high-five from the arrest team several times. After no more victims were present, the fire was extinguished and the property was handed over to the police. 112 track During work on a train, in a grease pit, in the workshop of Strukton Rail, an entrapment occurred for unknown reasons. An employee got his leg stuck under a pallet of ironwork. His colleague assisted him and kept talking to him until the emergency services arrived. An emergency response officer, who was quite panicked, led the firefighters to the place where his colleague was. The emergency response officer and the victim were then calmed down and the trapped victim could be liberated. Less than five minutes later…. The emergency response officer: "Fire!" Armed with a fire extinguisher, he jumped into the train and tried to extinguish the fire. However, he got himself into trouble and had to be rescued by the fire brigade himself. While other firefighters dealt with the trapped victim under the train, others prepared to extinguish the fire and rescue the emergency response officer. During the fire there was a lot of smoke development and the other victim was put on a mask so as not to inhale smoke. A short time later, the trapped victim was freed and brought outside. SatisfiedBoth the Zutphen fire brigade and the ABWC can look back on a successful day. The influx of the public and the beautiful weather played a major role in this. Participating corps: Kesteren, Elburg, Elspeet, Neerijnen West, Wageningen, Lingewaal, Creil, Oldebroek, Elst, Zetten, Lichtenvoorde, Culemborg, Maasdriel, Groenlo, Ens, Lienden, Otterlo, Gameren and Wehl. Responding to this article is no longer possible 112Doetinchem is looking for photographers, will you join our team? Are you interested in local news and the work of emergency services? Read more here</t>
+  </si>
+  <si>
     <t>Integrity Good business practices, integrity, respect, supervision, transparent reporting and accountability are the leading aspects of our business. We owe our success to our core competencies in the implementation of projects at world level, and to always acting ethically correct and with integrity. In all operating companies worldwide, we insist on integrity in doing business. Strukton All Right is the title of our policy of acting with integrity. With this programme, we use training courses, presentation and internal communication to pay intensive attention to our company culture to make employees more aware of ethical rules, authorisations, compliance with legislation and regulations both at home and abroad, and risk management when collaborating with domestic and foreign parties. We have various rules and by-laws indicating the framework for the performance and operations. Our Code of Conduct Honest Business Practice sets out the key rules that Strukton imposes for fair and just business. It helps determine what is fair and just at work, in addition to the existing local legislation. The Code has an integral structure, clearly connecting into various existing policy documents and rules, including the policy for dealing with gifts and invitations, the policy for countering bribes and corruption, the human rights policy and the regulations regarding undesirable behaviour. The regulations regarding undesirable behaviour allow employees to report any actual or suspected irregularities to a confidential counsellor. Additionally, we offer employees the possibility to anonymously report any suspected abuse of or non-compliance with the regulations to an external party. (116 kb) Open document (223 kb) (83 kb) (990 kb) (45 kb) (121 kb) (141 kb) Do you wish to know more about the Strukton All Right Integrity Programme? The compliance officers will be happy to tell you more: Ingrid de Jong (ingrid.dejong@strukton.com) Jan van de Riet (jan.vanderiet@strukton.com) Stephan Lutters (stephan.lutters@strukton.com)</t>
   </si>
   <si>
@@ -739,22 +720,19 @@
     <t>Concrete repair Building in concrete. We understand that. With specialist knowledge and years of experience, we offer high-quality craftsmanship in concrete repair. Concrete, a widely used material for those looking for a sturdy, massive and relatively cheap solution. Concrete has extremely many advantages compared to other materials, which makes it very interesting to use. Building in an inhabited environment places high demands on the contractors. The building space is almost always limited, the time margin minimal. That is why our work does not lack smart techniques that support and make the construction process possible. Just like professional ways to improve or restore the lifespan and quality of concrete structures. However, concrete can lose its strength if it is compromised. Damage can be caused by aging, fire, implementation or design errors, but also by factors such as the weather or, for example, acid or chlorides. Another common damage pattern is that the reinforcement starts to rust. Due to the expansion of rust, the concrete can be pressed around the reinforcement (cover). It is very important that the concrete is renovated if it no longer meets the requirements. Concrete must always be in good condition to guarantee the (structural) safety of a structure. SMT Betontechniek can sustainably renovate the concrete so that it can last for years. Within Strukton Milieutechniek, we have brought together the inspection, repair, renovation and conservation of concrete structures in a specialized Concrete Repair team. We carry out inspections and repairs, advise on maintenance and realize small and large-scale repairs to concrete structures. We work on quays, bridges, tunnels, underpasses and roads, among other things. We also have experience in carrying out (concrete) maintenance at industrial factory locations. Our knowledge of different types of concrete, such as reinforced concrete, prestressed concrete, lightweight concrete and underwater concrete, in combination with knowledge of the various concrete repair techniques, ensures the sustainability of the repair work we carry out. Quality and comfort are central to this, for now and in the future. SMT Betontechniek is fully certified to carry out concrete repairs in accordance with the rules of NEN-EN 1504, CUR recommendation 118 and BRL 3201 part 1 and 2. This means that we can provide aesthetic, technical and constructive concrete repairs. There is also a concrete maintenance expert in our team. We carry out our repair work ourselves. SMT Betontechniek carries out the work itself. We immediately convert advice into suitable solutions. The team is trained from various disciplines so that we can advise and unburden you with our own experts on larger or more complex projects. When concrete is damaged, it must be renovated. First of all, it is important to find out why damage to the concrete could have occurred. It is necessary to find out so that it can be avoided in the future. Our concrete maintenance expert is happy to assist you. We can carry out a repair by means of manual repair, we often repair larger concrete damage by pouring the repair spot or by applying shotcrete. We can also apply the shotcrete in the right color, making the repair virtually invisible. For example, to prevent concrete damage, the use of carbonation-inhibiting liquid-tight coatings is a good solution. This coating protects the concrete against weather influences, among other things. Marco de Ruiter Project leader marco.deruiter@smtbetontechniek.com 0627458757 Page Page Project</t>
   </si>
   <si>
-    <t>Strukton CEO Sanderink suspected of bribery in Saudi Arabia The investigation by the Public Prosecution Service (OM) is still in the management phase. This means that the Public Prosecution Service has not yet sent a summons. It is still unclear whether the Public Prosecution Service will eventually prosecute Sanderink, according to his lawyer Paul Acda. The Fiscal Intelligence and Investigation Service (FIOD) raided Strukton in 2019 because of a metro project in the Saudi capital Riyadh. The Dutch construction company was awarded a contract of 1 billion euros for the construction of the metro network in the city. Sanderink is suspected of leading the official bribery of a Saudi prince to get that job. Acda has asked the investigating judge to question several witnesses. They would paint a more complete picture of the Saudi issue than the FIOD. The counsel says that between the raid in 2019 and the beginning of this year, Strukton was guessing what the exact suspicions were. An OM spokesperson does not want to say much more about the suspicions and the suspects. The OM expects to bring the case to court in 2023 or 2024. ©2022 DPG Media B.V. - all rights reserved</t>
-  </si>
-  <si>
     <t>Long-term no train traffic possible between Dronten and Lelystad (update) News Published on September 3, 2022 - Latest update: September 7, 2022 1:18 PM The damage to the infrastructure of the railway between Dronten and Lelystad is enormous. As a result, no train traffic will be possible until at least the beginning of October 2022. A new forecast will follow in the week of September 12. This forecast is expected to shift further due to the extent of the damage. ProRail inspectors are currently investigating the exact damage together with maintenance contractor Strukton. We are working hard to map the damage from the power outage in Swifterbant and to provide a forecast for the period of recovery. We cannot give a realistic prognosis at this time. We know that no trains will run on the Lelystad - Dronten route until at least the beginning of October, but this is expected to take longer. The period from the beginning of October, which can be seen in travel planners since today, is intended not to give wrong expectations when planning travel in the future. In the week of September 12, we expect to be able to give an initial forecast about how long the recovery will take. The damage is a result of the incident on Friday afternoon, September 2. A high-voltage cable from grid operator TenneT then ended up on the overhead line near Swifterbant. The incident caused an enormous amount of power to pass through our systems in a short period of time. As a result, relay boxes have become defective underground. Cables and switches are burnt out. A lot of equipment damage was caused in both a substation and a switching station. There is also a lot of damage underground that still needs to be investigated. It may be that over a distance of several kilometers all infrastructure for the energy supply and train protection systems must be renewed. It is already clear that the damage will run into the millions and the recovery will be a huge operation. Once the exact damage has been mapped out, we can indicate how long the recovery will take. November 22, 2022 November 7, 2022 October 26, 2022 Do you live or work within 300 meters of the railway? Then use our rail check. You can immediately see which activities are planned in your area. This field is required and only accepts numbers and letters This field is required and only accepts numbers When you visit our website you will receive cookies. No filled cakes or stroopwafels, but temporary digital files. We use functional, analytical and marketing cookies. The functional cookies are necessary for this website to work properly. So they are always on. You can give your consent below for the analytical cookies and marketing cookies. More information about our cookies can be found in our cookie policy</t>
   </si>
   <si>
-    <t>Treinenweb.nl Most likely, there will be no train traffic between Dronten and Lelystad for weeks due to the short circuit of a TenneT high-voltage cable that hit the overhead lines on Friday afternoon. ProRail cautiously expects that no train traffic will run on this route until at least September 15, but this could take even longer. This forecast is expected to shift further due to the extent of the damage. ProRail inspectors are currently investigating the exact damage together with maintenance contractor Strukton. It is now clear that many electrical installations and cables have failed due to the enormous power surge. The incident caused an enormous amount of power to pass through our systems in a short period of time. As a result, relay boxes have become defective underground. Cables and switches are burnt out. A lot of equipment damage was caused in both a substation and a switching station. There is also a lot of damage underground that still needs to be investigated. It may be that over a distance of several kilometers all infrastructure for the energy supply and train protection systems must be renewed. It is currently clear to the rail manager that the damage will run into the millions and the repair will be a huge operation. Once the exact damage has been mapped out, ProRail can indicate how long the repair will take. Long-term no train traffic possible between Dronten and Lelystad. The damage to the rail infrastructure in Flevoland is extensive. The recovery will take a long time. The prognosis is now on September 15, but there is a good chance that it will take much longer: https://t.co/E9t1emQuwo #short circuit pic.twitter.com/zrCt87gnOU Source: ProRail © 2007 - 2022 Treinenweb.nl. All rights reserved Contact Our friends Disclaimer</t>
-  </si>
-  <si>
     <t>Train collides with empty city bus News Published on October 17, 2022 - Latest update: October 21, 2022 10:18 AM On Monday, October 17, a train collided with a stationary, empty city bus at a level crossing on Marconilaan in Bergen op Zoom. The collision caused havoc, but luckily there were no injuries. It was a traumatic experience for both the bus driver and the train driver. Our thoughts go out to them. An investigation has been carried out into the cause of the accident. It was quite a job, but after four days of hard work, the track at Bergen op zoom has been fully repaired. On Friday morning, October 21, the train service could be restarted. Immediately after the accident, our contractor Strukton set to work together with subcontractors and suppliers to get an overall picture of the damage and what was needed to repair it as quickly as possible. The damage only really became apparent after the bus was towed away. Over a length of 250 metres, all rails and sleepers were broken. In addition, there was a lot of oil on the track. A small repair was also necessary to the overhead line. But the biggest challenge was still the logistical operation to have enough people and material available in a short time. People from all over the country have traveled to Zeeland to participate. We would therefore like to thank everyone who contributed to this for the hard work that has been done these days. And a special thanks to the driving school owner who made his terrain available to us. Unfortunately, we need more time to repair the track in Bergen op Zoom. As a result, no trains will run between Bergen op Zoom and Roosendaal until 07:30 on Friday morning. Previously, the hope was that train traffic could be restarted on Thursday afternoon, but we already indicated that this was not certain. The work is large and therefore requires time. Contractor Strukton is busy repairing broken sleepers and 300 meters of rail, among other things. A completely new level crossing must also be installed. Consult travel planner Train traffic between Bergen op Zoom and Vlissingen largely resumed yesterday evening. Train traffic between Bergen op Zoom and Roosendaal will remain blocked until at least Thursday afternoon, October 20. Buses replace rail traffic between these two cities. In order to properly investigate the accident, we initially had to supply power over a large part of the overhead line. Also at Bergen op Zoom station. Therefore, the station could temporarily not be used at all. Now that is possible again, so that a large part of the trains can run to Zeeland. It is expected that we will be working on repairing the track at the accident site until at least Thursday afternoon. Among other things, a new level crossing installation must be installed and the soil must be cleaned up. Diesel was released during the collision. In addition, a piece of track is damaged: that must first be repaired. The rail contractor has mapped out the damage and shared an initial prognosis. The repair work is expected to take at least three days. There is currently no train traffic between Bergen op Zoom and Roosendaal. We are evacuating the passengers from the train. The rail contractor is on site to assess the damage and draw up a plan for the repair. We are currently unable to indicate when trains will be able to run on this route again. John Voppen, CEO at ProRail, responded to the incident: "This could have been a dramatic day for the railway. Several people have had an angel on their shoulders. And yet this must be a traumatic experience for both the driver and the driver . Our thoughts go out to them in the first instance. Our colleagues will ensure that the track becomes passable again. That is where the focus is now. In addition, we want to get to the bottom of how this could have happened. That is why we will also fully participate in the investigation." September 29, 2022 May 16, 2022 December 30, 2021 Do you live or work within 300 meters of the railway? Then use our rail check. You can immediately see which activities are planned in your area. This field is required and only accepts numbers and letters This field is required and only accepts numbers When you visit our website you will receive cookies. No filled cakes or stroopwafels, but temporary digital files. We use functional, analytical and marketing cookies. The functional cookies are necessary for this website to work properly. So they are always on. You can give your consent below for the analytical cookies and marketing cookies. More information about our cookies can be found in our cookie policy</t>
   </si>
   <si>
-    <t>Here you can see how a huge tunnel is pushed under the A2 A mega job, but shown with this video in just a few minutes. Here you can see how a huge tunnel box weighing millions of kilos is pushed under the A2 at the Batadorp junction in Eindhoven.   Earlier this week, the municipality and Strukton described the precise positioning of the tunnel box as a real masterpiece. The job was preceded by more than a year of preparation together with ‘Rijkswaterstaat‘ (Directorate-General for Public Works and Water Management). Joystick The tunnel’s components were placed under the A2 with millimetre precision using special machines controlled by a joystick. In total, some 200 men are working on the job. Traffic pressure The tunnel should make it easier for freight traffic to leave the large GDC industrial estate in Acht. This business park is growing rapidly. The connection between GDC and the Brainport Industries Campus and Eindhoven Airport should also be improved. The tunnel should also reduce the amount of traffic at the Batadorp junction and the Antony Fokkerweg. Work It will take another year before traffic can use the new subway. First the tunnel has to be finished and the roads around it constructed. Due to the work, there may be considerable traffic jams in the near future. The municipality of Eindhoven and Paul Poels Fotografie made the images and the editing. Source: Studio040 Save my name, email, and website in this browser for the next time I comment. Δ</t>
+    <t>Treinenweb.nl Train traffic in Zeeland was partly resumed on Monday evening. Due to a collision with a bus without passengers, major damage was caused to the track and infrastructure. Trains are now running again between Bergen op Zoom and Vlissingen, but between Bergen op Zoom and Roosendaal, ProRail expects to run trains again on Friday morning. "Unfortunately, we need more time to repair the track in Bergen op Zoom. As a result, no trains will run between Bergen op Zoom and Roosendaal until 07:30 on Friday morning," the rail manager reports. Earlier it was expected that train traffic could be restarted on Thursday afternoon, but a blow was given. Contractor Strukton is busy repairing broken sleepers and 300 meters of rail, a new installation for the level crossing and cabling along the track. On Monday morning at a level crossing in Bergen op Zoom, a train collided with a bus that was stopped at the level crossing for unknown reasons. The train ran right through the bus. There were no passengers on the bus. The bus driver would have left the bus in time to warn the driver of the approaching train. John Voppen, CEO of ProRail, responded to the incident: "This could have been a dramatic day for the railway. Several people have had an angel on their shoulders. And yet this must be a traumatic experience for both the driver and the driver. Our thoughts initially go out to them. Eelco van Asch, Director of Operations at the Dutch Railways, spoke of "a terrible accident that fortunately did not cause any casualties". "Colleagues have taken them over to talk about their experiences." © 2007 - 2022 Treinenweb.nl All rights reserved Contact Our friends Disclaimer</t>
   </si>
   <si>
     <t>IRJ InnoTrans 2022 preview; R - Z We have split the article alphabetically across four separate posts. In this final part we include companies from R-Z . Part one (A-E) is available here, part two (F-K) here, and part three (L-P) here. Rail Vision (Hall 9, stand 455) will showcase its driver assistance system which harnesses AI and advanced electro-optical sensor technologies, and which can identify and categorise obstacles on or near the track. The supplier is working with Hitachi Rail to equip the AutoHaul system used by Rio Tinto in Australia following successful tests at Hitachi’s test track in Naples. Robel Group (Hall 26, stand 470 and Track area O3/70 plus Plasser Robel Services Track area O3/65) will present more than 20 machines and solutions for track maintenance. At the outside exhibit, Robel Rail Construction Machines will show various hand-operated machines with electric and hybrid drives. Robel’s rail vehicles include the brand new Roclean Cleaning System, which combines automated surface extraction with manual cleaning using suction hoses, and which the manufacturer says is designed to significantly reduce fire load and fine dust in underground railways. The exhibitor will also show the Romill Urban E³ milling train, which is optimised for use on underground lines. The machine is equipped with hybrid drive and milling technology from Schweerbau International (Track Area O3/90/95) and measuring equipment from Vogel &amp; Plötscher. On the Robel stand, Vogel &amp; Plötscher will exhibit its Rail Surface Crack Measurement (RSCM) device for measuring crack depths and irregularities in the rail surface. New company Plasser Robel Services will present its multi-brand service programme for rail vehicles, and the latest addition to the group, Robel Rail Automation, will present studies on the automation of labour-intensive manual maintenance tasks. SAB Bröckskes Special Cables (Hall 14.1, stand 210) will display the new SAB RailLine 560 cable, which the supplier says, with the help of the latest materials, is continuously flexible, halogen-free, and possesses the highest level of flame protection as well as non-toxic characteristics. The cable is able to withstand a range of weather conditions during outdoor use and at the same time has good ozone, UV, oil and fuel resistance. It is also resistant against mechanical stress. Outside Siemens Mobility (Hall 27, stand 230 and Track Areas 04/36, 06/40, 50, 60, 07/40, 50, 70) will show seven vehicles: the Mireo Plus H hydrogen multiple unit (p38), a Desiro HC, a Vectron Dual Mode locomotive and a 230km/h Vectron Multi System, along with a four-car Siemens Avenio LRV and an X-Wagen automated metro train for Vienna. Highlights of the inside exhibit include the launch of its open digital business platform, Siemens Xcelerator. Clean, smart, safe and accurate is the theme of the Speno (Hall 26, stand 120) exhibit. The supplier will present its track cleaning machines, which employ a specialised technique to recover debris and metal shavings from the grinding process. Speno will also highlight its solutions to identify the most appropriate grinding patterns and to self-diagnose potential faults; and technology to help operators avoid any interference between grinding equipment and trackside devices such as axle-counters and hot box detectors. Other highlights include real-time monitoring equipment for track conditions. For the first time Stadler (Hall 2.2, stand 160 for main stand; Hall hub 27, stand 750 for signalling) will have a separate stand dedicated to its signalling portfolio, including ATO, ETCS, CBTC and railway safety systems. In addition, the supplier will present seven new rail vehicles at the outside track area: the Hydrogen Flirt H2 multiple-unit for the San Bernadino County Transportation Authority in the United States; a two-car battery Flirt for the NAH.SH network in Schleswig-Holstein, Germany; a Tina LRV for the Heag Mobilo transport company in the Darmstadt-Dieburg district of Germany; and a new Euro 9000 locomotive for European Loc Pool (ELP) in Switzerland. There will also be three trains for the British market: a Flirt tri-mode train for Transport for Wales (TfW); a Citylink tram-train for TfW; and a battery-electric EMU for Merseyrail. Infrastructure construction, renewal and maintenance company Strukton Rail (Hall 25, stand 285) will present “Leonardo,” a form of Google Street View for railway lines. Strukton will also show its robot for monitoring crane track systems and automatic rail structures. In addition, it will demonstrate an exoskeleton with an incorporated safety harness for working on overhead wires, which it has developed alongside the TU Delft Robotics Institute. Company representatives will also be on hand to demonstrate the HoloLens augmented reality application for training and instruction. Visitors to the Thales (Hall 27, stand 570) exhibit will be met by a digital wall, which will showcase projects the company has worked on around the world. Visitors can also test the latest generation of Thales’ digital integrated platform to supervise all wayside and onboard subsystems with a single click, as well as platforms for revenue collection and sharing. Thales will also showcase its latest digital train control and smart maintenance technology, as well as its end-to-end cybersecurity products. Outside, visitors can also board Lucy, Thales’ ERTMS test train (Track Area T04/29). Traktionssyteme Austria (TSA) (Hall 18, stand 310) will display traction motors for the new type J/JK metro train fleet for BVG, Berlin, built by Stadler; for CAF DEMUs for Transport for New South Wales’ TrainLink regional train project in Australia; and for Renfe’s latest series 106 and 122 high-speed trains built by Talgo (Hall 4.2, stand 450). TSA will also show its traction drive for the type X metro fleet for Vienna built by Siemens. Among the latest products on show at the Voith (Hall 1.2, stand 130) exhibit is the CargoFlex Digital Automatic Coupler (DAC) (pictured). Based on the Scharfenberg design, the coupler has already demonstrated high reliability in winter tests under extreme climate conditions in Sweden, in the Swiss mountains and in the climate chamber of DB Cargo in Minden. Voith will also show its MultiMode gear units for passenger rolling stock. The supplier says the transverse drives combine the advantages of modularised and parameterised products, ensuring speedy delivery and high level of gear unit availability. Vollert (Hall 21, stand 160) will showcase its battery-powered shunting solutions, including the road-rail robot Vlex. Vollert has supplied the model to Fret SNCF’s maintenance site in Modane. The compact road-rail robot shunts locomotives weighing up to 120 tonnes into the site’s 14 maintenance areas and is able to withstand the mountain region’s harsh weather conditions. Vollert will also present in a live demo the new IIoT service module, which offers virtual monitoring of shunting operations to allow resolution of errors as they arise. Vossloh (Hall 26, stand 975) is focusing its exhibit around three key themes: advanced infrastructure, future turnout environment, and smart maintenance. The supplier says it is focusing on tailored solutions that improve the durability and resilience of track infrastructure to increasing demand. The supplier will show its range of products, tools and services as well as its digital offering. VTG (Hall 6.2, stand 410) subsidiary Waggonwerk Brühl is a provider of wagon repair and maintenance services at its main facility in Wesseling near Cologne, and satellite workshops at Syke near Bremen and Schwarzheide near Dresden. At InnoTrans the service provider will bring its offer to life by demonstrating its wagon repair workshop to visitors through VR. Wabtec (Hall 1.2, stand 210) will highlight products to decarbonise the rail industry, including FLXdrive, the world’s first 100% battery-powered heavy-haul locomotive. The company will also showcase its latest signalling and digital solutions. Also featured will be the latest Wabtec braking technologies such as DistanceMaster, Green Friction and Regioflex, as well as products to transform the commuter experience with HVAC solutions such as Green Air and Bluefilter, along with passenger information systems such as the iSmart Displays. ZF Innovation (Hall 20, stand 580) will highlight its digital condition monitoring system [email protected], and will demonstrate how integrated sensors and advanced data analysis tools can further improve efficiency, reliability and safety in rail. Modular in design and compatible with new and existing rail vehicles, [email protected]’s functions range from wireless component identification to monitoring of flat spots, wheel tread wear, track and driveline components. In addition, ZF experts will give a presentation on connectivity solutions to partners and customers at the stand on September 22 at 16.00. Zonegreen (Hall 2.2, stand 230) will present its technology designed to automate depot safety procedures, removing manual processes and the risk of human error while allowing the effective movement of vehicles. Among the highlights are demonstrations of Depot Personal Protection System (DPPS), which safeguards workers by using Network Rail-approved powered derailers, linked to road end panels that control vehicle movements. Staff log on via RFID tags that record where they are working, with access permission for trains only granted if the route is clear. Zonegreen systems embody the concept of distributed intelligence, meaning there is no master controller or single point failures</t>
+  </si>
+  <si>
+    <t>Eindhoven begins construction of underpass A2 The construction of the tunnel under the A2 motorway has started. The project is part of improving the accessibility of Eindhoven North-West. The tunnel is to connect the new road through BIC North to the GDC business park. The tunnel will be connected to the traffic circle on Mispelhoefstraat. Construction company Strukton Civiel will perform the work. The renewal of the road infrastructure in North-West includes other projects as well. The construction of the Tegenbosch bicycle bridge and the connection between Anthony Fokkerweg and Spottersweg were also part of the renewal. Making Eindhoven Northwest more accessible should benefit Eindhoven Airport, FlightForum, and the BIC, among others. The underpass of the A2 is expected to be completed by the end of 2023. Source: www.studio040.nl Translation: Chaitali Sengupta. She also gives online INBURGERING classes. Save my name, email, and website in this browser for the next time I comment. Δ</t>
   </si>
   <si>
     <t>ProRail and NS on pole position News Published on September 5, 2022 Professional work prior to the Dutch Grand Prix has ensured that a train came to Zandvoort almost every 5 minutes this weekend. Tens of thousands of train passengers have arrived safely and on time at the track and have been brought home. During the race days, employees of the traffic control posts in Alkmaar and Amsterdam monitored the situation on the track for days. They had to intervene a few times due to unexpected malfunctions. They were resolved in record time. Our incident responders were also constantly on standby. They were on pole position along the track but hardly used their safety car. There were no significant incidents. The crowd management for which NS was responsible also worked well. It was extremely busy at the stations along the Amsterdam – Zandvoort aan Zee route from time to time. The clear signage and the many colleagues who steered fans in the right direction with a smile ensured that no panic broke out anywhere. In general, everyone is enthusiastic about the railway. As one of the travelers exclaimed: "It's going like a train!" Mirjam van Velthuizen, Chief Financial Officer of ProRail, has had an exciting Formula 1 afternoon. “It's fantastic to be part of this event. I have great admiration for our railway performance: hundreds of trains, three days in a row. And tens of thousands of cheerful fans who come by train and then relax to the circuit via the event platforms, the widened stairs and the 'events bridge'. It is wonderful to see that all this has been achieved through the dedication and expertise within our company.” Harro Homan, regional director of Randstad North, is also very enthusiastic. “Last year we ran twelve trains per hour for the first time. Then it went very well, of course, but the stands were 'only' 75% full. This year it was full house. And that also meant many more train passengers.” The NS said that from time to time it was very busy in Haarlem and Amsterdam, but that the crowd managers did an excellent job. Harro Homan: “There were no unsafe situations anywhere. Of course, the travelers also took into account the crowds in advance. They behaved very disciplined. But they also had great days!” Those twelve trains per hour did not just run. Behind the scenes, a lot of hard work has gone into making Zandvoort accessible. And so the race for ProRail started long before the Dutch Grand Prix weekend. Rails to the race Train traffic has been hampered a few times by disruptions. On Friday morning there was a broken down train and on Saturday a bus crashed into a railway viaduct. This caused some delays on the track. “The breakdown teams of contractors Strukton and VolkerRail were present in no time to ensure that the track was safe for use again,” Mirjam van Velthuizen looks back. “Later in the day it turned out that a beam had ended up on the overhead line at Sloterdijk. This incident was also resolved quite quickly. The traveler hardly noticed.” This Formula 1 race will be held annually in Zandvoort for the time being. ProRail will therefore continue to work on this in the coming years. “We now know for sure that we can handle this together,” says Harro Homan. “But there was a huge amount of events this weekend: Hiswa te water, Elrow Town Festival, the Ajax-Cambuur match, the Kensington concert… Hopefully next year we can persuade event organizers to skip this weekend . Then there is more room to allow train traffic in the rest of the country to run normally. In any case, we have delivered craftsmanship again. And we will do that again next year. To the Maxx!” September 2, 2022 Do you live or work within 300 meters of the railway? Then use our rail check. You can immediately see which activities are planned in your area. This field is required and only accepts numbers and letters This field is required and only accepts numbers When you visit our website you will receive cookies. No filled cakes or stroopwafels, but temporary digital files. We use functional, analytical and marketing cookies. The functional cookies are necessary for this website to work properly. So they are always on. You can give your consent below for the analytical cookies and marketing cookies. More information about our cookies can be found in our cookie policy</t>
@@ -764,13 +742,30 @@
  December 30, 2020, 11:49 • 3 minutes reading time Do you have a news tip or new information? Tip the editors via WhatsApp or via email. © 2022 RTV East</t>
   </si>
   <si>
+    <t>Data of probably all current and former Strukton Rail employees stolen In addition, the data of Eurailscout employees was also stolen. This company is half owned by Strukton. It is unclear exactly how many victims are involved in total. An investigation revealed that the data was allegedly stolen by a former employee who had access to the systems. This person would have taken pictures of it. According to the spokesperson, no data from international branches of Strukton and Eurailscout has been stolen. A Strukton spokesperson was unable to answer additional questions on Wednesday. For example, it is not known why the data of former employees was kept, and how far back this data goes. ©2022 DPG Media B.V. - all rights reserved</t>
+  </si>
+  <si>
+    <t>Eindhoven starts with the construction of the A2 underpass
+ Municipality of Eindhoven Editors March 10, 2022 - 2:54 PM March 10, 2022 - 3:00 PM The construction of the tunnel under the A2 has started. The project is part of improving the accessibility of Eindhoven Northwest. The tunnel is intended to connect the new road through the BIC North to the GDC business park. The tunnel is connected to the roundabout on Mispelhoefstraat. Construction company Strukton Civiel is carrying out the work. The renewal of the road infrastructure in Northwest also includes other projects. For example, the construction of the Tegenbosch bicycle bridge and the connection between Anthony Fokkerweg and Spottersweg were also parts of the renovation. Making Eindhoven Northwest more accessible should benefit Eindhoven Airport, FlightForum and the BIC, among others. The A2 underpass is expected to be completed by the end of 2023. The tunnel is intended to connect the new road through the BIC North to the GDC business park. The tunnel is connected to the roundabout on Mispelhoefstraat. Construction company Strukton Civiel is carrying out the work. The renewal of the road infrastructure in Northwest also includes other projects. For example, the construction of the Tegenbosch bicycle bridge and the connection between Anthony Fokkerweg and Spottersweg were also parts of the renovation. Making Eindhoven Northwest more accessible should benefit Eindhoven Airport, FlightForum and the BIC, among others. The A2 underpass is expected to be completed by the end of 2023. Share this article: Large fire at apartment complex in Eindhoven Many more parking fines issued in city due to use of scan car Students occupy boardroom TU/e ​​building Eindhoven resident threatens to set fire to apartment if arrested Neighborhood shocked by huge fire in Vaartbroek 040News: Monday 5 December 040News: Friday 2 December 040News: Thursday 1 December Studio Stadhuis - Studentenhuisvesting 040News: Wednesday 30 November Tue 6º 4º 0.0mm Wed 6º 3º 0.3mm Thu 3º 1º 0.0mm The shock is still there, in the Eindhoven district of Vaartbroek, after the great fire Sunday night in an apartment complex. Local residents came to take a look at the flat in their neighborhood on Monday. yesterday 3:23 pm The police have questioned a 17-year-old boy from Geldrop for possible involvement in arson in a nature reserve around Eindhoven. yesterday 2:46 pm Ten climate activists have occupied a boardroom in the Atlas building of Eindhoven University of Technology. Among other things, the students want the university to break its ties with the fossil fuel industry. yesterday 12:15 pm Due to the price increases in construction, the new construction of the Eindhoven swimming pool De Tongelreep is considerably more expensive than previously estimated. The city council informs the city council that money is therefore needed. yesterday 11:02 am The number of parking fines issued in Eindhoven has risen sharply. This year, around 58,000 vouchers have already been issued. That is much more than in the corona years, but also considerably more than before the pandemic. yesterday 07:31 a.m. A large fire raged in an apartment complex at the Amandelpark in Eindhoven on Sunday evening. Several apartments were ablaze, reports the fire service. 04 December 2022 - 8:52 pm Due to the price increases in construction, the new construction of the Eindhoven swimming pool De Tongelreep is considerably more expensive than previously estimated. The city council informs the city council that money is therefore needed. yesterday 11:02 am The number of parking fines issued in Eindhoven has risen sharply. This year, around 58,000 vouchers have already been issued. That is much more than in the corona years, but also considerably more than before the pandemic. yesterday 07:31 a.m. A large fire raged in an apartment complex at the Amandelpark in Eindhoven on Sunday evening. Several apartments were ablaze, reports the fire service. December 04, 2022 - 8:52 PM</t>
+  </si>
+  <si>
     <t>ProRail and Strukton Rail in talks to improve safety at Kijfhoek Login name Password Remember login ProRail and Strukton Rail are going to take measures to improve safety at the Kijfhoek shunting yard. The contractor and rail manager made this known in response to a report from the Human Environment and Transport Inspectorate, which states that the safety culture at the shunting yard is not up to standard. “We endorse the need to improve safety at the Kijfhoek shunting yard,” says ProRail spokesperson Coen van Kranenburg. The work at Kijfhoek was halted by ILT on 19 July following an accident on 15 June. Then the lorry derailed when it collided with a tank wagon. There was a flammable substance in the wagon, but there was no danger because it was not damaged. It was the fourth incident in a short time. In an investigation into the accident, the ILT says that both ProRail and Strukton Rail did not comply with safety instructions. According to the regulator, the problem is structural: deviations from the safety procedures would have occurred more often. The Inspectorate stated that there were insufficient guarantees in the field of supervision, management and evaluations to ensure that people could work safely and that the railways remained safe. This violates the Railways Act. ProRail and Strukton are therefore required by ILT to make a thorough analysis of the safety risks and take measures to guarantee safety before work can be restarted. The rail manager says that it is in talks with contractors such as Strukton Rail and with ILT about the possibilities of improving the safety culture at Kijfhoek. The Municipality of Zwijndrecht also plays an important role in this process, says Van Kranenburg. “The municipality is very critical, and rightly so. We will therefore keep the municipality closely involved in this process.” Strukton Rail also says it wants to improve safety at Kijfhoek. A spokesperson for the rail company says it finds it unacceptable that Strukton employees have not complied with safety instructions at Kijfhoek. “Deviating behavior in which we do not comply with safety instructions or agreed work processes is something we do not want and cannot accept,” says the spokesperson. “We are therefore constantly working on increasing our safety awareness. Sometimes we do that by learning from a deviation or incident.” The railway company indicates that it will use the intervention of the Inspectorate to improve the safety culture. “We have informed our employees and we are tightening up the procedures. Consultations with ProRail and ILT have also started for this.” The spokesperson cannot yet say what ProRail will actually do to improve the situation: “ILT has said: it cannot go on like this. We agree with that. Now we are conducting all kinds of studies to see what steps we can take to improve safety.” What is clear is that the mound system is outdated: “It must indeed be replaced. It is in the planning, but money must be available for this. We will discuss this with ILT.” According to the ProRail spokesperson, the consequences for freight transporters of stopping work are manageable: “We had discussions with the transporters about this on Wednesday. We have the consequences under control so far. The contractor also plays a role in this and they have also let us know that this is working well.” ProRail does not yet know when the work can be restarted. “We have not set a deadline for this. We must first have confidence that all employees can perform their work safely and that it is also safe for the environment.” The spokesman for Strukton Rail agrees: "Regular activities will only be resumed once all parties involved are convinced that the workplace is safe for all employees." Read also: Do ​​you want to read unlimited? Take out a promotional subscription now and  get unlimited access to specialist information about the rail market. start promotion subscription Are you already a subscriber? Log in Carlijn Kruidhof is an editor at SpoorPro, RailTech and RailFreight. She also writes for the other professional magazines of ProMedia Group. Maximum characters left Log in via one of the following social media partners to leave your comment. Register for free and receive the latest news directly by e-mail every week. © 2012–2022 SpoorPro.nl</t>
   </si>
   <si>
     <t>Phase One Drone Supports 3D Bridge Inspection in the Netherlands Acquiring High-resolution Aerial Data in Congested Areas and Controlled Airspace The use of a Phase One iXM-100 enabled EyeFly BV to fly closer to the Buggenum rail bridge in the Netherlands for the required annual bridge inspection. This achieved a resolution of close to 1mm ground sampling distance (GSD) and an image footprint of 12m x 9m from a flight height of 10m distance. The data has been used to create a 3D mesh of the structure.  Dutch company EyeFly BV is one of the few fully certified operators of unmanned aerial vehicles (UAVs or ‘drones’) in the Netherlands. The company has obtained all the permits regarding the commercial use of drones as well as additional certificates for flying in congested areas and controlled airspace. EyeFly is focused on performing inspections and mapping (2D and 3D models) using aircraft that have been tested by the Netherlands Aerospace Centre and registered in the aviation records. ​​ The company offers a specialist level of expertise and skills in infrastructure, construction, geoinformation and surveying. Achieving the best possible results using EyeFly’s existing certified equipment means acquiring high-resolution cameras that are ready to integrate. The Phase One Industrial iXM-100 camera easily incorporates with the company’s DJI M600 and Freefly Alta UAVs, plus it provides close-to-1mm resolution data with a large footprint at a safe enough distance from the object to meet the safety requirements.    Phase One iXM-100   Annual maintenance inspection of Buggenum bridge ​EyeFly supports Strukton Rail with the annual maintenance inspection of Buggenum rail bridge in order to identify changes in the structure from year to year. Areas of wear and damage are identified, and areas with the biggest changes are given priority for repair.​​ Previously, EyeFly faced the challenge of obtaining a resolution/GSD of close to 1mm while keeping the UAVs at a safe distance from the bridge. Lower-resolution sensors meant tens of thousands of images with smaller footprints had to be captured over a number of days. It was difficult if not impossible to generate a 3D mesh of the structure.​ Images were provided to the client using a sharing platform such as WeTransfer. There was no ability to correctly trace back every image.  Buggenum Bridge   Large footprint without reducing the level of detail​​​ Remco Kootstra, director of EyeFly, explains: “We chose the iXM-100 as it easily integrates with our DJI M600 platform in combination with the IOS IX Capture application. ​The camera is used on both our DJI M600 and Freefly Alta UAVs. The M600 is used for capturing the top and sides of the structure and the Alta enables us to perform an inspection from the underside of the bridge because of the ability to mount the IXM-100 on top.”​​ EyeFly uses the RSM 35mm lens as it has a focus of 10m to ∞ while the RSM 80mm AF lens is only 30m to ∞. The 35mm lens enables the UAV to be flown closer to the bridge and achieve a resolution of nearly 1mm with an image footprint of 12m x 9m from a flight height of 10m distance from the object. Integrated system​ ​​The system includes:​ Phase One Industrial iXM-100 medium-format camera​RSM 35mm lens​RSM 80mm AF lens​DJI M600​Freefly Alta UAV Data acquisition​ ​Since availability of GPS is limited on the underside of the bridge, the images are captured with a large overlap so that the processing software can provide orientation parameters and position data.​ The iXM-100 has enabled EyeFly to significantly reduce the number of images; 5,000 100MP images were captured in two days covering the top, side and bottom of the structure.  Additionally, it is now possible to create a 3D model of the entire project on EyeFly’s web-based platform with inspection functionality. This allows clients to perform an inspection much more efficiently, without losing detail or making any compromises.   Satisfied end users “Phase One’s 100MP camera is the best on the market and integrates very well into existing UAVs. The sensor never compromises on detail or accuracy and it always delivers. The large dynamic range means that fine details are captured, even in areas that are not well lit,” states Kootstra. “Our business has grown since we started with Phase One cameras as we are able to provide our customers with all the data that they need in one flight. The result is satisfied end users who come back time and again, as we can provide them with more details and better accuracy than we could with lower-resolution sensors,” he concludes.       Dutch company EyeFly BV is one of the few fully certified operators of unmanned aerial vehicles (UAVs or ‘drones’) in the Netherlands. The company has obtained all the permits regarding the commercial use of drones as well as additional certificates for flying in congested areas and controlled airspace. EyeFly is focused on performing inspections and mapping (2D and 3D models) using aircraft that have been tested by the Netherlands Aerospace Centre and registered in the aviation records. ​​ The company offers a specialist level of expertise and skills in infrastructure, construction, geoinformation and surveying. Achieving the best possible results using EyeFly’s existing certified equipment means acquiring high-resolution cameras that are ready to integrate. The Phase One Industrial iXM-100 camera easily incorporates with the company’s DJI M600 and Freefly Alta UAVs, plus it provides close-to-1mm resolution data with a large footprint at a safe enough distance from the object to meet the safety requirements.    Phase One iXM-100   Annual maintenance inspection of Buggenum bridge ​EyeFly supports Strukton Rail with the annual maintenance inspection of Buggenum rail bridge in order to identify changes in the structure from year to year. Areas of wear and damage are identified, and areas with the biggest changes are given priority for repair.​​ Previously, EyeFly faced the challenge of obtaining a resolution/GSD of close to 1mm while keeping the UAVs at a safe distance from the bridge. Lower-resolution sensors meant tens of thousands of images with smaller footprints had to be captured over a number of days. It was difficult if not impossible to generate a 3D mesh of the structure.​ Images were provided to the client using a sharing platform such as WeTransfer. There was no ability to correctly trace back every image.  Buggenum Bridge   Large footprint without reducing the level of detail​​​ Remco Kootstra, director of EyeFly, explains: “We chose the iXM-100 as it easily integrates with our DJI M600 platform in combination with the IOS IX Capture application. ​The camera is used on both our DJI M600 and Freefly Alta UAVs. The M600 is used for capturing the top and sides of the structure and the Alta enables us to perform an inspection from the underside of the bridge because of the ability to mount the IXM-100 on top.”​​ EyeFly uses the RSM 35mm lens as it has a focus of 10m to ∞ while the RSM 80mm AF lens is only 30m to ∞. The 35mm lens enables the UAV to be flown closer to the bridge and achieve a resolution of nearly 1mm with an image footprint of 12m x 9m from a flight height of 10m distance from the object. Integrated system​ ​​The system includes:​ Phase One Industrial iXM-100 medium-format camera​RSM 35mm lens​RSM 80mm AF lens​DJI M600​Freefly Alta UAV Data acquisition​ ​Since availability of GPS is limited on the underside of the bridge, the images are captured with a large overlap so that the processing software can provide orientation parameters and position data.​ The iXM-100 has enabled EyeFly to significantly reduce the number of images; 5,000 100MP images were captured in two days covering the top, side and bottom of the structure.  Additionally, it is now possible to create a 3D model of the entire project on EyeFly’s web-based platform with inspection functionality. This allows clients to perform an inspection much more efficiently, without losing detail or making any compromises.   Satisfied end users “Phase One’s 100MP camera is the best on the market and integrates very well into existing UAVs. The sensor never compromises on detail or accuracy and it always delivers. The large dynamic range means that fine details are captured, even in areas that are not well lit,” states Kootstra. “Our business has grown since we started with Phase One cameras as we are able to provide our customers with all the data that they need in one flight. The result is satisfied end users who come back time and again, as we can provide them with more details and better accuracy than we could with lower-resolution sensors,” he concludes.       The company offers a specialist level of expertise and skills in infrastructure, construction, geoinformation and surveying. Achieving the best possible results using EyeFly’s existing certified equipment means acquiring high-resolution cameras that are ready to integrate. The Phase One Industrial iXM-100 camera easily incorporates with the company’s DJI M600 and Freefly Alta UAVs, plus it provides close-to-1mm resolution data with a large footprint at a safe enough distance from the object to meet the safety requirements.    Phase One iXM-100   Annual maintenance inspection of Buggenum bridge ​EyeFly supports Strukton Rail with the annual maintenance inspection of Buggenum rail bridge in order to identify changes in the structure from year to year. Areas of wear and damage are identified, and areas with the biggest changes are given priority for repair.​​ Previously, EyeFly faced the challenge of obtaining a resolution/GSD of close to 1mm while keeping the UAVs at a safe distance from the bridge. Lower-resolution sensors meant tens of thousands of images with smaller footprints had to be captured over a number of days. It was difficult if not impossible to generate a 3D mesh of the structure.​ Images were provided to the client using a sharing platform such as WeTransfer. There was no ability to correctly trace back every image.  Buggenum Bridge   Large footprint without reducing the level of detail​​​ Remco Kootstra, director of EyeFly, explains: “We chose the iXM-100 as it easily integrates with our DJI M600 platform in combination with the IOS IX Capture application. ​The camera is used on both our DJI M600 and Freefly Alta UAVs. The M600 is used for capturing the top and sides of the structure and the Alta enables us to perform an inspection from the underside of the bridge because of the ability to mount the IXM-100 on top.”​​ EyeFly uses the RSM 35mm lens as it has a focus of 10m to ∞ while the RSM 80mm AF lens is only 30m to ∞. The 35mm lens enables the UAV to be flown closer to the bridge and achieve a resolution of nearly 1mm with an image footprint of 12m x 9m from a flight height of 10m distance from the object. Integrated system​ ​​The system includes:​ Phase One Industrial iXM-100 medium-format camera​RSM 35mm lens​RSM 80mm AF lens​DJI M600​Freefly Alta UAV Data acquisition​ ​Since availability of GPS is limited on the underside of the bridge, the images are captured with a large overlap so that the processing software can provide orientation parameters and position data.​ The iXM-100 has enabled EyeFly to significantly reduce the number of images; 5,000 100MP images were captured in two days covering the top, side and bottom of the structure.  Additionally, it is now possible to create a 3D model of the entire project on EyeFly’s web-based platform with inspection functionality. This allows clients to perform an inspection much more efficiently, without losing detail or making any compromises.   Satisfied end users “Phase One’s 100MP camera is the best on the market and integrates very well into existing UAVs. The sensor never compromises on detail or accuracy and it always delivers. The large dynamic range means that fine details are captured, even in areas that are not well lit,” states Kootstra. “Our business has grown since we started with Phase One cameras as we are able to provide our customers with all the data that they need in one flight. The result is satisfied end users who come back time and again, as we can provide them with more details and better accuracy than we could with lower-resolution sensors,” he concludes.         Phase One iXM-100   Annual maintenance inspection of Buggenum bridge ​EyeFly supports Strukton Rail with the annual maintenance inspection of Buggenum rail bridge in order to identify changes in the structure from year to year. Areas of wear and damage are identified, and areas with the biggest changes are given priority for repair.​​ Previously, EyeFly faced the challenge of obtaining a resolution/GSD of close to 1mm while keeping the UAVs at a safe distance from the bridge. Lower-resolution sensors meant tens of thousands of images with smaller footprints had to be captured over a number of days. It was difficult if not impossible to generate a 3D mesh of the structure.​ Images were provided to the client using a sharing platform such as WeTransfer. There was no ability to correctly trace back every image.  Buggenum Bridge   Large footprint without reducing the level of detail​​​ Remco Kootstra, director of EyeFly, explains: “We chose the iXM-100 as it easily integrates with our DJI M600 platform in combination with the IOS IX Capture application. ​The camera is used on both our DJI M600 and Freefly Alta UAVs. The M600 is used for capturing the top and sides of the structure and the Alta enables us to perform an inspection from the underside of the bridge because of the ability to mount the IXM-100 on top.”​​ EyeFly uses the RSM 35mm lens as it has a focus of 10m to ∞ while the RSM 80mm AF lens is only 30m to ∞. The 35mm lens enables the UAV to be flown closer to the bridge and achieve a resolution of nearly 1mm with an image footprint of 12m x 9m from a flight height of 10m distance from the object. Integrated system​ ​​The system includes:​ Phase One Industrial iXM-100 medium-format camera​RSM 35mm lens​RSM 80mm AF lens​DJI M600​Freefly Alta UAV Data acquisition​ ​Since availability of GPS is limited on the underside of the bridge, the images are captured with a large overlap so that the processing software can provide orientation parameters and position data.​ The iXM-100 has enabled EyeFly to significantly reduce the number of images; 5,000 100MP images were captured in two days covering the top, side and bottom of the structure.  Additionally, it is now possible to create a 3D model of the entire project on EyeFly’s web-based platform with inspection functionality. This allows clients to perform an inspection much more efficiently, without losing detail or making any compromises.   Satisfied end users “Phase One’s 100MP camera is the best on the market and integrates very well into existing UAVs. The sensor never compromises on detail or accuracy and it always delivers. The large dynamic range means that fine details are captured, even in areas that are not well lit,” states Kootstra. “Our business has grown since we started with Phase One cameras as we are able to provide our customers with all the data that they need in one flight. The result is satisfied end users who come back time and again, as we can provide them with more details and better accuracy than we could with lower-resolution sensors,” he concludes.       Phase One iXM-100   Annual maintenance inspection of Buggenum bridge ​EyeFly supports Strukton Rail with the annual maintenance inspection of Buggenum rail bridge in order to identify changes in the structure from year to year. Areas of wear and damage are identified, and areas with the biggest changes are given priority for repair.​​ Previously, EyeFly faced the challenge of obtaining a resolution/GSD of close to 1mm while keeping the UAVs at a safe distance from the bridge. Lower-resolution sensors meant tens of thousands of images with smaller footprints had to be captured over a number of days. It was difficult if not impossible to generate a 3D mesh of the structure.​ Images were provided to the client using a sharing platform such as WeTransfer. There was no ability to correctly trace back every image.  Buggenum Bridge   Large footprint without reducing the level of detail​​​ Remco Kootstra, director of EyeFly, explains: “We chose the iXM-100 as it easily integrates with our DJI M600 platform in combination with the IOS IX Capture application. ​The camera is used on both our DJI M600 and Freefly Alta UAVs. The M600 is used for capturing the top and sides of the structure and the Alta enables us to perform an inspection from the underside of the bridge because of the ability to mount the IXM-100 on top.”​​ EyeFly uses the RSM 35mm lens as it has a focus of 10m to ∞ while the RSM 80mm AF lens is only 30m to ∞. The 35mm lens enables the UAV to be flown closer to the bridge and achieve a resolution of nearly 1mm with an image footprint of 12m x 9m from a flight height of 10m distance from the object. Integrated system​ ​​The system includes:​ Phase One Industrial iXM-100 medium-format camera​RSM 35mm lens​RSM 80mm AF lens​DJI M600​Freefly Alta UAV Data acquisition​ ​Since availability of GPS is limited on the underside of the bridge, the images are captured with a large overlap so that the processing software can provide orientation parameters and position data.​ The iXM-100 has enabled EyeFly to significantly reduce the number of images; 5,000 100MP images were captured in two days covering the top, side and bottom of the structure.  Additionally, it is now possible to create a 3D model of the entire project on EyeFly’s web-based platform with inspection functionality. This allows clients to perform an inspection much more efficiently, without losing detail or making any compromises.   Satisfied end users “Phase One’s 100MP camera is the best on the market and integrates very well into existing UAVs. The sensor never compromises on detail or accuracy and it always delivers. The large dynamic range means that fine details are captured, even in areas that are not well lit,” states Kootstra. “Our business has grown since we started with Phase One cameras as we are able to provide our customers with all the data that they need in one flight. The result is satisfied end users who come back time and again, as we can provide them with more details and better accuracy than we could with lower-resolution sensors,” he concludes.       ​EyeFly supports Strukton Rail with the annual maintenance inspection of Buggenum rail bridge in order to identify changes in the structure from year to year. Areas of wear and damage are identified, and areas with the biggest changes are given priority for repair.​​ Previously, EyeFly faced the challenge of obtaining a resolution/GSD of close to 1mm while keeping the UAVs at a safe distance from the bridge. Lower-resolution sensors meant tens of thousands of images with smaller footprints had to be captured over a number of days. It was difficult if not impossible to generate a 3D mesh of the structure.​ Images were provided to the client using a sharing platform such as WeTransfer. There was no ability to correctly trace back every image.  Buggenum Bridge   Large footprint without reducing the level of detail​​​ Remco Kootstra, director of EyeFly, explains: “We chose the iXM-100 as it easily integrates with our DJI M600 platform in combination with the IOS IX Capture application. ​The camera is used on both our DJI M600 and Freefly Alta UAVs. The M600 is used for capturing the top and sides of the structure and the Alta enables us to perform an inspection from the underside of the bridge because of the ability to mount the IXM-100 on top.”​​ EyeFly uses the RSM 35mm lens as it has a focus of 10m to ∞ while the RSM 80mm AF lens is only 30m to ∞. The 35mm lens enables the UAV to be flown closer to the bridge and achieve a resolution of nearly 1mm with an image footprint of 12m x 9m from a flight height of 10m distance from the object. Integrated system​ ​​The system includes:​ Phase One Industrial iXM-100 medium-format camera​RSM 35mm lens​RSM 80mm AF lens​DJI M600​Freefly Alta UAV Data acquisition​ ​Since availability of GPS is limited on the underside of the bridge, the images are captured with a large overlap so that the processing software can provide orientation parameters and position data.​ The iXM-100 has enabled EyeFly to significantly reduce the number of images; 5,000 100MP images were captured in two days covering the top, side and bottom of the structure.  Additionally, it is now possible to create a 3D model of the entire project on EyeFly’s web-based platform with inspection functionality. This allows clients to perform an inspection much more efficiently, without losing detail or making any compromises.   Satisfied end users “Phase One’s 100MP camera is the best on the market and integrates very well into existing UAVs. The sensor never compromises on detail or accuracy and it always delivers. The large dynamic range means that fine details are captured, even in areas that are not well lit,” states Kootstra. “Our business has grown since we started with Phase One cameras as we are able to provide our customers with all the data that they need in one flight. The result is satisfied end users who come back time and again, as we can provide them with more details and better accuracy than we could with lower-resolution sensors,” he concludes.       Previously, EyeFly faced the challenge of obtaining a resolution/GSD of close to 1mm while keeping the UAVs at a safe distance from the bridge. Lower-resolution sensors meant tens of thousands of images with smaller footprints had to be captured over a number of days. It was difficult if not impossible to generate a 3D mesh of the structure.​ Images were provided to the client using a sharing platform such as WeTransfer. There was no ability to correctly trace back every image.  Buggenum Bridge   Large footprint without reducing the level of detail​​​ Remco Kootstra, director of EyeFly, explains: “We chose the iXM-100 as it easily integrates with our DJI M600 platform in combination with the IOS IX Capture application. ​The camera is used on both our DJI M600 and Freefly Alta UAVs. The M600 is used for capturing the top and sides of the structure and the Alta enables us to perform an inspection from the underside of the bridge because of the ability to mount the IXM-100 on top.”​​ EyeFly uses the RSM 35mm lens as it has a focus of 10m to ∞ while the RSM 80mm AF lens is only 30m to ∞. The 35mm lens enables the UAV to be flown closer to the bridge and achieve a resolution of nearly 1mm with an image footprint of 12m x 9m from a flight height of 10m distance from the object. Integrated system​ ​​The system includes:​ Phase One Industrial iXM-100 medium-format camera​RSM 35mm lens​RSM 80mm AF lens​DJI M600​Freefly Alta UAV Data acquisition​ ​Since availability of GPS is limited on the underside of the bridge, the images are captured with a large overlap so that the processing software can provide orientation parameters and position data.​ The iXM-100 has enabled EyeFly to significantly reduce the number of images; 5,000 100MP images were captured in two days covering the top, side and bottom of the structure.  Additionally, it is now possible to create a 3D model of the entire project on EyeFly’s web-based platform with inspection functionality. This allows clients to perform an inspection much more efficiently, without losing detail or making any compromises.   Satisfied end users “Phase One’s 100MP camera is the best on the market and integrates very well into existing UAVs. The sensor never compromises on detail or accuracy and it always delivers. The large dynamic range means that fine details are captured, even in areas that are not well lit,” states Kootstra. “Our business has grown since we started with Phase One cameras as we are able to provide our customers with all the data that they need in one flight. The result is satisfied end users who come back time and again, as we can provide them with more details and better accuracy than we could with lower-resolution sensors,” he concludes.       Buggenum Bridge   Large footprint without reducing the level of detail​​​ Remco Kootstra, director of EyeFly, explains: “We chose the iXM-100 as it easily integrates with our DJI M600 platform in combination with the IOS IX Capture application. ​The camera is used on both our DJI M600 and Freefly Alta UAVs. The M600 is used for capturing the top and sides of the structure and the Alta enables us to perform an inspection from the underside of the bridge because of the ability to mount the IXM-100 on top.”​​ EyeFly uses the RSM 35mm lens as it has a focus of 10m to ∞ while the RSM 80mm AF lens is only 30m to ∞. The 35mm lens enables the UAV to be flown closer to the bridge and achieve a resolution of nearly 1mm with an image footprint of 12m x 9m from a flight height of 10m distance from the object. Integrated system​ ​​The system includes:​ Phase One Industrial iXM-100 medium-format camera​RSM 35mm lens​RSM 80mm AF lens​DJI M600​Freefly Alta UAV Data acquisition​ ​Since availability of GPS is limited on the underside of the bridge, the images are captured with a large overlap so that the processing software can provide orientation parameters and position data.​ The iXM-100 has enabled EyeFly to significantly reduce the number of images; 5,000 100MP images were captured in two days covering the top, side and bottom of the structure.  Additionally, it is now possible to create a 3D model of the entire project on EyeFly’s web-based platform with inspection functionality. This allows clients to perform an inspection much more efficiently, without losing detail or making any compromises.   Satisfied end users “Phase One’s 100MP camera is the best on the market and integrates very well into existing UAVs. The sensor never compromises on detail or accuracy and it always delivers. The large dynamic range means that fine details are captured, even in areas that are not well lit,” states Kootstra. “Our business has grown since we started with Phase One cameras as we are able to provide our customers with all the data that they need in one flight. The result is satisfied end users who come back time and again, as we can provide them with more details and better accuracy than we could with lower-resolution sensors,” he concludes.         Large footprint without reducing the level of detail​​​ Remco Kootstra, director of EyeFly, explains: “We chose the iXM-100 as it easily integrates with our DJI M600 platform in combination with the IOS IX Capture application. ​The camera is used on both our DJI M600 and Freefly Alta UAVs. The M600 is used for capturing the top and sides of the structure and the Alta enables us to perform an inspection from the underside of the bridge because of the ability to mount the IXM-100 on top.”​​ EyeFly uses the RSM 35mm lens as it has a focus of 10m to ∞ while the RSM 80mm AF lens is only 30m to ∞. The 35mm lens enables the UAV to be flown closer to the bridge and achieve a resolution of nearly 1mm with an image footprint of 12m x 9m from a flight height of 10m distance from the object. Integrated system​ ​​The system includes:​ Phase One Industrial iXM-100 medium-format camera​RSM 35mm lens​RSM 80mm AF lens​DJI M600​Freefly Alta UAV Data acquisition​ ​Since availability of GPS is limited on the underside of the bridge, the images are captured with a large overlap so that the processing software can provide orientation parameters and position data.​ The iXM-100 has enabled EyeFly to significantly reduce the number of images; 5,000 100MP images were captured in two days covering the top, side and bottom of the structure.  Additionally, it is now possible to create a 3D model of the entire project on EyeFly’s web-based platform with inspection functionality. This allows clients to perform an inspection much more efficiently, without losing detail or making any compromises.   Satisfied end users “Phase One’s 100MP camera is the best on the market and integrates very well into existing UAVs. The sensor never compromises on detail or accuracy and it always delivers. The large dynamic range means that fine details are captured, even in areas that are not well lit,” states Kootstra. “Our business has grown since we started with Phase One cameras as we are able to provide our customers with all the data that they need in one flight. The result is satisfied end users who come back time and again, as we can provide them with more details and better accuracy than we could with lower-resolution sensors,” he concludes.       Remco Kootstra, director of EyeFly, explains: “We chose the iXM-100 as it easily integrates with our DJI M600 platform in combination with the IOS IX Capture application. ​The camera is used on both our DJI M600 and Freefly Alta UAVs. The M600 is used for capturing the top and sides of the structure and the Alta enables us to perform an inspection from the underside of the bridge because of the ability to mount the IXM-100 on top.”​​ EyeFly uses the RSM 35mm lens as it has a focus of 10m to ∞ while the RSM 80mm AF lens is only 30m to ∞. The 35mm lens enables the UAV to be flown closer to the bridge and achieve a resolution of nearly 1mm with an image footprint of 12m x 9m from a flight height of 10m distance from the object. Integrated system​ ​​The system includes:​ Phase One Industrial iXM-100 medium-format camera​RSM 35mm lens​RSM 80mm AF lens​DJI M600​Freefly Alta UAV Data acquisition​ ​Since availability of GPS is limited on the underside of the bridge, the images are captured with a large overlap so that the processing software can provide orientation parameters and position data.​ The iXM-100 has enabled EyeFly to significantly reduce the number of images; 5,000 100MP images were captured in two days covering the top, side and bottom of the structure.  Additionally, it is now possible to create a 3D model of the entire project on EyeFly’s web-based platform with inspection functionality. This allows clients to perform an inspection much more efficiently, without losing detail or making any compromises.   Satisfied end users “Phase One’s 100MP camera is the best on the market and integrates very well into existing UAVs. The sensor never compromises on detail or accuracy and it always delivers. The large dynamic range means that fine details are captured, even in areas that are not well lit,” states Kootstra. “Our business has grown since we started with Phase One cameras as we are able to provide our customers with all the data that they need in one flight. The result is satisfied end users who come back time and again, as we can provide them with more details and better accuracy than we could with lower-resolution sensors,” he concludes.       EyeFly uses the RSM 35mm lens as it has a focus of 10m to ∞ while the RSM 80mm AF lens is only 30m to ∞. The 35mm lens enables the UAV to be flown closer to the bridge and achieve a resolution of nearly 1mm with an image footprint of 12m x 9m from a flight height of 10m distance from the object. Integrated system​ ​​The system includes:​ Phase One Industrial iXM-100 medium-format camera​RSM 35mm lens​RSM 80mm AF lens​DJI M600​Freefly Alta UAV Data acquisition​ ​Since availability of GPS is limited on the underside of the bridge, the images are captured with a large overlap so that the processing software can provide orientation parameters and position data.​ The iXM-100 has enabled EyeFly to significantly reduce the number of images; 5,000 100MP images were captured in two days covering the top, side and bottom of the structure.  Additionally, it is now possible to create a 3D model of the entire project on EyeFly’s web-based platform with inspection functionality. This allows clients to perform an inspection much more efficiently, without losing detail or making any compromises.   Satisfied end users “Phase One’s 100MP camera is the best on the market and integrates very well into existing UAVs. The sensor never compromises on detail or accuracy and it always delivers. The large dynamic range means that fine details are captured, even in areas that are not well lit,” states Kootstra. “Our business has grown since we started with Phase One cameras as we are able to provide our customers with all the data that they need in one flight. The result is satisfied end users who come back time and again, as we can provide them with more details and better accuracy than we could with lower-resolution sensors,” he concludes.       ​​The system includes:​ Phase One Ind</t>
   </si>
   <si>
-    <t>Strukton secures ATB Vv train protection system installation contract from Prorail Strukton Systems has secured a contract from infrastructure manager Prorail to install the ATB Vv train protection system on the Brabant Route from Rotterdam to Venlo and the A2 corridor from Alkmaar to Maastricht in the Netherlands. By Srivani Venna Strukton Systems has secured a contract from infrastructure manager ProRail to install the ATB Vv train protection system on the Brabant Route from Rotterdam to Venlo and the A2 corridor from Alkmaar to Maastricht in the Netherlands. The ATB Vv train protection system automatically stops trains reaching a red signal at speeds higher than 40 km/hour and increases the safety level. It also stops trains approaching a red signal at speeds lower than 40 km/hour. Funding for the launch will be provided by the Dutch Ministry of Infrastructure and the Environment. The existing traditional ATB system is expected to be replaced with the European Rail Traffic Management System (ERTMS). The Brabant route will be installed with ATB Vv as freight trains will frequently be redirected over this route during the construction of a third track between Emmerich and Oberhausen in Germany. Data Feeds + 0 More ProRail and Dutch Railways are planning to start a programme enabling high-frequency rail transport with one train every ten minutes between Eindhoven and Amsterdam in 2018. Image: Patrick Buck and Lex van Seventer signing the contract. Photo: courtesy of Strukton. Automated Non-Destructive Testing and Measurement Systems for Rails, Rail Wheels and Axles Rail Passenger Information Displays Railway Wheel Sets, Freight Wagons and Passenger Coaches Thank you for subscribing to Railway Technology</t>
+    <t>Collection point for fireworks mainly harvests innocent stars
+ Firecrackers float in water Studio040 / Pleun Wolters December 29, 2020 - 2:18 PM December 29, 2020 - 6:41 PM The collection point for illegal fireworks that have landed at the De Hondsheuvels sports complex until Tuesday, mainly harvests feathery firecrackers and innocent stars. "Bring it back with you for the grandchildren, madam," says Mark Drenth of the collection point for fireworks to a lady who has just handed in a plastic bag. He hands her two packets of stars with a smile. She takes them back in surprise and gets into the car, with her three smiling fellow passengers. "Indeed. They will still come on," she says. To put it mildly, it's not a storm at the collection point for fireworks. The long driveway leading to the location remains almost completely empty. Only a few hundred grams have been handed in, especially the lighter classes of fireworks. Strings or other illegal stuff is hardly among them. Market Drenth, fireworks collection point Nevertheless, Strukton's Incident Management Team, which has been hired by the municipality of Eindhoven for this task, is fully present. Among other things to ensure correct processing. "Once we have taken the fireworks, they go into a container with water. It must lie there for seven days before it can be sent on to the party that receives the fireworks afterwards. Those are the rules," says employee Daan Claereboets. Is it naive to assume that people will personally hand in their illegal fireworks? "I won't comment on that," says Mark Drenth. "But it is important that such a point exists. Even if only for the principle." Share this article: Large fire at apartment complex in Eindhoven Many more parking fines issued in city due to use of scan car Students occupy boardroom TU/e ​​building Eindhoven resident threatens to set fire to apartment if arrested Neighborhood shocked by huge fire in Vaartbroek 040News: Monday 5 December 040News: Friday 2 December 040News: Thursday 1 December Studio Stadhuis - Studentenhuisvesting 040News: Wednesday 30 November Tue 6º 4º 0.0mm Wed 6º 3º 0.3mm Thu 3º 1º 0.0mm The shock is still there, in the Eindhoven district of Vaartbroek, after the great fire Sunday night in an apartment complex. Local residents came to take a look at the flat in their neighborhood on Monday. yesterday 3:23 pm The police have questioned a 17-year-old boy from Geldrop for possible involvement in arson in a nature reserve around Eindhoven. yesterday 2:46 pm Ten climate activists have occupied a boardroom in the Atlas building of Eindhoven University of Technology. Among other things, the students want the university to break its ties with the fossil fuel industry. yesterday 12:15 pm Due to the price increases in construction, the new construction of the Eindhoven swimming pool De Tongelreep is considerably more expensive than previously estimated. The city council informs the city council that money is therefore needed. yesterday 11:02 am The number of parking fines issued in Eindhoven has risen sharply. This year, around 58,000 vouchers have already been issued. That is much more than in the corona years, but also considerably more than before the pandemic. yesterday 07:31 a.m. A large fire raged in an apartment complex at the Amandelpark in Eindhoven on Sunday evening. Several apartments were ablaze, reports the fire service. 04 December 2022 - 8:52 pm Due to the price increases in construction, the new construction of the Eindhoven swimming pool De Tongelreep is considerably more expensive than previously estimated. The city council informs the city council that money is therefore needed. yesterday 11:02 am The number of parking fines issued in Eindhoven has risen sharply. This year, around 58,000 vouchers have already been issued. That is much more than in the corona years, but also considerably more than before the pandemic. yesterday 07:31 a.m. A large fire raged in an apartment complex at the Amandelpark in Eindhoven on Sunday evening. Several apartments were ablaze, reports the fire service. December 04, 2022 - 8:52 PM</t>
+  </si>
+  <si>
+    <t>GVB awards Strukton the renewal of the metro railway bridge in Amsterdam Login name Password Remember login In July of this year, Strukton Rail will renew the Amstelveenseweg crossing complex and the rail constructions on the metro railway bridge over the Schinkel in Amsterdam. Client GVB awarded the project to the rail contractor “on the basis of the best price-quality ratio”. The movable metro railway bridge is located next to two railway bridges between the carriageways of the A10 motorway. In total there are five bridges next to each other. There are movable bridge valves in all bridges, so that they can be opened for shipping. The metro railway bridge is one of the few only movable bridges in the Netherlands that is part of a metro line. There are also two movable railway bridges on the Hoekse Lijn metro connection between Hoek van Holland and the center of Rotterdam. According to Strukton Rail, the metro railway bridge is comparable to ProRail bridges, because they are “complex in their combination of construction, control and protection”. During the track renovation, employees of Baan, Kabel, Seinwezen, point heating and works of art from the railway contractor work together. After the work, the Schinkel Bridge must be rebalanced. In addition to the technical challenges presented by the project, Strukton reports that there are also logistics issues that need to be resolved. The work site is located between the two directions of the A10 and next to two other railway bridges. A temporary construction site is created for the supply and removal of materials and equipment. This site is accessible via a temporary exit lane on the left side of the carriageway and can only be used at night. “During the preparation, all logistics matters must be in view, so that all necessary materials and equipment are present during the day to be able to carry out the work,” the rail company reports. Strukton drew up an action plan in collaboration with MW Project Management and Advice, which extensively discussed planning, organization and logistics. Do you want unlimited reading? Take out a promotional subscription now and  get unlimited access to specialist information about the rail market. start promotion subscription Are you already a subscriber? Login Marieke van Gompel is a journalist for SpoorPro and general editor-in-chief of ProMedia Group. Maximum characters left Log in via one of the following social media partners to leave your comment. Register for free and receive the latest news directly by e-mail every week. © 2012–2022 SpoorPro.nl</t>
+  </si>
+  <si>
+    <t>Reorganization at Strukton Rail A spokeswoman confirmed this on Saturday. The company is also cutting jobs. "We are not yet making any statements about the number of jobs," said the spokeswoman. In a few weeks there will be more clarity about the reorganization and the number of jobs to be lost. The company says it has already agreed on a social plan with the unions. The rail sector is currently struggling with uncertainty about the expenditure that Prorail has reserved for major maintenance and new rail projects. Various rail companies run into problems due to the lack of orders. Trade union FNV Spoor does not know how many jobs are at risk, but takes into account a loss of "at least a few dozen jobs". Two hundred jobs have already disappeared at Strukton in recent years. Strukton has approximately seven thousand employees. Half of these work for the Strukton Rail division. ©2022 DPG Media B.V. - all rights reserved</t>
+  </si>
+  <si>
+    <t>Strukton and Centric have confidence in the expertise of Rian van Rijbroek Strukton and Centric have complete confidence in the expertise of (self-appointed) cyber expert Rian van Rijbroek, the Strukton website reports. The statement comes after various reports about a lawsuit between Centric and Strukton boss Gerard Sanderink and his former (business) partner Brigitte van Egten. Rian van Rijbroek now has an influential role within the business empire of Centric and Oranjewoud owner Gerard Sanderink. Strukton reports on its website: "Reports appeared in the media this week in response to summary proceedings brought by Brigitte van Egten against Gerard Sanderink. These reports state that Rian van Rijbroek plays a role in this. This is not the case. It concerns a dispute between Brigitte van Egten and Gerard Sanderink. It is also stated in the media that Rian van Rijbroek would play a role in the departure of two top managers within Gerard Sanderink's companies. Gerard Sanderink is working on the organization within Centric Inherent to this is that changes are taking place in the management. The management teams of both Strukton and Centric have full confidence in the expertise of Rian van Rijbroek. They deeply regret that the name of Rian van Rijbroek has been mentioned in a negative sense in the media with regard to the procedure referred to above.New foundationAs can be read in the media coverage, Gerard S Anderink established a new foundation, the Technology &amp; Cybersecurity Gerard Sanderink Foundation. This foundation was established with a view to the continuity of its businesses and to stimulate young talented students from Twente by providing scholarships. In addition, the foundation focuses on both high-quality technology and cyber security. The importance of cyber security appears to be increasing, as also described by Rian van Rijbroek in the book “Unhacked” with afterword by prof. dr. Ben van Lier CMC. More and more is happening in the world in the digital field, both at work and privately. On the one hand, this makes life easier. On the other hand, there are risks involved. Due to the speed of technological developments, our digital front door is increasingly wide open. And that offers opportunities for cybercrime. Together with the Foundation Technology &amp; Cybersecurity Gerard Sanderink, we will make every effort to prevent cybercrime as much as possible or to combat cybercrime as much as possible." Update: The NOS reports that Rian van Rijbroek has never worked for the AIVD.     06-12-2022 06- 12-2022 06-12-2022 06-12-2022 06-12-2022 06-12-2022 06-12-2022 06-12-2022 06-12-2022 06-12-2022</t>
   </si>
   <si>
     <t>Strukton Rail takes an interest in A1 Elektronics Login name Password Remember login Strukton Rail has acquired a fifty percent interest in A1 Elektronics in Almelo. The other fifty percent is in the hands of the current management. Strukton Rail has announced this. A1 Electronics is making a new start from this new ownership structure under the leadership of the current director Rudy Oude Vrielink. A1 Electronics was part of the V4 Group. Due to external circumstances within the V4 Group, the company was declared bankrupt on July 25, 2012. A1 Electronics BV has healthy business operations and has always been profitable. The prospect is therefore that 2012 will be closed profitably. “The components of A1 Electronics are of strategic importance to Strukton Rail,” says Aike Schoots, CEO of Strukton Rail. “We use the printed circuit boards and the electrical and electronic components in train systems. This purchase guarantees the quality of this.” Strukton Rail develops, builds, installs and maintains rail systems with the aim of making rail optimally available, reliable, safe and measurable. Strukton Rail is active in five European countries. It employs 3,200 employees. A1 Electronics is engaged in the assembly of electronic printed circuit boards and complete products and, as a separate discipline, repair for third parties. The company works for customers who mainly operate in the industrial, medical and transport sectors, traffic systems, message boards and communication technology. A1 Electronics has 22 employees. Do you want unlimited reading? Take out a promotional subscription now and  get unlimited access to specialist information about the rail market. start promotion subscription Are you already a subscriber? Login Marieke van Gompel is a journalist for SpoorPro and general editor-in-chief of ProMedia Group. Maximum characters left Log in via one of the following social media partners to leave your comment. Register for free and receive the latest news directly by e-mail every week. © 2012–2022 SpoorPro.nl</t>
@@ -788,41 +783,39 @@
     <t>Rail manager ProRail concludes four ten-year PGO contracts Login name Password Remember login Rail contractors Asset Rail, Strukton Rail, BAM Rail and VolkerRail and rail manager ProRail have signed contracts for four maintenance areas using the performance-based maintenance (PGO) method. The agreement is intended to give further substance to the covenant that was concluded with the contractors in 2013. The contracts now have a term of ten years, where previously it was five years. This is to stimulate long-term investments. Maintenance based on the new contracts will start in the 'Gelre2' contract areas with Asset Rail, Strukton Rail in the 'Wadden' contract area, The Hague contract area with BAM Rail and the Twente contract area with VolkerRail. The new contracts differ from the previous PGO contracts and are mainly aimed at prevention and quality improvement, according to BAM Rail. Stricter rules for, among other things, fault recovery, the number of faults and safety values ​​have been included. “On the other hand, the contracts stimulate a quality circle of continuous learning and improvement.” According to the rail contractor, this should ultimately result in a continuous improvement process resulting in a more robust track. An important change in the current contracts compared to the previous agreements is that they now have a term of ten years. Previously this was five years. The idea behind the expansion is that it should stimulate contractors and make it possible to make more investments for the long term. In training of personnel and infrastructure, for example. The contract form will be further developed in the coming period, it is stated. ProRail checks the quality of the track during the term of the contracts. Since 2008, rail management has been working with contracts based on performance-based maintenance. This arose from the wish of the Nma and the European Commission to put rail maintenance out to public tender, as was already common practice in other construction sectors. Maintenance in eleven contract areas is now carried out via the PGO method (public tender). In the remaining areas, the classic OPC method (no competition) is currently still used. Those areas will be put out to tender until 2018. Do you want unlimited reading? Take out a promotional subscription now and  get unlimited access to specialist information about the rail market. start promotion subscription Are you already a subscriber? Log in Maximum characters left Log in via one of the following social media partners to leave your comment. Register for free and receive the latest news directly by e-mail every week. © 2012–2022 SpoorPro.nl</t>
   </si>
   <si>
+    <t>GEFCO builds lightweight in-vehicle equipment for Strukton v/d Nat Wessels Logistics B.V. Almelo Wessels Logistics B.V. Almelo Wessels Logistics B.V. Almelo J.J. Ardon Transport J.J. Ardon Transport Send your photos to our editors and we will post them for you. To the photo album Send your photos to our editors and we will post them for you. Current fuel prices Euro951,942 Diesel1,916 Supplied by UnitedConsumers More fuel prices Supplied by UnitedConsumers More fuel prices Mercedes-Benz Trucks puts drivers in the spotlight on Truck Driver's Day 06-12-2022 | Company news LEUSDEN - On Thursday 8 December it is Truck Driver's Day again. On this day Mer</t>
+  </si>
+  <si>
     <t>Low-dust work train used for railway works in Gouda Login name Password Remember login Rail contractor Strukton Rail is renewing nineteen points and two kilometers of track at Gouda on behalf of ProRail until Tuesday 14 August. Due to the dusty conditions that the warm weather entails, the special low-dust unloading train (SALT) from rail supplier Voestalpine Railpro is being used for this. During the unloading of ballast, dust is created that is harmful to railway workers and local residents. The SALT has been developed to enable rail workers to work healthily. The installation on the train precipitates the dust with water spray. Wagon owner Voestalpine Railpro and ProRail have developed the special work train together with sector parties. Around Gouda, 75 percent of the rail network will be renewed to ensure that the routes from Utrecht via Gouda to Rotterdam and The Hague remain safe and easily accessible for passenger and freight transport. The extensive sub-projects are spread over periods in order to cause as little inconvenience as possible to travelers and goods transport. At the same time, some other work is being carried out, such as the removal of platform covers at Rotterdam-Alexander station. Do you want unlimited reading? Take out a promotional subscription now and  get unlimited access to specialist information about the rail market. start promotion subscription Are you already a subscriber? Login Marieke van Gompel is a journalist for SpoorPro and general editor-in-chief of ProMedia Group. Maximum characters left Log in via one of the following social media partners to leave your comment. Register for free and receive the latest news directly by e-mail every week. © 2012–2022 SpoorPro.nl</t>
   </si>
   <si>
     <t>ILT: ProRail did not learn enough from train collisions Login name Password Remember login A near-collision at Utrecht central station last year was the result of ProRail not learning enough from previous serious incidents such as the train collision at Amsterdam Westerpark. This is the conclusion of the Human Environment and Transport Inspectorate in an investigation into the near-collision. According to the ILT, the train driver's error in judgment when passing a red signal, together with an error in the planning, could have had major consequences. Also, too few measures have been taken to reduce the risk of an STS passage (stop signal passage). On 25 April, an NS sprinter almost collided with a Strukton Rail freight train coming from the opposite direction. The slow train was on its way to Breukelen, the freight train ran from Maarssen via Utrecht Central Station to Roosendaal. The driver of the sprinter passed a red signal, but applied emergency braking when he saw the freight train approaching. Because he intervened, the trains did not collide. No one was injured in the incident. However, the infrastructure was damaged and train traffic was delayed. The Inspectorate states that ProRail's traffic control did not report the incident correctly. The railway manager reported that it was an STS passage without risk of collision, while in reality there was a near-collision. According to ILT, the near-collision in Utrecht corresponds to previous serious incidents such as the train collisions at Amsterdam Westerpark in 2012, in Barendrecht in 2009 and at Amsterdam Central Station in 2004. For example, the train collision in Amsterdam also involved a timetable that did not comply with the planning standards and then went unnoticed by ProRail. Several people were injured in the train collisions in Amsterdam Westerpark and Barendrecht. One person was also killed in both cases. Several people were injured at Amsterdam CS. ILT states that ProRail in particular has not learned enough from these incidents, especially those in 2009 and 2004. Shortly after the incident in Utrecht, ProRail took measures to prevent a recurrence. Driving on a single track by the local train on the Breukelen-Utrecht CS route has been removed from the timetable. This allowed trains from opposite directions to approach each other on the same track. The passed signal is also equipped with Automatic Train Influencing, Improved version (ATB Vv), so that safety now depends less on the actions and observations of a train driver. The ATB-EG automatic protection system did not intervene because the slow train was traveling at approximately 40 kilometers per hour when it passed the signal. ATB-EG only intervenes at speeds higher than 40 kilometers per hour. The now installed ATB Vv also intervenes at speeds below 40 kilometers per hour. The near-train collision in Utrecht is included in the stricter supervision that the Inspectorate has instituted in response to the Amsterdam Westerpark train collision. Marieke van Gompel Unlimited reading? Take advantage of the exclusive annual offer: € 7.50 instead of € 10.50. View the offer Are you already a subscriber? Log in Maximum characters left Log in via one of the following social media partners to leave your comment. The best-read public transport news in your mailbox every Tuesday. Register for free and receive the latest news directly by e-mail every week. © 2011–2022 OVPro.nl</t>
   </si>
   <si>
-    <t>German train lays new sleepers on line 139 © Erik Roosens © Erik Roosens © Erik Roosens © Erik Roosens Railway manager Infrabel will carry out works on railway line 139 between Heverlee and Sint-Joris-Weert this weekend and next weekend. The P-machine - a giant train - removes the old sleepers and replaces them with new ones. Train traffic will come to a complete standstill during the works. The rail sleepers will be replaced between Ophemstraat and Reigerstraat on the track in the direction of Wavre. For this work, main contractor Strukton Rail had the Strabag renewal train come from Germany to Oud-Heverlee. It removes the old sleepers (biblock) from 1992 from under the tracks and replaces them with sleepers in one piece (monoblock). It concerns a 1600-metre stretch from level crossing 7 (Ophemstraat) to level crossing 8 (Reigerstraat). You can see how that works in this video. At the same time, Infrabel is carrying out other works. Stumbling mats were placed at the level crossing of the Naamsesteenweg in Heverlee to prevent track running and new rails will be installed at the level crossing of the Beekstraat in Sint-Joris-Weert. Due to the works, the level crossings on Ophemstraat and Reigerstraat will be closed until 7 a.m. Monday morning. The level crossing on Reigerstraat will close again from Saturday 12 October (5 a.m.) to Monday 14 October (7 a.m.). The level crossing at Beekstraat from Saturday 12 October (5 a.m.) to Sunday 13 October (4 p.m.). Do you want access to all articles of Het Nieuwsblad? Dive into our plus articles and read 3 of them for free every month. It happened. The women of OH Leuven can still lose. In the quarterfinals of the Belgian Cup, Standard turned out to be 2-0 too strong on Tuesday. To complete the disaster evening, the … The boys of the regional U21 football team OHL became champions in their series last weekend. Below you will find an overview of all goalscorers of this weekend in Flemish Brabant football. Haasrode Leuven continues to string together victories. The stiff Borgworm also turned out not to be able to cope with the sometimes spry attacking game of the team from Leuven on Sunday evening. Thanks to the 0-3 win... The women of Haasrode Leuven continue to look for their first league win of the season. Despite the win in the first set, they couldn't get off to a good start when visiting Antwerp Ladies... La Louvière broke off the Leuven series of fifteen to fifteen. But the U23 of OHL do not give up. “We have to face it again on Saturday evening against Olympic Charleroi to … Almost no matches on Sunday in amateur football. Due to the Red Devils' World Cup match, all matches will be played on Saturday, or they will be moved to the weekend of 7 and 8… Today, they are all world stars and can hardly walk the streets anonymously anymore. But of course our Red Devils also started playing football as a little boy at their … The World Cup fever is now also starting to rise in our region. On Wednesday, our Red Devils will play their first match at the Football World Cup. Of course, various catering establishments will … No first competition victory for the women of Haasrode Leuven. Erine Brems and co lost for their own people. Saturday with 2-3 against Tchalou, but that also meant that they finally had a first … Deaths in Oud-Heverlee. No new deaths have been recently added. Is your loved one not listed on inmemoriam.be or are you looking for additional information? View all jobs</t>
-  </si>
-  <si>
-    <t>Chemie-Pack begins remediation of polluted soil The chemical company was destroyed by a huge fire more than three years ago. Contractor Strukton is demolishing the floors, foundations and sewers. The contaminated soil is then excavated. The site should be usable again in 2016. Remediation of the deeper subsoil will take much longer, possibly another ten years. The province of North Brabant is leading the soil remediation and has reserved a total of 38 million euros for this. The fire at Chemie-Pack started because an employee tried to defrost a frozen pump with a gas burner. The court sentenced three of the company's executives to community service for culpable fire and violation of permit regulations. The appeal in the criminal case will begin on July 30. ©2022 DPG Media B.V. - all rights reserved</t>
+    <t>German train lays new sleepers on line 139 © Erik Roosens © Erik Roosens © Erik Roosens © Erik Roosens Railway manager Infrabel will carry out works on railway line 139 between Heverlee and Sint-Joris-Weert this weekend and next weekend. The P-machine - a giant train - removes the old sleepers and replaces them with new ones. Train traffic will come to a complete standstill during the works. The rail sleepers will be replaced between Ophemstraat and Reigerstraat on the track in the direction of Wavre. For this work, main contractor Strukton Rail had the Strabag renewal train come from Germany to Oud-Heverlee. It removes the old sleepers (biblock) from 1992 from under the tracks and replaces them with sleepers in one piece (monoblock). It concerns a 1600-metre stretch from level crossing 7 (Ophemstraat) to level crossing 8 (Reigerstraat). You can see how that works in this video. At the same time, Infrabel is carrying out other works. Stumbling mats were placed at the level crossing of the Naamsesteenweg in Heverlee to prevent track running and new rails will be installed at the level crossing of the Beekstraat in Sint-Joris-Weert. Due to the works, the level crossings on Ophemstraat and Reigerstraat will be closed until 7 a.m. Monday morning. The level crossing on Reigerstraat will close again from Saturday 12 October (5 a.m.) to Monday 14 October (7 a.m.). The level crossing at Beekstraat from Saturday 12 October (5 a.m.) to Sunday 13 October (4 p.m.). Do you want access to all articles of Het Nieuwsblad? Dive into our plus articles and read 3 of them for free every month. Forget the Red Devils, forget the World Cup in Qatar. From this weekend there will be Sunday games again in the lower leagues. An overview of all scheduled games this weekend (subject to change... At 31 years old, Elien Mattheuwsen is one of the more experienced players of Haasrode Leuven. In five days' time, two confrontations against Asterix Kieldrecht await, with a win as a reward... The next home game of OHL , on December 17 against Club YLA, will be played at the stadium in den Dreef for once. It happened. The women of OH Leuven can still lose. In the quarterfinals of the Belgian Cup, Standard turned out to be 2-0 on Tuesday too strong. To complete the disaster evening, the ... The boys of the regional U21 football team OHL became champions in their series last weekend. Haasrode Leuven continues to string together the victories. The stiff Waremme also proved unable to cope with the at times brisk attacking play from the team from Leuven Thanks to the 0-3 win … The women of Haasrode Leuven continue to look for their first league victory of the season kiss. Despite the win in the first set, they couldn't get off to a good start when visiting Antwerp Ladies... La Louvière broke off the Leuven series of fifteen to fifteen. But the U23 of OHL do not give up. “We have to face it again on Saturday evening against Olympic Charleroi to … Today they are all world stars and they can hardly walk the streets anonymously anymore. But of course our Red Devils also started playing football as a little boy at their … The World Cup fever is now also starting to rise in our region. On Wednesday, our Red Devils will play their first match at the Football World Cup. Of course, various catering establishments … Deaths in Oud-Heverlee. No new deaths have been recently added. Is your loved one not listed on inmemoriam.be or are you looking for additional information? View all jobs</t>
+  </si>
+  <si>
+    <t>Death of construction worker Kees is still unpalatable
+ The client, the municipality of Eindhoven, has never been held accountable. The clock at the International School Eindhoven has stopped forever at ten to two. It is the memory of the fatal accident during the construction of the new wing of the school in December 2012. A day that Maikel Gloudemans often relives. He worked with his father René and uncle Kees for the contractor company that was pouring concrete on the day of the accident. With the permission of the International School, which is hidden in the woods on the Oirschotsedijk, we are going to look in the new building hall where it happened. Maikel points to the height where he stood, together with his father, when the floor collapsed in its entirety. "Suddenly there was a loud noise. The sound of creaking ice. Then you are lying down. That goes very quickly." They fall at least five meters and end up in the rubble. Maikel sustains a back injury, but is able to get up and walk away on his own. His father is also slightly injured. But his 54-year-old uncle Kees was standing one floor below, right under the collapsed ceiling. The men immediately fear the worst. And hours later their fear becomes reality: Kees' dead body is found among the debris. Text continues below the video The death of Kees comes as a blow to the family from Heesch. Kees leaves an adolescent daughter and a wife. What makes it especially unpalatable is that Kees saw the accident coming himself. His widow Hannie says: "Days before the concrete had to be poured, he was brooding at night. Kees was an experienced concrete pourer and did not trust the construction and the calculations. went to work." Kees Gloudemans raises the alarm with the clients up to three times. In vain. Maikel: "We all had that unrest because we actually had no confidence in the construction. We indicated this several times to the clients. But every time the green light came back. Then we started pouring on the basis of confidence. And yes , then it turned out that we were right in our mistrust. But then it was already too late." widow of Kees Gloudemans December 2012 Huibert Borsje, TNO A few weeks after the accident, the whole thing takes a bizarre turn. Even before the investigation into the cause of the accident has been completed, one of the companies involved blames itself. It is Betonson from Son, which is declared bankrupt shortly after the admission of guilt. This event has a major impact on the settlement of the case. Because no party can be held liable, the insurers start a hard battle with the family to pay out as little as possible. And there will be no criminal case to find out where the blame lies. The Public Prosecution Service dismisses the case, which is the normal procedure if the suspect is a bankrupt company. When TNO's conclusions are known, Maikel Gloudemans falls off his chair in surprise. "The wet concrete mass would have been calculated incorrectly. But I am not satisfied with that. That is too simple. It would have been beginner's mistake number one. While we have repeatedly indicated that we believe the calculation was incorrect." Maikel Gloudemans Huibert Borsje, TNO, learning from collapses Because the bankruptcy of Betonson has left no criminal case, the client does not have to explain anything to the municipality of Eindhoven and does not have to pay anything. The same applies to contractor Strukton. For Maikel it feels like a great injustice. He himself is still negotiating with the insurers, who question whether his broken back is related to the accident. And he would like to find out where the responsibility lies. "Betonson and the municipality of Eindhoven</t>
   </si>
   <si>
     <t>Positive initial experiences with low-dust work train Login name Password Remember login ProRail and Voestalpine Railpro have developed a new work train together with industry parties that makes dumping ballast easier and much less dusty. The dust-free unloading train (SALT) was used for the first time during the recent track renewal between Almelo and Mariënberg. With the help of the SALT, Strukton Rail brought 56,000 tons of new ballast into work in a healthy, safer and efficient way. During the unloading of ballast, dust is created that is harmful to railway workers and local residents. The new ballast train is intended to enable rail workers to work in a healthy and sound way from a health and safety point of view. The newly developed installation on the train precipitates the dust with water spray. Wagon owner Voestalpine Railpro and ProRail worked intensively with sector parties to develop this new installation. During the development of the SALT, the rail workers were asked to think about solutions that would make the unloading of ballast with the voestalpine Railpro ballast train safer and less stressful. These have been included in the final design. The unloading of the train is now hydraulically controlled and operated by remote control. Lighting has also been installed on the wagons. According to the inventors, this entails 'an entirely new method of unloading ballast'. Rail workers followed a training to learn how to unload with the SALT. The test was put to the test in Mariënberg. The response to the dust reduction and the new working method was positive. Voestalpine Railpro is now going to convert all its ballast trains into new low-dust unloading trains. Do you want unlimited reading? Take out a promotional subscription now and  get unlimited access to specialist information about the rail market. start promotion subscription Are you already a subscriber? Login Marieke van Gompel is a journalist for SpoorPro and general editor-in-chief of ProMedia Group. Positive action in the context of healthy working and staying healthy! Good thing. Maximum characters left Log in via one of the following social media partners to leave your comment. Register for free and receive the latest news directly by e-mail every week. © 2012–2022 SpoorPro.nl</t>
   </si>
   <si>
-    <t>News overview: This gentleman defrauded a healthcare institution for hundreds of thousands of dollars (and celebrated) After tourists, now also bankers hated in Amsterdam Dagblad Trouw prints an opinion piece. Argument: get rid of bankers. 'Expensively paid system analysts are not backpackers who come to smoke weed for a weekend. But they do contribute to the same problem. The people of Amsterdam no longer know their own city – and are getting less and less chance to do so because they can no longer live there. The charm offensive with which the financial City-aan-de-Amstel is promoted may not be such a good idea. Why don't the remaining European countries concentrate the London exodus on one European city? – someone recently suggested. The City derives its appeal mainly from the fact that all international banks, insurance companies and the like are located together. The race of European capitals for a few crumbs of the cake is then rather counterproductive. Channel everything into one place and you really have an alternative. Only Frankfurt, seat of the European Central Bank, could compete with London.' A sprinter's Porsche Do you remember Brazil? Dafne Schippers wanted to win everything at the Olympic Games, but she only won silver in the 200 meters. Now she is taking revenge and, more muscular than ever, she takes bronze in the 100 meters at the World Cup. That's great, because not even her distance. The reason for the success is a new trainer, say connoisseurs, and her tendency to ignore the outside world, according to de Volkskrant: 'The contrast between the athletics track and the photo studio is enormous. Everything can be polished in advertising campaigns. Schippers hung on meters-high posters in numerous cities of the world, stripped of every unevenness by the wonderful technique of digital image processing: the symbol of athletic perfection in the eyes of its sponsor. 'Schippers seems to be able to separate these different worlds better this year than in the run-up to the Games. The sponsored 2015 Volkswagen Polo may have been swapped for a sponsored Porsche Macan (recommended retail price 131,000 euros), but she has recognized the relativity of glitter and glamour.' Porsche from a healthcare entrepreneur Nice, the FD is also becoming more and more like the Telegraaf. This headline would not have been out of place in the newspaper of the awake and especially angry Netherlands 'Care money for a Porsche.' The text: 'According to the Public Prosecution Service, the director of a care institution for mildly disabled youngsters spent millions of euros in care money in a few years' time on luxury holidays, cars and apartments.' Who is it about? To Darryl Nooitmeer (38) and to his girlfriend. Here in the photo: This Mr. Nooitmeer pulls care institution Vivence, which he takes over from bankruptcy, completely empty with an extreme rent and transferring money to himself and family members. The FD continues: 'While Darryl is still negotiating this settlement, he will become the sole director of ZSV. On paper it is a foundation, but in fact it is a family business. Father, mother, cousins ​​and other (in-law) relatives are on the payroll, without the rest of the staff knowing about it.' Another passage: 'On his Facebook page you can see where that money went. Numerous photos bear witness to luxurious holidays: Darryl playing golf, Darryl with (girlfriend) Dominique in the jungle. Darryl in a helicopter over Hollywood. 'We already found that he was often on holiday as a director,' says a former employee of ZSV. There is no holiday for Darryl for the time being. He will be held until December 8. The FD has made several attempts to ask Darryl for a response. Shortly after the FD had sent a message to its Facebook page, photos on it were removed. There was no response. Almost all of the family members drive a luxury lease car. At the expense of ZSV. Champion lease driver is director Darryl N. himself. He drives a Porsche 911 Targa 4S, an Audi A8 and a BMW i8, each with a purchase price of at least one ton. 'Of course we as staff sometimes asked questions about Darryl's cars. For example, he once drove up to Amsterdam in a car with a driver. But his story was that he had a lot of money because he had sold his ICT company with a lot of profit,' says a former manager of ZSV. The Foundation has since been declared bankrupt. The turnover in 2014 amounted to € 5.4 million, the profit was over 5 tons. Orange coins We can't pay with it in the store, but it does breed that nostalgic golden feeling. The Orange Lionesses get their own currency because they have become European Football Champions. Even more successful women Anouk Vetter has given the Dutch athletics team the first medal at the World Athletics Championships in London. The reigning European champion won bronze in the sold-out Olympic Stadium with 6636 points, an improvement on her Dutch record. Data from at least one hundred thousand lease drivers on the street Have you been wrong on the road? Your boss can check it all out. Personal data of at least one hundred thousand lease drivers are on the street. The security of more than fifty leasing companies was so poor that names, addresses, lease contracts and even fines could be traced. Banks agree with Strukton Strukton's financiers are demanding more control over the construction company. Partly at the insistence of house banks ABN Amro, Rabobank and NIBC, the construction company will have its own supervisory board this year. This can be deduced from the recently published annual report. Furthermore, new financing has been agreed, but only until June next year. This means that Strukton will have to make new credit agreements relatively quickly. With a turnover of €1.9 billion, Strukton is one of the largest Dutch construction companies. In the Netherlands, the company is active in rail and tunnel construction, among other things, and built the A2 tunnel in Maastricht. Abroad, Strukton is involved in projects such as the construction of the metro in Riyadh in Saudi Arabia. Be kind to Baudet Baudet is a relief. Stop character assassination writes @AfshinEllian1 https://t.co/aXmKt6Extt pic.twitter.com/54gJg6CV2G These kitchen trends will sell your home faster 7 kitchen trends that will help get your home sold fast https://t .co/AiZlvMemQP Taylor Swift is going to tackle sexual assault culture Singer Taylor Swift is expected to appear in court this week as a witness in a case that affects her enormously and coincidentally also generates a lot of publicity. Four years ago, a radio presenter said she grabbed her under her dress by the buttocks during a photo shoot. Taylor Swift is not demanding money, well $ 1, but wants to set an example for other women who have been subjected to such "disgraceful and humiliating acts". Just to be clear: the radio host denies everything and demands damages from Swift for defamation. Swift called his boss after the incident, after which he was fired. The police did not call them</t>
+    <t>News overview: This gentleman defrauded a healthcare institution for hundreds of thousands of dollars (and celebrated) After tourists, now also bankers hated in Amsterdam Dagblad Trouw prints an opinion piece. Argument: get rid of bankers. 'Expensively paid system analysts are not backpackers who come to smoke weed for a weekend. But they do contribute to the same problem. The people of Amsterdam no longer know their own city – and are getting less and less chance to do so because they can no longer live there. The charm offensive with which the financial City-aan-de-Amstel is promoted may not be such a good idea. Why don't the remaining European countries concentrate the London exodus on one European city? – someone recently suggested. The City derives its appeal mainly from the fact that all international banks, insurance companies and the like are located together. The race of European capitals for a few crumbs of the cake is then rather counterproductive. Channel everything into one place and you really have an alternative. Only Frankfurt, seat of the European Central Bank, could compete with London.' A sprinter's Porsche Do you remember Brazil? Dafne Schippers wanted to win everything at the Olympic Games, but she only won silver in the 200 meters. Now she is taking revenge and, more muscular than ever, she takes bronze in the 100 meters at the World Cup. That's great, because not even her distance. The reason for the success is a new trainer, say connoisseurs, and her tendency to ignore the outside world, according to de Volkskrant: 'The contrast between the athletics track and the photo studio is enormous. Everything can be polished in advertising campaigns. Schippers hung on meters-high posters in numerous cities of the world, stripped of every unevenness by the wonderful technique of digital image processing: the symbol of athletic perfection in the eyes of its sponsor. 'Schippers seems to be able to separate these different worlds better this year than in the run-up to the Games. The sponsored 2015 Volkswagen Polo may have been swapped for a sponsored Porsche Macan (recommended retail price 131,000 euros), but she has recognized the relativity of glitter and glamour.' Porsche from a healthcare entrepreneur Nice, the FD is also becoming more and more like the Telegraaf. This headline would not have been out of place in the newspaper of the awake and especially angry Netherlands 'Care money for a Porsche.' The text: 'According to the Public Prosecution Service, the director of a care institution for mildly disabled youngsters spent millions of euros in care money in a few years' time on luxury holidays, cars and apartments.' Who is it about? To Darryl Nooitmeer (38) and to his girlfriend. Here in the photo: This Mr. Nooitmeer pulls care institution Vivence, which he takes over from bankruptcy, completely empty with an extreme rent and transferring money to himself and family members. The FD continues: 'While Darryl is still negotiating this settlement, he will become the sole director of ZSV. On paper it is a foundation, but in fact it is a family business. Father, mother, cousins ​​and other (in-law) relatives are on the payroll, without the rest of the staff knowing about it.' Another passage: 'On his Facebook page you can see where that money went. Numerous photos bear witness to luxurious holidays: Darryl playing golf, Darryl with (girlfriend) Dominique in the jungle. Darryl in a helicopter over Hollywood. 'We already found that he was often on holiday as a director,' says a former employee of ZSV. There is no holiday for Darryl for the time being. He will be held until December 8. The FD has made several attempts to ask Darryl for a response. Shortly after the FD had sent a message to its Facebook page, photos on it were removed. There was no reaction. Almost all of the family members drive a luxury lease car. At the expense of ZSV. Champion lease driver is director Darryl N. himself. He drives a Porsche 911 Targa 4S, an Audi A8 and a BMW i8, each with a purchase price of at least one ton. 'Of course we as staff sometimes asked questions about Darryl's cars. For example, he once drove up to Amsterdam in a car with a driver. But his story was that he had a lot of money because he had sold his ICT company with a lot of profit,' says a former manager of ZSV. The Foundation has since been declared bankrupt. The turnover in 2014 amounted to € 5.4 million, the profit was over 5 tons. Orange coins We can't pay with it in the store, but it does breed that nostalgic golden feeling. The Orange Lionesses get their own currency because they have become European Football Champions. Even more successful women Anouk Vetter has given the Dutch athletics team the first medal at the World Athletics Championships in London. The reigning European champion won bronze in the sold-out Olympic Stadium with 6636 points, an improvement on her Dutch record. Data from at least one hundred thousand lease drivers on the street Have you been wrong on the road? Your boss can check it all out. Personal data of at least one hundred thousand lease drivers are on the street. The security of more than fifty leasing companies was so poor that names, addresses, lease contracts and even fines could be traced. Banks agree with Strukton Strukton's financiers are demanding more control over the construction company. Partly at the insistence of house banks ABN Amro, Rabobank and NIBC, the construction company will have its own supervisory board this year. This can be deduced from the recently published annual report. Furthermore, new financing has been agreed, but only until June next year. This means that Strukton will have to make new credit agreements relatively quickly. With a turnover of €1.9 billion, Strukton is one of the largest Dutch construction companies. In the Netherlands, the company is active in rail and tunnel construction, among other things, and built the A2 tunnel in Maastricht. Abroad, Strukton is involved in projects such as the construction of the metro in Riyadh in Saudi Arabia. Be kind to Baudet Baudet is a relief. Stop character assassination writes @AfshinEllian1 https://t.co/aXmKt6Extt pic.twitter.com/54gJg6CV2G These kitchen trends will sell your home faster 7 kitchen trends that will help get your home sold fast https://t .co/AiZlvMemQP Taylor Swift is going to tackle sexual assault culture Singer Taylor Swift is expected to appear in court this week as a witness in a case that affects her enormously and coincidentally also generates a lot of publicity. Four years ago, a radio presenter said she grabbed her under her dress by the buttocks during a photo shoot. Taylor Swift is not demanding money, well $ 1, but wants to set an example for other women who have been subjected to such "disgraceful and humiliating acts". Just to be clear: the radio host denies everything and demands damages from Swift for defamation. Swift called his boss after the incident, after which he was fired. The police did not call them</t>
   </si>
   <si>
     <t>Een giftige cocktail: vier dode kinderen, paniek en House of Cards RTL Nieuws heeft zich na het ongeval in Oss op 20 september verdiept in de toelating van de stint op de Nederlandse wegen. En de manier waarop het ministerie daarna de stint verbood. Dit is onze reconstructie. De overheid is in 2011 gewaarschuwd voor de grote problemen die konden ontstaan met de invoering van de 'bijzondere bromfiets', zoals de elektronische bolderkar stint. Geen toezicht op veiligheid, geen controle, geen handhaving, geen zicht op de ontwikkeling van dit soort voertuigen. Daarom brak op de dag van het dramatisch ongeluk met de stint grote paniek uit op het ministerie en bij de inspectie. De reconstructie van bestuurlijk falen en een politieke cover-up in zes delen. 20 september. Een ongeluk op het spoor in Oss. De bestuurster van een stint raakt de macht over de bolderkar kwijt. Vier kinderen komen om het leven. Er raakt nog een kind zwaargewond, net als de begeleidster. In Oss en heel Nederland is er verdriet en ontreddering. Op het ministerie van Infrastructuur en Waterstaat (IenW) en bij de Inspectie Leefomgeving en Transport (ILT) dringt direct door dat er een probleem is. "Er ontstond grote paniek," zeggen meerdere bronnen. In het verleden zijn inschattingsfouten gemaakt en er zijn waarschuwingen genegeerd. Er zijn documenten achtergehouden en er zijn geen duidelijke regels gemaakt. Er ontstaat paniek. Het eigen falen van ministerie en de inspectie staat in het geheugen gebrand, door de parlementaire enquête naar de Fyra. ''Dat ding moet onmiddellijk de weg af", zegt de senior beleidsmedewerker Verkeersveiligheid op die eerste dag tegen zijn bazen. Minister, secretaris-generaal, directeur-generaal, directeur, beleidsmedewerkers en juristen werken vanaf dat moment aan een witwasoperatie: al het vuil uit het verleden moet zo snel mogelijk, maar goed gedoseerd de deur uit, zodat het niet te veel opvalt.  Er moet snel gehandeld worden, zodat fouten uit het verleden zich niet tegen de huidige minister en ambtenaren keren. Er is voorlopig geen bewijs dat de stint in Oss iets mankeerde. Maar alles wijst erop dat er redenen gevonden moeten worden om de stint zo snel mogelijk van de weg te halen. Ook als dat bestuurlijk of juridisch helemaal niet kan, omdat de bewijsvoering ontbreekt. Om dat mogelijk te maken is gemanipuleerd met bewijsvoering, om voldoende 'twijfel' te zaaien. Dit blijkt uit een reconstructie die RTL Nieuws op basis van geheime stukken, openbare documenten en gesprekken met direct betrokkenen en klokkenluiders heeft gemaakt. Veel informatie is jarenlang niet gegeven aan de Tweede Kamer; ook nu zijn er nog talloze documenten waarover het parlement niet is geïnformeerd, blijkt uit ons onderzoek. Al op die fatale 20ste september maken juristen een 'concept-besluit' om de stint van de weg te halen. Om 16.30 uur ligt een eerste versie klaar. "Het was stuitend", zegt een klokkenluider tegen RTL Nieuws. ''Eigen falen toedekken, alleen maar naar anderen wijzen, proberen het de fabrikant in de schoenen te schuiven, tijd kopen met een onderzoek. En geen enkel gevoel voor de grote problemen die dit weer veroorzaakt bij scholen en de kinderopvang." Het ministerie erkent dat dit document toen al op tafel lag. Het was bedoeld om een 'handelingsperspectief' voor de minister te schetsen. ''Later op de dag bleek dat er geen informatie was om op dat moment tot schorsing over te gaan." ''Het is een giftige cocktail", zegt een goed ingevoerde waarnemer. ''Dode kinderen. Alle emoties die dat losmaakt. Een zwakke minister. Een slecht functionerende inspectie." Wat volgt is een politiek kat-en-muisspel met informatie. House of Cards in Den Haag. De dag na het ongeluk in Oss meldt minister Cora van Nieuwenhuizen aan de Tweede Kamer dat er geen informatie is dat stints onveilig zijn. Achter de schermen is iets anders gaande dan de minister op dat moment doet voorkomen. De Inspectie Leefomgeving en Transport (ILT) is al direct betrokken bij het politieonderzoek naar het ongeval, omdat de ILT onderzoek doet naar veilig vervoer en ongelukken op het spoor. Uit ons onderzoek blijkt dat de ILT er op 20 september opeens achter komt dat deze inspectie zelf ook verantwoordelijk was voor het toezicht op de stint, na een telefoontje van een andere toezichthouder, de Nederlandse Voedsel en Waren Autoriteit, om 12.33 uur. ''Na mijn vraag of het voertuig een kentekenplaat had, kreeg ik het antwoord dat het was goedgekeurd door de RDW (Rijksdienst Wegverkeer)." Conclusie: ''Waarop ik heb aangegeven dat het dan voor ILT is." Op dat moment drong bij de inspectie door dat zij zelf toezicht hadden moeten houden. De inspecteur alarmeert het afdelingshoofd van de afdeling Markttoezicht. De ILT heeft al die jaren geen toezicht gehouden. Daarom gelast de top van de inspectie die dag om 15.00 uur dat een onderzoek wordt ingesteld naar het 'product stint', naar 'informatie van en rondom het verkeersproduct' en 'naar alles wat daaromheen relevant lijkt': ''In dit stadium wordt het van belang geacht direct te handelen." Van Nieuwenhuizen meldt op 21 september het parlement niet dat dit productonderzoek door de ILT is ingesteld. Het ministerie zegt afgelopen zaterdagavond in een formele reactie dat de minister niet wist van dit onderzoek: ''Het was geen onderwerp van gesprek met de minister en derhalve is het niet vermeld in de Kamerbrief." De inspectie laat juist weten dat, hoewel afstemming formeel niet nodig is, bij een ernstig ongeluk als in Oss het ministerie wel op de hoogte wordt gebracht. ''Uiteraard wordt het ministerie in zo'n geval wel geïnformeerd." De minister maakt in de brief van 21 september ook niet duidelijk dat zij op de dag van het ongeluk al een verbod op de stint onderzocht. Ze maakt dan wel de eerste stukken openbaar die de Tweede Kamer daarvóór niet kreeg. Die vrijdagavond maken topambtenaren van het ministerie een WhatsApp-groep aan, voor 'eventuele ontwikkelingen dit weekend'. Krap een week later, op woensdag 26 september, blijkt dat de inspectie sowieso aankoerst op een nader onderzoek. Ook als er geen informatie opduikt dat de stint onveilig is. Dit blijkt uit wat een inspecteur opschrijft, na een gesprek met de Dienst Wegverkeer (RDW), die de stint eerder keurde: ''Hiermee staat voor ILT de mogelijkheid open om een ander gecertificeerd instituut te vragen andere stints objectief te onderzoeken." Zijn teamleider concludeert op dezelfde dag dat een instituut 'op korte termijn het onderzoek naar de stint als product' moet gaan bekijken. In reactie op het onderzoek van RTL Nieuws laat de inspectie ons zaterdagavond weten: ''Al direct nadat door de ILT onderzoek was ingesteld, was op basis van de eerste observaties van de betrokken ILT-inspecteurs duidelijk dat voor het verdere onderzoek externe technische expertise nodig zou zijn." Op maandag 24 september, vier dagen na het ongeval, staat vast dat er een extern onderzoek komt, dat naar verwachting maanden zal duren. ''De ILT heeft vanaf maandag 24 september bezien welke onderzoeksinstituten geëquipeerd zouden zijn om de technische onderzoeken uit te voeren." Daarmee was feitelijk het lot van de stint bezegeld. Het op de weg laten van de stint tijdens zo'n onderzoek naar de veiligheid, lijkt politiek en bestuurlijk uitgesloten. Het aansturen op een aanvullend onderzoek heeft alle kenmerken van een cover-up. De beslissing wordt genomen voordat het NFI een dag later, op donderdag 26 september 'bewijs' vindt dat er problemen zouden kunnen zijn. Nou ja, bewijs… Vorige week meldde RTL Nieuws al dat het ministerie en de ILT selectief citeerden uit dat onderzoek van NFI; dat er slechts met een klein percentage stints een probleem zou kunnen zijn, werd weggelaten. Ook dat dit volgens het NFI eenvoudig te verhelpen viel, werd niet vermeld. Onder druk van de Kamer gaf de minister het stuk een dag later vrij, maar ze vertelde niet waarom niet het hele verhaal was verteld. Ze zei slechts dat er een beeld ontstond dat er sprake was van een onvolledige weergave van feiten, en dat die verwarring niet de bedoeling was. Wat in de officiële NFI-rapportage nergens wordt vermeld, is dat een ILT-inspecteur aanwezig was bij de 'quick scan' naar het onderzoek en dat onderzoek beïnvloedde. De ILT-inspecteur dus, die onvoldoende technische kennis had, en bewijsvoering zocht dat een stint 'op hol' kon slaan, zoals hij later zou schrijven. Het NFI wil geen antwoord geven op onze vraag waarom in het verslag niet staat dat het onderzoek samen met een ILT-inspecteur is gedaan. Het NFI zou het onderzoek uitvoeren voor het strafrechtelijk onderzoek, zodat later de verongelukte stint daarmee kon worden onderzocht. Maar de ILT had een 'quick scan' en een 'werkhypothese' nodig voor het eigen productonderzoek, om de stint van de weg te kunnen halen. Het onderzoek werd gekaapt. Daarmee legt de ILT een rookgordijn en stelt in officiële stukken dat de inspectie door de politie (de opdrachtgever) is geïnformeerd over de resultaten van het NFI-onderzoek, alsof er geen bemoeienis was met dat onderzoek. Het wegpoetsen van – eigen – vingerafdrukken. Het NFI wijst er in de rapportage nog wel fijntjes op dat bij het vervolgonderzoek een rechter-commissaris vooraf deskundigen moet aanwijzen. Het ministerie noemde de quick-scan en de werkhypothese 'verkennend technisch onderzoek'. Vrijwel ieder onderdeel van het feitenrelaas van de ILT, op basis waarvan de stint op 1 oktober werd verboden, blijkt niet te kloppen. Dat geldt bijvoorbeeld voor het gebruikte soldeer in de stint, dat volgens de ILT zou kunnen smelten. Het is de suggestie dat er iets gevaarlijks is, maar dat is onzin. Alle inhoudelijke weerleggingen van de fabrikant, waar de ILT wel over beschikte, worden in het 'feitenrelaas' óf niet vermeld, of doelbewust verdraaid. Terwijl de teamleider van ILT exact beschrijft wat het verweer is. In het nog vertrouwelijke gespreksverslag van 29 en 30 september heeft de jurist van ILT die tegenwerpingen zoveel mogelijk weggelaten. Veel documenten waarop de minister zich baseerde bij haar besluit om de stint van de weg te halen, zijn geheim. Wie preciezer kijkt, snapt waarom. Het gaat om 'persoonlijke waarnemingen' van een medewerker van Strukton, waar Strukton zichzelf van distantieert. Ook is er een onderzoek van een adviesbureau over incidenten met een stint in Delfzijl. Dat onderzoek blijkt te bestaan uit interviews en is geen technisch onderzoek. Ten slotte schermden minister en ILT in het feitenrelaas met een proces-verbaal van bevindingen naar aanleiding van een incident met een stint in Amsterdam; het gaat om dit document. Wat daarna gebeurt, lijkt voer voor de Rijksrecherche. Op 20 september – de dag van Oss – doet een medewerkster van een kinderopvang in Amsterdam bij de politie telefonisch melding van 'rem en stopproblemen' met stints. Ruim een week later, op 28 september, belt een brigadier van de politie Oost-Brabant. De medewerkster vertelt, volgens het proces-verbaal: een stint zou bij het loslaten van het gas geen vaart minderen, de rem zou onvoldoende werken en de bolderkar zou door de sleutel eruit te halen tot stilstand zijn gebracht. Op zaterdag 29 september schrijft de ILT-inspecteur dat hij wordt gebeld door zijn afdelingshoofd die over deze melding zegt dat een stint 'op hol zou zijn geslagen'. Het lijkt de druppel voor de inspectie. Het is de trigger voor spoedoverleg met stint-baas Edwin Renzen, op die zaterdag 29 september. Dit is belangrijk en kan niet wachten, laat de ILT weten. Renzen wordt door de ILT geconfronteerd met het 'op hol slaan' van een stint. Het keert ook terug in een volgend spoedoverleg, op zondag. Renzen herkent zich niet in de melding, want zijn bedrijf was betrokken bij de afhandeling van het incident. Renzen spreekt de directrice van de kinderopvang. Ook die herkent zich niet in de weergave. De directrice laat de ILT die zondagavond weten dat het niet klopt: ''Wat jullie doen is niet onze intentie. Er zijn geen grote incidenten geweest. Voor zover er een verklaring is, trekken wij die in." De ILT wijst door naar de politie. Ook het ministerie wordt op zondagavond 30 september op twee manieren geïnformeerd dat het proces-verbaal niet deugt en van tafel moet. Op 1 oktober om 11.00 uur laat de kinderopvang formeel aan de politie weten dat de verklaring moet worden ingetrokken. En als dat niet wordt gedaan, zal een aanvullende verklaring moeten worden opgenomen, waarin het proces-verbaal sterk zal worden genuanceerd. Ook de suggestie van het op hol slaan moet er uit. De betrokken politiemedewerker zegt dat hij een aanvullende verklaring zal opnemen en dat hij de ILT zal informeren. Die avond zal de minister de stint van de weg laten halen, mede op basis van een proces-verbaal dat onjuist is. Op 3 oktober sluit de politie Oost-Brabant het proces-verbaal, als het officieel wordt overgedragen aan de ILT. 'Aldus naar waarheid opgemaakt'. De aanvullende verklaring staat er niet in; ook niet dat de melding wordt ingetrokken en genuanceerd. Als de Tweede Kamer de minister schriftelijk vraagt of haar ministerie bemoeienis had met deze gang van zaken, antwoordt ze dat de ILT hier contact over had met de politie. Wat de minister er niet bij vertelt, is dat een seniorjurist van haar ministerie voor het kort geding op 18 oktober schriftelijk bij de kinderopvang vraagt om de oorspronkelijke verklaring tóch te mogen gebruiken. Nee, zegt de kinderopvang. In ieder geval niet zonder de aanvullende verklaring. Tijdens het kort geding zwijgt de landsadvocaat wijselijk over het proces-verbaal. Ná het kort geding probeert de jurist van het ministerie het nogmaals: mag de oorspronkelijke verklaring dan worden gebruikt voor het debat van de minister met de Tweede Kamer, op donderdag 1 november? Nee, zegt de kinderopvang. Niet zonder de aanvullende verklaring. Dit weekeinde laat het ministerie RTL Nieuws weten dat er geen aanvullende verklaring bij de politie is. ''Een aanvullende verklaring is ons dus niet bekend." Nee, maar de informatie daarover wel. Vanaf zondagavond 30 september, blijkt uit ons onderzoek. Als de minister de stint per 2 oktober van de weg haalt, wordt gezegd dat de fabrikant wijzigingen doorvoerde die hij had moeten melden. En dat hij die had moeten laten toetsen. Maar dat staat juist niet in de beschikking die de fabrikant in november 2011 van het ministerie kreeg. De stint kreeg in 2014 een zwaardere accu, maar dat was binnen de gestelde technische eisen. Alle experts die RTL Nieuws raadpleegt, zeggen dat de regeling in de Wegenverkeerswet over de bijzondere bromfiets juist geen melding of toetsingsplicht aangeeft. De minister volhardt: ''Wanneer de fabrikant het toegelaten voertuig wijzigt, moet dit altijd worden gemeld bij het ministerie." Uit ons onderzoek blijkt dat datzelfde ministerie in 2017 tegen een fabrikant van een andere 'bijzondere bromfiets' iets anders zegt. Namelijk, dat het 'moeilijk blijft een exacte grens te trekken over wat wel of niet is toegestaan'. Die valt niet te geven. Het hoofd van de afdeling Verkeersveiligheid en Wegvervoer schrijft: ''U moet hier uw eigen verantwoordelijkheid volgen. Zolang de oorspronkelijke constructie geen geweld wordt aangedaan, is er geen probleem." Het ministerie wil verder ook geen overleg met deze fabrikant. Als de veiligheid verbetert, zijn aanpassingen geen probleem. Dit was exact de reden voor de stint om een zwaardere motor te nemen; die remt beter. Dat het ministerie weet dat hier iets niet klopt, blijkt ook uit een brief die het ministerie op 3 oktober naar alle fabrikanten van bijzondere bromfietsen stuurt. Daarin drukt het ministerie de bedrijven op het hart om veranderingen aan het product in het vervolg vooral te melden. Volgens jurist Werner van Bentem, die een kinderopvang in Almere bijstond in een kort geding tegen de minister, is de informatie die de minister aan de Tweede Kamer geeft ronduit misleidend. Het zit hem zo dwars dat hij hier afgelopen donderdag een brief stuurde naar het parlement. Opvallend is dat ook de Landsadvocaat de stelling van de minister niet overneemt Ook dit document is niet openbaar, net zoals het gespreksverslag van 29 en 30 september, waarin ILT aankondigt dat de inspectie maatregelen zal nemen. Maatregelen van ILT en RDW blijven uit, omdat de juridische basis daarvoor niet zorgvuldig kan worden onderbouwd. Er volgt geen 'recall' op last van de RDW. De ILT handhaaft zelf ook niet – de ILT geeft geen formele opdracht aan de fabrikant om alle Stints terug te roepen of stil te zetten. De fabrikant zou zo'n opdracht hebben kunnen aanvechten via de rechter. Daarom besluit de minister 'uit voorzorg' te schorsen, omdat er 'potentiele veiligheidsrisico's' zijn, en er twijfel is over de stint. Tijd dus voor TNO-onderzoek. Het is het begin van het einde van de stint. Wie de paniek en de misleiding wil begrijpen, moet terug naar 2008. Dan geeft een ruime meerderheid in de Tweede Kamer het ministerie de opdracht om de Segway (foto) toe te laten tot het verkeer. Omdat dat strijdig lijkt met Europese regels, verzint het ministerie een oplossing, en wordt de Segway gedoogd. Eigenlijk is een nationale oplossing alleen mogelijk voor een voertuig dat niet harder gaat dan 6 km per uur, op het voetpad. Maar het ministerie komt er achter dat de Europese regels gebruik op de weg 'niet verbieden', althans niet expliciet. Het is niet de bedoeling van Europa, maar als Nederland belooft dat men een 'notificatie' naar Brussel stuurt, is er geen haan die ernaar kraait. Er ontstond de mogelijkheid om 'nationaal iets te regelen'. In 2011 wordt die wetgeving voorbereid. De Rijksdienst voor het Wegverkeer (RDW) krijgt op 5 april 2011 een briefje van het ministerie. De gebruikelijke, grondige typegoedkeuring vervalt, juist omdat het een bijzondere bromfiets is. Of de RDW voortaan wil toetsen aan een paar technische eisen, en klaar. De RDW antwoordt op 27 april 2011. Die brief liegt er niet om. Medewerkers van de RDW hadden het al duidelijk aangegeven tegen het ministerie. Strijdig met de Europese regels, vindt de RDW. Maatregelen om toe te zien op 'conformiteit' van de nieuwe voertuigen ontbreken. De RDW kan maar één voertuig testen. Er is dus geen zicht of controle op het hele productieproces, zoals gebruikelijk. Met andere woorden: na de toelating is er geen kwaliteitscontrole en toezicht. De RDW vroeg om aanpassing van de plannen. Op  4 juli 2011 komt er een antwoord van het ministerie, met excuus voor de late beantwoording. Nee, we gaan de boel niet aanpassen, zegt de directeur Wegen en Verkeersveiligheid. Dit is juist de bedoeling. Het is waar dat controle en toezicht afnemen, en het is waar dat na de toelating de RDW voertuigen niet meer ziet. Er zijn een paar technische eisen gesteld, en that's it: ''Daardoor is er inderdaad minder toezicht door de overheid op bijzondere bromfietsen dan op andere voertuigen." De directeur concludeert: ''Dit risico wordt, gelet op de kleine aantallen, aanvaardbaar geacht." Het alarmerende advies van de RDW wordt al die jaren verzwegen. Het ministerie geeft het stuk ook niet vrij op 21 september, als de minister zegt dat zij na Oss alle feiten op een rij heeft gezet. Het document wordt ook niet vrijgegeven als de minister besluit de stint te schorsen. De correspondentie wordt pas vrijgegeven op 18 oktober 2018, na de rechtszaak over de schorsing, 's avonds – nadat de Tweede Kamer erom heeft gevraagd. Als je terugleest wat de toenmalig minister van Verkeer en Waterstaat in 2008 zei, bij de introductie van de eerste bijzondere bromfiets (de Segway) dan valt eigenlijk alles op zijn plaats: ''Tegelijk moeten wij de zaken wel juridisch kunnen regelen. Mijn ambtgenoot van Justitie heeft in het algemeen overleg ook gesproken over zaken als aansprakelijkheid. Ik heb eerder ook gezegd dat wij, hoe geinig deze nieuwe step ook mag zijn, ook moeten bedenken hoe wij zouden reageren wanneer er ongelukken gaan gebeuren."</t>
-  </si>
-  <si>
-    <t>Preliminary design renovation station Groningen presented By: Editors The preliminary design of the station in Groningen, made by Koen van Velsen architects, was presented on Monday. Strukton Civiel is the company designated as the preferred provider for the major renovations and modifications at and around Groningen station. This means that it is also largely known what the station and its surroundings will look like after the renovation. The design is based on sustainable, robust and reusable materials. Trees and greenery are also given a prominent place. The monumental roofs and the signal box will be retained and will become important again. The new platform covers are inspired by the existing ones and art is given an important place in the pedestrian passage. Old and new form a coherent whole in this design. The plan includes a larger bus station, more and longer train platforms, 8,000 bicycle parking spaces, a bicycle tunnel and a wide pedestrian passage that connects the north and south sides of the city and the extension of the tracks. The aim of the adjustments is that travelers can reach their destination even more comfortably, faster and easier in the future. The Strukton Civiel team includes Koen van Velsen architects, RoyalHaskoningDHV, Robert Jan Vos, TAK restoration architects and artist Gabriel Lester. In addition to price, their tender scored best on criteria such as design, sustainability, limitation of nuisance and connection to monumental parts of the station. The design by Koen van Velsen architects takes as a starting point that Groningen already has a beautiful station building and draws inspiration from this. Alderman Roeland van der Schaaf of the municipality of Groningen is enthusiastic: “Our beautiful main station will soon be even more beautiful and functional. In this way, the southern inhabitants of the city of Groningen will soon be able to reach the city center under the station and the station will have a fully-fledged southern entrance. In addition, our monumental signal box will be given a prominent place and there will soon be plenty of room for bicycles again, completely in line with Groningen as a cycling city.” Work on the station is expected to start in 2020. The tender design will be worked out in more detail in the coming months. The final award is expected at the end of October. It will then be clear whether Strukton Civiel, as the preferred provider, will receive the order definitively. Due to the growth of the economy and the associated increasing demand in the construction industry, a total of 26 million extra budget is needed to get all project components of Groningen Spoorzone implemented. In the coming period, the parties will jointly look for a solution to raise this additional budget. The adjustments to Groningen's main station fall under the Groningen Spoorzone project, part of the Northern Netherlands Railway Plan. For more information: www.groningenspoorzone.nl. Nieuws.nl has been bringing the Dutch news, nationally and locally, from your own municipality since 2002. Sign up now for our newsletter Sign up</t>
-  </si>
-  <si>
-    <t>Riyadh metro megaproject reaches halfway mark Keith Barrow looks at this mammoth project and its potential impact on this rapidly-growing city. The Saudi capital is making rapid progress with its $US 23bn project to build six metro lines by the end of the decade, with construction reaching 50% completion in early 2017. Keith Barrow looks at this mammoth project and its potential impact on this rapidly-growing city. PERHAPS unsurprisingly for the capital city of the world’s largest oil producing nation, the private car has had a defining impact on the urban landscape of Riyadh. In the early 1950s, when Riyadh was home to just 80,000 people, a new planning policy was adopted which designed new residential areas around a grid system, with wide arterial roads linking these expanding communities to the urban core. Over following decades the city continued to expand rapidly, with population growth averaging 8.2% between 1974 and 1992. Riyadh’s population rose from 5.4 million in 2010 to 6.5 million in 2016 and is projected to reach 8.3 million in 2030 - the equivalent of 26 new residents per hour. The High Commission for the Development of Arriyadh has acknowledged that congestion, pollution, and reduced mobility will constrain economic growth unless it takes radical steps to reorganise the transport network and develop a system that works for a much larger city. By 2030, the number of daily car trips is projected to double from 7.4 million to 15 million and the number of hours spent on the city’s roads will climb from 2 million to 4.7 million as the average speed of a journey plummets from 45km/h to 18km/h. The road network is expanding to meet the challenge of a rising population, with more than 1500km of new roads planned by 2030, but in itself this will not be sufficient to prevent gridlock. The solution is to build a sustainable, attractive, world-class public transport network - and build it quickly. By 2019 the King Abdulaziz Project for Riyadh Public Transport will create a 176.7km six-line automated metro network at a cost of nearly $US 23bn, together with a 1230km, 24-line bus network, representing a further investment of $US 4bn. This project - billed as a massive strategic investment in the future of Riyadh - aims to boost public transport’s share of journeys in the city from just 2% to around 20%. In July 2013 Arriyadh Development Authority (ADA) awarded three turnkey design-and-build contracts for the construction of the metro network. By early 2017, this vast undertaking had already reached 50% completion and ADA says it remains on schedule for completion in 2019. The BACS consortium led by Bechtel, and including Aecom, Saudi company Almabani General Contractors, Middle East-based Consolidated Contractors Company, and Siemens, was awarded Package 1, a $US 9.45bn contract for design, construction, rolling stock, signalling, electrification and integration of lines 1 and 2. As E&amp;M partner in BACS, Siemens is supplying 45 four-car Inspiro driverless trains for Line 1 and 29 two-car trains for Line 2, which are being built at the company’s Simmering plant in Vienna, as well as automatic train control systems and electrification for the two lines. Package 2 for the construction of Line 3 is worth $US 5.21bn and was awarded to the Arriyadh New Mobility Group, which is led by Salini Impregilo and includes partners Larsen &amp; Toubro (India), Nesma (Saudi Arabia), Ansaldo STS, Bombardier, Idom (Spain) and WorleyParsons (Australia). Ansaldo STS’ share is worth $US 680m and covers automatic train control (ATC), CBTC, power supplies including third-rail electrification, the operational control centre, telecommunications, and fitting out depots. The contract includes an option for 10 years’ maintenance. Bombardier’s share of the contract is worth $US 383m and includes 47 two-car Innova Metro 300 driverless trains, which are being assembled at the company’s plant in Sahagún, Mexico. In 2015 BACS awarded Larsen &amp; Toubro, India, a $US 161.3m contract to install 62.9km of ballastless track on lines 1 and 2, while Voestalpine is supplying rails and turnouts for the two lines. ThyssenKrupp is supplying 251 elevators and 390 escalators for lines 1 and 2. A joint venture of Parsons, Egis Rail, and Systra was awarded a €425m contract to supervise construction and provide project management services on lines 1, 2, and 3. The $US 7.8bn design-and-build contract for lines 4, 5 and 6 was awarded to the FCC-led Fast consortium, which includes Alstom, Samsung, Freyssinet Saudi Arabia, Strukton, Setec and Typsa. The three lines have a total length of 63.8km (29.8km elevated, 26.6km underground, 8.2km at grade) with 26 stations. Alstom is supplying 69 two-car Metropolis trains, which are being assembled at the company’s plant in Katowice. The company is also supplying its Urbalis communications-based train control (CBTC) system, power supply and its Hesop energy recovery system as part of its e1.2bn contract. Construction supervision services and project management on lines 4, 5, and 6 are the responsibility the Riyadh Advanced Metro Project Execution &amp; Delivery consortium, which comprises Louis Berger and Hill International. Lloyds Register Rail (now Ricardo Rail) was appointed independent safety assessor for all six lines in autumn 2014. In January 2015 ADA awarded Indra a 54-month contract to supply fare collection systems for the metro network and 1000 buses in a deal that includes 10 years’ maintenance. A unified rolling stock design has been adopted for the metro and the three suppliers developed exterior and interior designs for the fleet in collaboration with French design bureau Avant Premiere. The design of the trains was inspired by elements of traditional architecture, with interior and exterior colour schemes appropriate to each line. The metro project includes the construction of 85 stations, including 50 underground, 31 elevated and four at-grade stations. There will be 25 park-and-ride stations and five major interchanges. Seven depots are being built to maintain the rolling stock fleet. ADA has commissioned leading international architects to develop iconic designs for four major stations, which will help to create a distinctive visual identity for the metro. These include King Abdullah Financial District (designed by Zaha Hadid, Britain), Qasr AlHukm (Snohetta, Norway), Western Station (Omrania, Saudi Arabia) and Olaya (Gerber Architekten, Germany). Construction Naturally the logistics of construction reflect the huge scale of the project. ADA has more than 1000 staff working on the project, with 30 nationalities speaking 23 languages. More than 43,000 construction workers are employed on the public transport project, directed from various command centres around the city. Construction activity is scheduled by the hour, around the clock, seven days a week. Infrastructure work includes the excavation of 52km of tunnels using a combination of TBMs, cut-and-cover, and the New Austrian Tunnelling Method. Extensive viaduct construction is also required, and six different construction methods are being used to build the elevated sections of the network, which total 87.4km. On Package 3, the Fast consortium is employing the Full-Span Launching Method (FSLM), the first time this technique has been used in the Middle East. Full-span girders weighing up to 450 tonnes are pre-cast and lifted into a girder carrier, which transports them across the existing spans to a launching gantry, which lifts them into their final position. Fast is installing 256 spans using FSLM. ADA estimates that by the end of the first quarter of 2017, contractors will have excavated 15 million cubic metres of earth, poured nearly three million cubic metres of concrete, and used more 400,000 tonnes of steel. Utilities diversions alone are a vast undertaking - to date ADA has arranged the relocation of more than 170km of power cables, 43km of water mains, 38km of telecoms lines, 18km of sewage pipes and 26km of irrigation channels. So far, the metro project has involved more than 230 million man hours of work. ADA says a key challenge has been unifying the various elements of a complicated and multifaceted contract into a focussed and accountable schedule of deliverables. Before groundbreaking in April 2014, extensive discussions were held with all of the consortia to prepare detailed strategies for the implementation of each construction programme. In addition to its role as project owner, ADA’s responsibilities include facilitating relationships between stakeholders and the organisation manages a wide range of resource issues for the contractors and consultants. ADA’s project office in Oruba employs a matrix system with a ‘one-stop’ work group in direct contact with various stakeholders. Representatives from the Ministry of Transportation, the municipality of Riyadh, the traffic police, and all the various utility companies are seconded to the project offices to enable a rapid and co-ordinated response to any issues. ADA says adding this extra layer of management over the stakeholders and developing empowered teams across seven organisations has been extremely successful and opened the path to the critical scheduling of construction phases. With construction underway simultaneously at hundreds of worksites across the city and significant impacts on the city’s road network, mitigating disruption to communities and businesses has been a paramount consideration and ADA says that from the outset it has aimed for ‘total transparency’ in its communications. As well as engaging the public, ADA also sought to encourage the city’s residents to take ownership of the metro project. The extent of this task reflects the scale and complexity of the metro project and a range of channels including social media and public meetings have been used to establish regular two-way communication with the community. ADA has sought to ensure its call centre phone number is widely known, which enables the escalation of any issues through the organisation’s hierarchy. ADA is encouraging Riyadh’s population to keep looking ahead to the opening of the network, which will have an immediate impact on mobility in the city. Ridership is forecast to reach 1.16 million passengers per day during the initial phase of operation, ultimately increasing to 3.6 million passengers per day. ADA anticipates the metro and bus network will cut car usage by 803 million journeys per year or 10.9 billion vehicle-km. This is expected to reduce the cost of congestion to Riyadh’s economy by around $US 320m per year. ADA calculates that every $US 1 spent on public transport in the city will generate $US 3.40 in economic returns. The public transport project will undoubtedly have a transformative impact on mobility in Riyadh, equipping the city for future growth and achieving in the space of just a few years what many cities have strived for over a period of decades. While few cities could realistically afford to build so much so quickly, Riyadh demonstrates a confidence in public transport that others would do well to emulate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -899,14 +892,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -953,7 +938,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -985,27 +970,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1037,24 +1004,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1230,28 +1179,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J78"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="29.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.21875" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1283,7 +1218,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1291,13 +1226,13 @@
         <v>79</v>
       </c>
       <c r="E2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -1306,71 +1241,71 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3">
-        <v>44474</v>
-      </c>
       <c r="C3" t="s">
         <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H3">
-        <v>0.98799999999999999</v>
+        <v>0.9778</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
       <c r="J3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B4" s="3">
+        <v>44474</v>
+      </c>
       <c r="C4" t="s">
         <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H4">
-        <v>0.97070000000000001</v>
+        <v>0.988</v>
       </c>
       <c r="I4">
         <v>3</v>
       </c>
       <c r="J4">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1381,19 +1316,19 @@
         <v>82</v>
       </c>
       <c r="D5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H5">
-        <v>3.3000000000000002E-2</v>
+        <v>0.033</v>
       </c>
       <c r="I5">
         <v>4</v>
@@ -1402,7 +1337,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1413,60 +1348,60 @@
         <v>83</v>
       </c>
       <c r="D6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F6">
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H6">
-        <v>4.3999999999999997E-2</v>
+        <v>0.044</v>
       </c>
       <c r="I6">
         <v>5</v>
       </c>
       <c r="J6">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="3">
-        <v>44894</v>
+        <v>42863</v>
       </c>
       <c r="C7" t="s">
         <v>84</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H7">
-        <v>3.2000000000000001E-2</v>
+        <v>0.026</v>
       </c>
       <c r="I7">
         <v>6</v>
       </c>
       <c r="J7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1477,289 +1412,277 @@
         <v>85</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H8">
-        <v>0.51219999999999999</v>
+        <v>0.5122</v>
       </c>
       <c r="I8">
         <v>7</v>
       </c>
       <c r="J8">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="3">
-        <v>42863</v>
+        <v>41950</v>
       </c>
       <c r="C9" t="s">
         <v>86</v>
       </c>
       <c r="D9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H9">
-        <v>2.5999999999999999E-2</v>
+        <v>0.038</v>
       </c>
       <c r="I9">
         <v>8</v>
       </c>
       <c r="J9">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="3">
-        <v>41977</v>
+        <v>41879</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H10">
-        <v>5.7000000000000002E-2</v>
+        <v>0.757</v>
       </c>
       <c r="I10">
         <v>9</v>
       </c>
       <c r="J10">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="3">
-        <v>41950</v>
+        <v>44873</v>
       </c>
       <c r="C11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H11">
-        <v>3.7999999999999999E-2</v>
+        <v>0.9973</v>
       </c>
       <c r="I11">
         <v>10</v>
       </c>
       <c r="J11">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="3">
-        <v>41879</v>
-      </c>
       <c r="C12" t="s">
         <v>88</v>
       </c>
-      <c r="D12" t="s">
-        <v>129</v>
-      </c>
       <c r="E12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H12">
-        <v>0.75700000000000001</v>
+        <v>0.003</v>
       </c>
       <c r="I12">
         <v>11</v>
       </c>
       <c r="J12">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="3">
-        <v>44868</v>
-      </c>
       <c r="C13" t="s">
         <v>89</v>
       </c>
-      <c r="D13" t="s">
-        <v>129</v>
-      </c>
       <c r="E13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H13">
-        <v>0.99250000000000005</v>
+        <v>0.9821</v>
       </c>
       <c r="I13">
         <v>12</v>
       </c>
       <c r="J13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="3">
-        <v>44868</v>
-      </c>
       <c r="C14" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="E14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="H14">
-        <v>0.88070000000000004</v>
+        <v>0</v>
       </c>
       <c r="I14">
         <v>13</v>
       </c>
       <c r="J14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C15" t="s">
         <v>90</v>
       </c>
+      <c r="D15" t="s">
+        <v>129</v>
+      </c>
       <c r="E15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>211</v>
-      </c>
-      <c r="H15">
-        <v>3.0000000000000001E-3</v>
+        <v>3</v>
       </c>
       <c r="I15">
         <v>14</v>
       </c>
       <c r="J15">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="B16" s="3">
+        <v>43525</v>
+      </c>
       <c r="C16" t="s">
         <v>91</v>
       </c>
+      <c r="D16" t="s">
+        <v>128</v>
+      </c>
       <c r="E16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H16">
-        <v>0.98209999999999997</v>
+        <v>0.8725000000000001</v>
       </c>
       <c r="I16">
         <v>15</v>
       </c>
       <c r="J16">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>79</v>
+        <v>92</v>
+      </c>
+      <c r="D17" t="s">
+        <v>127</v>
       </c>
       <c r="E17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G17" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>0.2481</v>
       </c>
       <c r="I17">
         <v>16</v>
@@ -1768,364 +1691,376 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="B18" s="3">
+        <v>44873</v>
+      </c>
       <c r="C18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F18">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>211</v>
+      </c>
+      <c r="H18">
+        <v>0.053</v>
       </c>
       <c r="I18">
         <v>17</v>
       </c>
       <c r="J18">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="B19" s="3">
+        <v>44887</v>
+      </c>
       <c r="C19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D19" t="s">
         <v>128</v>
       </c>
       <c r="E19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H19">
-        <v>0.24809999999999999</v>
+        <v>0.029</v>
       </c>
       <c r="I19">
         <v>18</v>
       </c>
       <c r="J19">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B20" s="3">
-        <v>43525</v>
+        <v>44677</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H20">
-        <v>0.87250000000000005</v>
+        <v>0.9968</v>
       </c>
       <c r="I20">
         <v>19</v>
       </c>
       <c r="J20">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B21" s="3">
-        <v>44882</v>
+        <v>43511</v>
       </c>
       <c r="C21" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="D21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H21">
-        <v>2.9000000000000001E-2</v>
+        <v>0.034</v>
       </c>
       <c r="I21">
         <v>20</v>
       </c>
       <c r="J21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="3">
-        <v>44677</v>
+        <v>44873</v>
       </c>
       <c r="C22" t="s">
         <v>96</v>
       </c>
       <c r="D22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H22">
-        <v>0.99680000000000002</v>
+        <v>0.9755</v>
       </c>
       <c r="I22">
         <v>21</v>
       </c>
       <c r="J22">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="3">
-        <v>43511</v>
+        <v>44595</v>
       </c>
       <c r="C23" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="D23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F23">
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H23">
-        <v>3.4000000000000002E-2</v>
+        <v>0.7269</v>
       </c>
       <c r="I23">
         <v>22</v>
       </c>
       <c r="J23">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="3">
-        <v>44868</v>
+        <v>43549</v>
       </c>
       <c r="C24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F24">
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H24">
-        <v>0.97550000000000003</v>
+        <v>0.9905</v>
       </c>
       <c r="I24">
         <v>23</v>
       </c>
       <c r="J24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="3">
-        <v>43549</v>
+        <v>44311</v>
       </c>
       <c r="C25" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D25" t="s">
-        <v>129</v>
-      </c>
-      <c r="E25" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
       <c r="F25">
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H25">
-        <v>0.99050000000000005</v>
+        <v>0.9965000000000001</v>
       </c>
       <c r="I25">
         <v>24</v>
       </c>
       <c r="J25">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B26" s="3">
-        <v>44311</v>
+        <v>44706</v>
       </c>
       <c r="C26" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D26" t="s">
-        <v>129</v>
+        <v>128</v>
+      </c>
+      <c r="E26" t="s">
+        <v>153</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H26">
-        <v>0.99650000000000005</v>
+        <v>0.9983</v>
       </c>
       <c r="I26">
         <v>25</v>
       </c>
       <c r="J26">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B27" s="3">
-        <v>44706</v>
+        <v>44771</v>
       </c>
       <c r="C27" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H27">
-        <v>0.998</v>
+        <v>0.8312</v>
       </c>
       <c r="I27">
         <v>26</v>
       </c>
       <c r="J27">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B28" s="3">
-        <v>44771</v>
+        <v>43392</v>
       </c>
       <c r="C28" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H28">
-        <v>0.83120000000000005</v>
+        <v>0.013</v>
       </c>
       <c r="I28">
         <v>27</v>
       </c>
       <c r="J28">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B29" s="3">
-        <v>44641</v>
+        <v>43132</v>
       </c>
       <c r="C29" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F29">
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -2134,475 +2069,460 @@
         <v>28</v>
       </c>
       <c r="J29">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="2" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="B30" s="3">
-        <v>43392</v>
+        <v>42607</v>
       </c>
       <c r="C30" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="D30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E30" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>224</v>
+        <v>203</v>
       </c>
       <c r="H30">
-        <v>1.2999999999999999E-2</v>
+        <v>0.5122</v>
       </c>
       <c r="I30">
         <v>29</v>
       </c>
       <c r="J30">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" s="3">
-        <v>43132</v>
+        <v>43262</v>
       </c>
       <c r="C31" t="s">
         <v>103</v>
       </c>
       <c r="D31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E31" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>0.037</v>
       </c>
       <c r="I31">
         <v>30</v>
       </c>
       <c r="J31">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="2" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B32" s="3">
-        <v>44868</v>
+        <v>42863</v>
       </c>
       <c r="C32" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E32" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="F32">
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
       <c r="H32">
-        <v>0.99729999999999996</v>
+        <v>0.026</v>
       </c>
       <c r="I32">
         <v>31</v>
       </c>
       <c r="J32">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="2" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B33" s="3">
-        <v>42607</v>
+        <v>42621</v>
       </c>
       <c r="C33" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="D33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E33" t="s">
-        <v>137</v>
+        <v>158</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="H33">
-        <v>0.51219999999999999</v>
+        <v>0.02</v>
       </c>
       <c r="I33">
         <v>32</v>
       </c>
       <c r="J33">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="3">
-        <v>43262</v>
+        <v>42879</v>
       </c>
       <c r="C34" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E34" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F34">
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H34">
-        <v>3.6999999999999998E-2</v>
+        <v>0.025</v>
       </c>
       <c r="I34">
         <v>33</v>
       </c>
       <c r="J34">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B35" s="3">
-        <v>43874</v>
+        <v>42027</v>
       </c>
       <c r="C35" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E35" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F35">
         <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H35">
-        <v>2.4E-2</v>
+        <v>0.029</v>
       </c>
       <c r="I35">
         <v>34</v>
       </c>
       <c r="J35">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" s="2" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B36" s="3">
-        <v>42621</v>
+        <v>41950</v>
       </c>
       <c r="C36" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="D36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E36" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="F36">
         <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
       <c r="H36">
-        <v>0.02</v>
+        <v>0.038</v>
       </c>
       <c r="I36">
         <v>35</v>
       </c>
       <c r="J36">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" s="2" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="B37" s="3">
-        <v>42879</v>
+        <v>44873</v>
       </c>
       <c r="C37" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="D37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E37" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="F37">
         <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="H37">
-        <v>2.5000000000000001E-2</v>
+        <v>0.9973</v>
       </c>
       <c r="I37">
         <v>36</v>
       </c>
       <c r="J37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="B38" s="3">
-        <v>44582</v>
+        <v>44896</v>
       </c>
       <c r="C38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E38" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F38">
         <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="H38">
-        <v>1E-3</v>
+        <v>0.004</v>
       </c>
       <c r="I38">
         <v>37</v>
       </c>
       <c r="J38">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="B39" s="3">
-        <v>42863</v>
+        <v>44873</v>
       </c>
       <c r="C39" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E39" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="F39">
         <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>205</v>
+        <v>228</v>
       </c>
       <c r="H39">
-        <v>2.5999999999999999E-2</v>
+        <v>0.053</v>
       </c>
       <c r="I39">
         <v>38</v>
       </c>
       <c r="J39">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B40" s="3">
-        <v>43613</v>
+        <v>44430</v>
       </c>
       <c r="C40" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="D40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E40" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F40">
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H40">
-        <v>2E-3</v>
+        <v>0.9955000000000001</v>
       </c>
       <c r="I40">
         <v>39</v>
       </c>
       <c r="J40">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B41" s="3">
-        <v>42027</v>
+        <v>45</v>
       </c>
       <c r="C41" t="s">
         <v>109</v>
       </c>
-      <c r="D41" t="s">
-        <v>129</v>
-      </c>
       <c r="E41" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F41">
         <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H41">
-        <v>2.9000000000000001E-2</v>
+        <v>0.054</v>
       </c>
       <c r="I41">
         <v>40</v>
       </c>
       <c r="J41">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="3">
-        <v>41950</v>
+        <v>46</v>
       </c>
       <c r="C42" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="D42" t="s">
         <v>129</v>
       </c>
-      <c r="E42" t="s">
-        <v>140</v>
-      </c>
       <c r="F42">
-        <v>1</v>
-      </c>
-      <c r="G42" t="s">
-        <v>207</v>
-      </c>
-      <c r="H42">
-        <v>3.7999999999999999E-2</v>
+        <v>3</v>
       </c>
       <c r="I42">
         <v>41</v>
       </c>
       <c r="J42">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" s="2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B43" s="3">
-        <v>44868</v>
+        <v>44356</v>
       </c>
       <c r="C43" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="D43" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E43" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="F43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G43" t="s">
-        <v>210</v>
+        <v>231</v>
       </c>
       <c r="H43">
-        <v>0.88070000000000004</v>
+        <v>0.024</v>
       </c>
       <c r="I43">
         <v>42</v>
       </c>
       <c r="J43">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C44" t="s">
-        <v>110</v>
+        <v>112</v>
+      </c>
+      <c r="D44" t="s">
+        <v>127</v>
       </c>
       <c r="E44" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G44" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H44">
-        <v>5.3999999999999999E-2</v>
+        <v>0.01</v>
       </c>
       <c r="I44">
         <v>43</v>
@@ -2611,15 +2531,18 @@
         <v>72</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10">
       <c r="A45" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C45" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D45" t="s">
-        <v>130</v>
+        <v>129</v>
+      </c>
+      <c r="E45" t="s">
+        <v>167</v>
       </c>
       <c r="F45">
         <v>3</v>
@@ -2631,896 +2554,908 @@
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10">
       <c r="A46" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="3">
-        <v>44356</v>
-      </c>
       <c r="C46" t="s">
-        <v>112</v>
-      </c>
-      <c r="D46" t="s">
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="E46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G46" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H46">
-        <v>2.4E-2</v>
+        <v>0.061</v>
       </c>
       <c r="I46">
         <v>45</v>
       </c>
       <c r="J46">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="B47" s="3">
+        <v>44807</v>
+      </c>
       <c r="C47" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D47" t="s">
         <v>128</v>
       </c>
       <c r="E47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G47" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H47">
-        <v>0.01</v>
+        <v>0.9636</v>
       </c>
       <c r="I47">
         <v>46</v>
       </c>
       <c r="J47">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="B48" s="3">
+        <v>44873</v>
+      </c>
       <c r="C48" t="s">
         <v>114</v>
       </c>
       <c r="D48" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F48">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="G48" t="s">
+        <v>235</v>
+      </c>
+      <c r="H48">
+        <v>0.9938</v>
       </c>
       <c r="I48">
         <v>47</v>
       </c>
       <c r="J48">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="B49" s="3">
+        <v>44873</v>
+      </c>
       <c r="C49" t="s">
-        <v>90</v>
+        <v>115</v>
+      </c>
+      <c r="D49" t="s">
+        <v>128</v>
       </c>
       <c r="E49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F49">
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H49">
-        <v>6.0999999999999999E-2</v>
+        <v>0.9772</v>
       </c>
       <c r="I49">
         <v>48</v>
       </c>
       <c r="J49">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B50" s="3">
-        <v>44827</v>
+        <v>44819</v>
       </c>
       <c r="C50" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="D50" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E50" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F50">
         <v>1</v>
       </c>
       <c r="G50" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H50">
-        <v>0.95299999999999996</v>
+        <v>0.019</v>
       </c>
       <c r="I50">
         <v>49</v>
       </c>
       <c r="J50">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B51" s="3">
-        <v>44807</v>
+        <v>44631</v>
       </c>
       <c r="C51" t="s">
         <v>116</v>
       </c>
       <c r="D51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E51" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F51">
         <v>1</v>
       </c>
       <c r="G51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H51">
-        <v>0.96360000000000001</v>
+        <v>0</v>
       </c>
       <c r="I51">
         <v>50</v>
       </c>
       <c r="J51">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B52" s="3">
-        <v>44807</v>
+        <v>44809</v>
       </c>
       <c r="C52" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D52" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E52" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F52">
         <v>1</v>
       </c>
       <c r="G52" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H52">
-        <v>0.97350000000000003</v>
+        <v>0.023</v>
       </c>
       <c r="I52">
         <v>51</v>
       </c>
       <c r="J52">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B53" s="3">
-        <v>44868</v>
+        <v>44195</v>
       </c>
       <c r="C53" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D53" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E53" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F53">
         <v>1</v>
       </c>
       <c r="G53" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H53">
-        <v>0.99380000000000002</v>
+        <v>0.5266999999999999</v>
       </c>
       <c r="I53">
         <v>52</v>
       </c>
       <c r="J53">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B54" s="3">
-        <v>44778</v>
+        <v>43747</v>
       </c>
       <c r="C54" t="s">
         <v>118</v>
       </c>
       <c r="D54" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E54" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F54">
         <v>1</v>
       </c>
       <c r="G54" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H54">
-        <v>1.4999999999999999E-2</v>
+        <v>0.9538</v>
       </c>
       <c r="I54">
         <v>53</v>
       </c>
       <c r="J54">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B55" s="3">
-        <v>44819</v>
+        <v>44630</v>
       </c>
       <c r="C55" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="D55" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E55" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F55">
         <v>1</v>
       </c>
       <c r="G55" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H55">
-        <v>1.9E-2</v>
+        <v>0.9637</v>
       </c>
       <c r="I55">
         <v>54</v>
       </c>
       <c r="J55">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B56" s="3">
-        <v>44809</v>
+        <v>43321</v>
       </c>
       <c r="C56" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D56" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E56" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F56">
         <v>1</v>
       </c>
       <c r="G56" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H56">
-        <v>2.3E-2</v>
+        <v>0.052</v>
       </c>
       <c r="I56">
         <v>55</v>
       </c>
       <c r="J56">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B57" s="3">
-        <v>44195</v>
+        <v>44659</v>
       </c>
       <c r="C57" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D57" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E57" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F57">
         <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H57">
-        <v>0.52669999999999995</v>
+        <v>0.016</v>
       </c>
       <c r="I57">
         <v>56</v>
       </c>
       <c r="J57">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B58" s="3">
-        <v>43321</v>
+        <v>44194</v>
       </c>
       <c r="C58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E58" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F58">
         <v>1</v>
       </c>
       <c r="G58" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H58">
-        <v>5.1999999999999998E-2</v>
+        <v>0.9822</v>
       </c>
       <c r="I58">
         <v>57</v>
       </c>
       <c r="J58">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B59" s="3">
-        <v>44659</v>
+        <v>43910</v>
       </c>
       <c r="C59" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D59" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E59" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F59">
         <v>1</v>
       </c>
       <c r="G59" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H59">
-        <v>1.6E-2</v>
+        <v>0.003</v>
       </c>
       <c r="I59">
         <v>58</v>
       </c>
       <c r="J59">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B60" s="3">
-        <v>42578</v>
+        <v>41965</v>
       </c>
       <c r="C60" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D60" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E60" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F60">
         <v>1</v>
       </c>
       <c r="G60" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H60">
-        <v>1.9E-2</v>
+        <v>0.7966</v>
       </c>
       <c r="I60">
         <v>59</v>
       </c>
       <c r="J60">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B61" s="3">
-        <v>41124</v>
+        <v>43560</v>
       </c>
       <c r="C61" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D61" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E61" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F61">
         <v>1</v>
       </c>
       <c r="G61" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H61">
-        <v>1.4E-2</v>
+        <v>0.035</v>
       </c>
       <c r="I61">
         <v>60</v>
       </c>
       <c r="J61">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B62" s="3">
-        <v>41842</v>
+        <v>41124</v>
       </c>
       <c r="C62" t="s">
         <v>120</v>
       </c>
       <c r="D62" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E62" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F62">
         <v>1</v>
       </c>
       <c r="G62" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H62">
-        <v>2.1999999999999999E-2</v>
+        <v>0.014</v>
       </c>
       <c r="I62">
         <v>61</v>
       </c>
       <c r="J62">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B63" s="3">
-        <v>41198</v>
+        <v>41842</v>
       </c>
       <c r="C63" t="s">
         <v>120</v>
       </c>
       <c r="D63" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E63" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F63">
         <v>1</v>
       </c>
       <c r="G63" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H63">
-        <v>1.0999999999999999E-2</v>
+        <v>0.022</v>
       </c>
       <c r="I63">
         <v>62</v>
       </c>
       <c r="J63">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B64" s="3">
-        <v>41199</v>
+        <v>41198</v>
       </c>
       <c r="C64" t="s">
         <v>120</v>
       </c>
       <c r="D64" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E64" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F64">
         <v>1</v>
       </c>
       <c r="G64" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H64">
-        <v>4.0000000000000001E-3</v>
+        <v>0.011</v>
       </c>
       <c r="I64">
         <v>63</v>
       </c>
       <c r="J64">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B65" s="3">
-        <v>41855</v>
+        <v>41199</v>
       </c>
       <c r="C65" t="s">
         <v>120</v>
       </c>
       <c r="D65" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E65" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F65">
         <v>1</v>
       </c>
       <c r="G65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H65">
-        <v>1.4999999999999999E-2</v>
+        <v>0.004</v>
       </c>
       <c r="I65">
         <v>64</v>
       </c>
       <c r="J65">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B66" s="3">
-        <v>43315</v>
+        <v>41855</v>
       </c>
       <c r="C66" t="s">
         <v>120</v>
       </c>
       <c r="D66" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E66" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F66">
         <v>1</v>
       </c>
       <c r="G66" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H66">
-        <v>1.2E-2</v>
+        <v>0.015</v>
       </c>
       <c r="I66">
         <v>65</v>
       </c>
       <c r="J66">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B67" s="3">
-        <v>41430</v>
+        <v>40847</v>
       </c>
       <c r="C67" t="s">
         <v>123</v>
       </c>
       <c r="D67" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E67" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F67">
         <v>1</v>
       </c>
       <c r="G67" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H67">
-        <v>0.97829999999999995</v>
+        <v>0</v>
       </c>
       <c r="I67">
         <v>66</v>
       </c>
       <c r="J67">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B68" s="3">
-        <v>43744</v>
+        <v>43315</v>
       </c>
       <c r="C68" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D68" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E68" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F68">
         <v>1</v>
       </c>
       <c r="G68" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H68">
-        <v>0.92469999999999997</v>
+        <v>0.012</v>
       </c>
       <c r="I68">
         <v>67</v>
       </c>
       <c r="J68">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B69" s="3">
-        <v>41773</v>
+        <v>41430</v>
       </c>
       <c r="C69" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="D69" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E69" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F69">
         <v>1</v>
       </c>
       <c r="G69" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H69">
-        <v>0.95009999999999994</v>
+        <v>0.9782999999999999</v>
       </c>
       <c r="I69">
         <v>68</v>
       </c>
       <c r="J69">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B70" s="3">
-        <v>42579</v>
+        <v>43744</v>
       </c>
       <c r="C70" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D70" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E70" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F70">
         <v>1</v>
       </c>
       <c r="G70" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H70">
-        <v>1.6E-2</v>
+        <v>0.1017</v>
       </c>
       <c r="I70">
         <v>69</v>
       </c>
       <c r="J70">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B71" s="3">
-        <v>42954</v>
+        <v>44184</v>
       </c>
       <c r="C71" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D71" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E71" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F71">
         <v>1</v>
       </c>
       <c r="G71" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H71">
-        <v>6.7000000000000004E-2</v>
+        <v>0.9987</v>
       </c>
       <c r="I71">
         <v>70</v>
       </c>
       <c r="J71">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
       <c r="A72" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B72" s="3">
-        <v>43402</v>
+        <v>42579</v>
       </c>
       <c r="C72" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D72" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E72" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F72">
         <v>1</v>
       </c>
       <c r="G72" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H72">
-        <v>0.99919999999999998</v>
+        <v>0.016</v>
       </c>
       <c r="I72">
         <v>71</v>
       </c>
       <c r="J72">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
       <c r="A73" s="2" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="B73" s="3">
-        <v>43262</v>
+        <v>42954</v>
       </c>
       <c r="C73" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="D73" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E73" t="s">
-        <v>161</v>
+        <v>195</v>
       </c>
       <c r="F73">
         <v>1</v>
       </c>
       <c r="G73" t="s">
-        <v>227</v>
+        <v>260</v>
       </c>
       <c r="H73">
-        <v>3.6999999999999998E-2</v>
+        <v>0.067</v>
       </c>
       <c r="I73">
         <v>72</v>
       </c>
       <c r="J73">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
       <c r="A74" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B74" s="3">
-        <v>43614</v>
+        <v>43402</v>
       </c>
       <c r="C74" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="D74" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E74" t="s">
         <v>196</v>
@@ -3532,222 +3467,156 @@
         <v>261</v>
       </c>
       <c r="H74">
-        <v>7.0000000000000001E-3</v>
+        <v>0.9992</v>
       </c>
       <c r="I74">
         <v>73</v>
       </c>
       <c r="J74">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
       <c r="A75" s="2" t="s">
-        <v>78</v>
+        <v>15</v>
       </c>
       <c r="B75" s="3">
-        <v>43388</v>
+        <v>42863</v>
       </c>
       <c r="C75" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="D75" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E75" t="s">
-        <v>197</v>
+        <v>135</v>
       </c>
       <c r="F75">
         <v>1</v>
       </c>
       <c r="G75" t="s">
-        <v>262</v>
+        <v>202</v>
       </c>
       <c r="H75">
-        <v>6.0000000000000001E-3</v>
+        <v>0.026</v>
       </c>
       <c r="I75">
         <v>74</v>
       </c>
       <c r="J75">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B76" s="3">
-        <v>43874</v>
+        <v>43262</v>
       </c>
       <c r="C76" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D76" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E76" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F76">
         <v>1</v>
       </c>
       <c r="G76" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="H76">
-        <v>2.4E-2</v>
+        <v>0.037</v>
       </c>
       <c r="I76">
         <v>75</v>
       </c>
       <c r="J76">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A77" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B77" s="3">
-        <v>42863</v>
-      </c>
-      <c r="C77" t="s">
-        <v>86</v>
-      </c>
-      <c r="D77" t="s">
-        <v>129</v>
-      </c>
-      <c r="E77" t="s">
-        <v>138</v>
-      </c>
-      <c r="F77">
-        <v>1</v>
-      </c>
-      <c r="G77" t="s">
-        <v>205</v>
-      </c>
-      <c r="H77">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="I77">
-        <v>76</v>
-      </c>
-      <c r="J77">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A78" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B78" s="3">
-        <v>42027</v>
-      </c>
-      <c r="C78" t="s">
-        <v>109</v>
-      </c>
-      <c r="D78" t="s">
-        <v>129</v>
-      </c>
-      <c r="E78" t="s">
-        <v>167</v>
-      </c>
-      <c r="F78">
-        <v>1</v>
-      </c>
-      <c r="G78" t="s">
-        <v>233</v>
-      </c>
-      <c r="H78">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="I78">
-        <v>77</v>
-      </c>
-      <c r="J78">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="A10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="A11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="A12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="A13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="A14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="A15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="A16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="A17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="A18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="A19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="A20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="A21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="A22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="A23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="A24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="A25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="A26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="A27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="A28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="A29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="A30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="A31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="A32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="A33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="A34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="A35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="A36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="A37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="A38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="A39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="A40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="A41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="A42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="A43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="A44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="A45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="A46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="A47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="A48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="A49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="A50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="A51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="A52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="A53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="A54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="A55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="A56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="A57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="A58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="A59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="A60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="A61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="A62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="A63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="A64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="A65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="A66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="A67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="A68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="A69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="A70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="A71" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="A72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="A73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="A74" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="A75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="A76" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="A77" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="A78" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
+    <hyperlink ref="A10" r:id="rId9"/>
+    <hyperlink ref="A11" r:id="rId10"/>
+    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A13" r:id="rId12"/>
+    <hyperlink ref="A14" r:id="rId13"/>
+    <hyperlink ref="A15" r:id="rId14"/>
+    <hyperlink ref="A16" r:id="rId15"/>
+    <hyperlink ref="A17" r:id="rId16"/>
+    <hyperlink ref="A18" r:id="rId17"/>
+    <hyperlink ref="A19" r:id="rId18"/>
+    <hyperlink ref="A20" r:id="rId19"/>
+    <hyperlink ref="A21" r:id="rId20"/>
+    <hyperlink ref="A22" r:id="rId21"/>
+    <hyperlink ref="A23" r:id="rId22"/>
+    <hyperlink ref="A24" r:id="rId23"/>
+    <hyperlink ref="A25" r:id="rId24"/>
+    <hyperlink ref="A26" r:id="rId25"/>
+    <hyperlink ref="A27" r:id="rId26"/>
+    <hyperlink ref="A28" r:id="rId27"/>
+    <hyperlink ref="A29" r:id="rId28"/>
+    <hyperlink ref="A30" r:id="rId29"/>
+    <hyperlink ref="A31" r:id="rId30"/>
+    <hyperlink ref="A32" r:id="rId31"/>
+    <hyperlink ref="A33" r:id="rId32"/>
+    <hyperlink ref="A34" r:id="rId33"/>
+    <hyperlink ref="A35" r:id="rId34"/>
+    <hyperlink ref="A36" r:id="rId35"/>
+    <hyperlink ref="A37" r:id="rId36"/>
+    <hyperlink ref="A38" r:id="rId37"/>
+    <hyperlink ref="A39" r:id="rId38"/>
+    <hyperlink ref="A40" r:id="rId39"/>
+    <hyperlink ref="A41" r:id="rId40"/>
+    <hyperlink ref="A42" r:id="rId41"/>
+    <hyperlink ref="A43" r:id="rId42"/>
+    <hyperlink ref="A44" r:id="rId43"/>
+    <hyperlink ref="A45" r:id="rId44"/>
+    <hyperlink ref="A46" r:id="rId45"/>
+    <hyperlink ref="A47" r:id="rId46"/>
+    <hyperlink ref="A48" r:id="rId47"/>
+    <hyperlink ref="A49" r:id="rId48"/>
+    <hyperlink ref="A50" r:id="rId49"/>
+    <hyperlink ref="A51" r:id="rId50"/>
+    <hyperlink ref="A52" r:id="rId51"/>
+    <hyperlink ref="A53" r:id="rId52"/>
+    <hyperlink ref="A54" r:id="rId53"/>
+    <hyperlink ref="A55" r:id="rId54"/>
+    <hyperlink ref="A56" r:id="rId55"/>
+    <hyperlink ref="A57" r:id="rId56"/>
+    <hyperlink ref="A58" r:id="rId57"/>
+    <hyperlink ref="A59" r:id="rId58"/>
+    <hyperlink ref="A60" r:id="rId59"/>
+    <hyperlink ref="A61" r:id="rId60"/>
+    <hyperlink ref="A62" r:id="rId61"/>
+    <hyperlink ref="A63" r:id="rId62"/>
+    <hyperlink ref="A64" r:id="rId63"/>
+    <hyperlink ref="A65" r:id="rId64"/>
+    <hyperlink ref="A66" r:id="rId65"/>
+    <hyperlink ref="A67" r:id="rId66"/>
+    <hyperlink ref="A68" r:id="rId67"/>
+    <hyperlink ref="A69" r:id="rId68"/>
+    <hyperlink ref="A70" r:id="rId69"/>
+    <hyperlink ref="A71" r:id="rId70"/>
+    <hyperlink ref="A72" r:id="rId71"/>
+    <hyperlink ref="A73" r:id="rId72"/>
+    <hyperlink ref="A74" r:id="rId73"/>
+    <hyperlink ref="A75" r:id="rId74"/>
+    <hyperlink ref="A76" r:id="rId75"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>